<commit_message>
Norway is empty remove from spreadsheet
</commit_message>
<xml_diff>
--- a/data/spss_files.xlsx
+++ b/data/spss_files.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jarvisc1\Documents\projects\comix_data_clean\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE983EB5-5824-41D2-A4EA-D0D158089072}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A58D775-BFCA-4FA5-B9CD-155E3A347FB6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8175" yWindow="3675" windowWidth="21600" windowHeight="11475" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5340" yWindow="1388" windowWidth="21600" windowHeight="11475" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="5" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="81">
   <si>
     <t>country</t>
   </si>
@@ -265,15 +265,9 @@
     <t>no</t>
   </si>
   <si>
-    <t>20-023770-01_LSHTM_PanelA_NO_Wave1_Final_v1_01052020</t>
-  </si>
-  <si>
     <t xml:space="preserve">20-023770-01_LSHTM_NO_Wave2_Final_v1_29052020_ICUO </t>
   </si>
   <si>
-    <t>20-025859_NO_W3_Final_v1_Intclientuse</t>
-  </si>
-  <si>
     <t xml:space="preserve">20-025859_NO_Wave4_Final_v1_31072020_ICUO </t>
   </si>
   <si>
@@ -284,6 +278,9 @@
   </si>
   <si>
     <t>r_saved</t>
+  </si>
+  <si>
+    <t>Empty</t>
   </si>
 </sst>
 </file>
@@ -651,7 +648,7 @@
         <v>8</v>
       </c>
       <c r="J1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="K1" t="s">
         <v>9</v>
@@ -2033,7 +2030,7 @@
         <v>7</v>
       </c>
       <c r="I1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="J1" t="s">
         <v>9</v>
@@ -2311,7 +2308,7 @@
         <v>8</v>
       </c>
       <c r="J1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="K1" t="s">
         <v>9</v>
@@ -2555,7 +2552,7 @@
   <dimension ref="A1:M7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2589,7 +2586,7 @@
         <v>8</v>
       </c>
       <c r="J1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="K1" t="s">
         <v>9</v>
@@ -2605,6 +2602,9 @@
       <c r="A2" t="s">
         <v>74</v>
       </c>
+      <c r="B2" t="s">
+        <v>80</v>
+      </c>
       <c r="C2">
         <v>1</v>
       </c>
@@ -2616,17 +2616,11 @@
       </c>
       <c r="F2" s="1">
         <v>43952</v>
-      </c>
-      <c r="G2" t="s">
-        <v>75</v>
       </c>
       <c r="H2" t="str">
         <f t="shared" ref="H2:H7" si="0">A2&amp;"_"&amp;"wk"&amp;TEXT(C2,"00")&amp;"_"&amp;YEAR(F2)&amp;TEXT(F2,"MM")&amp;TEXT(F2,"DD")&amp;"_p"&amp;D2&amp;"_wv"&amp;TEXT(E2,"00")&amp;""</f>
         <v>no_wk01_20200501_pA_wv01</v>
       </c>
-      <c r="J2">
-        <v>1</v>
-      </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
@@ -2645,7 +2639,7 @@
         <v>43980</v>
       </c>
       <c r="G3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="H3" t="str">
         <f t="shared" si="0"/>
@@ -2659,6 +2653,9 @@
       <c r="A4" t="s">
         <v>74</v>
       </c>
+      <c r="B4" t="s">
+        <v>80</v>
+      </c>
       <c r="C4">
         <v>5</v>
       </c>
@@ -2671,15 +2668,9 @@
       <c r="F4" s="1">
         <v>44004</v>
       </c>
-      <c r="G4" t="s">
-        <v>77</v>
-      </c>
       <c r="H4" t="str">
         <f t="shared" si="0"/>
         <v>no_wk05_20200622_pA_wv03</v>
-      </c>
-      <c r="J4">
-        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.45">
@@ -2700,7 +2691,7 @@
         <v>44043</v>
       </c>
       <c r="G5" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="H5" t="str">
         <f t="shared" si="0"/>
@@ -2728,7 +2719,7 @@
         <v>44080</v>
       </c>
       <c r="G6" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="H6" t="str">
         <f t="shared" si="0"/>
@@ -2756,7 +2747,7 @@
         <v>44105</v>
       </c>
       <c r="G7" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="H7" t="str">
         <f t="shared" si="0"/>

</xml_diff>

<commit_message>
Update to run all and for this weeks data
</commit_message>
<xml_diff>
--- a/data/spss_files.xlsx
+++ b/data/spss_files.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jarvisc1\Documents\projects\comix_data_clean\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A58D775-BFCA-4FA5-B9CD-155E3A347FB6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBDF8EF8-FCC0-422F-A25C-EC5EA0F1B37F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5340" yWindow="1388" windowWidth="21600" windowHeight="11475" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="83">
   <si>
     <t>country</t>
   </si>
@@ -280,7 +280,13 @@
     <t>r_saved</t>
   </si>
   <si>
-    <t>Empty</t>
+    <t>20-023770-01_LSHTM_PanelA_NO_Wave1_Final_v1_01052020</t>
+  </si>
+  <si>
+    <t>20-025859_NO_W3_Final_v1_Intclientuse</t>
+  </si>
+  <si>
+    <t>20-040199-01_Final_PEW7_v1_061120_Intclientuse</t>
   </si>
 </sst>
 </file>
@@ -613,11 +619,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M52"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+    <sheetView topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="J44" sqref="J44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="6" max="6" width="10.19921875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="58.265625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="25.33203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
@@ -680,8 +691,11 @@
         <v>14</v>
       </c>
       <c r="H2" t="str">
-        <f t="shared" ref="H2:H43" si="0">A2&amp;"_"&amp;"wk"&amp;TEXT(C2,"00")&amp;"_"&amp;YEAR(F2)&amp;TEXT(F2,"MM")&amp;TEXT(F2,"DD")&amp;"_p"&amp;D2&amp;"_wv"&amp;TEXT(E2,"00")&amp;""</f>
+        <f t="shared" ref="H2:H44" si="0">A2&amp;"_"&amp;"wk"&amp;TEXT(C2,"00")&amp;"_"&amp;YEAR(F2)&amp;TEXT(F2,"MM")&amp;TEXT(F2,"DD")&amp;"_p"&amp;D2&amp;"_wv"&amp;TEXT(E2,"00")&amp;""</f>
         <v>uk_wk01_20200402_pA_wv01</v>
+      </c>
+      <c r="I2">
+        <v>1</v>
       </c>
       <c r="J2">
         <v>1</v>
@@ -710,6 +724,9 @@
         <f t="shared" si="0"/>
         <v>uk_wk02_20200214_pB_wv01</v>
       </c>
+      <c r="I3">
+        <v>1</v>
+      </c>
       <c r="J3">
         <v>1</v>
       </c>
@@ -737,6 +754,9 @@
         <f t="shared" si="0"/>
         <v>uk_wk03_20200513_pA_wv02</v>
       </c>
+      <c r="I4">
+        <v>1</v>
+      </c>
       <c r="J4">
         <v>1</v>
       </c>
@@ -764,6 +784,9 @@
         <f t="shared" si="0"/>
         <v>uk_wk04_20200427_pB_wv02</v>
       </c>
+      <c r="I5">
+        <v>1</v>
+      </c>
       <c r="J5">
         <v>1</v>
       </c>
@@ -791,6 +814,9 @@
         <f t="shared" si="0"/>
         <v>uk_wk05_20200428_pA_wv03</v>
       </c>
+      <c r="I6">
+        <v>1</v>
+      </c>
       <c r="J6">
         <v>1</v>
       </c>
@@ -818,6 +844,9 @@
         <f t="shared" si="0"/>
         <v>uk_wk06_20200512_pB_wv03</v>
       </c>
+      <c r="I7">
+        <v>1</v>
+      </c>
       <c r="J7">
         <v>1</v>
       </c>
@@ -848,6 +877,9 @@
         <f t="shared" si="0"/>
         <v>uk_wk07_20200513_pA_wv04</v>
       </c>
+      <c r="I8">
+        <v>1</v>
+      </c>
       <c r="J8">
         <v>1</v>
       </c>
@@ -874,6 +906,9 @@
       <c r="H9" t="str">
         <f t="shared" si="0"/>
         <v>uk_wk07_20200519_pC_wv01</v>
+      </c>
+      <c r="I9">
+        <v>1</v>
       </c>
       <c r="J9">
         <v>1</v>
@@ -903,6 +938,9 @@
         <f t="shared" si="0"/>
         <v>uk_wk08_20200522_pB_wv04</v>
       </c>
+      <c r="I10">
+        <v>1</v>
+      </c>
       <c r="J10">
         <v>1</v>
       </c>
@@ -931,6 +969,9 @@
         <f t="shared" si="0"/>
         <v>uk_wk08_20200611_pD_wv01</v>
       </c>
+      <c r="I11">
+        <v>1</v>
+      </c>
       <c r="J11">
         <v>1</v>
       </c>
@@ -959,6 +1000,9 @@
         <f t="shared" si="0"/>
         <v>uk_wk09_20200529_pA_wv05</v>
       </c>
+      <c r="I12">
+        <v>1</v>
+      </c>
       <c r="J12">
         <v>1</v>
       </c>
@@ -988,6 +1032,9 @@
         <f t="shared" si="0"/>
         <v>uk_wk09_20200528_pC_wv02</v>
       </c>
+      <c r="I13">
+        <v>1</v>
+      </c>
       <c r="J13">
         <v>1</v>
       </c>
@@ -1016,6 +1063,9 @@
         <f t="shared" si="0"/>
         <v>uk_wk10_20200604_pB_wv05</v>
       </c>
+      <c r="I14">
+        <v>1</v>
+      </c>
       <c r="J14">
         <v>1</v>
       </c>
@@ -1044,6 +1094,9 @@
         <f t="shared" si="0"/>
         <v>uk_wk10_20200608_pD_wv02</v>
       </c>
+      <c r="I15">
+        <v>1</v>
+      </c>
       <c r="J15">
         <v>1</v>
       </c>
@@ -1072,6 +1125,9 @@
         <f t="shared" si="0"/>
         <v>uk_wk11_20200612_pA_wv06</v>
       </c>
+      <c r="I16">
+        <v>1</v>
+      </c>
       <c r="J16">
         <v>1</v>
       </c>
@@ -1100,6 +1156,9 @@
         <f t="shared" si="0"/>
         <v>uk_wk11_20200612_pC_wv03</v>
       </c>
+      <c r="I17">
+        <v>1</v>
+      </c>
       <c r="J17">
         <v>1</v>
       </c>
@@ -1128,6 +1187,9 @@
         <f t="shared" si="0"/>
         <v>uk_wk12_20200619_pB_wv06</v>
       </c>
+      <c r="I18">
+        <v>1</v>
+      </c>
       <c r="J18">
         <v>1</v>
       </c>
@@ -1156,6 +1218,9 @@
         <f t="shared" si="0"/>
         <v>uk_wk12_20200619_pD_wv03</v>
       </c>
+      <c r="I19">
+        <v>1</v>
+      </c>
       <c r="J19">
         <v>1</v>
       </c>
@@ -1184,6 +1249,9 @@
         <f t="shared" si="0"/>
         <v>uk_wk13_20200625_pA_wv07</v>
       </c>
+      <c r="I20">
+        <v>1</v>
+      </c>
       <c r="J20">
         <v>1</v>
       </c>
@@ -1211,6 +1279,9 @@
       <c r="H21" t="str">
         <f t="shared" si="0"/>
         <v>uk_wk13_20200625_pC_wv04</v>
+      </c>
+      <c r="I21">
+        <v>1</v>
       </c>
       <c r="J21">
         <v>1</v>
@@ -1240,6 +1311,9 @@
         <f t="shared" si="0"/>
         <v>uk_wk14_20200702_pB_wv07</v>
       </c>
+      <c r="I22">
+        <v>1</v>
+      </c>
       <c r="J22">
         <v>1</v>
       </c>
@@ -1268,6 +1342,9 @@
         <f t="shared" si="0"/>
         <v>uk_wk14_20200703_pD_wv04</v>
       </c>
+      <c r="I23">
+        <v>1</v>
+      </c>
       <c r="J23">
         <v>1</v>
       </c>
@@ -1296,6 +1373,9 @@
         <f t="shared" si="0"/>
         <v>uk_wk15_20200710_pA_wv08</v>
       </c>
+      <c r="I24">
+        <v>1</v>
+      </c>
       <c r="J24">
         <v>1</v>
       </c>
@@ -1324,6 +1404,9 @@
         <f t="shared" si="0"/>
         <v>uk_wk15_20200709_pC_wv05</v>
       </c>
+      <c r="I25">
+        <v>1</v>
+      </c>
       <c r="J25">
         <v>1</v>
       </c>
@@ -1352,6 +1435,9 @@
         <f t="shared" si="0"/>
         <v>uk_wk16_20200717_pB_wv08</v>
       </c>
+      <c r="I26">
+        <v>1</v>
+      </c>
       <c r="J26">
         <v>1</v>
       </c>
@@ -1380,6 +1466,9 @@
         <f t="shared" si="0"/>
         <v>uk_wk16_20200717_pD_wv05</v>
       </c>
+      <c r="I27">
+        <v>1</v>
+      </c>
       <c r="J27">
         <v>1</v>
       </c>
@@ -1411,6 +1500,9 @@
         <f t="shared" si="0"/>
         <v>uk_wk17_20200724_pA_wv09</v>
       </c>
+      <c r="I28">
+        <v>1</v>
+      </c>
       <c r="J28">
         <v>1</v>
       </c>
@@ -1442,6 +1534,9 @@
         <f t="shared" si="0"/>
         <v>uk_wk18_20200731_pB_wv09</v>
       </c>
+      <c r="I29">
+        <v>1</v>
+      </c>
       <c r="J29">
         <v>1</v>
       </c>
@@ -1470,6 +1565,9 @@
         <f t="shared" si="0"/>
         <v>uk_wk19_20200807_pA_wv10</v>
       </c>
+      <c r="I30">
+        <v>1</v>
+      </c>
       <c r="J30">
         <v>1</v>
       </c>
@@ -1497,6 +1595,9 @@
         <f t="shared" si="0"/>
         <v>uk_wk19_20200810_pC_wv06</v>
       </c>
+      <c r="I31">
+        <v>1</v>
+      </c>
       <c r="J31">
         <v>1</v>
       </c>
@@ -1527,6 +1628,9 @@
         <f t="shared" si="0"/>
         <v>uk_wk20_20200821_pE_wv01</v>
       </c>
+      <c r="I32">
+        <v>1</v>
+      </c>
       <c r="J32">
         <v>1</v>
       </c>
@@ -1553,6 +1657,9 @@
       <c r="H33" t="str">
         <f t="shared" si="0"/>
         <v>uk_wk21_20200827_pF_wv01</v>
+      </c>
+      <c r="I33">
+        <v>1</v>
       </c>
       <c r="J33">
         <v>1</v>
@@ -1582,6 +1689,9 @@
         <f t="shared" si="0"/>
         <v>uk_wk22_20200903_pE_wv02</v>
       </c>
+      <c r="I34">
+        <v>1</v>
+      </c>
       <c r="J34">
         <v>1</v>
       </c>
@@ -1610,6 +1720,9 @@
         <f t="shared" si="0"/>
         <v>uk_wk23_20200907_pF_wv02</v>
       </c>
+      <c r="I35">
+        <v>1</v>
+      </c>
       <c r="J35">
         <v>1</v>
       </c>
@@ -1638,6 +1751,9 @@
         <f t="shared" si="0"/>
         <v>uk_wk24_20200914_pE_wv03</v>
       </c>
+      <c r="I36">
+        <v>1</v>
+      </c>
       <c r="J36">
         <v>1</v>
       </c>
@@ -1666,6 +1782,9 @@
         <f t="shared" si="0"/>
         <v>uk_wk25_20200918_pF_wv03</v>
       </c>
+      <c r="I37">
+        <v>1</v>
+      </c>
       <c r="J37">
         <v>1</v>
       </c>
@@ -1694,6 +1813,9 @@
         <f t="shared" si="0"/>
         <v>uk_wk26_20200925_pE_wv04</v>
       </c>
+      <c r="I38">
+        <v>1</v>
+      </c>
       <c r="J38">
         <v>1</v>
       </c>
@@ -1722,6 +1844,9 @@
         <f t="shared" si="0"/>
         <v>uk_wk27_20201002_pF_wv04</v>
       </c>
+      <c r="I39">
+        <v>1</v>
+      </c>
       <c r="J39">
         <v>1</v>
       </c>
@@ -1750,6 +1875,9 @@
         <f t="shared" si="0"/>
         <v>uk_wk28_20201009_pE_wv05</v>
       </c>
+      <c r="I40">
+        <v>1</v>
+      </c>
       <c r="J40">
         <v>1</v>
       </c>
@@ -1778,6 +1906,9 @@
         <f t="shared" si="0"/>
         <v>uk_wk29_20201018_pF_wv05</v>
       </c>
+      <c r="I41">
+        <v>1</v>
+      </c>
       <c r="J41">
         <v>1</v>
       </c>
@@ -1806,6 +1937,9 @@
         <f t="shared" si="0"/>
         <v>uk_wk30_20201023_pE_wv06</v>
       </c>
+      <c r="I42">
+        <v>1</v>
+      </c>
       <c r="J42">
         <v>1</v>
       </c>
@@ -1834,6 +1968,9 @@
         <f t="shared" si="0"/>
         <v>uk_wk31_20201030_pF_wv06</v>
       </c>
+      <c r="I43">
+        <v>1</v>
+      </c>
       <c r="J43">
         <v>1</v>
       </c>
@@ -1852,7 +1989,19 @@
         <f t="shared" si="4"/>
         <v>7</v>
       </c>
-      <c r="F44" s="1"/>
+      <c r="F44" s="1">
+        <v>44141</v>
+      </c>
+      <c r="G44" t="s">
+        <v>82</v>
+      </c>
+      <c r="H44" t="str">
+        <f t="shared" si="0"/>
+        <v>uk_wk32_20201106_pE_wv07</v>
+      </c>
+      <c r="I44">
+        <v>1</v>
+      </c>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A45" t="s">
@@ -2552,7 +2701,7 @@
   <dimension ref="A1:M7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2602,9 +2751,6 @@
       <c r="A2" t="s">
         <v>74</v>
       </c>
-      <c r="B2" t="s">
-        <v>80</v>
-      </c>
       <c r="C2">
         <v>1</v>
       </c>
@@ -2616,6 +2762,9 @@
       </c>
       <c r="F2" s="1">
         <v>43952</v>
+      </c>
+      <c r="G2" t="s">
+        <v>80</v>
       </c>
       <c r="H2" t="str">
         <f t="shared" ref="H2:H7" si="0">A2&amp;"_"&amp;"wk"&amp;TEXT(C2,"00")&amp;"_"&amp;YEAR(F2)&amp;TEXT(F2,"MM")&amp;TEXT(F2,"DD")&amp;"_p"&amp;D2&amp;"_wv"&amp;TEXT(E2,"00")&amp;""</f>
@@ -2653,9 +2802,6 @@
       <c r="A4" t="s">
         <v>74</v>
       </c>
-      <c r="B4" t="s">
-        <v>80</v>
-      </c>
       <c r="C4">
         <v>5</v>
       </c>
@@ -2667,6 +2813,9 @@
       </c>
       <c r="F4" s="1">
         <v>44004</v>
+      </c>
+      <c r="G4" t="s">
+        <v>81</v>
       </c>
       <c r="H4" t="str">
         <f t="shared" si="0"/>

</xml_diff>

<commit_message>
Add latest data to spss_file
</commit_message>
<xml_diff>
--- a/data/spss_files.xlsx
+++ b/data/spss_files.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jarvisc1\Documents\projects\comix_data_clean\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{939F16FA-BDAF-45F4-8AA2-A14CFAFDFE65}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC814162-C190-4260-8961-EDC8F728AEF6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="5" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="86">
   <si>
     <t>country</t>
   </si>
@@ -293,6 +293,9 @@
   </si>
   <si>
     <t>locked</t>
+  </si>
+  <si>
+    <t>20-056790_Final_PFW7_v1_IntUse</t>
   </si>
 </sst>
 </file>
@@ -625,8 +628,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O52"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="A45" sqref="A45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -711,7 +714,7 @@
         <v>14</v>
       </c>
       <c r="I2" t="str">
-        <f>C2&amp;"_"&amp;"wk"&amp;TEXT(D2,"00")&amp;"_"&amp;YEAR(G2)&amp;TEXT(G2,"MM")&amp;TEXT(G2,"DD")&amp;"_p"&amp;E2&amp;"_wv"&amp;TEXT(F2,"00")&amp;""</f>
+        <f t="shared" ref="I2:I45" si="0">C2&amp;"_"&amp;"wk"&amp;TEXT(D2,"00")&amp;"_"&amp;YEAR(G2)&amp;TEXT(G2,"MM")&amp;TEXT(G2,"DD")&amp;"_p"&amp;E2&amp;"_wv"&amp;TEXT(F2,"00")&amp;""</f>
         <v>uk_wk01_20200402_pA_wv01</v>
       </c>
       <c r="J2">
@@ -747,7 +750,7 @@
         <v>16</v>
       </c>
       <c r="I3" t="str">
-        <f>C3&amp;"_"&amp;"wk"&amp;TEXT(D3,"00")&amp;"_"&amp;YEAR(G3)&amp;TEXT(G3,"MM")&amp;TEXT(G3,"DD")&amp;"_p"&amp;E3&amp;"_wv"&amp;TEXT(F3,"00")&amp;""</f>
+        <f t="shared" si="0"/>
         <v>uk_wk02_20200214_pB_wv01</v>
       </c>
       <c r="J3">
@@ -783,7 +786,7 @@
         <v>17</v>
       </c>
       <c r="I4" t="str">
-        <f>C4&amp;"_"&amp;"wk"&amp;TEXT(D4,"00")&amp;"_"&amp;YEAR(G4)&amp;TEXT(G4,"MM")&amp;TEXT(G4,"DD")&amp;"_p"&amp;E4&amp;"_wv"&amp;TEXT(F4,"00")&amp;""</f>
+        <f t="shared" si="0"/>
         <v>uk_wk03_20200513_pA_wv02</v>
       </c>
       <c r="J4">
@@ -819,7 +822,7 @@
         <v>18</v>
       </c>
       <c r="I5" t="str">
-        <f>C5&amp;"_"&amp;"wk"&amp;TEXT(D5,"00")&amp;"_"&amp;YEAR(G5)&amp;TEXT(G5,"MM")&amp;TEXT(G5,"DD")&amp;"_p"&amp;E5&amp;"_wv"&amp;TEXT(F5,"00")&amp;""</f>
+        <f t="shared" si="0"/>
         <v>uk_wk04_20200427_pB_wv02</v>
       </c>
       <c r="J5">
@@ -855,7 +858,7 @@
         <v>19</v>
       </c>
       <c r="I6" t="str">
-        <f>C6&amp;"_"&amp;"wk"&amp;TEXT(D6,"00")&amp;"_"&amp;YEAR(G6)&amp;TEXT(G6,"MM")&amp;TEXT(G6,"DD")&amp;"_p"&amp;E6&amp;"_wv"&amp;TEXT(F6,"00")&amp;""</f>
+        <f t="shared" si="0"/>
         <v>uk_wk05_20200428_pA_wv03</v>
       </c>
       <c r="J6">
@@ -891,7 +894,7 @@
         <v>20</v>
       </c>
       <c r="I7" t="str">
-        <f>C7&amp;"_"&amp;"wk"&amp;TEXT(D7,"00")&amp;"_"&amp;YEAR(G7)&amp;TEXT(G7,"MM")&amp;TEXT(G7,"DD")&amp;"_p"&amp;E7&amp;"_wv"&amp;TEXT(F7,"00")&amp;""</f>
+        <f t="shared" si="0"/>
         <v>uk_wk06_20200512_pB_wv03</v>
       </c>
       <c r="J7">
@@ -927,7 +930,7 @@
         <v>22</v>
       </c>
       <c r="I8" t="str">
-        <f>C8&amp;"_"&amp;"wk"&amp;TEXT(D8,"00")&amp;"_"&amp;YEAR(G8)&amp;TEXT(G8,"MM")&amp;TEXT(G8,"DD")&amp;"_p"&amp;E8&amp;"_wv"&amp;TEXT(F8,"00")&amp;""</f>
+        <f t="shared" si="0"/>
         <v>uk_wk07_20200513_pA_wv04</v>
       </c>
       <c r="J8">
@@ -966,7 +969,7 @@
         <v>24</v>
       </c>
       <c r="I9" t="str">
-        <f>C9&amp;"_"&amp;"wk"&amp;TEXT(D9,"00")&amp;"_"&amp;YEAR(G9)&amp;TEXT(G9,"MM")&amp;TEXT(G9,"DD")&amp;"_p"&amp;E9&amp;"_wv"&amp;TEXT(F9,"00")&amp;""</f>
+        <f t="shared" si="0"/>
         <v>uk_wk07_20200519_pC_wv01</v>
       </c>
       <c r="J9">
@@ -1003,7 +1006,7 @@
         <v>25</v>
       </c>
       <c r="I10" t="str">
-        <f>C10&amp;"_"&amp;"wk"&amp;TEXT(D10,"00")&amp;"_"&amp;YEAR(G10)&amp;TEXT(G10,"MM")&amp;TEXT(G10,"DD")&amp;"_p"&amp;E10&amp;"_wv"&amp;TEXT(F10,"00")&amp;""</f>
+        <f t="shared" si="0"/>
         <v>uk_wk08_20200522_pB_wv04</v>
       </c>
       <c r="J10">
@@ -1040,7 +1043,7 @@
         <v>27</v>
       </c>
       <c r="I11" t="str">
-        <f>C11&amp;"_"&amp;"wk"&amp;TEXT(D11,"00")&amp;"_"&amp;YEAR(G11)&amp;TEXT(G11,"MM")&amp;TEXT(G11,"DD")&amp;"_p"&amp;E11&amp;"_wv"&amp;TEXT(F11,"00")&amp;""</f>
+        <f t="shared" si="0"/>
         <v>uk_wk08_20200611_pD_wv01</v>
       </c>
       <c r="J11">
@@ -1061,7 +1064,7 @@
         <v>12</v>
       </c>
       <c r="D12">
-        <f t="shared" ref="D12:D21" si="0">D10+1</f>
+        <f t="shared" ref="D12:D21" si="1">D10+1</f>
         <v>9</v>
       </c>
       <c r="E12" t="s">
@@ -1077,7 +1080,7 @@
         <v>28</v>
       </c>
       <c r="I12" t="str">
-        <f>C12&amp;"_"&amp;"wk"&amp;TEXT(D12,"00")&amp;"_"&amp;YEAR(G12)&amp;TEXT(G12,"MM")&amp;TEXT(G12,"DD")&amp;"_p"&amp;E12&amp;"_wv"&amp;TEXT(F12,"00")&amp;""</f>
+        <f t="shared" si="0"/>
         <v>uk_wk09_20200529_pA_wv05</v>
       </c>
       <c r="J12">
@@ -1098,7 +1101,7 @@
         <v>12</v>
       </c>
       <c r="D13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>9</v>
       </c>
       <c r="E13" t="s">
@@ -1108,14 +1111,14 @@
         <v>2</v>
       </c>
       <c r="G13" s="1">
-        <f t="shared" ref="G13" si="1">G14-7</f>
+        <f t="shared" ref="G13" si="2">G14-7</f>
         <v>43979</v>
       </c>
       <c r="H13" t="s">
         <v>29</v>
       </c>
       <c r="I13" t="str">
-        <f>C13&amp;"_"&amp;"wk"&amp;TEXT(D13,"00")&amp;"_"&amp;YEAR(G13)&amp;TEXT(G13,"MM")&amp;TEXT(G13,"DD")&amp;"_p"&amp;E13&amp;"_wv"&amp;TEXT(F13,"00")&amp;""</f>
+        <f t="shared" si="0"/>
         <v>uk_wk09_20200528_pC_wv02</v>
       </c>
       <c r="J13">
@@ -1136,7 +1139,7 @@
         <v>12</v>
       </c>
       <c r="D14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>10</v>
       </c>
       <c r="E14" t="s">
@@ -1152,7 +1155,7 @@
         <v>30</v>
       </c>
       <c r="I14" t="str">
-        <f>C14&amp;"_"&amp;"wk"&amp;TEXT(D14,"00")&amp;"_"&amp;YEAR(G14)&amp;TEXT(G14,"MM")&amp;TEXT(G14,"DD")&amp;"_p"&amp;E14&amp;"_wv"&amp;TEXT(F14,"00")&amp;""</f>
+        <f t="shared" si="0"/>
         <v>uk_wk10_20200604_pB_wv05</v>
       </c>
       <c r="J14">
@@ -1173,7 +1176,7 @@
         <v>12</v>
       </c>
       <c r="D15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>10</v>
       </c>
       <c r="E15" t="s">
@@ -1189,7 +1192,7 @@
         <v>31</v>
       </c>
       <c r="I15" t="str">
-        <f>C15&amp;"_"&amp;"wk"&amp;TEXT(D15,"00")&amp;"_"&amp;YEAR(G15)&amp;TEXT(G15,"MM")&amp;TEXT(G15,"DD")&amp;"_p"&amp;E15&amp;"_wv"&amp;TEXT(F15,"00")&amp;""</f>
+        <f t="shared" si="0"/>
         <v>uk_wk10_20200608_pD_wv02</v>
       </c>
       <c r="J15">
@@ -1210,7 +1213,7 @@
         <v>12</v>
       </c>
       <c r="D16">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>11</v>
       </c>
       <c r="E16" t="s">
@@ -1226,7 +1229,7 @@
         <v>32</v>
       </c>
       <c r="I16" t="str">
-        <f>C16&amp;"_"&amp;"wk"&amp;TEXT(D16,"00")&amp;"_"&amp;YEAR(G16)&amp;TEXT(G16,"MM")&amp;TEXT(G16,"DD")&amp;"_p"&amp;E16&amp;"_wv"&amp;TEXT(F16,"00")&amp;""</f>
+        <f t="shared" si="0"/>
         <v>uk_wk11_20200612_pA_wv06</v>
       </c>
       <c r="J16">
@@ -1247,7 +1250,7 @@
         <v>12</v>
       </c>
       <c r="D17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>11</v>
       </c>
       <c r="E17" t="s">
@@ -1263,7 +1266,7 @@
         <v>33</v>
       </c>
       <c r="I17" t="str">
-        <f>C17&amp;"_"&amp;"wk"&amp;TEXT(D17,"00")&amp;"_"&amp;YEAR(G17)&amp;TEXT(G17,"MM")&amp;TEXT(G17,"DD")&amp;"_p"&amp;E17&amp;"_wv"&amp;TEXT(F17,"00")&amp;""</f>
+        <f t="shared" si="0"/>
         <v>uk_wk11_20200612_pC_wv03</v>
       </c>
       <c r="J17">
@@ -1284,7 +1287,7 @@
         <v>12</v>
       </c>
       <c r="D18">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>12</v>
       </c>
       <c r="E18" t="s">
@@ -1300,7 +1303,7 @@
         <v>34</v>
       </c>
       <c r="I18" t="str">
-        <f>C18&amp;"_"&amp;"wk"&amp;TEXT(D18,"00")&amp;"_"&amp;YEAR(G18)&amp;TEXT(G18,"MM")&amp;TEXT(G18,"DD")&amp;"_p"&amp;E18&amp;"_wv"&amp;TEXT(F18,"00")&amp;""</f>
+        <f t="shared" si="0"/>
         <v>uk_wk12_20200619_pB_wv06</v>
       </c>
       <c r="J18">
@@ -1321,7 +1324,7 @@
         <v>12</v>
       </c>
       <c r="D19">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>12</v>
       </c>
       <c r="E19" t="s">
@@ -1337,7 +1340,7 @@
         <v>35</v>
       </c>
       <c r="I19" t="str">
-        <f>C19&amp;"_"&amp;"wk"&amp;TEXT(D19,"00")&amp;"_"&amp;YEAR(G19)&amp;TEXT(G19,"MM")&amp;TEXT(G19,"DD")&amp;"_p"&amp;E19&amp;"_wv"&amp;TEXT(F19,"00")&amp;""</f>
+        <f t="shared" si="0"/>
         <v>uk_wk12_20200619_pD_wv03</v>
       </c>
       <c r="J19">
@@ -1358,7 +1361,7 @@
         <v>12</v>
       </c>
       <c r="D20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>13</v>
       </c>
       <c r="E20" t="s">
@@ -1374,7 +1377,7 @@
         <v>36</v>
       </c>
       <c r="I20" t="str">
-        <f>C20&amp;"_"&amp;"wk"&amp;TEXT(D20,"00")&amp;"_"&amp;YEAR(G20)&amp;TEXT(G20,"MM")&amp;TEXT(G20,"DD")&amp;"_p"&amp;E20&amp;"_wv"&amp;TEXT(F20,"00")&amp;""</f>
+        <f t="shared" si="0"/>
         <v>uk_wk13_20200625_pA_wv07</v>
       </c>
       <c r="J20">
@@ -1395,7 +1398,7 @@
         <v>12</v>
       </c>
       <c r="D21">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>13</v>
       </c>
       <c r="E21" t="s">
@@ -1411,7 +1414,7 @@
         <v>37</v>
       </c>
       <c r="I21" t="str">
-        <f>C21&amp;"_"&amp;"wk"&amp;TEXT(D21,"00")&amp;"_"&amp;YEAR(G21)&amp;TEXT(G21,"MM")&amp;TEXT(G21,"DD")&amp;"_p"&amp;E21&amp;"_wv"&amp;TEXT(F21,"00")&amp;""</f>
+        <f t="shared" si="0"/>
         <v>uk_wk13_20200625_pC_wv04</v>
       </c>
       <c r="J21">
@@ -1448,7 +1451,7 @@
         <v>38</v>
       </c>
       <c r="I22" t="str">
-        <f>C22&amp;"_"&amp;"wk"&amp;TEXT(D22,"00")&amp;"_"&amp;YEAR(G22)&amp;TEXT(G22,"MM")&amp;TEXT(G22,"DD")&amp;"_p"&amp;E22&amp;"_wv"&amp;TEXT(F22,"00")&amp;""</f>
+        <f t="shared" si="0"/>
         <v>uk_wk14_20200702_pB_wv07</v>
       </c>
       <c r="J22">
@@ -1485,7 +1488,7 @@
         <v>39</v>
       </c>
       <c r="I23" t="str">
-        <f>C23&amp;"_"&amp;"wk"&amp;TEXT(D23,"00")&amp;"_"&amp;YEAR(G23)&amp;TEXT(G23,"MM")&amp;TEXT(G23,"DD")&amp;"_p"&amp;E23&amp;"_wv"&amp;TEXT(F23,"00")&amp;""</f>
+        <f t="shared" si="0"/>
         <v>uk_wk14_20200703_pD_wv04</v>
       </c>
       <c r="J23">
@@ -1506,7 +1509,7 @@
         <v>12</v>
       </c>
       <c r="D24">
-        <f t="shared" ref="D24:D28" si="2">D22+1</f>
+        <f t="shared" ref="D24:D28" si="3">D22+1</f>
         <v>15</v>
       </c>
       <c r="E24" t="s">
@@ -1522,7 +1525,7 @@
         <v>40</v>
       </c>
       <c r="I24" t="str">
-        <f>C24&amp;"_"&amp;"wk"&amp;TEXT(D24,"00")&amp;"_"&amp;YEAR(G24)&amp;TEXT(G24,"MM")&amp;TEXT(G24,"DD")&amp;"_p"&amp;E24&amp;"_wv"&amp;TEXT(F24,"00")&amp;""</f>
+        <f t="shared" si="0"/>
         <v>uk_wk15_20200710_pA_wv08</v>
       </c>
       <c r="J24">
@@ -1543,7 +1546,7 @@
         <v>12</v>
       </c>
       <c r="D25">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>15</v>
       </c>
       <c r="E25" t="s">
@@ -1559,7 +1562,7 @@
         <v>41</v>
       </c>
       <c r="I25" t="str">
-        <f>C25&amp;"_"&amp;"wk"&amp;TEXT(D25,"00")&amp;"_"&amp;YEAR(G25)&amp;TEXT(G25,"MM")&amp;TEXT(G25,"DD")&amp;"_p"&amp;E25&amp;"_wv"&amp;TEXT(F25,"00")&amp;""</f>
+        <f t="shared" si="0"/>
         <v>uk_wk15_20200709_pC_wv05</v>
       </c>
       <c r="J25">
@@ -1580,7 +1583,7 @@
         <v>12</v>
       </c>
       <c r="D26">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>16</v>
       </c>
       <c r="E26" t="s">
@@ -1596,7 +1599,7 @@
         <v>42</v>
       </c>
       <c r="I26" t="str">
-        <f>C26&amp;"_"&amp;"wk"&amp;TEXT(D26,"00")&amp;"_"&amp;YEAR(G26)&amp;TEXT(G26,"MM")&amp;TEXT(G26,"DD")&amp;"_p"&amp;E26&amp;"_wv"&amp;TEXT(F26,"00")&amp;""</f>
+        <f t="shared" si="0"/>
         <v>uk_wk16_20200717_pB_wv08</v>
       </c>
       <c r="J26">
@@ -1617,7 +1620,7 @@
         <v>12</v>
       </c>
       <c r="D27">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>16</v>
       </c>
       <c r="E27" t="s">
@@ -1633,7 +1636,7 @@
         <v>43</v>
       </c>
       <c r="I27" t="str">
-        <f>C27&amp;"_"&amp;"wk"&amp;TEXT(D27,"00")&amp;"_"&amp;YEAR(G27)&amp;TEXT(G27,"MM")&amp;TEXT(G27,"DD")&amp;"_p"&amp;E27&amp;"_wv"&amp;TEXT(F27,"00")&amp;""</f>
+        <f t="shared" si="0"/>
         <v>uk_wk16_20200717_pD_wv05</v>
       </c>
       <c r="J27">
@@ -1654,7 +1657,7 @@
         <v>12</v>
       </c>
       <c r="D28">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>17</v>
       </c>
       <c r="E28" t="s">
@@ -1670,7 +1673,7 @@
         <v>45</v>
       </c>
       <c r="I28" t="str">
-        <f>C28&amp;"_"&amp;"wk"&amp;TEXT(D28,"00")&amp;"_"&amp;YEAR(G28)&amp;TEXT(G28,"MM")&amp;TEXT(G28,"DD")&amp;"_p"&amp;E28&amp;"_wv"&amp;TEXT(F28,"00")&amp;""</f>
+        <f t="shared" si="0"/>
         <v>uk_wk17_20200724_pA_wv09</v>
       </c>
       <c r="J28">
@@ -1710,7 +1713,7 @@
         <v>46</v>
       </c>
       <c r="I29" t="str">
-        <f>C29&amp;"_"&amp;"wk"&amp;TEXT(D29,"00")&amp;"_"&amp;YEAR(G29)&amp;TEXT(G29,"MM")&amp;TEXT(G29,"DD")&amp;"_p"&amp;E29&amp;"_wv"&amp;TEXT(F29,"00")&amp;""</f>
+        <f t="shared" si="0"/>
         <v>uk_wk18_20200731_pB_wv09</v>
       </c>
       <c r="J29">
@@ -1750,7 +1753,7 @@
         <v>47</v>
       </c>
       <c r="I30" t="str">
-        <f>C30&amp;"_"&amp;"wk"&amp;TEXT(D30,"00")&amp;"_"&amp;YEAR(G30)&amp;TEXT(G30,"MM")&amp;TEXT(G30,"DD")&amp;"_p"&amp;E30&amp;"_wv"&amp;TEXT(F30,"00")&amp;""</f>
+        <f t="shared" si="0"/>
         <v>uk_wk19_20200807_pA_wv10</v>
       </c>
       <c r="J30">
@@ -1786,7 +1789,7 @@
         <v>48</v>
       </c>
       <c r="I31" t="str">
-        <f>C31&amp;"_"&amp;"wk"&amp;TEXT(D31,"00")&amp;"_"&amp;YEAR(G31)&amp;TEXT(G31,"MM")&amp;TEXT(G31,"DD")&amp;"_p"&amp;E31&amp;"_wv"&amp;TEXT(F31,"00")&amp;""</f>
+        <f t="shared" si="0"/>
         <v>uk_wk19_20200810_pC_wv06</v>
       </c>
       <c r="J31">
@@ -1822,7 +1825,7 @@
         <v>51</v>
       </c>
       <c r="I32" t="str">
-        <f>C32&amp;"_"&amp;"wk"&amp;TEXT(D32,"00")&amp;"_"&amp;YEAR(G32)&amp;TEXT(G32,"MM")&amp;TEXT(G32,"DD")&amp;"_p"&amp;E32&amp;"_wv"&amp;TEXT(F32,"00")&amp;""</f>
+        <f t="shared" si="0"/>
         <v>uk_wk20_20200821_pE_wv01</v>
       </c>
       <c r="J32">
@@ -1861,7 +1864,7 @@
         <v>53</v>
       </c>
       <c r="I33" t="str">
-        <f>C33&amp;"_"&amp;"wk"&amp;TEXT(D33,"00")&amp;"_"&amp;YEAR(G33)&amp;TEXT(G33,"MM")&amp;TEXT(G33,"DD")&amp;"_p"&amp;E33&amp;"_wv"&amp;TEXT(F33,"00")&amp;""</f>
+        <f t="shared" si="0"/>
         <v>uk_wk21_20200827_pF_wv01</v>
       </c>
       <c r="J33">
@@ -1888,7 +1891,7 @@
         <v>50</v>
       </c>
       <c r="F34">
-        <f t="shared" ref="F34:F52" si="3">F32+1</f>
+        <f t="shared" ref="F34:F52" si="4">F32+1</f>
         <v>2</v>
       </c>
       <c r="G34" s="1">
@@ -1898,7 +1901,7 @@
         <v>54</v>
       </c>
       <c r="I34" t="str">
-        <f>C34&amp;"_"&amp;"wk"&amp;TEXT(D34,"00")&amp;"_"&amp;YEAR(G34)&amp;TEXT(G34,"MM")&amp;TEXT(G34,"DD")&amp;"_p"&amp;E34&amp;"_wv"&amp;TEXT(F34,"00")&amp;""</f>
+        <f t="shared" si="0"/>
         <v>uk_wk22_20200903_pE_wv02</v>
       </c>
       <c r="J34">
@@ -1925,7 +1928,7 @@
         <v>52</v>
       </c>
       <c r="F35">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="G35" s="1">
@@ -1935,7 +1938,7 @@
         <v>55</v>
       </c>
       <c r="I35" t="str">
-        <f>C35&amp;"_"&amp;"wk"&amp;TEXT(D35,"00")&amp;"_"&amp;YEAR(G35)&amp;TEXT(G35,"MM")&amp;TEXT(G35,"DD")&amp;"_p"&amp;E35&amp;"_wv"&amp;TEXT(F35,"00")&amp;""</f>
+        <f t="shared" si="0"/>
         <v>uk_wk23_20200907_pF_wv02</v>
       </c>
       <c r="J35">
@@ -1962,7 +1965,7 @@
         <v>50</v>
       </c>
       <c r="F36">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>3</v>
       </c>
       <c r="G36" s="1">
@@ -1972,7 +1975,7 @@
         <v>56</v>
       </c>
       <c r="I36" t="str">
-        <f>C36&amp;"_"&amp;"wk"&amp;TEXT(D36,"00")&amp;"_"&amp;YEAR(G36)&amp;TEXT(G36,"MM")&amp;TEXT(G36,"DD")&amp;"_p"&amp;E36&amp;"_wv"&amp;TEXT(F36,"00")&amp;""</f>
+        <f t="shared" si="0"/>
         <v>uk_wk24_20200914_pE_wv03</v>
       </c>
       <c r="J36">
@@ -1999,7 +2002,7 @@
         <v>52</v>
       </c>
       <c r="F37">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>3</v>
       </c>
       <c r="G37" s="1">
@@ -2009,7 +2012,7 @@
         <v>57</v>
       </c>
       <c r="I37" t="str">
-        <f>C37&amp;"_"&amp;"wk"&amp;TEXT(D37,"00")&amp;"_"&amp;YEAR(G37)&amp;TEXT(G37,"MM")&amp;TEXT(G37,"DD")&amp;"_p"&amp;E37&amp;"_wv"&amp;TEXT(F37,"00")&amp;""</f>
+        <f t="shared" si="0"/>
         <v>uk_wk25_20200918_pF_wv03</v>
       </c>
       <c r="J37">
@@ -2036,7 +2039,7 @@
         <v>50</v>
       </c>
       <c r="F38">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>4</v>
       </c>
       <c r="G38" s="1">
@@ -2046,7 +2049,7 @@
         <v>58</v>
       </c>
       <c r="I38" t="str">
-        <f>C38&amp;"_"&amp;"wk"&amp;TEXT(D38,"00")&amp;"_"&amp;YEAR(G38)&amp;TEXT(G38,"MM")&amp;TEXT(G38,"DD")&amp;"_p"&amp;E38&amp;"_wv"&amp;TEXT(F38,"00")&amp;""</f>
+        <f t="shared" si="0"/>
         <v>uk_wk26_20200925_pE_wv04</v>
       </c>
       <c r="J38">
@@ -2073,7 +2076,7 @@
         <v>52</v>
       </c>
       <c r="F39">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>4</v>
       </c>
       <c r="G39" s="1">
@@ -2083,7 +2086,7 @@
         <v>59</v>
       </c>
       <c r="I39" t="str">
-        <f>C39&amp;"_"&amp;"wk"&amp;TEXT(D39,"00")&amp;"_"&amp;YEAR(G39)&amp;TEXT(G39,"MM")&amp;TEXT(G39,"DD")&amp;"_p"&amp;E39&amp;"_wv"&amp;TEXT(F39,"00")&amp;""</f>
+        <f t="shared" si="0"/>
         <v>uk_wk27_20201002_pF_wv04</v>
       </c>
       <c r="J39">
@@ -2110,7 +2113,7 @@
         <v>50</v>
       </c>
       <c r="F40">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>5</v>
       </c>
       <c r="G40" s="1">
@@ -2120,7 +2123,7 @@
         <v>60</v>
       </c>
       <c r="I40" t="str">
-        <f>C40&amp;"_"&amp;"wk"&amp;TEXT(D40,"00")&amp;"_"&amp;YEAR(G40)&amp;TEXT(G40,"MM")&amp;TEXT(G40,"DD")&amp;"_p"&amp;E40&amp;"_wv"&amp;TEXT(F40,"00")&amp;""</f>
+        <f t="shared" si="0"/>
         <v>uk_wk28_20201009_pE_wv05</v>
       </c>
       <c r="J40">
@@ -2147,7 +2150,7 @@
         <v>52</v>
       </c>
       <c r="F41">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>5</v>
       </c>
       <c r="G41" s="1">
@@ -2157,7 +2160,7 @@
         <v>61</v>
       </c>
       <c r="I41" t="str">
-        <f>C41&amp;"_"&amp;"wk"&amp;TEXT(D41,"00")&amp;"_"&amp;YEAR(G41)&amp;TEXT(G41,"MM")&amp;TEXT(G41,"DD")&amp;"_p"&amp;E41&amp;"_wv"&amp;TEXT(F41,"00")&amp;""</f>
+        <f t="shared" si="0"/>
         <v>uk_wk29_20201018_pF_wv05</v>
       </c>
       <c r="J41">
@@ -2184,7 +2187,7 @@
         <v>50</v>
       </c>
       <c r="F42">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>6</v>
       </c>
       <c r="G42" s="1">
@@ -2194,7 +2197,7 @@
         <v>62</v>
       </c>
       <c r="I42" t="str">
-        <f>C42&amp;"_"&amp;"wk"&amp;TEXT(D42,"00")&amp;"_"&amp;YEAR(G42)&amp;TEXT(G42,"MM")&amp;TEXT(G42,"DD")&amp;"_p"&amp;E42&amp;"_wv"&amp;TEXT(F42,"00")&amp;""</f>
+        <f t="shared" si="0"/>
         <v>uk_wk30_20201023_pE_wv06</v>
       </c>
       <c r="J42">
@@ -2221,7 +2224,7 @@
         <v>52</v>
       </c>
       <c r="F43">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>6</v>
       </c>
       <c r="G43" s="1">
@@ -2231,7 +2234,7 @@
         <v>63</v>
       </c>
       <c r="I43" t="str">
-        <f>C43&amp;"_"&amp;"wk"&amp;TEXT(D43,"00")&amp;"_"&amp;YEAR(G43)&amp;TEXT(G43,"MM")&amp;TEXT(G43,"DD")&amp;"_p"&amp;E43&amp;"_wv"&amp;TEXT(F43,"00")&amp;""</f>
+        <f t="shared" si="0"/>
         <v>uk_wk31_20201030_pF_wv06</v>
       </c>
       <c r="J43">
@@ -2258,7 +2261,7 @@
         <v>50</v>
       </c>
       <c r="F44">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>7</v>
       </c>
       <c r="G44" s="1">
@@ -2268,7 +2271,7 @@
         <v>82</v>
       </c>
       <c r="I44" t="str">
-        <f>C44&amp;"_"&amp;"wk"&amp;TEXT(D44,"00")&amp;"_"&amp;YEAR(G44)&amp;TEXT(G44,"MM")&amp;TEXT(G44,"DD")&amp;"_p"&amp;E44&amp;"_wv"&amp;TEXT(F44,"00")&amp;""</f>
+        <f t="shared" si="0"/>
         <v>uk_wk32_20201106_pE_wv07</v>
       </c>
       <c r="J44">
@@ -2292,10 +2295,25 @@
         <v>52</v>
       </c>
       <c r="F45">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>7</v>
       </c>
-      <c r="G45" s="1"/>
+      <c r="G45" s="1">
+        <v>44148</v>
+      </c>
+      <c r="H45" t="s">
+        <v>85</v>
+      </c>
+      <c r="I45" t="str">
+        <f t="shared" si="0"/>
+        <v>uk_wk33_20201113_pF_wv07</v>
+      </c>
+      <c r="J45">
+        <v>1</v>
+      </c>
+      <c r="K45">
+        <v>1</v>
+      </c>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A46">
@@ -2314,7 +2332,7 @@
         <v>50</v>
       </c>
       <c r="F46">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>8</v>
       </c>
       <c r="G46" s="1"/>
@@ -2336,7 +2354,7 @@
         <v>52</v>
       </c>
       <c r="F47">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>8</v>
       </c>
       <c r="G47" s="1"/>
@@ -2358,7 +2376,7 @@
         <v>50</v>
       </c>
       <c r="F48">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>9</v>
       </c>
       <c r="G48" s="1"/>
@@ -2380,7 +2398,7 @@
         <v>52</v>
       </c>
       <c r="F49">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>9</v>
       </c>
       <c r="G49" s="1"/>
@@ -2402,7 +2420,7 @@
         <v>50</v>
       </c>
       <c r="F50">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>10</v>
       </c>
       <c r="G50" s="1"/>
@@ -2424,7 +2442,7 @@
         <v>52</v>
       </c>
       <c r="F51">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>10</v>
       </c>
       <c r="G51" s="1"/>
@@ -2446,7 +2464,7 @@
         <v>50</v>
       </c>
       <c r="F52">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>11</v>
       </c>
       <c r="G52" s="1"/>
@@ -2880,7 +2898,7 @@
         <v>65</v>
       </c>
       <c r="I2" t="str">
-        <f>C2&amp;"_"&amp;"wk"&amp;TEXT(D2,"00")&amp;"_"&amp;YEAR(G2)&amp;TEXT(G2,"MM")&amp;TEXT(G2,"DD")&amp;"_p"&amp;E2&amp;"_wv"&amp;TEXT(F2,"00")&amp;""</f>
+        <f t="shared" ref="I2:I9" si="0">C2&amp;"_"&amp;"wk"&amp;TEXT(D2,"00")&amp;"_"&amp;YEAR(G2)&amp;TEXT(G2,"MM")&amp;TEXT(G2,"DD")&amp;"_p"&amp;E2&amp;"_wv"&amp;TEXT(F2,"00")&amp;""</f>
         <v>nl_wk01_20200429_pA_wv01</v>
       </c>
       <c r="K2">
@@ -2913,7 +2931,7 @@
         <v>66</v>
       </c>
       <c r="I3" t="str">
-        <f>C3&amp;"_"&amp;"wk"&amp;TEXT(D3,"00")&amp;"_"&amp;YEAR(G3)&amp;TEXT(G3,"MM")&amp;TEXT(G3,"DD")&amp;"_p"&amp;E3&amp;"_wv"&amp;TEXT(F3,"00")&amp;""</f>
+        <f t="shared" si="0"/>
         <v>nl_wk03_20200518_pA_wv02</v>
       </c>
       <c r="K3">
@@ -2947,7 +2965,7 @@
         <v>67</v>
       </c>
       <c r="I4" t="str">
-        <f>C4&amp;"_"&amp;"wk"&amp;TEXT(D4,"00")&amp;"_"&amp;YEAR(G4)&amp;TEXT(G4,"MM")&amp;TEXT(G4,"DD")&amp;"_p"&amp;E4&amp;"_wv"&amp;TEXT(F4,"00")&amp;""</f>
+        <f t="shared" si="0"/>
         <v>nl_wk05_20200601_pA_wv03</v>
       </c>
       <c r="K4">
@@ -2965,7 +2983,7 @@
         <v>73</v>
       </c>
       <c r="D5">
-        <f t="shared" ref="D5:D9" si="0">D4+2</f>
+        <f t="shared" ref="D5:D9" si="1">D4+2</f>
         <v>7</v>
       </c>
       <c r="E5" t="s">
@@ -2981,7 +2999,7 @@
         <v>68</v>
       </c>
       <c r="I5" t="str">
-        <f>C5&amp;"_"&amp;"wk"&amp;TEXT(D5,"00")&amp;"_"&amp;YEAR(G5)&amp;TEXT(G5,"MM")&amp;TEXT(G5,"DD")&amp;"_p"&amp;E5&amp;"_wv"&amp;TEXT(F5,"00")&amp;""</f>
+        <f t="shared" si="0"/>
         <v>nl_wk07_20200612_pA_wv04</v>
       </c>
       <c r="K5">
@@ -2999,7 +3017,7 @@
         <v>73</v>
       </c>
       <c r="D6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>9</v>
       </c>
       <c r="E6" t="s">
@@ -3015,7 +3033,7 @@
         <v>69</v>
       </c>
       <c r="I6" t="str">
-        <f>C6&amp;"_"&amp;"wk"&amp;TEXT(D6,"00")&amp;"_"&amp;YEAR(G6)&amp;TEXT(G6,"MM")&amp;TEXT(G6,"DD")&amp;"_p"&amp;E6&amp;"_wv"&amp;TEXT(F6,"00")&amp;""</f>
+        <f t="shared" si="0"/>
         <v>nl_wk09_20200626_pA_wv05</v>
       </c>
       <c r="K6">
@@ -3033,7 +3051,7 @@
         <v>73</v>
       </c>
       <c r="D7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>11</v>
       </c>
       <c r="E7" t="s">
@@ -3049,7 +3067,7 @@
         <v>70</v>
       </c>
       <c r="I7" t="str">
-        <f>C7&amp;"_"&amp;"wk"&amp;TEXT(D7,"00")&amp;"_"&amp;YEAR(G7)&amp;TEXT(G7,"MM")&amp;TEXT(G7,"DD")&amp;"_p"&amp;E7&amp;"_wv"&amp;TEXT(F7,"00")&amp;""</f>
+        <f t="shared" si="0"/>
         <v>nl_wk11_20200710_pA_wv06</v>
       </c>
       <c r="K7">
@@ -3067,7 +3085,7 @@
         <v>73</v>
       </c>
       <c r="D8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>13</v>
       </c>
       <c r="E8" t="s">
@@ -3083,7 +3101,7 @@
         <v>71</v>
       </c>
       <c r="I8" t="str">
-        <f>C8&amp;"_"&amp;"wk"&amp;TEXT(D8,"00")&amp;"_"&amp;YEAR(G8)&amp;TEXT(G8,"MM")&amp;TEXT(G8,"DD")&amp;"_p"&amp;E8&amp;"_wv"&amp;TEXT(F8,"00")&amp;""</f>
+        <f t="shared" si="0"/>
         <v>nl_wk13_20200724_pA_wv07</v>
       </c>
       <c r="K8">
@@ -3101,7 +3119,7 @@
         <v>73</v>
       </c>
       <c r="D9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>15</v>
       </c>
       <c r="E9" t="s">
@@ -3117,7 +3135,7 @@
         <v>72</v>
       </c>
       <c r="I9" t="str">
-        <f>C9&amp;"_"&amp;"wk"&amp;TEXT(D9,"00")&amp;"_"&amp;YEAR(G9)&amp;TEXT(G9,"MM")&amp;TEXT(G9,"DD")&amp;"_p"&amp;E9&amp;"_wv"&amp;TEXT(F9,"00")&amp;""</f>
+        <f t="shared" si="0"/>
         <v>nl_wk15_20200806_pA_wv08</v>
       </c>
       <c r="K9">
@@ -3133,7 +3151,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D2B755C-13CE-401F-B50D-AD8E835063B7}">
   <dimension ref="A1:O7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
@@ -3214,7 +3232,7 @@
         <v>80</v>
       </c>
       <c r="I2" t="str">
-        <f>C2&amp;"_"&amp;"wk"&amp;TEXT(D2,"00")&amp;"_"&amp;YEAR(G2)&amp;TEXT(G2,"MM")&amp;TEXT(G2,"DD")&amp;"_p"&amp;E2&amp;"_wv"&amp;TEXT(F2,"00")&amp;""</f>
+        <f t="shared" ref="I2:I7" si="0">C2&amp;"_"&amp;"wk"&amp;TEXT(D2,"00")&amp;"_"&amp;YEAR(G2)&amp;TEXT(G2,"MM")&amp;TEXT(G2,"DD")&amp;"_p"&amp;E2&amp;"_wv"&amp;TEXT(F2,"00")&amp;""</f>
         <v>no_wk01_20200501_pA_wv01</v>
       </c>
     </row>
@@ -3244,7 +3262,7 @@
         <v>75</v>
       </c>
       <c r="I3" t="str">
-        <f>C3&amp;"_"&amp;"wk"&amp;TEXT(D3,"00")&amp;"_"&amp;YEAR(G3)&amp;TEXT(G3,"MM")&amp;TEXT(G3,"DD")&amp;"_p"&amp;E3&amp;"_wv"&amp;TEXT(F3,"00")&amp;""</f>
+        <f t="shared" si="0"/>
         <v>no_wk03_20200529_pA_wv02</v>
       </c>
       <c r="K3">
@@ -3277,7 +3295,7 @@
         <v>81</v>
       </c>
       <c r="I4" t="str">
-        <f>C4&amp;"_"&amp;"wk"&amp;TEXT(D4,"00")&amp;"_"&amp;YEAR(G4)&amp;TEXT(G4,"MM")&amp;TEXT(G4,"DD")&amp;"_p"&amp;E4&amp;"_wv"&amp;TEXT(F4,"00")&amp;""</f>
+        <f t="shared" si="0"/>
         <v>no_wk05_20200622_pA_wv03</v>
       </c>
     </row>
@@ -3308,7 +3326,7 @@
         <v>76</v>
       </c>
       <c r="I5" t="str">
-        <f>C5&amp;"_"&amp;"wk"&amp;TEXT(D5,"00")&amp;"_"&amp;YEAR(G5)&amp;TEXT(G5,"MM")&amp;TEXT(G5,"DD")&amp;"_p"&amp;E5&amp;"_wv"&amp;TEXT(F5,"00")&amp;""</f>
+        <f t="shared" si="0"/>
         <v>no_wk07_20200731_pA_wv04</v>
       </c>
       <c r="K5">
@@ -3326,7 +3344,7 @@
         <v>74</v>
       </c>
       <c r="D6">
-        <f t="shared" ref="D6:D7" si="0">D5+2</f>
+        <f t="shared" ref="D6:D7" si="1">D5+2</f>
         <v>9</v>
       </c>
       <c r="E6" t="s">
@@ -3342,7 +3360,7 @@
         <v>77</v>
       </c>
       <c r="I6" t="str">
-        <f>C6&amp;"_"&amp;"wk"&amp;TEXT(D6,"00")&amp;"_"&amp;YEAR(G6)&amp;TEXT(G6,"MM")&amp;TEXT(G6,"DD")&amp;"_p"&amp;E6&amp;"_wv"&amp;TEXT(F6,"00")&amp;""</f>
+        <f t="shared" si="0"/>
         <v>no_wk09_20200906_pA_wv05</v>
       </c>
       <c r="K6">
@@ -3360,7 +3378,7 @@
         <v>74</v>
       </c>
       <c r="D7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>11</v>
       </c>
       <c r="E7" t="s">
@@ -3376,7 +3394,7 @@
         <v>78</v>
       </c>
       <c r="I7" t="str">
-        <f>C7&amp;"_"&amp;"wk"&amp;TEXT(D7,"00")&amp;"_"&amp;YEAR(G7)&amp;TEXT(G7,"MM")&amp;TEXT(G7,"DD")&amp;"_p"&amp;E7&amp;"_wv"&amp;TEXT(F7,"00")&amp;""</f>
+        <f t="shared" si="0"/>
         <v>no_wk11_20201001_pA_wv06</v>
       </c>
       <c r="K7">

</xml_diff>

<commit_message>
Added UK panel F wave 7 to spss_file
</commit_message>
<xml_diff>
--- a/data/spss_files.xlsx
+++ b/data/spss_files.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jarvisc1\Documents\projects\comix_data_clean\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC814162-C190-4260-8961-EDC8F728AEF6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34248944-BA50-49E6-BF55-4A542A7C0CCF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -629,7 +629,7 @@
   <dimension ref="A1:O52"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="A45" sqref="A45"/>
+      <selection activeCell="H45" sqref="H45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>

</xml_diff>

<commit_message>
Update for UK wk 34 Panel E Wave 8 & BE Panel B Wave 1
</commit_message>
<xml_diff>
--- a/data/spss_files.xlsx
+++ b/data/spss_files.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jarvisc1\Documents\projects\comix_data_clean\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34248944-BA50-49E6-BF55-4A542A7C0CCF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E0916EE-1A68-4BE9-8F8A-6C3D45A3E4EE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="5" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="88">
   <si>
     <t>country</t>
   </si>
@@ -296,6 +296,12 @@
   </si>
   <si>
     <t>20-056790_Final_PFW7_v1_IntUse</t>
+  </si>
+  <si>
+    <t>20-040199-01_Final_PEW8_v1_201120_Intclientuse</t>
+  </si>
+  <si>
+    <t>20_060765_BE2_Wave1_Final_v1_20112020_IntClientUse</t>
   </si>
 </sst>
 </file>
@@ -628,8 +634,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="H45" sqref="H45"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K46" sqref="K46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -714,7 +720,7 @@
         <v>14</v>
       </c>
       <c r="I2" t="str">
-        <f t="shared" ref="I2:I45" si="0">C2&amp;"_"&amp;"wk"&amp;TEXT(D2,"00")&amp;"_"&amp;YEAR(G2)&amp;TEXT(G2,"MM")&amp;TEXT(G2,"DD")&amp;"_p"&amp;E2&amp;"_wv"&amp;TEXT(F2,"00")&amp;""</f>
+        <f t="shared" ref="I2:I46" si="0">C2&amp;"_"&amp;"wk"&amp;TEXT(D2,"00")&amp;"_"&amp;YEAR(G2)&amp;TEXT(G2,"MM")&amp;TEXT(G2,"DD")&amp;"_p"&amp;E2&amp;"_wv"&amp;TEXT(F2,"00")&amp;""</f>
         <v>uk_wk01_20200402_pA_wv01</v>
       </c>
       <c r="J2">
@@ -2335,7 +2341,22 @@
         <f t="shared" si="4"/>
         <v>8</v>
       </c>
-      <c r="G46" s="1"/>
+      <c r="G46" s="1">
+        <v>44155</v>
+      </c>
+      <c r="H46" t="s">
+        <v>86</v>
+      </c>
+      <c r="I46" t="str">
+        <f t="shared" si="0"/>
+        <v>uk_wk34_20201120_pE_wv08</v>
+      </c>
+      <c r="J46">
+        <v>1</v>
+      </c>
+      <c r="K46">
+        <v>1</v>
+      </c>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A47">
@@ -2476,10 +2497,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C042354-CAAB-48AD-AFC2-2197A2D12C9D}">
-  <dimension ref="A1:N9"/>
+  <dimension ref="A1:N10"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3:C9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2563,7 +2584,7 @@
         <v>65</v>
       </c>
       <c r="I2" t="str">
-        <f t="shared" ref="I2:I9" si="0">A2&amp;"_"&amp;"wk"&amp;TEXT(D2,"00")&amp;"_"&amp;YEAR(G2)&amp;TEXT(G2,"MM")&amp;TEXT(G2,"DD")&amp;"_p"&amp;E2&amp;"_wv"&amp;TEXT(F2,"00")&amp;""</f>
+        <f t="shared" ref="I2:I10" si="0">A2&amp;"_"&amp;"wk"&amp;TEXT(D2,"00")&amp;"_"&amp;YEAR(G2)&amp;TEXT(G2,"MM")&amp;TEXT(G2,"DD")&amp;"_p"&amp;E2&amp;"_wv"&amp;TEXT(F2,"00")&amp;""</f>
         <v>be_wk01_20200429_pA_wv01</v>
       </c>
       <c r="J2">
@@ -2581,7 +2602,7 @@
         <v>0</v>
       </c>
       <c r="D3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E3" t="s">
         <v>13</v>
@@ -2597,7 +2618,7 @@
       </c>
       <c r="I3" t="str">
         <f t="shared" si="0"/>
-        <v>be_wk03_20200518_pA_wv02</v>
+        <v>be_wk02_20200518_pA_wv02</v>
       </c>
       <c r="J3">
         <v>1</v>
@@ -2614,8 +2635,7 @@
         <v>0</v>
       </c>
       <c r="D4">
-        <f>D3+2</f>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E4" t="s">
         <v>13</v>
@@ -2631,7 +2651,7 @@
       </c>
       <c r="I4" t="str">
         <f t="shared" si="0"/>
-        <v>be_wk05_20200601_pA_wv03</v>
+        <v>be_wk03_20200601_pA_wv03</v>
       </c>
       <c r="J4">
         <v>1</v>
@@ -2648,8 +2668,7 @@
         <v>0</v>
       </c>
       <c r="D5">
-        <f t="shared" ref="D5:D9" si="1">D4+2</f>
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E5" t="s">
         <v>13</v>
@@ -2665,7 +2684,7 @@
       </c>
       <c r="I5" t="str">
         <f t="shared" si="0"/>
-        <v>be_wk07_20200612_pA_wv04</v>
+        <v>be_wk04_20200612_pA_wv04</v>
       </c>
       <c r="J5">
         <v>1</v>
@@ -2682,8 +2701,7 @@
         <v>0</v>
       </c>
       <c r="D6">
-        <f t="shared" si="1"/>
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="E6" t="s">
         <v>13</v>
@@ -2699,7 +2717,7 @@
       </c>
       <c r="I6" t="str">
         <f t="shared" si="0"/>
-        <v>be_wk09_20200626_pA_wv05</v>
+        <v>be_wk05_20200626_pA_wv05</v>
       </c>
       <c r="J6">
         <v>1</v>
@@ -2716,8 +2734,7 @@
         <v>0</v>
       </c>
       <c r="D7">
-        <f t="shared" si="1"/>
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="E7" t="s">
         <v>13</v>
@@ -2733,7 +2750,7 @@
       </c>
       <c r="I7" t="str">
         <f t="shared" si="0"/>
-        <v>be_wk11_20200710_pA_wv06</v>
+        <v>be_wk06_20200710_pA_wv06</v>
       </c>
       <c r="J7">
         <v>1</v>
@@ -2750,8 +2767,7 @@
         <v>0</v>
       </c>
       <c r="D8">
-        <f t="shared" si="1"/>
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="E8" t="s">
         <v>13</v>
@@ -2767,7 +2783,7 @@
       </c>
       <c r="I8" t="str">
         <f t="shared" si="0"/>
-        <v>be_wk13_20200724_pA_wv07</v>
+        <v>be_wk07_20200724_pA_wv07</v>
       </c>
       <c r="J8">
         <v>1</v>
@@ -2784,8 +2800,7 @@
         <v>0</v>
       </c>
       <c r="D9">
-        <f t="shared" si="1"/>
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="E9" t="s">
         <v>13</v>
@@ -2801,10 +2816,40 @@
       </c>
       <c r="I9" t="str">
         <f t="shared" si="0"/>
-        <v>be_wk15_20200806_pA_wv08</v>
+        <v>be_wk08_20200806_pA_wv08</v>
       </c>
       <c r="J9">
         <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="A10" t="s">
+        <v>64</v>
+      </c>
+      <c r="B10">
+        <v>2</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>9</v>
+      </c>
+      <c r="E10" t="s">
+        <v>15</v>
+      </c>
+      <c r="F10">
+        <v>1</v>
+      </c>
+      <c r="G10" s="1">
+        <v>44155</v>
+      </c>
+      <c r="H10" t="s">
+        <v>87</v>
+      </c>
+      <c r="I10" t="str">
+        <f t="shared" si="0"/>
+        <v>be_wk09_20201120_pB_wv01</v>
       </c>
     </row>
   </sheetData>
@@ -2817,7 +2862,7 @@
   <dimension ref="A1:O9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2916,7 +2961,7 @@
         <v>73</v>
       </c>
       <c r="D3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E3" t="s">
         <v>13</v>
@@ -2932,7 +2977,7 @@
       </c>
       <c r="I3" t="str">
         <f t="shared" si="0"/>
-        <v>nl_wk03_20200518_pA_wv02</v>
+        <v>nl_wk02_20200518_pA_wv02</v>
       </c>
       <c r="K3">
         <v>1</v>
@@ -2949,8 +2994,7 @@
         <v>73</v>
       </c>
       <c r="D4">
-        <f>D3+2</f>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E4" t="s">
         <v>13</v>
@@ -2966,7 +3010,7 @@
       </c>
       <c r="I4" t="str">
         <f t="shared" si="0"/>
-        <v>nl_wk05_20200601_pA_wv03</v>
+        <v>nl_wk03_20200601_pA_wv03</v>
       </c>
       <c r="K4">
         <v>1</v>
@@ -2983,8 +3027,7 @@
         <v>73</v>
       </c>
       <c r="D5">
-        <f t="shared" ref="D5:D9" si="1">D4+2</f>
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E5" t="s">
         <v>13</v>
@@ -3000,7 +3043,7 @@
       </c>
       <c r="I5" t="str">
         <f t="shared" si="0"/>
-        <v>nl_wk07_20200612_pA_wv04</v>
+        <v>nl_wk04_20200612_pA_wv04</v>
       </c>
       <c r="K5">
         <v>1</v>
@@ -3017,8 +3060,7 @@
         <v>73</v>
       </c>
       <c r="D6">
-        <f t="shared" si="1"/>
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="E6" t="s">
         <v>13</v>
@@ -3034,7 +3076,7 @@
       </c>
       <c r="I6" t="str">
         <f t="shared" si="0"/>
-        <v>nl_wk09_20200626_pA_wv05</v>
+        <v>nl_wk05_20200626_pA_wv05</v>
       </c>
       <c r="K6">
         <v>1</v>
@@ -3051,8 +3093,7 @@
         <v>73</v>
       </c>
       <c r="D7">
-        <f t="shared" si="1"/>
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="E7" t="s">
         <v>13</v>
@@ -3068,7 +3109,7 @@
       </c>
       <c r="I7" t="str">
         <f t="shared" si="0"/>
-        <v>nl_wk11_20200710_pA_wv06</v>
+        <v>nl_wk06_20200710_pA_wv06</v>
       </c>
       <c r="K7">
         <v>1</v>
@@ -3085,8 +3126,7 @@
         <v>73</v>
       </c>
       <c r="D8">
-        <f t="shared" si="1"/>
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="E8" t="s">
         <v>13</v>
@@ -3102,7 +3142,7 @@
       </c>
       <c r="I8" t="str">
         <f t="shared" si="0"/>
-        <v>nl_wk13_20200724_pA_wv07</v>
+        <v>nl_wk07_20200724_pA_wv07</v>
       </c>
       <c r="K8">
         <v>1</v>
@@ -3119,8 +3159,7 @@
         <v>73</v>
       </c>
       <c r="D9">
-        <f t="shared" si="1"/>
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="E9" t="s">
         <v>13</v>
@@ -3136,7 +3175,7 @@
       </c>
       <c r="I9" t="str">
         <f t="shared" si="0"/>
-        <v>nl_wk15_20200806_pA_wv08</v>
+        <v>nl_wk08_20200806_pA_wv08</v>
       </c>
       <c r="K9">
         <v>1</v>
@@ -3151,7 +3190,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D2B755C-13CE-401F-B50D-AD8E835063B7}">
   <dimension ref="A1:O7"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
@@ -3247,7 +3288,7 @@
         <v>74</v>
       </c>
       <c r="D3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E3" t="s">
         <v>13</v>
@@ -3263,7 +3304,7 @@
       </c>
       <c r="I3" t="str">
         <f t="shared" si="0"/>
-        <v>no_wk03_20200529_pA_wv02</v>
+        <v>no_wk02_20200529_pA_wv02</v>
       </c>
       <c r="K3">
         <v>1</v>
@@ -3280,7 +3321,7 @@
         <v>74</v>
       </c>
       <c r="D4">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E4" t="s">
         <v>13</v>
@@ -3296,7 +3337,7 @@
       </c>
       <c r="I4" t="str">
         <f t="shared" si="0"/>
-        <v>no_wk05_20200622_pA_wv03</v>
+        <v>no_wk03_20200622_pA_wv03</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.45">
@@ -3310,8 +3351,7 @@
         <v>74</v>
       </c>
       <c r="D5">
-        <f>D4+2</f>
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E5" t="s">
         <v>13</v>
@@ -3327,7 +3367,7 @@
       </c>
       <c r="I5" t="str">
         <f t="shared" si="0"/>
-        <v>no_wk07_20200731_pA_wv04</v>
+        <v>no_wk04_20200731_pA_wv04</v>
       </c>
       <c r="K5">
         <v>1</v>
@@ -3344,8 +3384,7 @@
         <v>74</v>
       </c>
       <c r="D6">
-        <f t="shared" ref="D6:D7" si="1">D5+2</f>
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="E6" t="s">
         <v>13</v>
@@ -3361,7 +3400,7 @@
       </c>
       <c r="I6" t="str">
         <f t="shared" si="0"/>
-        <v>no_wk09_20200906_pA_wv05</v>
+        <v>no_wk05_20200906_pA_wv05</v>
       </c>
       <c r="K6">
         <v>1</v>
@@ -3378,8 +3417,7 @@
         <v>74</v>
       </c>
       <c r="D7">
-        <f t="shared" si="1"/>
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="E7" t="s">
         <v>13</v>
@@ -3395,7 +3433,7 @@
       </c>
       <c r="I7" t="str">
         <f t="shared" si="0"/>
-        <v>no_wk11_20201001_pA_wv06</v>
+        <v>no_wk06_20201001_pA_wv06</v>
       </c>
       <c r="K7">
         <v>1</v>

</xml_diff>

<commit_message>
remove latest belgium as not cleaned yet
</commit_message>
<xml_diff>
--- a/data/spss_files.xlsx
+++ b/data/spss_files.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jarvisc1\Documents\projects\comix_data_clean\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E0916EE-1A68-4BE9-8F8A-6C3D45A3E4EE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C69DC82-D0B6-40D4-88CA-4E8824599945}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2500,7 +2500,7 @@
   <dimension ref="A1:N10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2844,12 +2844,8 @@
       <c r="G10" s="1">
         <v>44155</v>
       </c>
-      <c r="H10" t="s">
+      <c r="I10" t="s">
         <v>87</v>
-      </c>
-      <c r="I10" t="str">
-        <f t="shared" si="0"/>
-        <v>be_wk09_20201120_pB_wv01</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update for new data UK E8 survey round 35
</commit_message>
<xml_diff>
--- a/data/spss_files.xlsx
+++ b/data/spss_files.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jarvisc1\Documents\projects\comix_data_clean\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C69DC82-D0B6-40D4-88CA-4E8824599945}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9EAEA06-9E7A-4997-A7A1-EB7EE10908C2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="5" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="89">
   <si>
     <t>country</t>
   </si>
@@ -302,6 +302,9 @@
   </si>
   <si>
     <t>20_060765_BE2_Wave1_Final_v1_20112020_IntClientUse</t>
+  </si>
+  <si>
+    <t>20-056790_Final_PFW8_v1_IntUse</t>
   </si>
 </sst>
 </file>
@@ -634,8 +637,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O52"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K46" sqref="K46"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="A47" sqref="A47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -720,7 +723,7 @@
         <v>14</v>
       </c>
       <c r="I2" t="str">
-        <f t="shared" ref="I2:I46" si="0">C2&amp;"_"&amp;"wk"&amp;TEXT(D2,"00")&amp;"_"&amp;YEAR(G2)&amp;TEXT(G2,"MM")&amp;TEXT(G2,"DD")&amp;"_p"&amp;E2&amp;"_wv"&amp;TEXT(F2,"00")&amp;""</f>
+        <f t="shared" ref="I2:I47" si="0">C2&amp;"_"&amp;"wk"&amp;TEXT(D2,"00")&amp;"_"&amp;YEAR(G2)&amp;TEXT(G2,"MM")&amp;TEXT(G2,"DD")&amp;"_p"&amp;E2&amp;"_wv"&amp;TEXT(F2,"00")&amp;""</f>
         <v>uk_wk01_20200402_pA_wv01</v>
       </c>
       <c r="J2">
@@ -2378,7 +2381,22 @@
         <f t="shared" si="4"/>
         <v>8</v>
       </c>
-      <c r="G47" s="1"/>
+      <c r="G47" s="1">
+        <v>44161</v>
+      </c>
+      <c r="H47" t="s">
+        <v>88</v>
+      </c>
+      <c r="I47" t="str">
+        <f t="shared" si="0"/>
+        <v>uk_wk35_20201126_pF_wv08</v>
+      </c>
+      <c r="J47">
+        <v>1</v>
+      </c>
+      <c r="K47">
+        <v>1</v>
+      </c>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A48">
@@ -2499,7 +2517,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C042354-CAAB-48AD-AFC2-2197A2D12C9D}">
   <dimension ref="A1:N10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
@@ -2584,7 +2602,7 @@
         <v>65</v>
       </c>
       <c r="I2" t="str">
-        <f t="shared" ref="I2:I10" si="0">A2&amp;"_"&amp;"wk"&amp;TEXT(D2,"00")&amp;"_"&amp;YEAR(G2)&amp;TEXT(G2,"MM")&amp;TEXT(G2,"DD")&amp;"_p"&amp;E2&amp;"_wv"&amp;TEXT(F2,"00")&amp;""</f>
+        <f t="shared" ref="I2:I9" si="0">A2&amp;"_"&amp;"wk"&amp;TEXT(D2,"00")&amp;"_"&amp;YEAR(G2)&amp;TEXT(G2,"MM")&amp;TEXT(G2,"DD")&amp;"_p"&amp;E2&amp;"_wv"&amp;TEXT(F2,"00")&amp;""</f>
         <v>be_wk01_20200429_pA_wv01</v>
       </c>
       <c r="J2">

</xml_diff>

<commit_message>
Updates from Kerry review closes #24
</commit_message>
<xml_diff>
--- a/data/spss_files.xlsx
+++ b/data/spss_files.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jarvisc1\Documents\projects\comix_data_clean\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9EAEA06-9E7A-4997-A7A1-EB7EE10908C2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{660CA9BD-8E67-419F-8B82-4C976ADF9302}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="90">
   <si>
     <t>country</t>
   </si>
@@ -305,6 +305,9 @@
   </si>
   <si>
     <t>20-056790_Final_PFW8_v1_IntUse</t>
+  </si>
+  <si>
+    <t>20-040199-01_Final_PEW9_v1_031220_Intclientuse</t>
   </si>
 </sst>
 </file>
@@ -638,7 +641,7 @@
   <dimension ref="A1:O52"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="A47" sqref="A47"/>
+      <selection activeCell="A48" sqref="A48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -723,7 +726,7 @@
         <v>14</v>
       </c>
       <c r="I2" t="str">
-        <f t="shared" ref="I2:I47" si="0">C2&amp;"_"&amp;"wk"&amp;TEXT(D2,"00")&amp;"_"&amp;YEAR(G2)&amp;TEXT(G2,"MM")&amp;TEXT(G2,"DD")&amp;"_p"&amp;E2&amp;"_wv"&amp;TEXT(F2,"00")&amp;""</f>
+        <f t="shared" ref="I2:I48" si="0">C2&amp;"_"&amp;"wk"&amp;TEXT(D2,"00")&amp;"_"&amp;YEAR(G2)&amp;TEXT(G2,"MM")&amp;TEXT(G2,"DD")&amp;"_p"&amp;E2&amp;"_wv"&amp;TEXT(F2,"00")&amp;""</f>
         <v>uk_wk01_20200402_pA_wv01</v>
       </c>
       <c r="J2">
@@ -2418,7 +2421,16 @@
         <f t="shared" si="4"/>
         <v>9</v>
       </c>
-      <c r="G48" s="1"/>
+      <c r="G48" s="1">
+        <v>43924</v>
+      </c>
+      <c r="H48" t="s">
+        <v>89</v>
+      </c>
+      <c r="I48" t="str">
+        <f t="shared" si="0"/>
+        <v>uk_wk36_20200403_pE_wv09</v>
+      </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A49">

</xml_diff>

<commit_message>
Add latest data to spss file
</commit_message>
<xml_diff>
--- a/data/spss_files.xlsx
+++ b/data/spss_files.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jarvisc1\Documents\projects\comix_data_clean\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49B0E404-2E9C-4D78-8CB7-BB3B25B411E9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{992DB4B9-5D55-49B9-B1E4-AE4EB13D7F5E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1950" yWindow="1950" windowWidth="21600" windowHeight="11130" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1073" yWindow="1073" windowWidth="21600" windowHeight="11542" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="5" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="92">
   <si>
     <t>country</t>
   </si>
@@ -311,6 +311,9 @@
   </si>
   <si>
     <t>20-056790_PFW9_Final_DPClean_IntUse</t>
+  </si>
+  <si>
+    <t>20-040199-01_Final_PEW10_v1_171220_Intclientuse</t>
   </si>
 </sst>
 </file>
@@ -633,7 +636,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -644,19 +647,19 @@
   <dimension ref="A1:O52"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="J49" sqref="J49"/>
+      <selection activeCell="H50" sqref="H50"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" customWidth="1"/>
-    <col min="7" max="7" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="58.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.3984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.3984375" customWidth="1"/>
+    <col min="7" max="7" width="10.73046875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="58.265625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="25.265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>83</v>
       </c>
@@ -703,7 +706,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A2">
         <v>1</v>
       </c>
@@ -729,7 +732,7 @@
         <v>14</v>
       </c>
       <c r="I2" t="str">
-        <f t="shared" ref="I2:I49" si="0">C2&amp;"_"&amp;"wk"&amp;TEXT(D2,"00")&amp;"_"&amp;YEAR(G2)&amp;TEXT(G2,"MM")&amp;TEXT(G2,"DD")&amp;"_p"&amp;E2&amp;"_wv"&amp;TEXT(F2,"00")&amp;""</f>
+        <f t="shared" ref="I2:I50" si="0">C2&amp;"_"&amp;"wk"&amp;TEXT(D2,"00")&amp;"_"&amp;YEAR(G2)&amp;TEXT(G2,"MM")&amp;TEXT(G2,"DD")&amp;"_p"&amp;E2&amp;"_wv"&amp;TEXT(F2,"00")&amp;""</f>
         <v>uk_wk01_20200402_pA_wv01</v>
       </c>
       <c r="J2">
@@ -739,7 +742,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A3">
         <v>1</v>
       </c>
@@ -775,7 +778,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A4">
         <v>1</v>
       </c>
@@ -811,7 +814,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A5">
         <v>1</v>
       </c>
@@ -847,7 +850,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A6">
         <v>1</v>
       </c>
@@ -883,7 +886,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A7">
         <v>1</v>
       </c>
@@ -919,7 +922,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A8">
         <v>1</v>
       </c>
@@ -958,7 +961,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A9">
         <v>2</v>
       </c>
@@ -994,7 +997,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A10">
         <v>1</v>
       </c>
@@ -1031,7 +1034,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A11">
         <v>2</v>
       </c>
@@ -1068,7 +1071,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A12">
         <v>1</v>
       </c>
@@ -1105,7 +1108,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A13">
         <v>2</v>
       </c>
@@ -1143,7 +1146,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A14">
         <v>1</v>
       </c>
@@ -1180,7 +1183,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A15">
         <v>2</v>
       </c>
@@ -1217,7 +1220,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A16">
         <v>1</v>
       </c>
@@ -1254,7 +1257,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A17">
         <v>2</v>
       </c>
@@ -1291,7 +1294,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A18">
         <v>1</v>
       </c>
@@ -1328,7 +1331,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A19">
         <v>2</v>
       </c>
@@ -1365,7 +1368,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A20">
         <v>1</v>
       </c>
@@ -1402,7 +1405,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A21">
         <v>2</v>
       </c>
@@ -1439,7 +1442,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A22">
         <v>1</v>
       </c>
@@ -1476,7 +1479,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A23">
         <v>2</v>
       </c>
@@ -1513,7 +1516,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A24">
         <v>1</v>
       </c>
@@ -1550,7 +1553,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A25">
         <v>2</v>
       </c>
@@ -1587,7 +1590,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A26">
         <v>1</v>
       </c>
@@ -1624,7 +1627,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A27">
         <v>2</v>
       </c>
@@ -1661,7 +1664,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A28">
         <v>1</v>
       </c>
@@ -1701,7 +1704,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A29">
         <v>1</v>
       </c>
@@ -1741,7 +1744,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A30">
         <v>1</v>
       </c>
@@ -1778,7 +1781,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A31">
         <v>2</v>
       </c>
@@ -1814,7 +1817,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A32">
         <v>3</v>
       </c>
@@ -1853,7 +1856,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A33">
         <v>3</v>
       </c>
@@ -1889,7 +1892,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A34">
         <v>3</v>
       </c>
@@ -1926,7 +1929,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A35">
         <v>3</v>
       </c>
@@ -1963,7 +1966,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A36">
         <v>3</v>
       </c>
@@ -2000,7 +2003,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A37">
         <v>3</v>
       </c>
@@ -2037,7 +2040,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A38">
         <v>3</v>
       </c>
@@ -2074,7 +2077,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A39">
         <v>3</v>
       </c>
@@ -2111,7 +2114,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A40">
         <v>3</v>
       </c>
@@ -2148,7 +2151,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A41">
         <v>3</v>
       </c>
@@ -2185,7 +2188,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A42">
         <v>3</v>
       </c>
@@ -2222,7 +2225,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A43">
         <v>3</v>
       </c>
@@ -2259,7 +2262,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A44">
         <v>3</v>
       </c>
@@ -2293,7 +2296,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A45">
         <v>3</v>
       </c>
@@ -2330,7 +2333,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A46">
         <v>3</v>
       </c>
@@ -2367,7 +2370,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A47">
         <v>3</v>
       </c>
@@ -2404,7 +2407,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A48">
         <v>3</v>
       </c>
@@ -2438,7 +2441,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A49">
         <v>3</v>
       </c>
@@ -2472,7 +2475,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A50">
         <v>3</v>
       </c>
@@ -2492,9 +2495,18 @@
         <f t="shared" si="4"/>
         <v>10</v>
       </c>
-      <c r="G50" s="1"/>
-    </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G50" s="1">
+        <v>44182</v>
+      </c>
+      <c r="H50" t="s">
+        <v>91</v>
+      </c>
+      <c r="I50" t="str">
+        <f t="shared" si="0"/>
+        <v>uk_wk38_20201217_pE_wv10</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A51">
         <v>3</v>
       </c>
@@ -2516,7 +2528,7 @@
       </c>
       <c r="G51" s="1"/>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A52">
         <v>3</v>
       </c>
@@ -2551,17 +2563,17 @@
       <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.42578125" customWidth="1"/>
+    <col min="2" max="2" width="12.3984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.3984375" customWidth="1"/>
     <col min="5" max="6" width="5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.5703125" customWidth="1"/>
-    <col min="8" max="8" width="58.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="30.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.59765625" customWidth="1"/>
+    <col min="8" max="8" width="58.59765625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="30.59765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2605,7 +2617,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>64</v>
       </c>
@@ -2638,7 +2650,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>64</v>
       </c>
@@ -2671,7 +2683,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>64</v>
       </c>
@@ -2704,7 +2716,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>64</v>
       </c>
@@ -2737,7 +2749,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>64</v>
       </c>
@@ -2770,7 +2782,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>64</v>
       </c>
@@ -2803,7 +2815,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>64</v>
       </c>
@@ -2836,7 +2848,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>64</v>
       </c>
@@ -2869,7 +2881,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>64</v>
       </c>
@@ -2908,12 +2920,12 @@
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="14" max="14" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.59765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>83</v>
       </c>
@@ -2960,7 +2972,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2993,7 +3005,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A3">
         <v>1</v>
       </c>
@@ -3026,7 +3038,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A4">
         <v>1</v>
       </c>
@@ -3059,7 +3071,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A5">
         <v>1</v>
       </c>
@@ -3092,7 +3104,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A6">
         <v>1</v>
       </c>
@@ -3125,7 +3137,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A7">
         <v>1</v>
       </c>
@@ -3158,7 +3170,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A8">
         <v>1</v>
       </c>
@@ -3191,7 +3203,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A9">
         <v>1</v>
       </c>
@@ -3237,13 +3249,13 @@
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" customWidth="1"/>
+    <col min="1" max="1" width="12.3984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.3984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>83</v>
       </c>
@@ -3290,7 +3302,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A2">
         <v>1</v>
       </c>
@@ -3320,7 +3332,7 @@
         <v>no_wk01_20200501_pA_wv01</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A3">
         <v>1</v>
       </c>
@@ -3353,7 +3365,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A4">
         <v>1</v>
       </c>
@@ -3383,7 +3395,7 @@
         <v>no_wk03_20200622_pA_wv03</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A5">
         <v>1</v>
       </c>
@@ -3416,7 +3428,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A6">
         <v>1</v>
       </c>
@@ -3449,7 +3461,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A7">
         <v>1</v>
       </c>

</xml_diff>

<commit_message>
Add latest UK data
</commit_message>
<xml_diff>
--- a/data/spss_files.xlsx
+++ b/data/spss_files.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jarvisc1\Documents\projects\comix_data_clean\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{992DB4B9-5D55-49B9-B1E4-AE4EB13D7F5E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82DC0BEA-7391-4056-AFBF-B4FA2B76B140}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1073" yWindow="1073" windowWidth="21600" windowHeight="11542" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18120" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="5" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="94">
   <si>
     <t>country</t>
   </si>
@@ -314,6 +314,12 @@
   </si>
   <si>
     <t>20-040199-01_Final_PEW10_v1_171220_Intclientuse</t>
+  </si>
+  <si>
+    <t>20-056790_PFW10_Final_DPClean_IntUse</t>
+  </si>
+  <si>
+    <t>20-040199_PEW11_Final_DPClean_IntUse</t>
   </si>
 </sst>
 </file>
@@ -636,7 +642,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -647,19 +653,19 @@
   <dimension ref="A1:O52"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="H50" sqref="H50"/>
+      <selection activeCell="I52" sqref="I52"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="12.3984375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.3984375" customWidth="1"/>
-    <col min="7" max="7" width="10.73046875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="58.265625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="25.265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.3828125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.3828125" customWidth="1"/>
+    <col min="7" max="7" width="10.69140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="58.23046875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="25.23046875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>83</v>
       </c>
@@ -706,7 +712,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A2">
         <v>1</v>
       </c>
@@ -732,7 +738,7 @@
         <v>14</v>
       </c>
       <c r="I2" t="str">
-        <f t="shared" ref="I2:I50" si="0">C2&amp;"_"&amp;"wk"&amp;TEXT(D2,"00")&amp;"_"&amp;YEAR(G2)&amp;TEXT(G2,"MM")&amp;TEXT(G2,"DD")&amp;"_p"&amp;E2&amp;"_wv"&amp;TEXT(F2,"00")&amp;""</f>
+        <f t="shared" ref="I2:I52" si="0">C2&amp;"_"&amp;"wk"&amp;TEXT(D2,"00")&amp;"_"&amp;YEAR(G2)&amp;TEXT(G2,"MM")&amp;TEXT(G2,"DD")&amp;"_p"&amp;E2&amp;"_wv"&amp;TEXT(F2,"00")&amp;""</f>
         <v>uk_wk01_20200402_pA_wv01</v>
       </c>
       <c r="J2">
@@ -742,7 +748,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A3">
         <v>1</v>
       </c>
@@ -778,7 +784,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A4">
         <v>1</v>
       </c>
@@ -814,7 +820,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A5">
         <v>1</v>
       </c>
@@ -850,7 +856,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A6">
         <v>1</v>
       </c>
@@ -886,7 +892,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A7">
         <v>1</v>
       </c>
@@ -922,7 +928,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A8">
         <v>1</v>
       </c>
@@ -961,7 +967,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A9">
         <v>2</v>
       </c>
@@ -997,7 +1003,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A10">
         <v>1</v>
       </c>
@@ -1034,7 +1040,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A11">
         <v>2</v>
       </c>
@@ -1071,7 +1077,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A12">
         <v>1</v>
       </c>
@@ -1108,7 +1114,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A13">
         <v>2</v>
       </c>
@@ -1146,7 +1152,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A14">
         <v>1</v>
       </c>
@@ -1183,7 +1189,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A15">
         <v>2</v>
       </c>
@@ -1220,7 +1226,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A16">
         <v>1</v>
       </c>
@@ -1257,7 +1263,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A17">
         <v>2</v>
       </c>
@@ -1294,7 +1300,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A18">
         <v>1</v>
       </c>
@@ -1331,7 +1337,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A19">
         <v>2</v>
       </c>
@@ -1368,7 +1374,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A20">
         <v>1</v>
       </c>
@@ -1405,7 +1411,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A21">
         <v>2</v>
       </c>
@@ -1442,7 +1448,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A22">
         <v>1</v>
       </c>
@@ -1479,7 +1485,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A23">
         <v>2</v>
       </c>
@@ -1516,7 +1522,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A24">
         <v>1</v>
       </c>
@@ -1553,7 +1559,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A25">
         <v>2</v>
       </c>
@@ -1590,7 +1596,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A26">
         <v>1</v>
       </c>
@@ -1627,7 +1633,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A27">
         <v>2</v>
       </c>
@@ -1664,7 +1670,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A28">
         <v>1</v>
       </c>
@@ -1704,7 +1710,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A29">
         <v>1</v>
       </c>
@@ -1744,7 +1750,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A30">
         <v>1</v>
       </c>
@@ -1781,7 +1787,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A31">
         <v>2</v>
       </c>
@@ -1817,7 +1823,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A32">
         <v>3</v>
       </c>
@@ -1856,7 +1862,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A33">
         <v>3</v>
       </c>
@@ -1892,7 +1898,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A34">
         <v>3</v>
       </c>
@@ -1929,7 +1935,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A35">
         <v>3</v>
       </c>
@@ -1966,7 +1972,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A36">
         <v>3</v>
       </c>
@@ -2003,7 +2009,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A37">
         <v>3</v>
       </c>
@@ -2040,7 +2046,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A38">
         <v>3</v>
       </c>
@@ -2077,7 +2083,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A39">
         <v>3</v>
       </c>
@@ -2114,7 +2120,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A40">
         <v>3</v>
       </c>
@@ -2151,7 +2157,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A41">
         <v>3</v>
       </c>
@@ -2188,7 +2194,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A42">
         <v>3</v>
       </c>
@@ -2225,7 +2231,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A43">
         <v>3</v>
       </c>
@@ -2262,7 +2268,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A44">
         <v>3</v>
       </c>
@@ -2296,7 +2302,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A45">
         <v>3</v>
       </c>
@@ -2333,7 +2339,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A46">
         <v>3</v>
       </c>
@@ -2370,7 +2376,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A47">
         <v>3</v>
       </c>
@@ -2407,7 +2413,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A48">
         <v>3</v>
       </c>
@@ -2441,7 +2447,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A49">
         <v>3</v>
       </c>
@@ -2475,7 +2481,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A50">
         <v>3</v>
       </c>
@@ -2505,8 +2511,11 @@
         <f t="shared" si="0"/>
         <v>uk_wk38_20201217_pE_wv10</v>
       </c>
-    </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="J50">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A51">
         <v>3</v>
       </c>
@@ -2526,9 +2535,21 @@
         <f t="shared" si="4"/>
         <v>10</v>
       </c>
-      <c r="G51" s="1"/>
-    </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="G51" s="1">
+        <v>44189</v>
+      </c>
+      <c r="H51" t="s">
+        <v>92</v>
+      </c>
+      <c r="I51" t="str">
+        <f t="shared" si="0"/>
+        <v>uk_wk39_20201224_pF_wv10</v>
+      </c>
+      <c r="J51">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A52">
         <v>3</v>
       </c>
@@ -2548,7 +2569,19 @@
         <f t="shared" si="4"/>
         <v>11</v>
       </c>
-      <c r="G52" s="1"/>
+      <c r="G52" s="1">
+        <v>44196</v>
+      </c>
+      <c r="H52" t="s">
+        <v>93</v>
+      </c>
+      <c r="I52" t="str">
+        <f t="shared" si="0"/>
+        <v>uk_wk40_20201231_pE_wv11</v>
+      </c>
+      <c r="J52">
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2563,17 +2596,17 @@
       <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="2" max="2" width="12.3984375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.3984375" customWidth="1"/>
+    <col min="2" max="2" width="12.3828125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.3828125" customWidth="1"/>
     <col min="5" max="6" width="5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.59765625" customWidth="1"/>
-    <col min="8" max="8" width="58.59765625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="30.59765625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.61328125" customWidth="1"/>
+    <col min="8" max="8" width="58.61328125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="30.61328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2617,7 +2650,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>64</v>
       </c>
@@ -2650,7 +2683,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>64</v>
       </c>
@@ -2683,7 +2716,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>64</v>
       </c>
@@ -2716,7 +2749,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>64</v>
       </c>
@@ -2749,7 +2782,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
         <v>64</v>
       </c>
@@ -2782,7 +2815,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
         <v>64</v>
       </c>
@@ -2815,7 +2848,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
         <v>64</v>
       </c>
@@ -2848,7 +2881,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
         <v>64</v>
       </c>
@@ -2881,7 +2914,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
         <v>64</v>
       </c>
@@ -2920,12 +2953,12 @@
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="14" max="14" width="9.59765625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.61328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>83</v>
       </c>
@@ -2972,7 +3005,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A2">
         <v>1</v>
       </c>
@@ -3005,7 +3038,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A3">
         <v>1</v>
       </c>
@@ -3038,7 +3071,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A4">
         <v>1</v>
       </c>
@@ -3071,7 +3104,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A5">
         <v>1</v>
       </c>
@@ -3104,7 +3137,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A6">
         <v>1</v>
       </c>
@@ -3137,7 +3170,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A7">
         <v>1</v>
       </c>
@@ -3170,7 +3203,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A8">
         <v>1</v>
       </c>
@@ -3203,7 +3236,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A9">
         <v>1</v>
       </c>
@@ -3249,13 +3282,13 @@
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="12.3984375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.3984375" customWidth="1"/>
+    <col min="1" max="1" width="12.3828125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.3828125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>83</v>
       </c>
@@ -3302,7 +3335,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A2">
         <v>1</v>
       </c>
@@ -3332,7 +3365,7 @@
         <v>no_wk01_20200501_pA_wv01</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A3">
         <v>1</v>
       </c>
@@ -3365,7 +3398,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A4">
         <v>1</v>
       </c>
@@ -3395,7 +3428,7 @@
         <v>no_wk03_20200622_pA_wv03</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A5">
         <v>1</v>
       </c>
@@ -3428,7 +3461,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A6">
         <v>1</v>
       </c>
@@ -3461,7 +3494,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A7">
         <v>1</v>
       </c>

</xml_diff>

<commit_message>
Add in latest data
</commit_message>
<xml_diff>
--- a/data/spss_files.xlsx
+++ b/data/spss_files.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jarvisc1\Documents\projects\comix_data_clean\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BF8E04E-5745-46C3-BD45-62470B15BAA4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73746B90-BE51-4CE7-9A8C-DC7E1043BE6F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="5" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="99">
   <si>
     <t>country</t>
   </si>
@@ -332,6 +332,9 @@
   </si>
   <si>
     <t>Panel E and F for UK</t>
+  </si>
+  <si>
+    <t>20-056790_PFW11_Final_DPClean_IntUse</t>
   </si>
 </sst>
 </file>
@@ -652,18 +655,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2637BBD4-AFF7-4386-815F-A64B43C0CC5D}">
   <dimension ref="A4:B7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1</v>
       </c>
@@ -671,7 +674,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2</v>
       </c>
@@ -679,7 +682,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>3</v>
       </c>
@@ -694,22 +697,22 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O52"/>
+  <dimension ref="A1:O53"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="I52" sqref="I52"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="J53" sqref="J53"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.3828125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.3828125" customWidth="1"/>
-    <col min="7" max="7" width="10.69140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="58.23046875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="25.23046875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" customWidth="1"/>
+    <col min="7" max="7" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="58.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="25.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>83</v>
       </c>
@@ -756,7 +759,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -782,7 +785,7 @@
         <v>14</v>
       </c>
       <c r="I2" t="str">
-        <f t="shared" ref="I2:I52" si="0">C2&amp;"_"&amp;"wk"&amp;TEXT(D2,"00")&amp;"_"&amp;YEAR(G2)&amp;TEXT(G2,"MM")&amp;TEXT(G2,"DD")&amp;"_p"&amp;E2&amp;"_wv"&amp;TEXT(F2,"00")&amp;""</f>
+        <f t="shared" ref="I2:I53" si="0">C2&amp;"_"&amp;"wk"&amp;TEXT(D2,"00")&amp;"_"&amp;YEAR(G2)&amp;TEXT(G2,"MM")&amp;TEXT(G2,"DD")&amp;"_p"&amp;E2&amp;"_wv"&amp;TEXT(F2,"00")&amp;""</f>
         <v>uk_wk01_20200402_pA_wv01</v>
       </c>
       <c r="J2">
@@ -792,7 +795,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -828,7 +831,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1</v>
       </c>
@@ -864,7 +867,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1</v>
       </c>
@@ -900,7 +903,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>1</v>
       </c>
@@ -936,7 +939,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>1</v>
       </c>
@@ -972,7 +975,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>1</v>
       </c>
@@ -1011,7 +1014,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>2</v>
       </c>
@@ -1047,7 +1050,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>1</v>
       </c>
@@ -1084,7 +1087,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>2</v>
       </c>
@@ -1121,7 +1124,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>1</v>
       </c>
@@ -1158,7 +1161,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>2</v>
       </c>
@@ -1196,7 +1199,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>1</v>
       </c>
@@ -1233,7 +1236,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>2</v>
       </c>
@@ -1270,7 +1273,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>1</v>
       </c>
@@ -1307,7 +1310,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>2</v>
       </c>
@@ -1344,7 +1347,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>1</v>
       </c>
@@ -1381,7 +1384,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>2</v>
       </c>
@@ -1418,7 +1421,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>1</v>
       </c>
@@ -1455,7 +1458,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>2</v>
       </c>
@@ -1492,7 +1495,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>1</v>
       </c>
@@ -1529,7 +1532,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>2</v>
       </c>
@@ -1566,7 +1569,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>1</v>
       </c>
@@ -1603,7 +1606,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>2</v>
       </c>
@@ -1640,7 +1643,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>1</v>
       </c>
@@ -1677,7 +1680,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>2</v>
       </c>
@@ -1714,7 +1717,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>1</v>
       </c>
@@ -1754,7 +1757,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>1</v>
       </c>
@@ -1794,7 +1797,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>1</v>
       </c>
@@ -1831,7 +1834,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>2</v>
       </c>
@@ -1867,7 +1870,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>3</v>
       </c>
@@ -1906,7 +1909,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>3</v>
       </c>
@@ -1942,7 +1945,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>3</v>
       </c>
@@ -1959,7 +1962,7 @@
         <v>50</v>
       </c>
       <c r="F34">
-        <f t="shared" ref="F34:F52" si="4">F32+1</f>
+        <f t="shared" ref="F34:F53" si="4">F32+1</f>
         <v>2</v>
       </c>
       <c r="G34" s="1">
@@ -1979,7 +1982,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>3</v>
       </c>
@@ -2016,7 +2019,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>3</v>
       </c>
@@ -2053,7 +2056,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>3</v>
       </c>
@@ -2090,7 +2093,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>3</v>
       </c>
@@ -2127,7 +2130,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>3</v>
       </c>
@@ -2164,7 +2167,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>3</v>
       </c>
@@ -2201,7 +2204,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>3</v>
       </c>
@@ -2238,7 +2241,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>3</v>
       </c>
@@ -2275,7 +2278,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>3</v>
       </c>
@@ -2312,7 +2315,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>3</v>
       </c>
@@ -2346,7 +2349,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>3</v>
       </c>
@@ -2383,7 +2386,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>3</v>
       </c>
@@ -2420,7 +2423,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>3</v>
       </c>
@@ -2457,7 +2460,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>3</v>
       </c>
@@ -2491,7 +2494,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>3</v>
       </c>
@@ -2525,7 +2528,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>3</v>
       </c>
@@ -2559,7 +2562,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>3</v>
       </c>
@@ -2593,7 +2596,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>3</v>
       </c>
@@ -2625,6 +2628,37 @@
       </c>
       <c r="J52">
         <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>3</v>
+      </c>
+      <c r="B53">
+        <v>0</v>
+      </c>
+      <c r="C53" t="s">
+        <v>12</v>
+      </c>
+      <c r="D53">
+        <v>41</v>
+      </c>
+      <c r="E53" t="s">
+        <v>52</v>
+      </c>
+      <c r="F53">
+        <f t="shared" si="4"/>
+        <v>11</v>
+      </c>
+      <c r="G53" s="1">
+        <v>44203</v>
+      </c>
+      <c r="H53" t="s">
+        <v>98</v>
+      </c>
+      <c r="I53" t="str">
+        <f t="shared" si="0"/>
+        <v>uk_wk41_20210107_pF_wv11</v>
       </c>
     </row>
   </sheetData>
@@ -2640,17 +2674,17 @@
       <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="12.3828125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.3828125" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.42578125" customWidth="1"/>
     <col min="5" max="6" width="5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.61328125" customWidth="1"/>
-    <col min="8" max="8" width="58.61328125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="30.61328125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.5703125" customWidth="1"/>
+    <col min="8" max="8" width="58.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="30.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2694,7 +2728,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>64</v>
       </c>
@@ -2727,7 +2761,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>64</v>
       </c>
@@ -2760,7 +2794,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>64</v>
       </c>
@@ -2793,7 +2827,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>64</v>
       </c>
@@ -2826,7 +2860,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>64</v>
       </c>
@@ -2859,7 +2893,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>64</v>
       </c>
@@ -2892,7 +2926,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>64</v>
       </c>
@@ -2925,7 +2959,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>64</v>
       </c>
@@ -2958,7 +2992,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>64</v>
       </c>
@@ -2997,12 +3031,12 @@
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="14" max="14" width="9.61328125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>83</v>
       </c>
@@ -3049,7 +3083,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -3082,7 +3116,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -3115,7 +3149,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1</v>
       </c>
@@ -3148,7 +3182,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1</v>
       </c>
@@ -3181,7 +3215,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>1</v>
       </c>
@@ -3214,7 +3248,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>1</v>
       </c>
@@ -3247,7 +3281,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>1</v>
       </c>
@@ -3280,7 +3314,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>1</v>
       </c>
@@ -3326,13 +3360,13 @@
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.3828125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.3828125" customWidth="1"/>
+    <col min="1" max="1" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>83</v>
       </c>
@@ -3379,7 +3413,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -3409,7 +3443,7 @@
         <v>no_wk01_20200501_pA_wv01</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -3442,7 +3476,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1</v>
       </c>
@@ -3472,7 +3506,7 @@
         <v>no_wk03_20200622_pA_wv03</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1</v>
       </c>
@@ -3505,7 +3539,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>1</v>
       </c>
@@ -3538,7 +3572,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>1</v>
       </c>

</xml_diff>

<commit_message>
Start version 5 for EU data
</commit_message>
<xml_diff>
--- a/data/spss_files.xlsx
+++ b/data/spss_files.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23530"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jarvisc1\Documents\projects\comix_data_clean\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96BBF966-885B-4689-93F1-43EE9E14E1C0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CCF68D0-2149-4F4A-9E49-7F4FFC90693A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="5" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="BE" sheetId="2" r:id="rId3"/>
     <sheet name="NL" sheetId="3" r:id="rId4"/>
     <sheet name="NO" sheetId="4" r:id="rId5"/>
+    <sheet name="Group1" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="113">
   <si>
     <t>country</t>
   </si>
@@ -335,6 +336,48 @@
   </si>
   <si>
     <t>20-056790_PFW11_Final_DPClean_IntUse</t>
+  </si>
+  <si>
+    <t>20-030971_AT_Wave1_Final_v1_110121_IntClientuse</t>
+  </si>
+  <si>
+    <t>at</t>
+  </si>
+  <si>
+    <t>dk</t>
+  </si>
+  <si>
+    <t>es</t>
+  </si>
+  <si>
+    <t>fr</t>
+  </si>
+  <si>
+    <t>it</t>
+  </si>
+  <si>
+    <t>pl</t>
+  </si>
+  <si>
+    <t>pt</t>
+  </si>
+  <si>
+    <t>20-030971_DK_Wave1_Final_v1_110121_IntClientuse</t>
+  </si>
+  <si>
+    <t>20-030971_ES_Wave1_Final_v1_110121_IntClientuse</t>
+  </si>
+  <si>
+    <t>20-030971_FR_Wave1_Final_v1_110121_IntClientuse</t>
+  </si>
+  <si>
+    <t>20-030971_IT_Wave1_Final_v1_110121_IntClientuse</t>
+  </si>
+  <si>
+    <t>20-030971_PL_Wave1_Final_v1_110121_IntClientuse</t>
+  </si>
+  <si>
+    <t>20-030971_PT_Wave1_Final_v1_110121_IntClientuse</t>
   </si>
 </sst>
 </file>
@@ -699,7 +742,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+    <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="H53" sqref="H53"/>
     </sheetView>
   </sheetViews>
@@ -2674,7 +2717,7 @@
   <dimension ref="A1:N10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection sqref="A1:M10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3611,4 +3654,302 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9984DEBA-9A58-467F-869B-4E55580BB1A4}">
+  <dimension ref="A1:M10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="7" max="7" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="59" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="27.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C1" t="s">
+        <v>84</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" t="s">
+        <v>79</v>
+      </c>
+      <c r="K1" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>100</v>
+      </c>
+      <c r="B2">
+        <v>5</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2" s="1">
+        <v>44207</v>
+      </c>
+      <c r="H2" t="s">
+        <v>99</v>
+      </c>
+      <c r="I2" t="str">
+        <f>A2&amp;"_"&amp;"wk"&amp;TEXT(D2,"00")&amp;"_"&amp;YEAR(G3)&amp;TEXT(G3,"MM")&amp;TEXT(G3,"DD")&amp;"_p"&amp;E2&amp;"_wv"&amp;TEXT(F2,"00")&amp;""</f>
+        <v>at_wk01_20210111_pA_wv01</v>
+      </c>
+      <c r="J2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>101</v>
+      </c>
+      <c r="B3">
+        <v>5</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="G3" s="1">
+        <v>44207</v>
+      </c>
+      <c r="H3" t="s">
+        <v>107</v>
+      </c>
+      <c r="I3" t="str">
+        <f t="shared" ref="I3:I9" si="0">A3&amp;"_"&amp;"wk"&amp;TEXT(D3,"00")&amp;"_"&amp;YEAR(G3)&amp;TEXT(G3,"MM")&amp;TEXT(G3,"DD")&amp;"_p"&amp;E3&amp;"_wv"&amp;TEXT(F3,"00")&amp;""</f>
+        <v>dk_wk01_20210111_pA_wv01</v>
+      </c>
+      <c r="J3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>102</v>
+      </c>
+      <c r="B4">
+        <v>5</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4" s="1">
+        <v>44207</v>
+      </c>
+      <c r="H4" t="s">
+        <v>108</v>
+      </c>
+      <c r="I4" t="str">
+        <f t="shared" si="0"/>
+        <v>es_wk01_20210111_pA_wv01</v>
+      </c>
+      <c r="J4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>103</v>
+      </c>
+      <c r="B5">
+        <v>5</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+      <c r="G5" s="1">
+        <v>44207</v>
+      </c>
+      <c r="H5" t="s">
+        <v>109</v>
+      </c>
+      <c r="I5" t="str">
+        <f t="shared" si="0"/>
+        <v>fr_wk01_20210111_pA_wv01</v>
+      </c>
+      <c r="J5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>104</v>
+      </c>
+      <c r="B6">
+        <v>5</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6" t="s">
+        <v>13</v>
+      </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
+      <c r="G6" s="1">
+        <v>44207</v>
+      </c>
+      <c r="H6" t="s">
+        <v>110</v>
+      </c>
+      <c r="I6" t="str">
+        <f t="shared" si="0"/>
+        <v>it_wk01_20210111_pA_wv01</v>
+      </c>
+      <c r="J6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>105</v>
+      </c>
+      <c r="B7">
+        <v>5</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F7">
+        <v>1</v>
+      </c>
+      <c r="G7" s="1">
+        <v>44207</v>
+      </c>
+      <c r="H7" t="s">
+        <v>111</v>
+      </c>
+      <c r="I7" t="str">
+        <f t="shared" si="0"/>
+        <v>pl_wk01_20210111_pA_wv01</v>
+      </c>
+      <c r="J7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>106</v>
+      </c>
+      <c r="B8">
+        <v>5</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8" t="s">
+        <v>13</v>
+      </c>
+      <c r="F8">
+        <v>1</v>
+      </c>
+      <c r="G8" s="1">
+        <v>44207</v>
+      </c>
+      <c r="H8" t="s">
+        <v>112</v>
+      </c>
+      <c r="I8" t="str">
+        <f t="shared" si="0"/>
+        <v>pt_wk01_20210111_pA_wv01</v>
+      </c>
+      <c r="J8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="G9" s="1"/>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="G10" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Update for new group 1 data
</commit_message>
<xml_diff>
--- a/data/spss_files.xlsx
+++ b/data/spss_files.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jarvisc1\Documents\projects\comix_data_clean\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CCF68D0-2149-4F4A-9E49-7F4FFC90693A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AA1EB04-2BDB-4678-BEFA-0F6727145726}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18120" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="5" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="115">
   <si>
     <t>country</t>
   </si>
@@ -378,6 +378,12 @@
   </si>
   <si>
     <t>20-030971_PT_Wave1_Final_v1_110121_IntClientuse</t>
+  </si>
+  <si>
+    <t>20-040199_PEW12_Final_DPClean_IntUse</t>
+  </si>
+  <si>
+    <t>20-030971_G1_Merged_Wave2_Final_v1_18012021_IntClientUse</t>
   </si>
 </sst>
 </file>
@@ -702,14 +708,14 @@
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <sheetData>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A5">
         <v>1</v>
       </c>
@@ -717,7 +723,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A6">
         <v>2</v>
       </c>
@@ -725,7 +731,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A7">
         <v>3</v>
       </c>
@@ -740,22 +746,22 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O53"/>
+  <dimension ref="A1:O54"/>
   <sheetViews>
     <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="H53" sqref="H53"/>
+      <selection activeCell="A54" sqref="A54"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" customWidth="1"/>
-    <col min="7" max="7" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="58.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.3828125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.3828125" customWidth="1"/>
+    <col min="7" max="7" width="10.69140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="58.3046875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="25.3046875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>83</v>
       </c>
@@ -802,7 +808,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A2">
         <v>1</v>
       </c>
@@ -828,7 +834,7 @@
         <v>14</v>
       </c>
       <c r="I2" t="str">
-        <f t="shared" ref="I2:I53" si="0">C2&amp;"_"&amp;"wk"&amp;TEXT(D2,"00")&amp;"_"&amp;YEAR(G2)&amp;TEXT(G2,"MM")&amp;TEXT(G2,"DD")&amp;"_p"&amp;E2&amp;"_wv"&amp;TEXT(F2,"00")&amp;""</f>
+        <f t="shared" ref="I2:I54" si="0">C2&amp;"_"&amp;"wk"&amp;TEXT(D2,"00")&amp;"_"&amp;YEAR(G2)&amp;TEXT(G2,"MM")&amp;TEXT(G2,"DD")&amp;"_p"&amp;E2&amp;"_wv"&amp;TEXT(F2,"00")&amp;""</f>
         <v>uk_wk01_20200402_pA_wv01</v>
       </c>
       <c r="J2">
@@ -838,7 +844,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A3">
         <v>1</v>
       </c>
@@ -874,7 +880,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A4">
         <v>1</v>
       </c>
@@ -910,7 +916,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A5">
         <v>1</v>
       </c>
@@ -946,7 +952,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A6">
         <v>1</v>
       </c>
@@ -982,7 +988,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A7">
         <v>1</v>
       </c>
@@ -1018,7 +1024,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A8">
         <v>1</v>
       </c>
@@ -1057,7 +1063,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A9">
         <v>2</v>
       </c>
@@ -1093,7 +1099,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A10">
         <v>1</v>
       </c>
@@ -1130,7 +1136,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A11">
         <v>2</v>
       </c>
@@ -1167,7 +1173,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A12">
         <v>1</v>
       </c>
@@ -1204,7 +1210,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A13">
         <v>2</v>
       </c>
@@ -1242,7 +1248,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A14">
         <v>1</v>
       </c>
@@ -1279,7 +1285,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A15">
         <v>2</v>
       </c>
@@ -1316,7 +1322,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A16">
         <v>1</v>
       </c>
@@ -1353,7 +1359,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A17">
         <v>2</v>
       </c>
@@ -1390,7 +1396,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A18">
         <v>1</v>
       </c>
@@ -1427,7 +1433,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A19">
         <v>2</v>
       </c>
@@ -1464,7 +1470,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A20">
         <v>1</v>
       </c>
@@ -1501,7 +1507,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A21">
         <v>2</v>
       </c>
@@ -1538,7 +1544,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A22">
         <v>1</v>
       </c>
@@ -1575,7 +1581,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A23">
         <v>2</v>
       </c>
@@ -1612,7 +1618,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A24">
         <v>1</v>
       </c>
@@ -1649,7 +1655,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A25">
         <v>2</v>
       </c>
@@ -1686,7 +1692,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A26">
         <v>1</v>
       </c>
@@ -1723,7 +1729,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A27">
         <v>2</v>
       </c>
@@ -1760,7 +1766,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A28">
         <v>1</v>
       </c>
@@ -1800,7 +1806,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A29">
         <v>1</v>
       </c>
@@ -1840,7 +1846,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A30">
         <v>1</v>
       </c>
@@ -1877,7 +1883,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A31">
         <v>2</v>
       </c>
@@ -1913,7 +1919,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A32">
         <v>3</v>
       </c>
@@ -1952,7 +1958,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A33">
         <v>3</v>
       </c>
@@ -1988,7 +1994,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A34">
         <v>3</v>
       </c>
@@ -2005,7 +2011,7 @@
         <v>50</v>
       </c>
       <c r="F34">
-        <f t="shared" ref="F34:F53" si="4">F32+1</f>
+        <f t="shared" ref="F34:F54" si="4">F32+1</f>
         <v>2</v>
       </c>
       <c r="G34" s="1">
@@ -2025,7 +2031,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A35">
         <v>3</v>
       </c>
@@ -2062,7 +2068,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A36">
         <v>3</v>
       </c>
@@ -2099,7 +2105,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A37">
         <v>3</v>
       </c>
@@ -2136,7 +2142,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A38">
         <v>3</v>
       </c>
@@ -2173,7 +2179,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A39">
         <v>3</v>
       </c>
@@ -2210,7 +2216,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A40">
         <v>3</v>
       </c>
@@ -2247,7 +2253,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A41">
         <v>3</v>
       </c>
@@ -2284,7 +2290,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A42">
         <v>3</v>
       </c>
@@ -2321,7 +2327,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A43">
         <v>3</v>
       </c>
@@ -2358,7 +2364,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A44">
         <v>3</v>
       </c>
@@ -2392,7 +2398,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A45">
         <v>3</v>
       </c>
@@ -2429,7 +2435,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A46">
         <v>3</v>
       </c>
@@ -2466,7 +2472,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A47">
         <v>3</v>
       </c>
@@ -2503,7 +2509,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A48">
         <v>3</v>
       </c>
@@ -2537,7 +2543,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A49">
         <v>3</v>
       </c>
@@ -2571,7 +2577,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A50">
         <v>3</v>
       </c>
@@ -2605,7 +2611,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A51">
         <v>3</v>
       </c>
@@ -2639,7 +2645,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A52">
         <v>3</v>
       </c>
@@ -2673,7 +2679,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A53">
         <v>3</v>
       </c>
@@ -2704,6 +2710,40 @@
         <v>uk_wk41_20210107_pF_wv11</v>
       </c>
       <c r="J53">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A54">
+        <v>3</v>
+      </c>
+      <c r="B54">
+        <v>0</v>
+      </c>
+      <c r="C54" t="s">
+        <v>12</v>
+      </c>
+      <c r="D54">
+        <v>42</v>
+      </c>
+      <c r="E54" t="s">
+        <v>50</v>
+      </c>
+      <c r="F54">
+        <f t="shared" si="4"/>
+        <v>12</v>
+      </c>
+      <c r="G54" s="1">
+        <v>44210</v>
+      </c>
+      <c r="H54" t="s">
+        <v>113</v>
+      </c>
+      <c r="I54" t="str">
+        <f t="shared" si="0"/>
+        <v>uk_wk42_20210114_pE_wv12</v>
+      </c>
+      <c r="J54">
         <v>1</v>
       </c>
     </row>
@@ -2716,21 +2756,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C042354-CAAB-48AD-AFC2-2197A2D12C9D}">
   <dimension ref="A1:N10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:M10"/>
+    <sheetView topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="I9" sqref="I9:I10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.42578125" customWidth="1"/>
+    <col min="2" max="2" width="12.3828125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.3828125" customWidth="1"/>
     <col min="5" max="6" width="5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.5703125" customWidth="1"/>
-    <col min="8" max="8" width="58.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="30.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.53515625" customWidth="1"/>
+    <col min="8" max="8" width="58.53515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="30.53515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2774,7 +2814,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>64</v>
       </c>
@@ -2800,14 +2840,14 @@
         <v>65</v>
       </c>
       <c r="I2" t="str">
-        <f t="shared" ref="I2:I9" si="0">A2&amp;"_"&amp;"wk"&amp;TEXT(D2,"00")&amp;"_"&amp;YEAR(G2)&amp;TEXT(G2,"MM")&amp;TEXT(G2,"DD")&amp;"_p"&amp;E2&amp;"_wv"&amp;TEXT(F2,"00")&amp;""</f>
+        <f t="shared" ref="I2:I10" si="0">A2&amp;"_"&amp;"wk"&amp;TEXT(D2,"00")&amp;"_"&amp;YEAR(G2)&amp;TEXT(G2,"MM")&amp;TEXT(G2,"DD")&amp;"_p"&amp;E2&amp;"_wv"&amp;TEXT(F2,"00")&amp;""</f>
         <v>be_wk01_20200429_pA_wv01</v>
       </c>
       <c r="J2">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>64</v>
       </c>
@@ -2840,7 +2880,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>64</v>
       </c>
@@ -2873,7 +2913,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>64</v>
       </c>
@@ -2906,7 +2946,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
         <v>64</v>
       </c>
@@ -2939,7 +2979,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
         <v>64</v>
       </c>
@@ -2972,7 +3012,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
         <v>64</v>
       </c>
@@ -3005,7 +3045,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
         <v>64</v>
       </c>
@@ -3038,7 +3078,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
         <v>64</v>
       </c>
@@ -3060,8 +3100,12 @@
       <c r="G10" s="1">
         <v>44155</v>
       </c>
-      <c r="I10" t="s">
+      <c r="H10" t="s">
         <v>87</v>
+      </c>
+      <c r="I10" t="str">
+        <f t="shared" si="0"/>
+        <v>be_wk09_20201120_pB_wv01</v>
       </c>
     </row>
   </sheetData>
@@ -3077,12 +3121,12 @@
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="14" max="14" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.53515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>83</v>
       </c>
@@ -3129,7 +3173,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A2">
         <v>1</v>
       </c>
@@ -3162,7 +3206,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A3">
         <v>1</v>
       </c>
@@ -3195,7 +3239,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A4">
         <v>1</v>
       </c>
@@ -3228,7 +3272,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A5">
         <v>1</v>
       </c>
@@ -3261,7 +3305,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A6">
         <v>1</v>
       </c>
@@ -3294,7 +3338,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A7">
         <v>1</v>
       </c>
@@ -3327,7 +3371,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A8">
         <v>1</v>
       </c>
@@ -3360,7 +3404,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A9">
         <v>1</v>
       </c>
@@ -3406,13 +3450,13 @@
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" customWidth="1"/>
+    <col min="1" max="1" width="12.3828125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.3828125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>83</v>
       </c>
@@ -3459,7 +3503,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A2">
         <v>1</v>
       </c>
@@ -3489,7 +3533,7 @@
         <v>no_wk01_20200501_pA_wv01</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A3">
         <v>1</v>
       </c>
@@ -3522,7 +3566,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A4">
         <v>1</v>
       </c>
@@ -3552,7 +3596,7 @@
         <v>no_wk03_20200622_pA_wv03</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A5">
         <v>1</v>
       </c>
@@ -3585,7 +3629,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A6">
         <v>1</v>
       </c>
@@ -3618,7 +3662,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A7">
         <v>1</v>
       </c>
@@ -3658,20 +3702,20 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9984DEBA-9A58-467F-869B-4E55580BB1A4}">
-  <dimension ref="A1:M10"/>
+  <dimension ref="A1:M15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="I8" sqref="I8:I15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="7" max="7" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.69140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="59" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="27.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="27.3046875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3712,7 +3756,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>100</v>
       </c>
@@ -3745,7 +3789,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>101</v>
       </c>
@@ -3771,14 +3815,14 @@
         <v>107</v>
       </c>
       <c r="I3" t="str">
-        <f t="shared" ref="I3:I9" si="0">A3&amp;"_"&amp;"wk"&amp;TEXT(D3,"00")&amp;"_"&amp;YEAR(G3)&amp;TEXT(G3,"MM")&amp;TEXT(G3,"DD")&amp;"_p"&amp;E3&amp;"_wv"&amp;TEXT(F3,"00")&amp;""</f>
+        <f t="shared" ref="I3:I15" si="0">A3&amp;"_"&amp;"wk"&amp;TEXT(D3,"00")&amp;"_"&amp;YEAR(G3)&amp;TEXT(G3,"MM")&amp;TEXT(G3,"DD")&amp;"_p"&amp;E3&amp;"_wv"&amp;TEXT(F3,"00")&amp;""</f>
         <v>dk_wk01_20210111_pA_wv01</v>
       </c>
       <c r="J3">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>102</v>
       </c>
@@ -3811,7 +3855,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>103</v>
       </c>
@@ -3844,7 +3888,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
         <v>104</v>
       </c>
@@ -3877,7 +3921,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
         <v>105</v>
       </c>
@@ -3910,7 +3954,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
         <v>106</v>
       </c>
@@ -3943,11 +3987,194 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="G9" s="1"/>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="G10" s="1"/>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A9" t="s">
+        <v>100</v>
+      </c>
+      <c r="B9">
+        <v>5</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>2</v>
+      </c>
+      <c r="F9">
+        <v>2</v>
+      </c>
+      <c r="G9" s="1">
+        <v>44214</v>
+      </c>
+      <c r="H9" t="s">
+        <v>114</v>
+      </c>
+      <c r="I9" t="str">
+        <f t="shared" si="0"/>
+        <v>at_wk02_20210118_p_wv02</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A10" t="s">
+        <v>101</v>
+      </c>
+      <c r="B10">
+        <v>5</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>2</v>
+      </c>
+      <c r="F10">
+        <v>2</v>
+      </c>
+      <c r="G10" s="1">
+        <v>44214</v>
+      </c>
+      <c r="H10" t="s">
+        <v>114</v>
+      </c>
+      <c r="I10" t="str">
+        <f t="shared" si="0"/>
+        <v>dk_wk02_20210118_p_wv02</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A11" t="s">
+        <v>102</v>
+      </c>
+      <c r="B11">
+        <v>5</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>2</v>
+      </c>
+      <c r="F11">
+        <v>2</v>
+      </c>
+      <c r="G11" s="1">
+        <v>44214</v>
+      </c>
+      <c r="H11" t="s">
+        <v>114</v>
+      </c>
+      <c r="I11" t="str">
+        <f t="shared" si="0"/>
+        <v>es_wk02_20210118_p_wv02</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A12" t="s">
+        <v>103</v>
+      </c>
+      <c r="B12">
+        <v>5</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <v>2</v>
+      </c>
+      <c r="F12">
+        <v>2</v>
+      </c>
+      <c r="G12" s="1">
+        <v>44214</v>
+      </c>
+      <c r="H12" t="s">
+        <v>114</v>
+      </c>
+      <c r="I12" t="str">
+        <f t="shared" si="0"/>
+        <v>fr_wk02_20210118_p_wv02</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A13" t="s">
+        <v>104</v>
+      </c>
+      <c r="B13">
+        <v>5</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <v>2</v>
+      </c>
+      <c r="F13">
+        <v>2</v>
+      </c>
+      <c r="G13" s="1">
+        <v>44214</v>
+      </c>
+      <c r="H13" t="s">
+        <v>114</v>
+      </c>
+      <c r="I13" t="str">
+        <f t="shared" si="0"/>
+        <v>it_wk02_20210118_p_wv02</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A14" t="s">
+        <v>105</v>
+      </c>
+      <c r="B14">
+        <v>5</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
+      <c r="D14">
+        <v>2</v>
+      </c>
+      <c r="F14">
+        <v>2</v>
+      </c>
+      <c r="G14" s="1">
+        <v>44214</v>
+      </c>
+      <c r="H14" t="s">
+        <v>114</v>
+      </c>
+      <c r="I14" t="str">
+        <f t="shared" si="0"/>
+        <v>pl_wk02_20210118_p_wv02</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A15" t="s">
+        <v>106</v>
+      </c>
+      <c r="B15">
+        <v>5</v>
+      </c>
+      <c r="C15">
+        <v>0</v>
+      </c>
+      <c r="D15">
+        <v>2</v>
+      </c>
+      <c r="F15">
+        <v>2</v>
+      </c>
+      <c r="G15" s="1">
+        <v>44214</v>
+      </c>
+      <c r="H15" t="s">
+        <v>114</v>
+      </c>
+      <c r="I15" t="str">
+        <f t="shared" si="0"/>
+        <v>pt_wk02_20210118_p_wv02</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Check EU and run for latest data
</commit_message>
<xml_diff>
--- a/data/spss_files.xlsx
+++ b/data/spss_files.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jarvisc1\Documents\projects\comix_data_clean\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AA1EB04-2BDB-4678-BEFA-0F6727145726}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A9D7553-97AB-4890-906D-613F43BCEBF9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18120" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -19,6 +19,7 @@
     <sheet name="NL" sheetId="3" r:id="rId4"/>
     <sheet name="NO" sheetId="4" r:id="rId5"/>
     <sheet name="Group1" sheetId="6" r:id="rId6"/>
+    <sheet name="Sheet1" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -2756,8 +2757,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C042354-CAAB-48AD-AFC2-2197A2D12C9D}">
   <dimension ref="A1:N10"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9:I10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -3083,7 +3084,7 @@
         <v>64</v>
       </c>
       <c r="B10">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C10">
         <v>0</v>
@@ -3705,7 +3706,7 @@
   <dimension ref="A1:M15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8:I15"/>
+      <selection activeCell="I9" sqref="I9:I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -4179,4 +4180,16 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9379CF0-E466-4164-B69D-1322B08B2D66}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
update for BE data
</commit_message>
<xml_diff>
--- a/data/spss_files.xlsx
+++ b/data/spss_files.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jarvisc1\Documents\projects\comix_data_clean\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A9D7553-97AB-4890-906D-613F43BCEBF9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85B91B72-F6EF-4EDA-8F1F-4E836616E448}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18120" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18120" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="5" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="120">
   <si>
     <t>country</t>
   </si>
@@ -303,9 +303,6 @@
     <t>20-040199-01_Final_PEW8_v1_201120_Intclientuse</t>
   </si>
   <si>
-    <t>20_060765_BE2_Wave1_Final_v1_20112020_IntClientUse</t>
-  </si>
-  <si>
     <t>20-056790_Final_PFW8_v1_IntUse</t>
   </si>
   <si>
@@ -385,6 +382,24 @@
   </si>
   <si>
     <t>20-030971_G1_Merged_Wave2_Final_v1_18012021_IntClientUse</t>
+  </si>
+  <si>
+    <t>be_wk09_20201120_pB_wv01</t>
+  </si>
+  <si>
+    <t>be_wk10_19000100_pB_wv02</t>
+  </si>
+  <si>
+    <t>be_wk11_19000100_pB_wv03</t>
+  </si>
+  <si>
+    <t>20_060765_BE2_Wave4_Final_v1_110121_IntClientUse</t>
+  </si>
+  <si>
+    <t>be_wk12_20200111_pB_wv04</t>
+  </si>
+  <si>
+    <t>Temp for Belguim</t>
   </si>
 </sst>
 </file>
@@ -420,7 +435,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
@@ -713,7 +730,7 @@
   <sheetData>
     <row r="4" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.4">
@@ -721,7 +738,7 @@
         <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.4">
@@ -729,7 +746,7 @@
         <v>2</v>
       </c>
       <c r="B6" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.4">
@@ -737,7 +754,7 @@
         <v>3</v>
       </c>
       <c r="B7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
   </sheetData>
@@ -2497,7 +2514,7 @@
         <v>44161</v>
       </c>
       <c r="H47" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="I47" t="str">
         <f t="shared" si="0"/>
@@ -2534,7 +2551,7 @@
         <v>43924</v>
       </c>
       <c r="H48" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="I48" t="str">
         <f t="shared" si="0"/>
@@ -2568,7 +2585,7 @@
         <v>43872</v>
       </c>
       <c r="H49" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="I49" t="str">
         <f t="shared" si="0"/>
@@ -2602,7 +2619,7 @@
         <v>44182</v>
       </c>
       <c r="H50" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="I50" t="str">
         <f t="shared" si="0"/>
@@ -2636,7 +2653,7 @@
         <v>44189</v>
       </c>
       <c r="H51" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="I51" t="str">
         <f t="shared" si="0"/>
@@ -2670,7 +2687,7 @@
         <v>44196</v>
       </c>
       <c r="H52" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I52" t="str">
         <f t="shared" si="0"/>
@@ -2704,7 +2721,7 @@
         <v>44203</v>
       </c>
       <c r="H53" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="I53" t="str">
         <f t="shared" si="0"/>
@@ -2738,7 +2755,7 @@
         <v>44210</v>
       </c>
       <c r="H54" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="I54" t="str">
         <f t="shared" si="0"/>
@@ -2755,10 +2772,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C042354-CAAB-48AD-AFC2-2197A2D12C9D}">
-  <dimension ref="A1:N10"/>
+  <dimension ref="A1:N13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -2841,7 +2858,7 @@
         <v>65</v>
       </c>
       <c r="I2" t="str">
-        <f t="shared" ref="I2:I10" si="0">A2&amp;"_"&amp;"wk"&amp;TEXT(D2,"00")&amp;"_"&amp;YEAR(G2)&amp;TEXT(G2,"MM")&amp;TEXT(G2,"DD")&amp;"_p"&amp;E2&amp;"_wv"&amp;TEXT(F2,"00")&amp;""</f>
+        <f t="shared" ref="I2:I9" si="0">A2&amp;"_"&amp;"wk"&amp;TEXT(D2,"00")&amp;"_"&amp;YEAR(G2)&amp;TEXT(G2,"MM")&amp;TEXT(G2,"DD")&amp;"_p"&amp;E2&amp;"_wv"&amp;TEXT(F2,"00")&amp;""</f>
         <v>be_wk01_20200429_pA_wv01</v>
       </c>
       <c r="J2">
@@ -3080,33 +3097,103 @@
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="A10" t="s">
+      <c r="A10" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="2"/>
+      <c r="C10" s="2">
+        <v>0</v>
+      </c>
+      <c r="D10" s="2">
+        <v>9</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F10" s="2">
+        <v>1</v>
+      </c>
+      <c r="G10" s="3">
+        <v>44155</v>
+      </c>
+      <c r="H10" s="2"/>
+      <c r="I10" s="2" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.4">
+      <c r="A11" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2">
+        <v>0</v>
+      </c>
+      <c r="D11" s="2">
+        <v>10</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F11" s="2">
+        <v>2</v>
+      </c>
+      <c r="G11" s="2"/>
+      <c r="H11" s="2"/>
+      <c r="I11" s="2" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.4">
+      <c r="A12" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2">
+        <v>0</v>
+      </c>
+      <c r="D12" s="2">
+        <v>11</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F12" s="2">
+        <v>3</v>
+      </c>
+      <c r="G12" s="2"/>
+      <c r="H12" s="2"/>
+      <c r="I12" s="2" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.4">
+      <c r="A13" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B13" s="2">
         <v>4</v>
       </c>
-      <c r="C10">
-        <v>0</v>
-      </c>
-      <c r="D10">
-        <v>9</v>
-      </c>
-      <c r="E10" t="s">
+      <c r="C13" s="2">
+        <v>0</v>
+      </c>
+      <c r="D13" s="2">
+        <v>12</v>
+      </c>
+      <c r="E13" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F10">
-        <v>1</v>
-      </c>
-      <c r="G10" s="1">
-        <v>44155</v>
-      </c>
-      <c r="H10" t="s">
-        <v>87</v>
-      </c>
-      <c r="I10" t="str">
-        <f t="shared" si="0"/>
-        <v>be_wk09_20201120_pB_wv01</v>
+      <c r="F13" s="2">
+        <v>4</v>
+      </c>
+      <c r="G13" s="3">
+        <v>43841</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="I13" s="2" t="s">
+        <v>118</v>
       </c>
     </row>
   </sheetData>
@@ -3705,7 +3792,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9984DEBA-9A58-467F-869B-4E55580BB1A4}">
   <dimension ref="A1:M15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I9" sqref="I9:I15"/>
     </sheetView>
   </sheetViews>
@@ -3759,7 +3846,7 @@
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B2">
         <v>5</v>
@@ -3780,7 +3867,7 @@
         <v>44207</v>
       </c>
       <c r="H2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="I2" t="str">
         <f>A2&amp;"_"&amp;"wk"&amp;TEXT(D2,"00")&amp;"_"&amp;YEAR(G3)&amp;TEXT(G3,"MM")&amp;TEXT(G3,"DD")&amp;"_p"&amp;E2&amp;"_wv"&amp;TEXT(F2,"00")&amp;""</f>
@@ -3792,7 +3879,7 @@
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B3">
         <v>5</v>
@@ -3813,7 +3900,7 @@
         <v>44207</v>
       </c>
       <c r="H3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="I3" t="str">
         <f t="shared" ref="I3:I15" si="0">A3&amp;"_"&amp;"wk"&amp;TEXT(D3,"00")&amp;"_"&amp;YEAR(G3)&amp;TEXT(G3,"MM")&amp;TEXT(G3,"DD")&amp;"_p"&amp;E3&amp;"_wv"&amp;TEXT(F3,"00")&amp;""</f>
@@ -3825,7 +3912,7 @@
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B4">
         <v>5</v>
@@ -3846,7 +3933,7 @@
         <v>44207</v>
       </c>
       <c r="H4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="I4" t="str">
         <f t="shared" si="0"/>
@@ -3858,7 +3945,7 @@
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B5">
         <v>5</v>
@@ -3879,7 +3966,7 @@
         <v>44207</v>
       </c>
       <c r="H5" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="I5" t="str">
         <f t="shared" si="0"/>
@@ -3891,7 +3978,7 @@
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B6">
         <v>5</v>
@@ -3912,7 +3999,7 @@
         <v>44207</v>
       </c>
       <c r="H6" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="I6" t="str">
         <f t="shared" si="0"/>
@@ -3924,7 +4011,7 @@
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B7">
         <v>5</v>
@@ -3945,7 +4032,7 @@
         <v>44207</v>
       </c>
       <c r="H7" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="I7" t="str">
         <f t="shared" si="0"/>
@@ -3957,7 +4044,7 @@
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B8">
         <v>5</v>
@@ -3978,7 +4065,7 @@
         <v>44207</v>
       </c>
       <c r="H8" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="I8" t="str">
         <f t="shared" si="0"/>
@@ -3990,7 +4077,7 @@
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B9">
         <v>5</v>
@@ -4008,7 +4095,7 @@
         <v>44214</v>
       </c>
       <c r="H9" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="I9" t="str">
         <f t="shared" si="0"/>
@@ -4017,7 +4104,7 @@
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B10">
         <v>5</v>
@@ -4035,7 +4122,7 @@
         <v>44214</v>
       </c>
       <c r="H10" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="I10" t="str">
         <f t="shared" si="0"/>
@@ -4044,7 +4131,7 @@
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B11">
         <v>5</v>
@@ -4062,7 +4149,7 @@
         <v>44214</v>
       </c>
       <c r="H11" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="I11" t="str">
         <f t="shared" si="0"/>
@@ -4071,7 +4158,7 @@
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A12" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B12">
         <v>5</v>
@@ -4089,7 +4176,7 @@
         <v>44214</v>
       </c>
       <c r="H12" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="I12" t="str">
         <f t="shared" si="0"/>
@@ -4098,7 +4185,7 @@
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A13" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B13">
         <v>5</v>
@@ -4116,7 +4203,7 @@
         <v>44214</v>
       </c>
       <c r="H13" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="I13" t="str">
         <f t="shared" si="0"/>
@@ -4125,7 +4212,7 @@
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A14" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B14">
         <v>5</v>
@@ -4143,7 +4230,7 @@
         <v>44214</v>
       </c>
       <c r="H14" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="I14" t="str">
         <f t="shared" si="0"/>
@@ -4152,7 +4239,7 @@
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A15" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B15">
         <v>5</v>
@@ -4170,7 +4257,7 @@
         <v>44214</v>
       </c>
       <c r="H15" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="I15" t="str">
         <f t="shared" si="0"/>
@@ -4189,7 +4276,13 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A1" t="s">
+        <v>119</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add panel to filenames EU
</commit_message>
<xml_diff>
--- a/data/spss_files.xlsx
+++ b/data/spss_files.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jarvisc1\Documents\projects\comix_data_clean\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85B91B72-F6EF-4EDA-8F1F-4E836616E448}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{709EBD96-F02E-4CD2-8B22-0CE24DD474BB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18120" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18120" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="5" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="361" uniqueCount="120">
   <si>
     <t>country</t>
   </si>
@@ -2774,8 +2774,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C042354-CAAB-48AD-AFC2-2197A2D12C9D}">
   <dimension ref="A1:N13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -3792,8 +3792,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9984DEBA-9A58-467F-869B-4E55580BB1A4}">
   <dimension ref="A1:M15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I9" sqref="I9:I15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9:E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -4088,6 +4088,9 @@
       <c r="D9">
         <v>2</v>
       </c>
+      <c r="E9" s="2" t="s">
+        <v>13</v>
+      </c>
       <c r="F9">
         <v>2</v>
       </c>
@@ -4099,7 +4102,7 @@
       </c>
       <c r="I9" t="str">
         <f t="shared" si="0"/>
-        <v>at_wk02_20210118_p_wv02</v>
+        <v>at_wk02_20210118_pA_wv02</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.4">
@@ -4115,6 +4118,9 @@
       <c r="D10">
         <v>2</v>
       </c>
+      <c r="E10" s="2" t="s">
+        <v>13</v>
+      </c>
       <c r="F10">
         <v>2</v>
       </c>
@@ -4126,7 +4132,7 @@
       </c>
       <c r="I10" t="str">
         <f t="shared" si="0"/>
-        <v>dk_wk02_20210118_p_wv02</v>
+        <v>dk_wk02_20210118_pA_wv02</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.4">
@@ -4142,6 +4148,9 @@
       <c r="D11">
         <v>2</v>
       </c>
+      <c r="E11" s="2" t="s">
+        <v>13</v>
+      </c>
       <c r="F11">
         <v>2</v>
       </c>
@@ -4153,7 +4162,7 @@
       </c>
       <c r="I11" t="str">
         <f t="shared" si="0"/>
-        <v>es_wk02_20210118_p_wv02</v>
+        <v>es_wk02_20210118_pA_wv02</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.4">
@@ -4169,6 +4178,9 @@
       <c r="D12">
         <v>2</v>
       </c>
+      <c r="E12" s="2" t="s">
+        <v>13</v>
+      </c>
       <c r="F12">
         <v>2</v>
       </c>
@@ -4180,7 +4192,7 @@
       </c>
       <c r="I12" t="str">
         <f t="shared" si="0"/>
-        <v>fr_wk02_20210118_p_wv02</v>
+        <v>fr_wk02_20210118_pA_wv02</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.4">
@@ -4196,6 +4208,9 @@
       <c r="D13">
         <v>2</v>
       </c>
+      <c r="E13" s="2" t="s">
+        <v>13</v>
+      </c>
       <c r="F13">
         <v>2</v>
       </c>
@@ -4207,7 +4222,7 @@
       </c>
       <c r="I13" t="str">
         <f t="shared" si="0"/>
-        <v>it_wk02_20210118_p_wv02</v>
+        <v>it_wk02_20210118_pA_wv02</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.4">
@@ -4223,6 +4238,9 @@
       <c r="D14">
         <v>2</v>
       </c>
+      <c r="E14" s="2" t="s">
+        <v>13</v>
+      </c>
       <c r="F14">
         <v>2</v>
       </c>
@@ -4234,7 +4252,7 @@
       </c>
       <c r="I14" t="str">
         <f t="shared" si="0"/>
-        <v>pl_wk02_20210118_p_wv02</v>
+        <v>pl_wk02_20210118_pA_wv02</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.4">
@@ -4250,6 +4268,9 @@
       <c r="D15">
         <v>2</v>
       </c>
+      <c r="E15" s="2" t="s">
+        <v>13</v>
+      </c>
       <c r="F15">
         <v>2</v>
       </c>
@@ -4261,7 +4282,7 @@
       </c>
       <c r="I15" t="str">
         <f t="shared" si="0"/>
-        <v>pt_wk02_20210118_p_wv02</v>
+        <v>pt_wk02_20210118_pA_wv02</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
move sample type col
</commit_message>
<xml_diff>
--- a/data/spss_files.xlsx
+++ b/data/spss_files.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11213"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jarvisc1\Documents\projects\comix_data_clean\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/amygimma/lshtm/comix_data_clean/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BCAA70E-0A03-4105-B98A-C6D121C390EA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39A6E211-A711-BE4A-A124-3C6145617E39}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15180" yWindow="651" windowWidth="16714" windowHeight="15052" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="5" r:id="rId1"/>
@@ -19,7 +19,6 @@
     <sheet name="NL" sheetId="3" r:id="rId4"/>
     <sheet name="NO" sheetId="4" r:id="rId5"/>
     <sheet name="Group1" sheetId="6" r:id="rId6"/>
-    <sheet name="Sheet1" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="364" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="120">
   <si>
     <t>country</t>
   </si>
@@ -303,6 +302,9 @@
     <t>20-040199-01_Final_PEW8_v1_201120_Intclientuse</t>
   </si>
   <si>
+    <t>20_060765_BE2_Wave1_Final_v1_20112020_IntClientUse</t>
+  </si>
+  <si>
     <t>20-056790_Final_PFW8_v1_IntUse</t>
   </si>
   <si>
@@ -378,12 +380,6 @@
     <t>20-030971_PT_Wave1_Final_v1_110121_IntClientuse</t>
   </si>
   <si>
-    <t>20-040199_PEW12_Final_DPClean_IntUse</t>
-  </si>
-  <si>
-    <t>20-030971_G1_Merged_Wave2_Final_v1_18012021_IntClientUse</t>
-  </si>
-  <si>
     <t>be_wk09_20201120_pB_wv01</t>
   </si>
   <si>
@@ -399,20 +395,26 @@
     <t>be_wk12_20200111_pB_wv04</t>
   </si>
   <si>
-    <t>Temp for Belguim</t>
-  </si>
-  <si>
-    <t>20-056790_PFW12_Final_ICUO</t>
+    <t>20_060765_BE2_Wave5_Final_v1_200121_IntClientUse</t>
+  </si>
+  <si>
+    <t>be_wk12_20200111_pB_wv05</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -438,9 +440,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
@@ -729,35 +729,35 @@
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.4">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.4">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>2</v>
       </c>
       <c r="B6" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.4">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>3</v>
       </c>
       <c r="B7" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
   </sheetData>
@@ -767,22 +767,22 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O55"/>
+  <dimension ref="A1:O53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D19" workbookViewId="0">
-      <selection activeCell="H55" sqref="H55"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="H53" sqref="H53"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.3828125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.3828125" customWidth="1"/>
-    <col min="7" max="7" width="10.69140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="58.3046875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="25.3046875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.5" customWidth="1"/>
+    <col min="7" max="7" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="58.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="25.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>83</v>
       </c>
@@ -829,7 +829,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -855,7 +855,7 @@
         <v>14</v>
       </c>
       <c r="I2" t="str">
-        <f t="shared" ref="I2:I55" si="0">C2&amp;"_"&amp;"wk"&amp;TEXT(D2,"00")&amp;"_"&amp;YEAR(G2)&amp;TEXT(G2,"MM")&amp;TEXT(G2,"DD")&amp;"_p"&amp;E2&amp;"_wv"&amp;TEXT(F2,"00")&amp;""</f>
+        <f t="shared" ref="I2:I53" si="0">C2&amp;"_"&amp;"wk"&amp;TEXT(D2,"00")&amp;"_"&amp;YEAR(G2)&amp;TEXT(G2,"MM")&amp;TEXT(G2,"DD")&amp;"_p"&amp;E2&amp;"_wv"&amp;TEXT(F2,"00")&amp;""</f>
         <v>uk_wk01_20200402_pA_wv01</v>
       </c>
       <c r="J2">
@@ -865,7 +865,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
@@ -901,7 +901,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>1</v>
       </c>
@@ -937,7 +937,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>1</v>
       </c>
@@ -973,7 +973,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>1</v>
       </c>
@@ -1009,7 +1009,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>1</v>
       </c>
@@ -1045,7 +1045,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>1</v>
       </c>
@@ -1084,7 +1084,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>2</v>
       </c>
@@ -1120,7 +1120,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>1</v>
       </c>
@@ -1157,7 +1157,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>2</v>
       </c>
@@ -1194,7 +1194,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>1</v>
       </c>
@@ -1231,7 +1231,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>2</v>
       </c>
@@ -1269,7 +1269,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>1</v>
       </c>
@@ -1306,7 +1306,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>2</v>
       </c>
@@ -1343,7 +1343,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>1</v>
       </c>
@@ -1380,7 +1380,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>2</v>
       </c>
@@ -1417,7 +1417,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>1</v>
       </c>
@@ -1454,7 +1454,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>2</v>
       </c>
@@ -1491,7 +1491,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>1</v>
       </c>
@@ -1528,7 +1528,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>2</v>
       </c>
@@ -1565,7 +1565,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>1</v>
       </c>
@@ -1602,7 +1602,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>2</v>
       </c>
@@ -1639,7 +1639,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>1</v>
       </c>
@@ -1676,7 +1676,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>2</v>
       </c>
@@ -1713,7 +1713,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>1</v>
       </c>
@@ -1750,7 +1750,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>2</v>
       </c>
@@ -1787,7 +1787,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>1</v>
       </c>
@@ -1827,7 +1827,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>1</v>
       </c>
@@ -1867,7 +1867,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>1</v>
       </c>
@@ -1904,7 +1904,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>2</v>
       </c>
@@ -1940,7 +1940,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>3</v>
       </c>
@@ -1979,7 +1979,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>3</v>
       </c>
@@ -2015,7 +2015,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>3</v>
       </c>
@@ -2032,7 +2032,7 @@
         <v>50</v>
       </c>
       <c r="F34">
-        <f t="shared" ref="F34:F55" si="4">F32+1</f>
+        <f t="shared" ref="F34:F53" si="4">F32+1</f>
         <v>2</v>
       </c>
       <c r="G34" s="1">
@@ -2052,7 +2052,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>3</v>
       </c>
@@ -2089,7 +2089,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>3</v>
       </c>
@@ -2126,7 +2126,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>3</v>
       </c>
@@ -2163,7 +2163,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>3</v>
       </c>
@@ -2200,7 +2200,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>3</v>
       </c>
@@ -2237,7 +2237,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>3</v>
       </c>
@@ -2274,7 +2274,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>3</v>
       </c>
@@ -2311,7 +2311,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>3</v>
       </c>
@@ -2348,7 +2348,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>3</v>
       </c>
@@ -2385,7 +2385,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>3</v>
       </c>
@@ -2419,7 +2419,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>3</v>
       </c>
@@ -2456,7 +2456,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>3</v>
       </c>
@@ -2493,7 +2493,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>3</v>
       </c>
@@ -2517,7 +2517,7 @@
         <v>44161</v>
       </c>
       <c r="H47" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="I47" t="str">
         <f t="shared" si="0"/>
@@ -2530,7 +2530,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>3</v>
       </c>
@@ -2554,7 +2554,7 @@
         <v>43924</v>
       </c>
       <c r="H48" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="I48" t="str">
         <f t="shared" si="0"/>
@@ -2564,7 +2564,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>3</v>
       </c>
@@ -2588,7 +2588,7 @@
         <v>43872</v>
       </c>
       <c r="H49" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="I49" t="str">
         <f t="shared" si="0"/>
@@ -2598,7 +2598,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>3</v>
       </c>
@@ -2622,7 +2622,7 @@
         <v>44182</v>
       </c>
       <c r="H50" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="I50" t="str">
         <f t="shared" si="0"/>
@@ -2632,7 +2632,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>3</v>
       </c>
@@ -2656,7 +2656,7 @@
         <v>44189</v>
       </c>
       <c r="H51" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="I51" t="str">
         <f t="shared" si="0"/>
@@ -2666,7 +2666,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>3</v>
       </c>
@@ -2690,7 +2690,7 @@
         <v>44196</v>
       </c>
       <c r="H52" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="I52" t="str">
         <f t="shared" si="0"/>
@@ -2700,7 +2700,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>3</v>
       </c>
@@ -2724,81 +2724,13 @@
         <v>44203</v>
       </c>
       <c r="H53" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="I53" t="str">
         <f t="shared" si="0"/>
         <v>uk_wk41_20210107_pF_wv11</v>
       </c>
       <c r="J53">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A54">
-        <v>3</v>
-      </c>
-      <c r="B54">
-        <v>0</v>
-      </c>
-      <c r="C54" t="s">
-        <v>12</v>
-      </c>
-      <c r="D54">
-        <v>42</v>
-      </c>
-      <c r="E54" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="F54">
-        <f t="shared" si="4"/>
-        <v>12</v>
-      </c>
-      <c r="G54" s="1">
-        <v>44210</v>
-      </c>
-      <c r="H54" t="s">
-        <v>112</v>
-      </c>
-      <c r="I54" t="str">
-        <f t="shared" si="0"/>
-        <v>uk_wk42_20210114_pE_wv12</v>
-      </c>
-      <c r="J54">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A55" s="2">
-        <v>3</v>
-      </c>
-      <c r="B55" s="2">
-        <v>0</v>
-      </c>
-      <c r="C55" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D55" s="2">
-        <v>43</v>
-      </c>
-      <c r="E55" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="F55" s="2">
-        <f t="shared" si="4"/>
-        <v>12</v>
-      </c>
-      <c r="G55" s="3">
-        <v>44216</v>
-      </c>
-      <c r="H55" t="s">
-        <v>120</v>
-      </c>
-      <c r="I55" t="str">
-        <f t="shared" si="0"/>
-        <v>uk_wk43_20210120_pF_wv12</v>
-      </c>
-      <c r="J55">
         <v>1</v>
       </c>
     </row>
@@ -2809,23 +2741,23 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C042354-CAAB-48AD-AFC2-2197A2D12C9D}">
-  <dimension ref="A1:N13"/>
+  <dimension ref="A1:N15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="12.3828125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.3828125" customWidth="1"/>
+    <col min="2" max="2" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.5" customWidth="1"/>
     <col min="5" max="6" width="5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.53515625" customWidth="1"/>
-    <col min="8" max="8" width="58.53515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="30.53515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.5" customWidth="1"/>
+    <col min="8" max="8" width="58.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="30.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2869,7 +2801,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>64</v>
       </c>
@@ -2902,7 +2834,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>64</v>
       </c>
@@ -2935,7 +2867,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>64</v>
       </c>
@@ -2968,7 +2900,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>64</v>
       </c>
@@ -3001,7 +2933,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>64</v>
       </c>
@@ -3034,7 +2966,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>64</v>
       </c>
@@ -3067,7 +2999,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>64</v>
       </c>
@@ -3100,7 +3032,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>64</v>
       </c>
@@ -3133,107 +3065,167 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="A10" s="2" t="s">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
         <v>64</v>
       </c>
-      <c r="B10" s="2"/>
-      <c r="C10" s="2">
-        <v>0</v>
-      </c>
-      <c r="D10" s="2">
+      <c r="B10">
+        <v>2</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
         <v>9</v>
       </c>
-      <c r="E10" s="2" t="s">
+      <c r="E10" t="s">
         <v>15</v>
       </c>
-      <c r="F10" s="2">
-        <v>1</v>
-      </c>
-      <c r="G10" s="3">
+      <c r="F10">
+        <v>1</v>
+      </c>
+      <c r="G10" s="1">
         <v>44155</v>
       </c>
-      <c r="H10" s="2"/>
-      <c r="I10" s="2" t="s">
+      <c r="I10" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>64</v>
+      </c>
+      <c r="B11">
+        <v>2</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>9</v>
+      </c>
+      <c r="E11" t="s">
+        <v>15</v>
+      </c>
+      <c r="F11">
+        <v>1</v>
+      </c>
+      <c r="G11" s="1">
+        <v>44155</v>
+      </c>
+      <c r="H11" t="s">
+        <v>87</v>
+      </c>
+      <c r="I11" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>64</v>
+      </c>
+      <c r="B12">
+        <v>2</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <v>10</v>
+      </c>
+      <c r="E12" t="s">
+        <v>15</v>
+      </c>
+      <c r="F12">
+        <v>2</v>
+      </c>
+      <c r="I12" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="A11" s="2" t="s">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
         <v>64</v>
       </c>
-      <c r="B11" s="2"/>
-      <c r="C11" s="2">
-        <v>0</v>
-      </c>
-      <c r="D11" s="2">
-        <v>10</v>
-      </c>
-      <c r="E11" s="2" t="s">
+      <c r="B13">
+        <v>2</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <v>11</v>
+      </c>
+      <c r="E13" t="s">
         <v>15</v>
       </c>
-      <c r="F11" s="2">
-        <v>2</v>
-      </c>
-      <c r="G11" s="2"/>
-      <c r="H11" s="2"/>
-      <c r="I11" s="2" t="s">
+      <c r="F13">
+        <v>3</v>
+      </c>
+      <c r="I13" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="A12" s="2" t="s">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
         <v>64</v>
       </c>
-      <c r="B12" s="2"/>
-      <c r="C12" s="2">
-        <v>0</v>
-      </c>
-      <c r="D12" s="2">
-        <v>11</v>
-      </c>
-      <c r="E12" s="2" t="s">
+      <c r="B14">
+        <v>4</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
+      <c r="D14">
+        <v>12</v>
+      </c>
+      <c r="E14" t="s">
         <v>15</v>
       </c>
-      <c r="F12" s="2">
-        <v>3</v>
-      </c>
-      <c r="G12" s="2"/>
-      <c r="H12" s="2"/>
-      <c r="I12" s="2" t="s">
+      <c r="F14">
+        <v>4</v>
+      </c>
+      <c r="G14" s="1">
+        <v>43841</v>
+      </c>
+      <c r="H14" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="A13" s="2" t="s">
+      <c r="I14" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
         <v>64</v>
       </c>
-      <c r="B13" s="2">
+      <c r="B15">
         <v>4</v>
       </c>
-      <c r="C13" s="2">
-        <v>0</v>
-      </c>
-      <c r="D13" s="2">
-        <v>12</v>
-      </c>
-      <c r="E13" s="2" t="s">
+      <c r="C15">
+        <v>0</v>
+      </c>
+      <c r="D15">
+        <v>12</v>
+      </c>
+      <c r="E15" t="s">
         <v>15</v>
       </c>
-      <c r="F13" s="2">
-        <v>4</v>
-      </c>
-      <c r="G13" s="3">
-        <v>43841</v>
-      </c>
-      <c r="H13" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="I13" s="2" t="s">
+      <c r="F15">
+        <v>5</v>
+      </c>
+      <c r="G15" s="1">
+        <v>43850</v>
+      </c>
+      <c r="H15" t="s">
         <v>118</v>
       </c>
+      <c r="I15" t="s">
+        <v>119</v>
+      </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -3246,12 +3238,12 @@
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="14" max="14" width="9.53515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>83</v>
       </c>
@@ -3298,7 +3290,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -3331,7 +3323,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
@@ -3364,7 +3356,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>1</v>
       </c>
@@ -3397,7 +3389,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>1</v>
       </c>
@@ -3430,7 +3422,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>1</v>
       </c>
@@ -3463,7 +3455,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>1</v>
       </c>
@@ -3496,7 +3488,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>1</v>
       </c>
@@ -3529,7 +3521,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>1</v>
       </c>
@@ -3575,13 +3567,13 @@
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.3828125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.3828125" customWidth="1"/>
+    <col min="1" max="1" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>83</v>
       </c>
@@ -3628,7 +3620,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -3658,7 +3650,7 @@
         <v>no_wk01_20200501_pA_wv01</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
@@ -3691,7 +3683,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>1</v>
       </c>
@@ -3721,7 +3713,7 @@
         <v>no_wk03_20200622_pA_wv03</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>1</v>
       </c>
@@ -3754,7 +3746,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>1</v>
       </c>
@@ -3787,7 +3779,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>1</v>
       </c>
@@ -3827,20 +3819,20 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9984DEBA-9A58-467F-869B-4E55580BB1A4}">
-  <dimension ref="A1:M15"/>
+  <dimension ref="A1:M10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E9" sqref="E9:E15"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="7" max="7" width="10.69140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.6640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="59" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="27.3046875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="27.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3881,9 +3873,9 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B2">
         <v>5</v>
@@ -3904,7 +3896,7 @@
         <v>44207</v>
       </c>
       <c r="H2" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="I2" t="str">
         <f>A2&amp;"_"&amp;"wk"&amp;TEXT(D2,"00")&amp;"_"&amp;YEAR(G3)&amp;TEXT(G3,"MM")&amp;TEXT(G3,"DD")&amp;"_p"&amp;E2&amp;"_wv"&amp;TEXT(F2,"00")&amp;""</f>
@@ -3914,9 +3906,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B3">
         <v>5</v>
@@ -3937,19 +3929,19 @@
         <v>44207</v>
       </c>
       <c r="H3" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="I3" t="str">
-        <f t="shared" ref="I3:I15" si="0">A3&amp;"_"&amp;"wk"&amp;TEXT(D3,"00")&amp;"_"&amp;YEAR(G3)&amp;TEXT(G3,"MM")&amp;TEXT(G3,"DD")&amp;"_p"&amp;E3&amp;"_wv"&amp;TEXT(F3,"00")&amp;""</f>
+        <f t="shared" ref="I3:I8" si="0">A3&amp;"_"&amp;"wk"&amp;TEXT(D3,"00")&amp;"_"&amp;YEAR(G3)&amp;TEXT(G3,"MM")&amp;TEXT(G3,"DD")&amp;"_p"&amp;E3&amp;"_wv"&amp;TEXT(F3,"00")&amp;""</f>
         <v>dk_wk01_20210111_pA_wv01</v>
       </c>
       <c r="J3">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B4">
         <v>5</v>
@@ -3970,7 +3962,7 @@
         <v>44207</v>
       </c>
       <c r="H4" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="I4" t="str">
         <f t="shared" si="0"/>
@@ -3980,9 +3972,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B5">
         <v>5</v>
@@ -4003,7 +3995,7 @@
         <v>44207</v>
       </c>
       <c r="H5" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="I5" t="str">
         <f t="shared" si="0"/>
@@ -4013,9 +4005,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B6">
         <v>5</v>
@@ -4036,7 +4028,7 @@
         <v>44207</v>
       </c>
       <c r="H6" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="I6" t="str">
         <f t="shared" si="0"/>
@@ -4046,9 +4038,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B7">
         <v>5</v>
@@ -4069,7 +4061,7 @@
         <v>44207</v>
       </c>
       <c r="H7" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="I7" t="str">
         <f t="shared" si="0"/>
@@ -4079,9 +4071,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B8">
         <v>5</v>
@@ -4102,7 +4094,7 @@
         <v>44207</v>
       </c>
       <c r="H8" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="I8" t="str">
         <f t="shared" si="0"/>
@@ -4112,233 +4104,11 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A9" t="s">
-        <v>99</v>
-      </c>
-      <c r="B9">
-        <v>5</v>
-      </c>
-      <c r="C9">
-        <v>0</v>
-      </c>
-      <c r="D9">
-        <v>2</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F9">
-        <v>2</v>
-      </c>
-      <c r="G9" s="1">
-        <v>44214</v>
-      </c>
-      <c r="H9" t="s">
-        <v>113</v>
-      </c>
-      <c r="I9" t="str">
-        <f t="shared" si="0"/>
-        <v>at_wk02_20210118_pA_wv02</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A10" t="s">
-        <v>100</v>
-      </c>
-      <c r="B10">
-        <v>5</v>
-      </c>
-      <c r="C10">
-        <v>0</v>
-      </c>
-      <c r="D10">
-        <v>2</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F10">
-        <v>2</v>
-      </c>
-      <c r="G10" s="1">
-        <v>44214</v>
-      </c>
-      <c r="H10" t="s">
-        <v>113</v>
-      </c>
-      <c r="I10" t="str">
-        <f t="shared" si="0"/>
-        <v>dk_wk02_20210118_pA_wv02</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A11" t="s">
-        <v>101</v>
-      </c>
-      <c r="B11">
-        <v>5</v>
-      </c>
-      <c r="C11">
-        <v>0</v>
-      </c>
-      <c r="D11">
-        <v>2</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F11">
-        <v>2</v>
-      </c>
-      <c r="G11" s="1">
-        <v>44214</v>
-      </c>
-      <c r="H11" t="s">
-        <v>113</v>
-      </c>
-      <c r="I11" t="str">
-        <f t="shared" si="0"/>
-        <v>es_wk02_20210118_pA_wv02</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A12" t="s">
-        <v>102</v>
-      </c>
-      <c r="B12">
-        <v>5</v>
-      </c>
-      <c r="C12">
-        <v>0</v>
-      </c>
-      <c r="D12">
-        <v>2</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F12">
-        <v>2</v>
-      </c>
-      <c r="G12" s="1">
-        <v>44214</v>
-      </c>
-      <c r="H12" t="s">
-        <v>113</v>
-      </c>
-      <c r="I12" t="str">
-        <f t="shared" si="0"/>
-        <v>fr_wk02_20210118_pA_wv02</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A13" t="s">
-        <v>103</v>
-      </c>
-      <c r="B13">
-        <v>5</v>
-      </c>
-      <c r="C13">
-        <v>0</v>
-      </c>
-      <c r="D13">
-        <v>2</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F13">
-        <v>2</v>
-      </c>
-      <c r="G13" s="1">
-        <v>44214</v>
-      </c>
-      <c r="H13" t="s">
-        <v>113</v>
-      </c>
-      <c r="I13" t="str">
-        <f t="shared" si="0"/>
-        <v>it_wk02_20210118_pA_wv02</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A14" t="s">
-        <v>104</v>
-      </c>
-      <c r="B14">
-        <v>5</v>
-      </c>
-      <c r="C14">
-        <v>0</v>
-      </c>
-      <c r="D14">
-        <v>2</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F14">
-        <v>2</v>
-      </c>
-      <c r="G14" s="1">
-        <v>44214</v>
-      </c>
-      <c r="H14" t="s">
-        <v>113</v>
-      </c>
-      <c r="I14" t="str">
-        <f t="shared" si="0"/>
-        <v>pl_wk02_20210118_pA_wv02</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A15" t="s">
-        <v>105</v>
-      </c>
-      <c r="B15">
-        <v>5</v>
-      </c>
-      <c r="C15">
-        <v>0</v>
-      </c>
-      <c r="D15">
-        <v>2</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F15">
-        <v>2</v>
-      </c>
-      <c r="G15" s="1">
-        <v>44214</v>
-      </c>
-      <c r="H15" t="s">
-        <v>113</v>
-      </c>
-      <c r="I15" t="str">
-        <f t="shared" si="0"/>
-        <v>pt_wk02_20210118_pA_wv02</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9379CF0-E466-4164-B69D-1322B08B2D66}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A1" t="s">
-        <v>119</v>
-      </c>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="G9" s="1"/>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="G10" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Add new UK data
</commit_message>
<xml_diff>
--- a/data/spss_files.xlsx
+++ b/data/spss_files.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jarvisc1\Documents\projects\comix_data_clean\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BCAA70E-0A03-4105-B98A-C6D121C390EA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEE53A03-1071-432D-93DF-7CB4D020E5B9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15180" yWindow="651" windowWidth="16714" windowHeight="15052" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18120" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="5" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="364" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="367" uniqueCount="122">
   <si>
     <t>country</t>
   </si>
@@ -403,6 +403,9 @@
   </si>
   <si>
     <t>20-056790_PFW12_Final_ICUO</t>
+  </si>
+  <si>
+    <t>20-100562_PEW13_Final</t>
   </si>
 </sst>
 </file>
@@ -767,10 +770,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O55"/>
+  <dimension ref="A1:O56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D19" workbookViewId="0">
-      <selection activeCell="H55" sqref="H55"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -855,7 +858,7 @@
         <v>14</v>
       </c>
       <c r="I2" t="str">
-        <f t="shared" ref="I2:I55" si="0">C2&amp;"_"&amp;"wk"&amp;TEXT(D2,"00")&amp;"_"&amp;YEAR(G2)&amp;TEXT(G2,"MM")&amp;TEXT(G2,"DD")&amp;"_p"&amp;E2&amp;"_wv"&amp;TEXT(F2,"00")&amp;""</f>
+        <f t="shared" ref="I2:I56" si="0">C2&amp;"_"&amp;"wk"&amp;TEXT(D2,"00")&amp;"_"&amp;YEAR(G2)&amp;TEXT(G2,"MM")&amp;TEXT(G2,"DD")&amp;"_p"&amp;E2&amp;"_wv"&amp;TEXT(F2,"00")&amp;""</f>
         <v>uk_wk01_20200402_pA_wv01</v>
       </c>
       <c r="J2">
@@ -2032,7 +2035,7 @@
         <v>50</v>
       </c>
       <c r="F34">
-        <f t="shared" ref="F34:F55" si="4">F32+1</f>
+        <f t="shared" ref="F34:F56" si="4">F32+1</f>
         <v>2</v>
       </c>
       <c r="G34" s="1">
@@ -2799,6 +2802,40 @@
         <v>uk_wk43_20210120_pF_wv12</v>
       </c>
       <c r="J55">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A56" s="2">
+        <v>3</v>
+      </c>
+      <c r="B56" s="2">
+        <v>0</v>
+      </c>
+      <c r="C56" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D56" s="2">
+        <v>44</v>
+      </c>
+      <c r="E56" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="F56" s="2">
+        <f t="shared" si="4"/>
+        <v>13</v>
+      </c>
+      <c r="G56" s="3">
+        <v>44224</v>
+      </c>
+      <c r="H56" t="s">
+        <v>121</v>
+      </c>
+      <c r="I56" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>uk_wk44_20210128_pE_wv13</v>
+      </c>
+      <c r="J56">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update spss_files for Group 1 data
</commit_message>
<xml_diff>
--- a/data/spss_files.xlsx
+++ b/data/spss_files.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jarvisc1\Documents\projects\comix_data_clean\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kw\Documents\comix_data_clean\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEE53A03-1071-432D-93DF-7CB4D020E5B9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{226743BD-F6F6-4937-8D52-741C6B5E7BBF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18120" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="13986" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="5" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="367" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="388" uniqueCount="123">
   <si>
     <t>country</t>
   </si>
@@ -406,6 +406,9 @@
   </si>
   <si>
     <t>20-100562_PEW13_Final</t>
+  </si>
+  <si>
+    <t>20-030971_G1_Merged_Wave3_Final_v1_29012021_IntClientUse</t>
   </si>
 </sst>
 </file>
@@ -732,14 +735,14 @@
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <sheetData>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A4" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A5">
         <v>1</v>
       </c>
@@ -747,7 +750,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A6">
         <v>2</v>
       </c>
@@ -755,7 +758,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A7">
         <v>3</v>
       </c>
@@ -772,20 +775,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="H34" sqref="H34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" width="12.3828125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.3828125" customWidth="1"/>
-    <col min="7" max="7" width="10.69140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="58.3046875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="25.3046875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.3515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.3515625" customWidth="1"/>
+    <col min="7" max="7" width="10.703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="58.29296875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="25.29296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A1" t="s">
         <v>83</v>
       </c>
@@ -832,7 +835,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A2">
         <v>1</v>
       </c>
@@ -868,7 +871,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A3">
         <v>1</v>
       </c>
@@ -904,7 +907,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A4">
         <v>1</v>
       </c>
@@ -940,7 +943,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A5">
         <v>1</v>
       </c>
@@ -976,7 +979,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A6">
         <v>1</v>
       </c>
@@ -1012,7 +1015,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A7">
         <v>1</v>
       </c>
@@ -1048,7 +1051,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A8">
         <v>1</v>
       </c>
@@ -1087,7 +1090,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A9">
         <v>2</v>
       </c>
@@ -1123,7 +1126,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A10">
         <v>1</v>
       </c>
@@ -1160,7 +1163,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A11">
         <v>2</v>
       </c>
@@ -1197,7 +1200,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A12">
         <v>1</v>
       </c>
@@ -1234,7 +1237,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A13">
         <v>2</v>
       </c>
@@ -1272,7 +1275,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A14">
         <v>1</v>
       </c>
@@ -1309,7 +1312,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A15">
         <v>2</v>
       </c>
@@ -1346,7 +1349,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A16">
         <v>1</v>
       </c>
@@ -1383,7 +1386,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A17">
         <v>2</v>
       </c>
@@ -1420,7 +1423,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A18">
         <v>1</v>
       </c>
@@ -1457,7 +1460,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A19">
         <v>2</v>
       </c>
@@ -1494,7 +1497,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A20">
         <v>1</v>
       </c>
@@ -1531,7 +1534,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A21">
         <v>2</v>
       </c>
@@ -1568,7 +1571,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A22">
         <v>1</v>
       </c>
@@ -1605,7 +1608,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A23">
         <v>2</v>
       </c>
@@ -1642,7 +1645,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A24">
         <v>1</v>
       </c>
@@ -1679,7 +1682,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A25">
         <v>2</v>
       </c>
@@ -1716,7 +1719,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A26">
         <v>1</v>
       </c>
@@ -1753,7 +1756,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A27">
         <v>2</v>
       </c>
@@ -1790,7 +1793,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A28">
         <v>1</v>
       </c>
@@ -1830,7 +1833,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A29">
         <v>1</v>
       </c>
@@ -1870,7 +1873,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A30">
         <v>1</v>
       </c>
@@ -1907,7 +1910,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A31">
         <v>2</v>
       </c>
@@ -1943,7 +1946,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A32">
         <v>3</v>
       </c>
@@ -1982,7 +1985,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A33">
         <v>3</v>
       </c>
@@ -2018,7 +2021,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A34">
         <v>3</v>
       </c>
@@ -2055,7 +2058,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A35">
         <v>3</v>
       </c>
@@ -2092,7 +2095,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A36">
         <v>3</v>
       </c>
@@ -2129,7 +2132,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A37">
         <v>3</v>
       </c>
@@ -2166,7 +2169,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A38">
         <v>3</v>
       </c>
@@ -2203,7 +2206,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A39">
         <v>3</v>
       </c>
@@ -2240,7 +2243,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A40">
         <v>3</v>
       </c>
@@ -2277,7 +2280,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A41">
         <v>3</v>
       </c>
@@ -2314,7 +2317,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A42">
         <v>3</v>
       </c>
@@ -2351,7 +2354,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A43">
         <v>3</v>
       </c>
@@ -2388,7 +2391,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A44">
         <v>3</v>
       </c>
@@ -2422,7 +2425,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A45">
         <v>3</v>
       </c>
@@ -2459,7 +2462,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A46">
         <v>3</v>
       </c>
@@ -2496,7 +2499,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A47">
         <v>3</v>
       </c>
@@ -2533,7 +2536,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A48">
         <v>3</v>
       </c>
@@ -2567,7 +2570,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A49">
         <v>3</v>
       </c>
@@ -2601,7 +2604,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A50">
         <v>3</v>
       </c>
@@ -2635,7 +2638,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A51">
         <v>3</v>
       </c>
@@ -2669,7 +2672,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A52">
         <v>3</v>
       </c>
@@ -2703,7 +2706,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A53">
         <v>3</v>
       </c>
@@ -2737,7 +2740,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A54">
         <v>3</v>
       </c>
@@ -2771,7 +2774,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A55" s="2">
         <v>3</v>
       </c>
@@ -2805,7 +2808,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A56" s="2">
         <v>3</v>
       </c>
@@ -2852,17 +2855,17 @@
       <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="2" max="2" width="12.3828125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.3828125" customWidth="1"/>
+    <col min="2" max="2" width="12.3515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.3515625" customWidth="1"/>
     <col min="5" max="6" width="5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.53515625" customWidth="1"/>
-    <col min="8" max="8" width="58.53515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="30.53515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.52734375" customWidth="1"/>
+    <col min="8" max="8" width="58.52734375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="30.52734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.5">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2906,7 +2909,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.5">
       <c r="A2" t="s">
         <v>64</v>
       </c>
@@ -2939,7 +2942,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.5">
       <c r="A3" t="s">
         <v>64</v>
       </c>
@@ -2972,7 +2975,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.5">
       <c r="A4" t="s">
         <v>64</v>
       </c>
@@ -3005,7 +3008,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.5">
       <c r="A5" t="s">
         <v>64</v>
       </c>
@@ -3038,7 +3041,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.5">
       <c r="A6" t="s">
         <v>64</v>
       </c>
@@ -3071,7 +3074,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.5">
       <c r="A7" t="s">
         <v>64</v>
       </c>
@@ -3104,7 +3107,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.5">
       <c r="A8" t="s">
         <v>64</v>
       </c>
@@ -3137,7 +3140,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.5">
       <c r="A9" t="s">
         <v>64</v>
       </c>
@@ -3170,7 +3173,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.5">
       <c r="A10" s="2" t="s">
         <v>64</v>
       </c>
@@ -3195,7 +3198,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.5">
       <c r="A11" s="2" t="s">
         <v>64</v>
       </c>
@@ -3218,7 +3221,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.5">
       <c r="A12" s="2" t="s">
         <v>64</v>
       </c>
@@ -3241,7 +3244,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.5">
       <c r="A13" s="2" t="s">
         <v>64</v>
       </c>
@@ -3283,12 +3286,12 @@
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="14" max="14" width="9.53515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.52734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A1" t="s">
         <v>83</v>
       </c>
@@ -3335,7 +3338,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A2">
         <v>1</v>
       </c>
@@ -3368,7 +3371,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A3">
         <v>1</v>
       </c>
@@ -3401,7 +3404,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A4">
         <v>1</v>
       </c>
@@ -3434,7 +3437,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A5">
         <v>1</v>
       </c>
@@ -3467,7 +3470,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A6">
         <v>1</v>
       </c>
@@ -3500,7 +3503,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A7">
         <v>1</v>
       </c>
@@ -3533,7 +3536,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A8">
         <v>1</v>
       </c>
@@ -3566,7 +3569,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A9">
         <v>1</v>
       </c>
@@ -3612,13 +3615,13 @@
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" width="12.3828125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.3828125" customWidth="1"/>
+    <col min="1" max="1" width="12.3515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.3515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A1" t="s">
         <v>83</v>
       </c>
@@ -3665,7 +3668,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A2">
         <v>1</v>
       </c>
@@ -3695,7 +3698,7 @@
         <v>no_wk01_20200501_pA_wv01</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A3">
         <v>1</v>
       </c>
@@ -3728,7 +3731,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A4">
         <v>1</v>
       </c>
@@ -3758,7 +3761,7 @@
         <v>no_wk03_20200622_pA_wv03</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A5">
         <v>1</v>
       </c>
@@ -3791,7 +3794,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A6">
         <v>1</v>
       </c>
@@ -3824,7 +3827,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A7">
         <v>1</v>
       </c>
@@ -3864,20 +3867,20 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9984DEBA-9A58-467F-869B-4E55580BB1A4}">
-  <dimension ref="A1:M15"/>
+  <dimension ref="A1:M22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E9" sqref="E9:E15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G17" sqref="G17:G22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="7" max="7" width="10.69140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.703125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="59" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="27.3046875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="27.29296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3918,7 +3921,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A2" t="s">
         <v>99</v>
       </c>
@@ -3951,7 +3954,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A3" t="s">
         <v>100</v>
       </c>
@@ -3984,7 +3987,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A4" t="s">
         <v>101</v>
       </c>
@@ -4017,7 +4020,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A5" t="s">
         <v>102</v>
       </c>
@@ -4050,7 +4053,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A6" t="s">
         <v>103</v>
       </c>
@@ -4083,7 +4086,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A7" t="s">
         <v>104</v>
       </c>
@@ -4116,7 +4119,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A8" t="s">
         <v>105</v>
       </c>
@@ -4149,7 +4152,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A9" t="s">
         <v>99</v>
       </c>
@@ -4179,7 +4182,7 @@
         <v>at_wk02_20210118_pA_wv02</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A10" t="s">
         <v>100</v>
       </c>
@@ -4209,7 +4212,7 @@
         <v>dk_wk02_20210118_pA_wv02</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A11" t="s">
         <v>101</v>
       </c>
@@ -4239,7 +4242,7 @@
         <v>es_wk02_20210118_pA_wv02</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A12" t="s">
         <v>102</v>
       </c>
@@ -4269,7 +4272,7 @@
         <v>fr_wk02_20210118_pA_wv02</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A13" t="s">
         <v>103</v>
       </c>
@@ -4299,7 +4302,7 @@
         <v>it_wk02_20210118_pA_wv02</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A14" t="s">
         <v>104</v>
       </c>
@@ -4329,7 +4332,7 @@
         <v>pl_wk02_20210118_pA_wv02</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A15" t="s">
         <v>105</v>
       </c>
@@ -4357,6 +4360,216 @@
       <c r="I15" t="str">
         <f t="shared" si="0"/>
         <v>pt_wk02_20210118_pA_wv02</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.5">
+      <c r="A16" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="B16" s="2">
+        <v>5</v>
+      </c>
+      <c r="C16" s="2">
+        <v>0</v>
+      </c>
+      <c r="D16" s="2">
+        <v>3</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F16" s="2">
+        <v>3</v>
+      </c>
+      <c r="G16" s="3">
+        <v>44225</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="I16" s="2" t="str">
+        <f t="shared" ref="I16:I22" si="1">A16&amp;"_"&amp;"wk"&amp;TEXT(D16,"00")&amp;"_"&amp;YEAR(G16)&amp;TEXT(G16,"MM")&amp;TEXT(G16,"DD")&amp;"_p"&amp;E16&amp;"_wv"&amp;TEXT(F16,"00")&amp;""</f>
+        <v>at_wk03_20210129_pA_wv03</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.5">
+      <c r="A17" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="B17" s="2">
+        <v>5</v>
+      </c>
+      <c r="C17" s="2">
+        <v>0</v>
+      </c>
+      <c r="D17" s="2">
+        <v>3</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F17" s="2">
+        <v>3</v>
+      </c>
+      <c r="G17" s="3">
+        <v>44225</v>
+      </c>
+      <c r="H17" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="I17" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>dk_wk03_20210129_pA_wv03</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.5">
+      <c r="A18" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="B18" s="2">
+        <v>5</v>
+      </c>
+      <c r="C18" s="2">
+        <v>0</v>
+      </c>
+      <c r="D18" s="2">
+        <v>3</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F18" s="2">
+        <v>3</v>
+      </c>
+      <c r="G18" s="3">
+        <v>44225</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="I18" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>es_wk03_20210129_pA_wv03</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.5">
+      <c r="A19" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="B19" s="2">
+        <v>5</v>
+      </c>
+      <c r="C19" s="2">
+        <v>0</v>
+      </c>
+      <c r="D19" s="2">
+        <v>3</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F19" s="2">
+        <v>3</v>
+      </c>
+      <c r="G19" s="3">
+        <v>44225</v>
+      </c>
+      <c r="H19" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="I19" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>fr_wk03_20210129_pA_wv03</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.5">
+      <c r="A20" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="B20" s="2">
+        <v>5</v>
+      </c>
+      <c r="C20" s="2">
+        <v>0</v>
+      </c>
+      <c r="D20" s="2">
+        <v>3</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F20" s="2">
+        <v>3</v>
+      </c>
+      <c r="G20" s="3">
+        <v>44225</v>
+      </c>
+      <c r="H20" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="I20" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>it_wk03_20210129_pA_wv03</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.5">
+      <c r="A21" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="B21" s="2">
+        <v>5</v>
+      </c>
+      <c r="C21" s="2">
+        <v>0</v>
+      </c>
+      <c r="D21" s="2">
+        <v>3</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F21" s="2">
+        <v>3</v>
+      </c>
+      <c r="G21" s="3">
+        <v>44225</v>
+      </c>
+      <c r="H21" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="I21" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>pl_wk03_20210129_pA_wv03</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.5">
+      <c r="A22" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="B22" s="2">
+        <v>5</v>
+      </c>
+      <c r="C22" s="2">
+        <v>0</v>
+      </c>
+      <c r="D22" s="2">
+        <v>3</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F22" s="2">
+        <v>3</v>
+      </c>
+      <c r="G22" s="3">
+        <v>44225</v>
+      </c>
+      <c r="H22" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="I22" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>pt_wk03_20210129_pA_wv03</v>
       </c>
     </row>
   </sheetData>
@@ -4370,9 +4583,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A1" t="s">
         <v>119</v>
       </c>

</xml_diff>

<commit_message>
version 4 5 6
</commit_message>
<xml_diff>
--- a/data/spss_files.xlsx
+++ b/data/spss_files.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10111"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kw\Documents\comix_data_clean\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/amygimma/lshtm/comix_data_clean/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{226743BD-F6F6-4937-8D52-741C6B5E7BBF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC943A78-7D4F-FB47-B149-7CF763E44E8A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="13986" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25780" windowHeight="13980" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="5" r:id="rId1"/>
@@ -19,7 +19,8 @@
     <sheet name="NL" sheetId="3" r:id="rId4"/>
     <sheet name="NO" sheetId="4" r:id="rId5"/>
     <sheet name="Group1" sheetId="6" r:id="rId6"/>
-    <sheet name="Sheet1" sheetId="7" r:id="rId7"/>
+    <sheet name="Group2" sheetId="8" r:id="rId7"/>
+    <sheet name="Sheet1" sheetId="7" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="388" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="415" uniqueCount="131">
   <si>
     <t>country</t>
   </si>
@@ -409,16 +410,46 @@
   </si>
   <si>
     <t>20-030971_G1_Merged_Wave3_Final_v1_29012021_IntClientUse</t>
+  </si>
+  <si>
+    <t>20-030971_G2_Merged_Wave1_Final_v1_04022021_IntClientUse</t>
+  </si>
+  <si>
+    <t>lt</t>
+  </si>
+  <si>
+    <t>fi</t>
+  </si>
+  <si>
+    <t>ch</t>
+  </si>
+  <si>
+    <t>20_060765_BE2_Wave5_Final_v1_200121_IntClientUse</t>
+  </si>
+  <si>
+    <t>be_wk12_20200111_pB_wv05</t>
+  </si>
+  <si>
+    <t>20_060765_BE2_Wave6_Final_v1_270121_IntClientUse</t>
+  </si>
+  <si>
+    <t>be_wk12_20200111_pB_wv06</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -735,14 +766,14 @@
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>1</v>
       </c>
@@ -750,7 +781,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>2</v>
       </c>
@@ -758,7 +789,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>3</v>
       </c>
@@ -779,16 +810,16 @@
       <selection activeCell="H34" sqref="H34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.3515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.3515625" customWidth="1"/>
-    <col min="7" max="7" width="10.703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="58.29296875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="25.29296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.33203125" customWidth="1"/>
+    <col min="7" max="7" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="58.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="25.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>83</v>
       </c>
@@ -835,7 +866,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -871,7 +902,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
@@ -907,7 +938,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>1</v>
       </c>
@@ -943,7 +974,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>1</v>
       </c>
@@ -979,7 +1010,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>1</v>
       </c>
@@ -1015,7 +1046,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>1</v>
       </c>
@@ -1051,7 +1082,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>1</v>
       </c>
@@ -1090,7 +1121,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>2</v>
       </c>
@@ -1126,7 +1157,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>1</v>
       </c>
@@ -1163,7 +1194,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>2</v>
       </c>
@@ -1200,7 +1231,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.5">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>1</v>
       </c>
@@ -1237,7 +1268,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.5">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>2</v>
       </c>
@@ -1275,7 +1306,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.5">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>1</v>
       </c>
@@ -1312,7 +1343,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.5">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>2</v>
       </c>
@@ -1349,7 +1380,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.5">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>1</v>
       </c>
@@ -1386,7 +1417,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.5">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>2</v>
       </c>
@@ -1423,7 +1454,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.5">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>1</v>
       </c>
@@ -1460,7 +1491,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.5">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>2</v>
       </c>
@@ -1497,7 +1528,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.5">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>1</v>
       </c>
@@ -1534,7 +1565,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.5">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>2</v>
       </c>
@@ -1571,7 +1602,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.5">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>1</v>
       </c>
@@ -1608,7 +1639,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.5">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>2</v>
       </c>
@@ -1645,7 +1676,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.5">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>1</v>
       </c>
@@ -1682,7 +1713,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.5">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>2</v>
       </c>
@@ -1719,7 +1750,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.5">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>1</v>
       </c>
@@ -1756,7 +1787,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.5">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>2</v>
       </c>
@@ -1793,7 +1824,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.5">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>1</v>
       </c>
@@ -1833,7 +1864,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.5">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>1</v>
       </c>
@@ -1873,7 +1904,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.5">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>1</v>
       </c>
@@ -1910,7 +1941,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.5">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>2</v>
       </c>
@@ -1946,7 +1977,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.5">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>3</v>
       </c>
@@ -1985,7 +2016,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>3</v>
       </c>
@@ -2021,7 +2052,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>3</v>
       </c>
@@ -2058,7 +2089,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>3</v>
       </c>
@@ -2095,7 +2126,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>3</v>
       </c>
@@ -2132,7 +2163,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>3</v>
       </c>
@@ -2169,7 +2200,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>3</v>
       </c>
@@ -2206,7 +2237,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>3</v>
       </c>
@@ -2243,7 +2274,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>3</v>
       </c>
@@ -2280,7 +2311,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>3</v>
       </c>
@@ -2317,7 +2348,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>3</v>
       </c>
@@ -2354,7 +2385,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>3</v>
       </c>
@@ -2391,7 +2422,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>3</v>
       </c>
@@ -2425,7 +2456,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>3</v>
       </c>
@@ -2462,7 +2493,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>3</v>
       </c>
@@ -2499,7 +2530,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>3</v>
       </c>
@@ -2536,7 +2567,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>3</v>
       </c>
@@ -2570,7 +2601,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>3</v>
       </c>
@@ -2604,7 +2635,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>3</v>
       </c>
@@ -2638,7 +2669,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>3</v>
       </c>
@@ -2672,7 +2703,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>3</v>
       </c>
@@ -2706,7 +2737,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>3</v>
       </c>
@@ -2740,7 +2771,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>3</v>
       </c>
@@ -2774,7 +2805,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A55" s="2">
         <v>3</v>
       </c>
@@ -2808,7 +2839,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A56" s="2">
         <v>3</v>
       </c>
@@ -2849,23 +2880,23 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C042354-CAAB-48AD-AFC2-2197A2D12C9D}">
-  <dimension ref="A1:N13"/>
+  <dimension ref="A1:N15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="12.3515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.3515625" customWidth="1"/>
+    <col min="2" max="2" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.33203125" customWidth="1"/>
     <col min="5" max="6" width="5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.52734375" customWidth="1"/>
-    <col min="8" max="8" width="58.52734375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="30.52734375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.5" customWidth="1"/>
+    <col min="8" max="8" width="58.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="30.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2909,7 +2940,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>64</v>
       </c>
@@ -2942,7 +2973,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>64</v>
       </c>
@@ -2975,7 +3006,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>64</v>
       </c>
@@ -3008,7 +3039,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>64</v>
       </c>
@@ -3041,7 +3072,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>64</v>
       </c>
@@ -3074,7 +3105,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>64</v>
       </c>
@@ -3107,7 +3138,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>64</v>
       </c>
@@ -3140,7 +3171,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>64</v>
       </c>
@@ -3173,7 +3204,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>64</v>
       </c>
@@ -3198,7 +3229,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>64</v>
       </c>
@@ -3221,7 +3252,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.5">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>64</v>
       </c>
@@ -3244,7 +3275,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.5">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>64</v>
       </c>
@@ -3264,7 +3295,7 @@
         <v>4</v>
       </c>
       <c r="G13" s="3">
-        <v>43841</v>
+        <v>44207</v>
       </c>
       <c r="H13" s="2" t="s">
         <v>117</v>
@@ -3273,7 +3304,66 @@
         <v>118</v>
       </c>
     </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A14" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B14" s="2">
+        <v>4</v>
+      </c>
+      <c r="C14" s="2">
+        <v>0</v>
+      </c>
+      <c r="D14" s="2">
+        <v>13</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F14" s="2">
+        <v>5</v>
+      </c>
+      <c r="G14" s="3">
+        <v>44216</v>
+      </c>
+      <c r="H14" t="s">
+        <v>127</v>
+      </c>
+      <c r="I14" s="2" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A15" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B15" s="2">
+        <v>4</v>
+      </c>
+      <c r="C15" s="2">
+        <v>0</v>
+      </c>
+      <c r="D15" s="2">
+        <v>13</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F15" s="2">
+        <v>6</v>
+      </c>
+      <c r="G15" s="3">
+        <v>44223</v>
+      </c>
+      <c r="H15" t="s">
+        <v>129</v>
+      </c>
+      <c r="I15" s="2" t="s">
+        <v>130</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -3286,12 +3376,12 @@
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="14" max="14" width="9.52734375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>83</v>
       </c>
@@ -3338,7 +3428,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -3371,7 +3461,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
@@ -3404,7 +3494,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>1</v>
       </c>
@@ -3437,7 +3527,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>1</v>
       </c>
@@ -3470,7 +3560,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>1</v>
       </c>
@@ -3503,7 +3593,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>1</v>
       </c>
@@ -3536,7 +3626,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>1</v>
       </c>
@@ -3569,7 +3659,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>1</v>
       </c>
@@ -3615,13 +3705,13 @@
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.3515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.3515625" customWidth="1"/>
+    <col min="1" max="1" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>83</v>
       </c>
@@ -3668,7 +3758,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -3698,7 +3788,7 @@
         <v>no_wk01_20200501_pA_wv01</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
@@ -3731,7 +3821,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>1</v>
       </c>
@@ -3761,7 +3851,7 @@
         <v>no_wk03_20200622_pA_wv03</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>1</v>
       </c>
@@ -3794,7 +3884,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>1</v>
       </c>
@@ -3827,7 +3917,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>1</v>
       </c>
@@ -3869,18 +3959,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9984DEBA-9A58-467F-869B-4E55580BB1A4}">
   <dimension ref="A1:M22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17:G22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="7" max="7" width="10.703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.6640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="59" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="27.29296875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="27.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3921,7 +4011,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>99</v>
       </c>
@@ -3954,7 +4044,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>100</v>
       </c>
@@ -3987,7 +4077,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>101</v>
       </c>
@@ -4020,7 +4110,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>102</v>
       </c>
@@ -4053,7 +4143,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>103</v>
       </c>
@@ -4086,7 +4176,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>104</v>
       </c>
@@ -4119,7 +4209,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>105</v>
       </c>
@@ -4152,7 +4242,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>99</v>
       </c>
@@ -4182,7 +4272,7 @@
         <v>at_wk02_20210118_pA_wv02</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>100</v>
       </c>
@@ -4212,7 +4302,7 @@
         <v>dk_wk02_20210118_pA_wv02</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>101</v>
       </c>
@@ -4242,7 +4332,7 @@
         <v>es_wk02_20210118_pA_wv02</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.5">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>102</v>
       </c>
@@ -4272,7 +4362,7 @@
         <v>fr_wk02_20210118_pA_wv02</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.5">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>103</v>
       </c>
@@ -4302,7 +4392,7 @@
         <v>it_wk02_20210118_pA_wv02</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.5">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>104</v>
       </c>
@@ -4332,7 +4422,7 @@
         <v>pl_wk02_20210118_pA_wv02</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.5">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>105</v>
       </c>
@@ -4362,7 +4452,7 @@
         <v>pt_wk02_20210118_pA_wv02</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.5">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
         <v>99</v>
       </c>
@@ -4392,7 +4482,7 @@
         <v>at_wk03_20210129_pA_wv03</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
         <v>100</v>
       </c>
@@ -4422,7 +4512,7 @@
         <v>dk_wk03_20210129_pA_wv03</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
         <v>101</v>
       </c>
@@ -4452,7 +4542,7 @@
         <v>es_wk03_20210129_pA_wv03</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
         <v>102</v>
       </c>
@@ -4482,7 +4572,7 @@
         <v>fr_wk03_20210129_pA_wv03</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
         <v>103</v>
       </c>
@@ -4512,7 +4602,7 @@
         <v>it_wk03_20210129_pA_wv03</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
         <v>104</v>
       </c>
@@ -4542,7 +4632,7 @@
         <v>pl_wk03_20210129_pA_wv03</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
         <v>105</v>
       </c>
@@ -4578,14 +4668,166 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B44EFFA-AC3D-0445-9643-71A374D3D58F}">
+  <dimension ref="A1:J4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="10.5" customWidth="1"/>
+    <col min="2" max="2" width="16.6640625" customWidth="1"/>
+    <col min="3" max="3" width="8.6640625" customWidth="1"/>
+    <col min="4" max="4" width="7.33203125" customWidth="1"/>
+    <col min="5" max="5" width="8.5" customWidth="1"/>
+    <col min="6" max="6" width="9.33203125" customWidth="1"/>
+    <col min="7" max="7" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="52.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="24.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="6.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="B2" s="2">
+        <v>6</v>
+      </c>
+      <c r="C2" s="2">
+        <v>0</v>
+      </c>
+      <c r="D2" s="2">
+        <v>1</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" s="2">
+        <v>1</v>
+      </c>
+      <c r="G2" s="3">
+        <v>44207</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="I2" s="2" t="str">
+        <f>A2&amp;"_"&amp;"wk"&amp;TEXT(D2,"00")&amp;"_"&amp;YEAR(G3)&amp;TEXT(G3,"MM")&amp;TEXT(G3,"DD")&amp;"_p"&amp;E2&amp;"_wv"&amp;TEXT(F2,"00")&amp;""</f>
+        <v>lt_wk01_20210112_pA_wv01</v>
+      </c>
+      <c r="J2" s="2"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>125</v>
+      </c>
+      <c r="B3" s="2">
+        <v>6</v>
+      </c>
+      <c r="C3" s="2">
+        <v>0</v>
+      </c>
+      <c r="D3" s="2">
+        <v>1</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" s="2">
+        <v>1</v>
+      </c>
+      <c r="G3" s="3">
+        <v>44208</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="I3" s="2" t="str">
+        <f t="shared" ref="I3:I4" si="0">A3&amp;"_"&amp;"wk"&amp;TEXT(D3,"00")&amp;"_"&amp;YEAR(G4)&amp;TEXT(G4,"MM")&amp;TEXT(G4,"DD")&amp;"_p"&amp;E3&amp;"_wv"&amp;TEXT(F3,"00")&amp;""</f>
+        <v>fi_wk01_20210113_pA_wv01</v>
+      </c>
+      <c r="J3" s="2"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>126</v>
+      </c>
+      <c r="B4" s="2">
+        <v>6</v>
+      </c>
+      <c r="C4" s="2">
+        <v>0</v>
+      </c>
+      <c r="D4" s="2">
+        <v>1</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" s="2">
+        <v>1</v>
+      </c>
+      <c r="G4" s="3">
+        <v>44209</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="I4" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>ch_wk01_19000100_pA_wv01</v>
+      </c>
+      <c r="J4" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9379CF0-E466-4164-B69D-1322B08B2D66}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>119</v>
       </c>

</xml_diff>

<commit_message>
clean eu-child data part 1
</commit_message>
<xml_diff>
--- a/data/spss_files.xlsx
+++ b/data/spss_files.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/amygimma/lshtm/comix_data_clean/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC943A78-7D4F-FB47-B149-7CF763E44E8A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8220A6E9-A456-D14F-B2E2-5BF5E4BBB045}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25780" windowHeight="13980" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25780" windowHeight="13980" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="5" r:id="rId1"/>
@@ -21,6 +21,7 @@
     <sheet name="Group1" sheetId="6" r:id="rId6"/>
     <sheet name="Group2" sheetId="8" r:id="rId7"/>
     <sheet name="Sheet1" sheetId="7" r:id="rId8"/>
+    <sheet name="EUchild" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="415" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="455" uniqueCount="134">
   <si>
     <t>country</t>
   </si>
@@ -434,13 +435,22 @@
   </si>
   <si>
     <t>be_wk12_20200111_pB_wv06</t>
+  </si>
+  <si>
+    <t>20-030971_G1_Merged_Wave1_Parents_Final_v1_12022021_IntClientUse</t>
+  </si>
+  <si>
+    <t>20-030971_G2_Merged_Wave1_Parents_Final_v1_12022021_IntClientUse</t>
+  </si>
+  <si>
+    <t>gr</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -450,6 +460,13 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -475,11 +492,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2882,8 +2901,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C042354-CAAB-48AD-AFC2-2197A2D12C9D}">
   <dimension ref="A1:N15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I19" sqref="I19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3960,7 +3979,7 @@
   <dimension ref="A1:M22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+      <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4672,7 +4691,7 @@
   <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection sqref="A1:J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4835,4 +4854,368 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BED03538-A030-6E4C-BA50-2D13272854A1}">
+  <dimension ref="A1:M10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="I13" sqref="I13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="7.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="58.33203125" customWidth="1"/>
+    <col min="9" max="9" width="25" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="6.83203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.83203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A2" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="B2" s="4">
+        <v>7</v>
+      </c>
+      <c r="C2" s="4">
+        <v>0</v>
+      </c>
+      <c r="D2" s="4">
+        <v>1</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F2" s="4">
+        <v>1</v>
+      </c>
+      <c r="G2" s="5">
+        <v>44207</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="I2" s="4" t="str">
+        <f>A2&amp;"_"&amp;"wk"&amp;TEXT(D2,"00")&amp;"_"&amp;YEAR(G2)&amp;TEXT(G2,"MM")&amp;TEXT(G2,"DD")&amp;"_p"&amp;E2&amp;"_wv"&amp;TEXT(F2,"00")&amp;""</f>
+        <v>at_wk01_20210111_pC_wv01</v>
+      </c>
+      <c r="J2" s="4"/>
+      <c r="K2" s="4"/>
+      <c r="L2" s="4"/>
+      <c r="M2" s="4"/>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A3" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="B3" s="4">
+        <v>7</v>
+      </c>
+      <c r="C3" s="4">
+        <v>0</v>
+      </c>
+      <c r="D3" s="4">
+        <v>1</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F3" s="4">
+        <v>1</v>
+      </c>
+      <c r="G3" s="5">
+        <v>44207</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="I3" s="4" t="str">
+        <f t="shared" ref="I3:I10" si="0">A3&amp;"_"&amp;"wk"&amp;TEXT(D3,"00")&amp;"_"&amp;YEAR(G3)&amp;TEXT(G3,"MM")&amp;TEXT(G3,"DD")&amp;"_p"&amp;E3&amp;"_wv"&amp;TEXT(F3,"00")&amp;""</f>
+        <v>dk_wk01_20210111_pC_wv01</v>
+      </c>
+      <c r="J3" s="4"/>
+      <c r="K3" s="4"/>
+      <c r="L3" s="4"/>
+      <c r="M3" s="4"/>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A4" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="B4" s="4">
+        <v>7</v>
+      </c>
+      <c r="C4" s="4">
+        <v>0</v>
+      </c>
+      <c r="D4" s="4">
+        <v>1</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F4" s="4">
+        <v>1</v>
+      </c>
+      <c r="G4" s="5">
+        <v>44207</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="I4" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>fr_wk01_20210111_pC_wv01</v>
+      </c>
+      <c r="J4" s="4"/>
+      <c r="K4" s="4"/>
+      <c r="L4" s="4"/>
+      <c r="M4" s="4"/>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A5" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="B5" s="4">
+        <v>7</v>
+      </c>
+      <c r="C5" s="4">
+        <v>0</v>
+      </c>
+      <c r="D5" s="4">
+        <v>1</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F5" s="4">
+        <v>1</v>
+      </c>
+      <c r="G5" s="5">
+        <v>44207</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="I5" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>it_wk01_20210111_pC_wv01</v>
+      </c>
+      <c r="J5" s="4"/>
+      <c r="K5" s="4"/>
+      <c r="L5" s="4"/>
+      <c r="M5" s="4"/>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A6" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="B6" s="4">
+        <v>7</v>
+      </c>
+      <c r="C6" s="4">
+        <v>0</v>
+      </c>
+      <c r="D6" s="4">
+        <v>1</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F6" s="4">
+        <v>1</v>
+      </c>
+      <c r="G6" s="5">
+        <v>44207</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="I6" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>pl_wk01_20210111_pC_wv01</v>
+      </c>
+      <c r="J6" s="4"/>
+      <c r="K6" s="4"/>
+      <c r="L6" s="4"/>
+      <c r="M6" s="4"/>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="B7" s="4">
+        <v>7</v>
+      </c>
+      <c r="C7" s="2">
+        <v>0</v>
+      </c>
+      <c r="D7" s="2">
+        <v>1</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F7" s="2">
+        <v>1</v>
+      </c>
+      <c r="G7" s="3">
+        <v>44207</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="I7" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>lt_wk01_20210111_pC_wv01</v>
+      </c>
+      <c r="J7" s="2"/>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="B8" s="4">
+        <v>7</v>
+      </c>
+      <c r="C8" s="2">
+        <v>0</v>
+      </c>
+      <c r="D8" s="2">
+        <v>1</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F8" s="2">
+        <v>1</v>
+      </c>
+      <c r="G8" s="3">
+        <v>44208</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="I8" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>fi_wk01_20210112_pC_wv01</v>
+      </c>
+      <c r="J8" s="2"/>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="B9" s="4">
+        <v>7</v>
+      </c>
+      <c r="C9" s="2">
+        <v>0</v>
+      </c>
+      <c r="D9" s="2">
+        <v>1</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F9" s="2">
+        <v>1</v>
+      </c>
+      <c r="G9" s="3">
+        <v>44209</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="I9" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>ch_wk01_20210113_pC_wv01</v>
+      </c>
+      <c r="J9" s="2"/>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A10" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="B10" s="4">
+        <v>7</v>
+      </c>
+      <c r="C10" s="2">
+        <v>0</v>
+      </c>
+      <c r="D10" s="2">
+        <v>1</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F10" s="2">
+        <v>1</v>
+      </c>
+      <c r="G10" s="3">
+        <v>44209</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="I10" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>gr_wk01_20210113_pC_wv01</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
cleaning for v5 with children
</commit_message>
<xml_diff>
--- a/data/spss_files.xlsx
+++ b/data/spss_files.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/amygimma/lshtm/comix_data_clean/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A13FBEDE-AB2D-6749-99A0-9CE7CAF2C2C4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6F390B4-7F9C-144D-9DED-8E5BA8AFF062}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2180" yWindow="5680" windowWidth="25780" windowHeight="13980" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2780" yWindow="2420" windowWidth="25780" windowHeight="13980" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="5" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="461" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="488" uniqueCount="136">
   <si>
     <t>country</t>
   </si>
@@ -3397,7 +3397,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7709FE3-57B1-4766-A5D4-6B378E0A5BA3}">
   <dimension ref="A1:O11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
@@ -4037,10 +4037,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9984DEBA-9A58-467F-869B-4E55580BB1A4}">
-  <dimension ref="A1:M22"/>
+  <dimension ref="A1:M27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H24" sqref="H24"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A28" sqref="A28:XFD28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4150,7 +4150,7 @@
         <v>106</v>
       </c>
       <c r="I3" t="str">
-        <f t="shared" ref="I3:I15" si="0">A3&amp;"_"&amp;"wk"&amp;TEXT(D3,"00")&amp;"_"&amp;YEAR(G3)&amp;TEXT(G3,"MM")&amp;TEXT(G3,"DD")&amp;"_p"&amp;E3&amp;"_wv"&amp;TEXT(F3,"00")&amp;""</f>
+        <f>A3&amp;"_"&amp;"wk"&amp;TEXT(D3,"00")&amp;"_"&amp;YEAR(G3)&amp;TEXT(G3,"MM")&amp;TEXT(G3,"DD")&amp;"_p"&amp;E3&amp;"_wv"&amp;TEXT(F3,"00")&amp;""</f>
         <v>dk_wk01_20210111_pA_wv01</v>
       </c>
       <c r="J3">
@@ -4183,7 +4183,7 @@
         <v>107</v>
       </c>
       <c r="I4" t="str">
-        <f t="shared" si="0"/>
+        <f>A4&amp;"_"&amp;"wk"&amp;TEXT(D4,"00")&amp;"_"&amp;YEAR(G4)&amp;TEXT(G4,"MM")&amp;TEXT(G4,"DD")&amp;"_p"&amp;E4&amp;"_wv"&amp;TEXT(F4,"00")&amp;""</f>
         <v>es_wk01_20210111_pA_wv01</v>
       </c>
       <c r="J4">
@@ -4216,7 +4216,7 @@
         <v>108</v>
       </c>
       <c r="I5" t="str">
-        <f t="shared" si="0"/>
+        <f>A5&amp;"_"&amp;"wk"&amp;TEXT(D5,"00")&amp;"_"&amp;YEAR(G5)&amp;TEXT(G5,"MM")&amp;TEXT(G5,"DD")&amp;"_p"&amp;E5&amp;"_wv"&amp;TEXT(F5,"00")&amp;""</f>
         <v>fr_wk01_20210111_pA_wv01</v>
       </c>
       <c r="J5">
@@ -4249,7 +4249,7 @@
         <v>109</v>
       </c>
       <c r="I6" t="str">
-        <f t="shared" si="0"/>
+        <f>A6&amp;"_"&amp;"wk"&amp;TEXT(D6,"00")&amp;"_"&amp;YEAR(G6)&amp;TEXT(G6,"MM")&amp;TEXT(G6,"DD")&amp;"_p"&amp;E6&amp;"_wv"&amp;TEXT(F6,"00")&amp;""</f>
         <v>it_wk01_20210111_pA_wv01</v>
       </c>
       <c r="J6">
@@ -4282,7 +4282,7 @@
         <v>110</v>
       </c>
       <c r="I7" t="str">
-        <f t="shared" si="0"/>
+        <f>A7&amp;"_"&amp;"wk"&amp;TEXT(D7,"00")&amp;"_"&amp;YEAR(G7)&amp;TEXT(G7,"MM")&amp;TEXT(G7,"DD")&amp;"_p"&amp;E7&amp;"_wv"&amp;TEXT(F7,"00")&amp;""</f>
         <v>pl_wk01_20210111_pA_wv01</v>
       </c>
       <c r="J7">
@@ -4315,7 +4315,7 @@
         <v>111</v>
       </c>
       <c r="I8" t="str">
-        <f t="shared" si="0"/>
+        <f>A8&amp;"_"&amp;"wk"&amp;TEXT(D8,"00")&amp;"_"&amp;YEAR(G8)&amp;TEXT(G8,"MM")&amp;TEXT(G8,"DD")&amp;"_p"&amp;E8&amp;"_wv"&amp;TEXT(F8,"00")&amp;""</f>
         <v>pt_wk01_20210111_pA_wv01</v>
       </c>
       <c r="J8">
@@ -4348,7 +4348,7 @@
         <v>113</v>
       </c>
       <c r="I9" t="str">
-        <f t="shared" si="0"/>
+        <f>A9&amp;"_"&amp;"wk"&amp;TEXT(D9,"00")&amp;"_"&amp;YEAR(G9)&amp;TEXT(G9,"MM")&amp;TEXT(G9,"DD")&amp;"_p"&amp;E9&amp;"_wv"&amp;TEXT(F9,"00")&amp;""</f>
         <v>at_wk02_20210118_pA_wv02</v>
       </c>
     </row>
@@ -4378,7 +4378,7 @@
         <v>113</v>
       </c>
       <c r="I10" t="str">
-        <f t="shared" si="0"/>
+        <f>A10&amp;"_"&amp;"wk"&amp;TEXT(D10,"00")&amp;"_"&amp;YEAR(G10)&amp;TEXT(G10,"MM")&amp;TEXT(G10,"DD")&amp;"_p"&amp;E10&amp;"_wv"&amp;TEXT(F10,"00")&amp;""</f>
         <v>dk_wk02_20210118_pA_wv02</v>
       </c>
     </row>
@@ -4408,7 +4408,7 @@
         <v>113</v>
       </c>
       <c r="I11" t="str">
-        <f t="shared" si="0"/>
+        <f>A11&amp;"_"&amp;"wk"&amp;TEXT(D11,"00")&amp;"_"&amp;YEAR(G11)&amp;TEXT(G11,"MM")&amp;TEXT(G11,"DD")&amp;"_p"&amp;E11&amp;"_wv"&amp;TEXT(F11,"00")&amp;""</f>
         <v>es_wk02_20210118_pA_wv02</v>
       </c>
     </row>
@@ -4438,7 +4438,7 @@
         <v>113</v>
       </c>
       <c r="I12" t="str">
-        <f t="shared" si="0"/>
+        <f>A12&amp;"_"&amp;"wk"&amp;TEXT(D12,"00")&amp;"_"&amp;YEAR(G12)&amp;TEXT(G12,"MM")&amp;TEXT(G12,"DD")&amp;"_p"&amp;E12&amp;"_wv"&amp;TEXT(F12,"00")&amp;""</f>
         <v>fr_wk02_20210118_pA_wv02</v>
       </c>
     </row>
@@ -4468,7 +4468,7 @@
         <v>113</v>
       </c>
       <c r="I13" t="str">
-        <f t="shared" si="0"/>
+        <f>A13&amp;"_"&amp;"wk"&amp;TEXT(D13,"00")&amp;"_"&amp;YEAR(G13)&amp;TEXT(G13,"MM")&amp;TEXT(G13,"DD")&amp;"_p"&amp;E13&amp;"_wv"&amp;TEXT(F13,"00")&amp;""</f>
         <v>it_wk02_20210118_pA_wv02</v>
       </c>
     </row>
@@ -4498,7 +4498,7 @@
         <v>113</v>
       </c>
       <c r="I14" t="str">
-        <f t="shared" si="0"/>
+        <f>A14&amp;"_"&amp;"wk"&amp;TEXT(D14,"00")&amp;"_"&amp;YEAR(G14)&amp;TEXT(G14,"MM")&amp;TEXT(G14,"DD")&amp;"_p"&amp;E14&amp;"_wv"&amp;TEXT(F14,"00")&amp;""</f>
         <v>pl_wk02_20210118_pA_wv02</v>
       </c>
     </row>
@@ -4528,7 +4528,7 @@
         <v>113</v>
       </c>
       <c r="I15" t="str">
-        <f t="shared" si="0"/>
+        <f>A15&amp;"_"&amp;"wk"&amp;TEXT(D15,"00")&amp;"_"&amp;YEAR(G15)&amp;TEXT(G15,"MM")&amp;TEXT(G15,"DD")&amp;"_p"&amp;E15&amp;"_wv"&amp;TEXT(F15,"00")&amp;""</f>
         <v>pt_wk02_20210118_pA_wv02</v>
       </c>
     </row>
@@ -4558,7 +4558,7 @@
         <v>122</v>
       </c>
       <c r="I16" s="2" t="str">
-        <f t="shared" ref="I16:I22" si="1">A16&amp;"_"&amp;"wk"&amp;TEXT(D16,"00")&amp;"_"&amp;YEAR(G16)&amp;TEXT(G16,"MM")&amp;TEXT(G16,"DD")&amp;"_p"&amp;E16&amp;"_wv"&amp;TEXT(F16,"00")&amp;""</f>
+        <f>A16&amp;"_"&amp;"wk"&amp;TEXT(D16,"00")&amp;"_"&amp;YEAR(G16)&amp;TEXT(G16,"MM")&amp;TEXT(G16,"DD")&amp;"_p"&amp;E16&amp;"_wv"&amp;TEXT(F16,"00")&amp;""</f>
         <v>at_wk03_20210129_pA_wv03</v>
       </c>
     </row>
@@ -4588,7 +4588,7 @@
         <v>122</v>
       </c>
       <c r="I17" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f>A17&amp;"_"&amp;"wk"&amp;TEXT(D17,"00")&amp;"_"&amp;YEAR(G17)&amp;TEXT(G17,"MM")&amp;TEXT(G17,"DD")&amp;"_p"&amp;E17&amp;"_wv"&amp;TEXT(F17,"00")&amp;""</f>
         <v>dk_wk03_20210129_pA_wv03</v>
       </c>
     </row>
@@ -4618,7 +4618,7 @@
         <v>122</v>
       </c>
       <c r="I18" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f>A18&amp;"_"&amp;"wk"&amp;TEXT(D18,"00")&amp;"_"&amp;YEAR(G18)&amp;TEXT(G18,"MM")&amp;TEXT(G18,"DD")&amp;"_p"&amp;E18&amp;"_wv"&amp;TEXT(F18,"00")&amp;""</f>
         <v>es_wk03_20210129_pA_wv03</v>
       </c>
     </row>
@@ -4648,7 +4648,7 @@
         <v>122</v>
       </c>
       <c r="I19" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f>A19&amp;"_"&amp;"wk"&amp;TEXT(D19,"00")&amp;"_"&amp;YEAR(G19)&amp;TEXT(G19,"MM")&amp;TEXT(G19,"DD")&amp;"_p"&amp;E19&amp;"_wv"&amp;TEXT(F19,"00")&amp;""</f>
         <v>fr_wk03_20210129_pA_wv03</v>
       </c>
     </row>
@@ -4678,7 +4678,7 @@
         <v>122</v>
       </c>
       <c r="I20" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f>A20&amp;"_"&amp;"wk"&amp;TEXT(D20,"00")&amp;"_"&amp;YEAR(G20)&amp;TEXT(G20,"MM")&amp;TEXT(G20,"DD")&amp;"_p"&amp;E20&amp;"_wv"&amp;TEXT(F20,"00")&amp;""</f>
         <v>it_wk03_20210129_pA_wv03</v>
       </c>
     </row>
@@ -4708,7 +4708,7 @@
         <v>122</v>
       </c>
       <c r="I21" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f>A21&amp;"_"&amp;"wk"&amp;TEXT(D21,"00")&amp;"_"&amp;YEAR(G21)&amp;TEXT(G21,"MM")&amp;TEXT(G21,"DD")&amp;"_p"&amp;E21&amp;"_wv"&amp;TEXT(F21,"00")&amp;""</f>
         <v>pl_wk03_20210129_pA_wv03</v>
       </c>
     </row>
@@ -4738,8 +4738,158 @@
         <v>122</v>
       </c>
       <c r="I22" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f>A22&amp;"_"&amp;"wk"&amp;TEXT(D22,"00")&amp;"_"&amp;YEAR(G22)&amp;TEXT(G22,"MM")&amp;TEXT(G22,"DD")&amp;"_p"&amp;E22&amp;"_wv"&amp;TEXT(F22,"00")&amp;""</f>
         <v>pt_wk03_20210129_pA_wv03</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A23" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="B23" s="4">
+        <v>5</v>
+      </c>
+      <c r="C23" s="4">
+        <v>0</v>
+      </c>
+      <c r="D23" s="4">
+        <v>1</v>
+      </c>
+      <c r="E23" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F23" s="4">
+        <v>1</v>
+      </c>
+      <c r="G23" s="5">
+        <v>44207</v>
+      </c>
+      <c r="H23" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="I23" s="4" t="str">
+        <f>A23&amp;"_"&amp;"wk"&amp;TEXT(D23,"00")&amp;"_"&amp;YEAR(G23)&amp;TEXT(G23,"MM")&amp;TEXT(G23,"DD")&amp;"_p"&amp;E23&amp;"_wv"&amp;TEXT(F23,"00")&amp;""</f>
+        <v>at_wk01_20210111_pC_wv01</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A24" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="B24" s="4">
+        <v>5</v>
+      </c>
+      <c r="C24" s="4">
+        <v>0</v>
+      </c>
+      <c r="D24" s="4">
+        <v>1</v>
+      </c>
+      <c r="E24" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F24" s="4">
+        <v>1</v>
+      </c>
+      <c r="G24" s="5">
+        <v>44207</v>
+      </c>
+      <c r="H24" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="I24" s="4" t="str">
+        <f>A24&amp;"_"&amp;"wk"&amp;TEXT(D24,"00")&amp;"_"&amp;YEAR(G24)&amp;TEXT(G24,"MM")&amp;TEXT(G24,"DD")&amp;"_p"&amp;E24&amp;"_wv"&amp;TEXT(F24,"00")&amp;""</f>
+        <v>dk_wk01_20210111_pC_wv01</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A25" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="B25" s="4">
+        <v>5</v>
+      </c>
+      <c r="C25" s="4">
+        <v>0</v>
+      </c>
+      <c r="D25" s="4">
+        <v>1</v>
+      </c>
+      <c r="E25" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F25" s="4">
+        <v>1</v>
+      </c>
+      <c r="G25" s="5">
+        <v>44207</v>
+      </c>
+      <c r="H25" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="I25" s="4" t="str">
+        <f>A25&amp;"_"&amp;"wk"&amp;TEXT(D25,"00")&amp;"_"&amp;YEAR(G25)&amp;TEXT(G25,"MM")&amp;TEXT(G25,"DD")&amp;"_p"&amp;E25&amp;"_wv"&amp;TEXT(F25,"00")&amp;""</f>
+        <v>fr_wk01_20210111_pC_wv01</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A26" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="B26" s="4">
+        <v>5</v>
+      </c>
+      <c r="C26" s="4">
+        <v>0</v>
+      </c>
+      <c r="D26" s="4">
+        <v>1</v>
+      </c>
+      <c r="E26" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F26" s="4">
+        <v>1</v>
+      </c>
+      <c r="G26" s="5">
+        <v>44207</v>
+      </c>
+      <c r="H26" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="I26" s="4" t="str">
+        <f>A26&amp;"_"&amp;"wk"&amp;TEXT(D26,"00")&amp;"_"&amp;YEAR(G26)&amp;TEXT(G26,"MM")&amp;TEXT(G26,"DD")&amp;"_p"&amp;E26&amp;"_wv"&amp;TEXT(F26,"00")&amp;""</f>
+        <v>it_wk01_20210111_pC_wv01</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A27" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="B27" s="4">
+        <v>5</v>
+      </c>
+      <c r="C27" s="4">
+        <v>0</v>
+      </c>
+      <c r="D27" s="4">
+        <v>1</v>
+      </c>
+      <c r="E27" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F27" s="4">
+        <v>1</v>
+      </c>
+      <c r="G27" s="5">
+        <v>44207</v>
+      </c>
+      <c r="H27" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="I27" s="4" t="str">
+        <f>A27&amp;"_"&amp;"wk"&amp;TEXT(D27,"00")&amp;"_"&amp;YEAR(G27)&amp;TEXT(G27,"MM")&amp;TEXT(G27,"DD")&amp;"_p"&amp;E27&amp;"_wv"&amp;TEXT(F27,"00")&amp;""</f>
+        <v>pl_wk01_20210111_pC_wv01</v>
       </c>
     </row>
   </sheetData>
@@ -4749,10 +4899,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B44EFFA-AC3D-0445-9643-71A374D3D58F}">
-  <dimension ref="A1:J4"/>
+  <dimension ref="A1:J8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:J4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4806,7 +4956,7 @@
         <v>124</v>
       </c>
       <c r="B2" s="2">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C2" s="2">
         <v>0</v>
@@ -4837,7 +4987,7 @@
         <v>125</v>
       </c>
       <c r="B3" s="2">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C3" s="2">
         <v>0</v>
@@ -4868,7 +5018,7 @@
         <v>126</v>
       </c>
       <c r="B4" s="2">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C4" s="2">
         <v>0</v>
@@ -4890,9 +5040,129 @@
       </c>
       <c r="I4" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>ch_wk01_19000100_pA_wv01</v>
+        <v>ch_wk01_20210112_pA_wv01</v>
       </c>
       <c r="J4" s="2"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="B5" s="4">
+        <v>5</v>
+      </c>
+      <c r="C5" s="2">
+        <v>0</v>
+      </c>
+      <c r="D5" s="2">
+        <v>1</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F5" s="2">
+        <v>1</v>
+      </c>
+      <c r="G5" s="3">
+        <v>44208</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="I5" s="4" t="str">
+        <f t="shared" ref="I5:I7" si="1">A5&amp;"_"&amp;"wk"&amp;TEXT(D5,"00")&amp;"_"&amp;YEAR(G5)&amp;TEXT(G5,"MM")&amp;TEXT(G5,"DD")&amp;"_p"&amp;E5&amp;"_wv"&amp;TEXT(F5,"00")&amp;""</f>
+        <v>fi_wk01_20210112_pC_wv01</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="B6" s="4">
+        <v>5</v>
+      </c>
+      <c r="C6" s="2">
+        <v>0</v>
+      </c>
+      <c r="D6" s="2">
+        <v>1</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F6" s="2">
+        <v>1</v>
+      </c>
+      <c r="G6" s="3">
+        <v>44209</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="I6" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>ch_wk01_20210113_pC_wv01</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="B7" s="4">
+        <v>5</v>
+      </c>
+      <c r="C7" s="2">
+        <v>0</v>
+      </c>
+      <c r="D7" s="2">
+        <v>1</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F7" s="2">
+        <v>1</v>
+      </c>
+      <c r="G7" s="3">
+        <v>44209</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="I7" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>gr_wk01_20210113_pC_wv01</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="B8" s="4">
+        <v>5</v>
+      </c>
+      <c r="C8" s="2">
+        <v>0</v>
+      </c>
+      <c r="D8" s="2">
+        <v>1</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F8" s="2">
+        <v>1</v>
+      </c>
+      <c r="G8" s="3">
+        <v>44207</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="I8" s="4" t="str">
+        <f>A8&amp;"_"&amp;"wk"&amp;TEXT(D8,"00")&amp;"_"&amp;YEAR(G8)&amp;TEXT(G8,"MM")&amp;TEXT(G8,"DD")&amp;"_p"&amp;E8&amp;"_wv"&amp;TEXT(F8,"00")&amp;""</f>
+        <v>lt_wk01_20210111_pC_wv01</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4922,7 +5192,7 @@
   <dimension ref="A1:M10"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+      <selection activeCell="A8" sqref="A8:I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Update to give options for either country or group in shell script
</commit_message>
<xml_diff>
--- a/data/spss_files.xlsx
+++ b/data/spss_files.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/amygimma/lshtm/comix_data_clean/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jarvisc1\Documents\projects\comix_data_clean\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6F390B4-7F9C-144D-9DED-8E5BA8AFF062}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5848D049-F5B0-4893-95B6-5D7630BC43A8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2780" yWindow="2420" windowWidth="25780" windowHeight="13980" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18120" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="5" r:id="rId1"/>
@@ -791,14 +791,14 @@
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.84375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <sheetData>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A5">
         <v>1</v>
       </c>
@@ -806,7 +806,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A6">
         <v>2</v>
       </c>
@@ -814,7 +814,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A7">
         <v>3</v>
       </c>
@@ -835,16 +835,16 @@
       <selection activeCell="H34" sqref="H34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.84375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.33203125" customWidth="1"/>
-    <col min="7" max="7" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="58.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="25.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.3046875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.3046875" customWidth="1"/>
+    <col min="7" max="7" width="10.69140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="58.3046875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="25.3046875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>83</v>
       </c>
@@ -891,7 +891,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A2">
         <v>1</v>
       </c>
@@ -927,7 +927,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A3">
         <v>1</v>
       </c>
@@ -963,7 +963,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A4">
         <v>1</v>
       </c>
@@ -999,7 +999,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A5">
         <v>1</v>
       </c>
@@ -1035,7 +1035,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A6">
         <v>1</v>
       </c>
@@ -1071,7 +1071,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A7">
         <v>1</v>
       </c>
@@ -1107,7 +1107,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A8">
         <v>1</v>
       </c>
@@ -1146,7 +1146,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A9">
         <v>2</v>
       </c>
@@ -1182,7 +1182,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A10">
         <v>1</v>
       </c>
@@ -1219,7 +1219,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A11">
         <v>2</v>
       </c>
@@ -1256,7 +1256,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A12">
         <v>1</v>
       </c>
@@ -1293,7 +1293,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A13">
         <v>2</v>
       </c>
@@ -1331,7 +1331,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A14">
         <v>1</v>
       </c>
@@ -1368,7 +1368,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A15">
         <v>2</v>
       </c>
@@ -1405,7 +1405,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A16">
         <v>1</v>
       </c>
@@ -1442,7 +1442,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A17">
         <v>2</v>
       </c>
@@ -1479,7 +1479,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A18">
         <v>1</v>
       </c>
@@ -1516,7 +1516,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A19">
         <v>2</v>
       </c>
@@ -1553,7 +1553,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A20">
         <v>1</v>
       </c>
@@ -1590,7 +1590,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A21">
         <v>2</v>
       </c>
@@ -1627,7 +1627,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A22">
         <v>1</v>
       </c>
@@ -1664,7 +1664,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A23">
         <v>2</v>
       </c>
@@ -1701,7 +1701,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A24">
         <v>1</v>
       </c>
@@ -1738,7 +1738,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A25">
         <v>2</v>
       </c>
@@ -1775,7 +1775,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A26">
         <v>1</v>
       </c>
@@ -1812,7 +1812,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A27">
         <v>2</v>
       </c>
@@ -1849,7 +1849,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A28">
         <v>1</v>
       </c>
@@ -1889,7 +1889,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A29">
         <v>1</v>
       </c>
@@ -1929,7 +1929,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A30">
         <v>1</v>
       </c>
@@ -1966,7 +1966,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A31">
         <v>2</v>
       </c>
@@ -2002,7 +2002,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A32">
         <v>3</v>
       </c>
@@ -2041,7 +2041,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A33">
         <v>3</v>
       </c>
@@ -2077,7 +2077,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A34">
         <v>3</v>
       </c>
@@ -2114,7 +2114,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A35">
         <v>3</v>
       </c>
@@ -2151,7 +2151,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A36">
         <v>3</v>
       </c>
@@ -2188,7 +2188,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A37">
         <v>3</v>
       </c>
@@ -2225,7 +2225,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A38">
         <v>3</v>
       </c>
@@ -2262,7 +2262,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A39">
         <v>3</v>
       </c>
@@ -2299,7 +2299,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A40">
         <v>3</v>
       </c>
@@ -2336,7 +2336,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A41">
         <v>3</v>
       </c>
@@ -2373,7 +2373,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A42">
         <v>3</v>
       </c>
@@ -2410,7 +2410,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A43">
         <v>3</v>
       </c>
@@ -2447,7 +2447,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A44">
         <v>3</v>
       </c>
@@ -2481,7 +2481,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A45">
         <v>3</v>
       </c>
@@ -2518,7 +2518,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A46">
         <v>3</v>
       </c>
@@ -2555,7 +2555,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A47">
         <v>3</v>
       </c>
@@ -2592,7 +2592,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A48">
         <v>3</v>
       </c>
@@ -2626,7 +2626,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A49">
         <v>3</v>
       </c>
@@ -2660,7 +2660,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A50">
         <v>3</v>
       </c>
@@ -2694,7 +2694,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A51">
         <v>3</v>
       </c>
@@ -2728,7 +2728,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A52">
         <v>3</v>
       </c>
@@ -2762,7 +2762,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A53">
         <v>3</v>
       </c>
@@ -2796,7 +2796,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A54">
         <v>3</v>
       </c>
@@ -2830,7 +2830,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A55" s="2">
         <v>3</v>
       </c>
@@ -2864,7 +2864,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A56" s="2">
         <v>3</v>
       </c>
@@ -2911,17 +2911,17 @@
       <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.84375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="2" max="2" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.33203125" customWidth="1"/>
+    <col min="2" max="2" width="12.3046875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.3046875" customWidth="1"/>
     <col min="5" max="6" width="5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.5" customWidth="1"/>
-    <col min="8" max="8" width="58.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="30.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.4609375" customWidth="1"/>
+    <col min="8" max="8" width="58.4609375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="30.4609375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2965,7 +2965,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>64</v>
       </c>
@@ -2998,7 +2998,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>64</v>
       </c>
@@ -3031,7 +3031,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>64</v>
       </c>
@@ -3064,7 +3064,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>64</v>
       </c>
@@ -3097,7 +3097,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
         <v>64</v>
       </c>
@@ -3130,7 +3130,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
         <v>64</v>
       </c>
@@ -3163,7 +3163,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
         <v>64</v>
       </c>
@@ -3196,7 +3196,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
         <v>64</v>
       </c>
@@ -3229,7 +3229,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A10" s="2" t="s">
         <v>64</v>
       </c>
@@ -3254,7 +3254,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A11" s="2" t="s">
         <v>64</v>
       </c>
@@ -3277,7 +3277,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A12" s="2" t="s">
         <v>64</v>
       </c>
@@ -3300,7 +3300,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A13" s="2" t="s">
         <v>64</v>
       </c>
@@ -3329,7 +3329,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A14" s="2" t="s">
         <v>64</v>
       </c>
@@ -3358,7 +3358,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A15" s="2" t="s">
         <v>64</v>
       </c>
@@ -3397,17 +3397,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7709FE3-57B1-4766-A5D4-6B378E0A5BA3}">
   <dimension ref="A1:O11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K13" sqref="K13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.84375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="7" max="7" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.4609375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.4609375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>83</v>
       </c>
@@ -3454,7 +3454,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A2">
         <v>1</v>
       </c>
@@ -3487,7 +3487,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A3">
         <v>1</v>
       </c>
@@ -3520,7 +3520,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A4">
         <v>1</v>
       </c>
@@ -3553,7 +3553,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A5">
         <v>1</v>
       </c>
@@ -3586,7 +3586,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A6">
         <v>1</v>
       </c>
@@ -3619,7 +3619,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A7">
         <v>1</v>
       </c>
@@ -3652,7 +3652,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A8">
         <v>1</v>
       </c>
@@ -3685,7 +3685,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A9">
         <v>1</v>
       </c>
@@ -3718,15 +3718,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A10">
         <v>4</v>
       </c>
+      <c r="B10">
+        <v>0</v>
+      </c>
       <c r="C10" t="s">
         <v>73</v>
       </c>
       <c r="D10">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="E10" t="s">
         <v>15</v>
@@ -3742,18 +3745,21 @@
       </c>
       <c r="I10" t="str">
         <f t="shared" si="0"/>
-        <v>nl_wk01_20210107_pB_wv01</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
+        <v>nl_wk09_20210107_pB_wv01</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A11">
         <v>4</v>
       </c>
+      <c r="B11">
+        <v>0</v>
+      </c>
       <c r="C11" t="s">
         <v>73</v>
       </c>
       <c r="D11">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="E11" t="s">
         <v>15</v>
@@ -3769,7 +3775,7 @@
       </c>
       <c r="I11" t="str">
         <f t="shared" si="0"/>
-        <v>nl_wk02_20210118_pB_wv02</v>
+        <v>nl_wk10_20210118_pB_wv02</v>
       </c>
     </row>
   </sheetData>
@@ -3785,13 +3791,13 @@
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.84375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.33203125" customWidth="1"/>
+    <col min="1" max="1" width="12.3046875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.3046875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>83</v>
       </c>
@@ -3838,7 +3844,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A2">
         <v>1</v>
       </c>
@@ -3868,7 +3874,7 @@
         <v>no_wk01_20200501_pA_wv01</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A3">
         <v>1</v>
       </c>
@@ -3901,7 +3907,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A4">
         <v>1</v>
       </c>
@@ -3931,7 +3937,7 @@
         <v>no_wk03_20200622_pA_wv03</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A5">
         <v>1</v>
       </c>
@@ -3964,7 +3970,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A6">
         <v>1</v>
       </c>
@@ -3997,7 +4003,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A7">
         <v>1</v>
       </c>
@@ -4043,14 +4049,14 @@
       <selection activeCell="A28" sqref="A28:XFD28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.84375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="7" max="7" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.69140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="59" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="27.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="27.3046875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4091,7 +4097,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>99</v>
       </c>
@@ -4124,7 +4130,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>100</v>
       </c>
@@ -4150,14 +4156,14 @@
         <v>106</v>
       </c>
       <c r="I3" t="str">
-        <f>A3&amp;"_"&amp;"wk"&amp;TEXT(D3,"00")&amp;"_"&amp;YEAR(G3)&amp;TEXT(G3,"MM")&amp;TEXT(G3,"DD")&amp;"_p"&amp;E3&amp;"_wv"&amp;TEXT(F3,"00")&amp;""</f>
+        <f t="shared" ref="I3:I27" si="0">A3&amp;"_"&amp;"wk"&amp;TEXT(D3,"00")&amp;"_"&amp;YEAR(G3)&amp;TEXT(G3,"MM")&amp;TEXT(G3,"DD")&amp;"_p"&amp;E3&amp;"_wv"&amp;TEXT(F3,"00")&amp;""</f>
         <v>dk_wk01_20210111_pA_wv01</v>
       </c>
       <c r="J3">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>101</v>
       </c>
@@ -4183,14 +4189,14 @@
         <v>107</v>
       </c>
       <c r="I4" t="str">
-        <f>A4&amp;"_"&amp;"wk"&amp;TEXT(D4,"00")&amp;"_"&amp;YEAR(G4)&amp;TEXT(G4,"MM")&amp;TEXT(G4,"DD")&amp;"_p"&amp;E4&amp;"_wv"&amp;TEXT(F4,"00")&amp;""</f>
+        <f t="shared" si="0"/>
         <v>es_wk01_20210111_pA_wv01</v>
       </c>
       <c r="J4">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>102</v>
       </c>
@@ -4216,14 +4222,14 @@
         <v>108</v>
       </c>
       <c r="I5" t="str">
-        <f>A5&amp;"_"&amp;"wk"&amp;TEXT(D5,"00")&amp;"_"&amp;YEAR(G5)&amp;TEXT(G5,"MM")&amp;TEXT(G5,"DD")&amp;"_p"&amp;E5&amp;"_wv"&amp;TEXT(F5,"00")&amp;""</f>
+        <f t="shared" si="0"/>
         <v>fr_wk01_20210111_pA_wv01</v>
       </c>
       <c r="J5">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
         <v>103</v>
       </c>
@@ -4249,14 +4255,14 @@
         <v>109</v>
       </c>
       <c r="I6" t="str">
-        <f>A6&amp;"_"&amp;"wk"&amp;TEXT(D6,"00")&amp;"_"&amp;YEAR(G6)&amp;TEXT(G6,"MM")&amp;TEXT(G6,"DD")&amp;"_p"&amp;E6&amp;"_wv"&amp;TEXT(F6,"00")&amp;""</f>
+        <f t="shared" si="0"/>
         <v>it_wk01_20210111_pA_wv01</v>
       </c>
       <c r="J6">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
         <v>104</v>
       </c>
@@ -4282,14 +4288,14 @@
         <v>110</v>
       </c>
       <c r="I7" t="str">
-        <f>A7&amp;"_"&amp;"wk"&amp;TEXT(D7,"00")&amp;"_"&amp;YEAR(G7)&amp;TEXT(G7,"MM")&amp;TEXT(G7,"DD")&amp;"_p"&amp;E7&amp;"_wv"&amp;TEXT(F7,"00")&amp;""</f>
+        <f t="shared" si="0"/>
         <v>pl_wk01_20210111_pA_wv01</v>
       </c>
       <c r="J7">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
         <v>105</v>
       </c>
@@ -4315,14 +4321,14 @@
         <v>111</v>
       </c>
       <c r="I8" t="str">
-        <f>A8&amp;"_"&amp;"wk"&amp;TEXT(D8,"00")&amp;"_"&amp;YEAR(G8)&amp;TEXT(G8,"MM")&amp;TEXT(G8,"DD")&amp;"_p"&amp;E8&amp;"_wv"&amp;TEXT(F8,"00")&amp;""</f>
+        <f t="shared" si="0"/>
         <v>pt_wk01_20210111_pA_wv01</v>
       </c>
       <c r="J8">
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
         <v>99</v>
       </c>
@@ -4348,11 +4354,11 @@
         <v>113</v>
       </c>
       <c r="I9" t="str">
-        <f>A9&amp;"_"&amp;"wk"&amp;TEXT(D9,"00")&amp;"_"&amp;YEAR(G9)&amp;TEXT(G9,"MM")&amp;TEXT(G9,"DD")&amp;"_p"&amp;E9&amp;"_wv"&amp;TEXT(F9,"00")&amp;""</f>
+        <f t="shared" si="0"/>
         <v>at_wk02_20210118_pA_wv02</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
         <v>100</v>
       </c>
@@ -4378,11 +4384,11 @@
         <v>113</v>
       </c>
       <c r="I10" t="str">
-        <f>A10&amp;"_"&amp;"wk"&amp;TEXT(D10,"00")&amp;"_"&amp;YEAR(G10)&amp;TEXT(G10,"MM")&amp;TEXT(G10,"DD")&amp;"_p"&amp;E10&amp;"_wv"&amp;TEXT(F10,"00")&amp;""</f>
+        <f t="shared" si="0"/>
         <v>dk_wk02_20210118_pA_wv02</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
         <v>101</v>
       </c>
@@ -4408,11 +4414,11 @@
         <v>113</v>
       </c>
       <c r="I11" t="str">
-        <f>A11&amp;"_"&amp;"wk"&amp;TEXT(D11,"00")&amp;"_"&amp;YEAR(G11)&amp;TEXT(G11,"MM")&amp;TEXT(G11,"DD")&amp;"_p"&amp;E11&amp;"_wv"&amp;TEXT(F11,"00")&amp;""</f>
+        <f t="shared" si="0"/>
         <v>es_wk02_20210118_pA_wv02</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A12" t="s">
         <v>102</v>
       </c>
@@ -4438,11 +4444,11 @@
         <v>113</v>
       </c>
       <c r="I12" t="str">
-        <f>A12&amp;"_"&amp;"wk"&amp;TEXT(D12,"00")&amp;"_"&amp;YEAR(G12)&amp;TEXT(G12,"MM")&amp;TEXT(G12,"DD")&amp;"_p"&amp;E12&amp;"_wv"&amp;TEXT(F12,"00")&amp;""</f>
+        <f t="shared" si="0"/>
         <v>fr_wk02_20210118_pA_wv02</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A13" t="s">
         <v>103</v>
       </c>
@@ -4468,11 +4474,11 @@
         <v>113</v>
       </c>
       <c r="I13" t="str">
-        <f>A13&amp;"_"&amp;"wk"&amp;TEXT(D13,"00")&amp;"_"&amp;YEAR(G13)&amp;TEXT(G13,"MM")&amp;TEXT(G13,"DD")&amp;"_p"&amp;E13&amp;"_wv"&amp;TEXT(F13,"00")&amp;""</f>
+        <f t="shared" si="0"/>
         <v>it_wk02_20210118_pA_wv02</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A14" t="s">
         <v>104</v>
       </c>
@@ -4498,11 +4504,11 @@
         <v>113</v>
       </c>
       <c r="I14" t="str">
-        <f>A14&amp;"_"&amp;"wk"&amp;TEXT(D14,"00")&amp;"_"&amp;YEAR(G14)&amp;TEXT(G14,"MM")&amp;TEXT(G14,"DD")&amp;"_p"&amp;E14&amp;"_wv"&amp;TEXT(F14,"00")&amp;""</f>
+        <f t="shared" si="0"/>
         <v>pl_wk02_20210118_pA_wv02</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A15" t="s">
         <v>105</v>
       </c>
@@ -4528,11 +4534,11 @@
         <v>113</v>
       </c>
       <c r="I15" t="str">
-        <f>A15&amp;"_"&amp;"wk"&amp;TEXT(D15,"00")&amp;"_"&amp;YEAR(G15)&amp;TEXT(G15,"MM")&amp;TEXT(G15,"DD")&amp;"_p"&amp;E15&amp;"_wv"&amp;TEXT(F15,"00")&amp;""</f>
+        <f t="shared" si="0"/>
         <v>pt_wk02_20210118_pA_wv02</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A16" s="2" t="s">
         <v>99</v>
       </c>
@@ -4558,11 +4564,11 @@
         <v>122</v>
       </c>
       <c r="I16" s="2" t="str">
-        <f>A16&amp;"_"&amp;"wk"&amp;TEXT(D16,"00")&amp;"_"&amp;YEAR(G16)&amp;TEXT(G16,"MM")&amp;TEXT(G16,"DD")&amp;"_p"&amp;E16&amp;"_wv"&amp;TEXT(F16,"00")&amp;""</f>
+        <f t="shared" si="0"/>
         <v>at_wk03_20210129_pA_wv03</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A17" s="2" t="s">
         <v>100</v>
       </c>
@@ -4588,11 +4594,11 @@
         <v>122</v>
       </c>
       <c r="I17" s="2" t="str">
-        <f>A17&amp;"_"&amp;"wk"&amp;TEXT(D17,"00")&amp;"_"&amp;YEAR(G17)&amp;TEXT(G17,"MM")&amp;TEXT(G17,"DD")&amp;"_p"&amp;E17&amp;"_wv"&amp;TEXT(F17,"00")&amp;""</f>
+        <f t="shared" si="0"/>
         <v>dk_wk03_20210129_pA_wv03</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A18" s="2" t="s">
         <v>101</v>
       </c>
@@ -4618,11 +4624,11 @@
         <v>122</v>
       </c>
       <c r="I18" s="2" t="str">
-        <f>A18&amp;"_"&amp;"wk"&amp;TEXT(D18,"00")&amp;"_"&amp;YEAR(G18)&amp;TEXT(G18,"MM")&amp;TEXT(G18,"DD")&amp;"_p"&amp;E18&amp;"_wv"&amp;TEXT(F18,"00")&amp;""</f>
+        <f t="shared" si="0"/>
         <v>es_wk03_20210129_pA_wv03</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A19" s="2" t="s">
         <v>102</v>
       </c>
@@ -4648,11 +4654,11 @@
         <v>122</v>
       </c>
       <c r="I19" s="2" t="str">
-        <f>A19&amp;"_"&amp;"wk"&amp;TEXT(D19,"00")&amp;"_"&amp;YEAR(G19)&amp;TEXT(G19,"MM")&amp;TEXT(G19,"DD")&amp;"_p"&amp;E19&amp;"_wv"&amp;TEXT(F19,"00")&amp;""</f>
+        <f t="shared" si="0"/>
         <v>fr_wk03_20210129_pA_wv03</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A20" s="2" t="s">
         <v>103</v>
       </c>
@@ -4678,11 +4684,11 @@
         <v>122</v>
       </c>
       <c r="I20" s="2" t="str">
-        <f>A20&amp;"_"&amp;"wk"&amp;TEXT(D20,"00")&amp;"_"&amp;YEAR(G20)&amp;TEXT(G20,"MM")&amp;TEXT(G20,"DD")&amp;"_p"&amp;E20&amp;"_wv"&amp;TEXT(F20,"00")&amp;""</f>
+        <f t="shared" si="0"/>
         <v>it_wk03_20210129_pA_wv03</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A21" s="2" t="s">
         <v>104</v>
       </c>
@@ -4708,11 +4714,11 @@
         <v>122</v>
       </c>
       <c r="I21" s="2" t="str">
-        <f>A21&amp;"_"&amp;"wk"&amp;TEXT(D21,"00")&amp;"_"&amp;YEAR(G21)&amp;TEXT(G21,"MM")&amp;TEXT(G21,"DD")&amp;"_p"&amp;E21&amp;"_wv"&amp;TEXT(F21,"00")&amp;""</f>
+        <f t="shared" si="0"/>
         <v>pl_wk03_20210129_pA_wv03</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A22" s="2" t="s">
         <v>105</v>
       </c>
@@ -4738,11 +4744,11 @@
         <v>122</v>
       </c>
       <c r="I22" s="2" t="str">
-        <f>A22&amp;"_"&amp;"wk"&amp;TEXT(D22,"00")&amp;"_"&amp;YEAR(G22)&amp;TEXT(G22,"MM")&amp;TEXT(G22,"DD")&amp;"_p"&amp;E22&amp;"_wv"&amp;TEXT(F22,"00")&amp;""</f>
+        <f t="shared" si="0"/>
         <v>pt_wk03_20210129_pA_wv03</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A23" s="4" t="s">
         <v>99</v>
       </c>
@@ -4768,11 +4774,11 @@
         <v>131</v>
       </c>
       <c r="I23" s="4" t="str">
-        <f>A23&amp;"_"&amp;"wk"&amp;TEXT(D23,"00")&amp;"_"&amp;YEAR(G23)&amp;TEXT(G23,"MM")&amp;TEXT(G23,"DD")&amp;"_p"&amp;E23&amp;"_wv"&amp;TEXT(F23,"00")&amp;""</f>
+        <f t="shared" si="0"/>
         <v>at_wk01_20210111_pC_wv01</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A24" s="4" t="s">
         <v>100</v>
       </c>
@@ -4798,11 +4804,11 @@
         <v>131</v>
       </c>
       <c r="I24" s="4" t="str">
-        <f>A24&amp;"_"&amp;"wk"&amp;TEXT(D24,"00")&amp;"_"&amp;YEAR(G24)&amp;TEXT(G24,"MM")&amp;TEXT(G24,"DD")&amp;"_p"&amp;E24&amp;"_wv"&amp;TEXT(F24,"00")&amp;""</f>
+        <f t="shared" si="0"/>
         <v>dk_wk01_20210111_pC_wv01</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A25" s="4" t="s">
         <v>102</v>
       </c>
@@ -4828,11 +4834,11 @@
         <v>131</v>
       </c>
       <c r="I25" s="4" t="str">
-        <f>A25&amp;"_"&amp;"wk"&amp;TEXT(D25,"00")&amp;"_"&amp;YEAR(G25)&amp;TEXT(G25,"MM")&amp;TEXT(G25,"DD")&amp;"_p"&amp;E25&amp;"_wv"&amp;TEXT(F25,"00")&amp;""</f>
+        <f t="shared" si="0"/>
         <v>fr_wk01_20210111_pC_wv01</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A26" s="4" t="s">
         <v>103</v>
       </c>
@@ -4858,11 +4864,11 @@
         <v>131</v>
       </c>
       <c r="I26" s="4" t="str">
-        <f>A26&amp;"_"&amp;"wk"&amp;TEXT(D26,"00")&amp;"_"&amp;YEAR(G26)&amp;TEXT(G26,"MM")&amp;TEXT(G26,"DD")&amp;"_p"&amp;E26&amp;"_wv"&amp;TEXT(F26,"00")&amp;""</f>
+        <f t="shared" si="0"/>
         <v>it_wk01_20210111_pC_wv01</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A27" s="4" t="s">
         <v>104</v>
       </c>
@@ -4888,7 +4894,7 @@
         <v>131</v>
       </c>
       <c r="I27" s="4" t="str">
-        <f>A27&amp;"_"&amp;"wk"&amp;TEXT(D27,"00")&amp;"_"&amp;YEAR(G27)&amp;TEXT(G27,"MM")&amp;TEXT(G27,"DD")&amp;"_p"&amp;E27&amp;"_wv"&amp;TEXT(F27,"00")&amp;""</f>
+        <f t="shared" si="0"/>
         <v>pl_wk01_20210111_pC_wv01</v>
       </c>
     </row>
@@ -4901,25 +4907,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B44EFFA-AC3D-0445-9643-71A374D3D58F}">
   <dimension ref="A1:J8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.07421875" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="10.5" customWidth="1"/>
-    <col min="2" max="2" width="16.6640625" customWidth="1"/>
-    <col min="3" max="3" width="8.6640625" customWidth="1"/>
-    <col min="4" max="4" width="7.33203125" customWidth="1"/>
-    <col min="5" max="5" width="8.5" customWidth="1"/>
-    <col min="6" max="6" width="9.33203125" customWidth="1"/>
-    <col min="7" max="7" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="52.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="24.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="6.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.4609375" customWidth="1"/>
+    <col min="2" max="2" width="16.69140625" customWidth="1"/>
+    <col min="3" max="3" width="8.69140625" customWidth="1"/>
+    <col min="4" max="4" width="7.3046875" customWidth="1"/>
+    <col min="5" max="5" width="8.4609375" customWidth="1"/>
+    <col min="6" max="6" width="9.3046875" customWidth="1"/>
+    <col min="7" max="7" width="11.69140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="52.69140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="24.69140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="6.84375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -4951,7 +4957,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A2" s="2" t="s">
         <v>124</v>
       </c>
@@ -4982,7 +4988,7 @@
       </c>
       <c r="J2" s="2"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>125</v>
       </c>
@@ -5013,7 +5019,7 @@
       </c>
       <c r="J3" s="2"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>126</v>
       </c>
@@ -5044,7 +5050,7 @@
       </c>
       <c r="J4" s="2"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A5" s="2" t="s">
         <v>125</v>
       </c>
@@ -5074,7 +5080,7 @@
         <v>fi_wk01_20210112_pC_wv01</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A6" s="2" t="s">
         <v>126</v>
       </c>
@@ -5104,7 +5110,7 @@
         <v>ch_wk01_20210113_pC_wv01</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A7" s="2" t="s">
         <v>133</v>
       </c>
@@ -5134,7 +5140,7 @@
         <v>gr_wk01_20210113_pC_wv01</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A8" s="2" t="s">
         <v>124</v>
       </c>
@@ -5175,9 +5181,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.84375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>119</v>
       </c>
@@ -5195,24 +5201,24 @@
       <selection activeCell="A8" sqref="A8:I10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.07421875" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="7.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.15234375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.3046875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.15234375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.3046875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="58.33203125" customWidth="1"/>
+    <col min="7" max="7" width="11.69140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="58.3046875" customWidth="1"/>
     <col min="9" max="9" width="25" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="6.83203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="6.84375" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="7" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="8.83203125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.84375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.69140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -5253,7 +5259,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A2" s="4" t="s">
         <v>99</v>
       </c>
@@ -5287,7 +5293,7 @@
       <c r="L2" s="4"/>
       <c r="M2" s="4"/>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A3" s="4" t="s">
         <v>100</v>
       </c>
@@ -5321,7 +5327,7 @@
       <c r="L3" s="4"/>
       <c r="M3" s="4"/>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A4" s="4" t="s">
         <v>102</v>
       </c>
@@ -5355,7 +5361,7 @@
       <c r="L4" s="4"/>
       <c r="M4" s="4"/>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A5" s="4" t="s">
         <v>103</v>
       </c>
@@ -5389,7 +5395,7 @@
       <c r="L5" s="4"/>
       <c r="M5" s="4"/>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A6" s="4" t="s">
         <v>104</v>
       </c>
@@ -5423,7 +5429,7 @@
       <c r="L6" s="4"/>
       <c r="M6" s="4"/>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A7" s="2" t="s">
         <v>124</v>
       </c>
@@ -5454,7 +5460,7 @@
       </c>
       <c r="J7" s="2"/>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A8" s="2" t="s">
         <v>125</v>
       </c>
@@ -5485,7 +5491,7 @@
       </c>
       <c r="J8" s="2"/>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A9" s="2" t="s">
         <v>126</v>
       </c>
@@ -5516,7 +5522,7 @@
       </c>
       <c r="J9" s="2"/>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A10" s="2" t="s">
         <v>133</v>
       </c>

</xml_diff>

<commit_message>
Change from Group1 to G1
</commit_message>
<xml_diff>
--- a/data/spss_files.xlsx
+++ b/data/spss_files.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jarvisc1\Documents\projects\comix_data_clean\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5848D049-F5B0-4893-95B6-5D7630BC43A8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A81FC42-23D8-41EC-890C-B67EE2513759}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18120" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18120" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="5" r:id="rId1"/>
@@ -18,8 +18,8 @@
     <sheet name="BE" sheetId="2" r:id="rId3"/>
     <sheet name="NL" sheetId="3" r:id="rId4"/>
     <sheet name="NO" sheetId="4" r:id="rId5"/>
-    <sheet name="Group1" sheetId="6" r:id="rId6"/>
-    <sheet name="Group2" sheetId="8" r:id="rId7"/>
+    <sheet name="G1" sheetId="6" r:id="rId6"/>
+    <sheet name="G2" sheetId="8" r:id="rId7"/>
     <sheet name="Sheet1" sheetId="7" r:id="rId8"/>
     <sheet name="EUchild" sheetId="9" r:id="rId9"/>
   </sheets>
@@ -3397,7 +3397,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7709FE3-57B1-4766-A5D4-6B378E0A5BA3}">
   <dimension ref="A1:O11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
@@ -4907,7 +4907,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B44EFFA-AC3D-0445-9643-71A374D3D58F}">
   <dimension ref="A1:J8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Add inside outside contacts to version 5 and put in new UK data
</commit_message>
<xml_diff>
--- a/data/spss_files.xlsx
+++ b/data/spss_files.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jarvisc1\Documents\projects\comix_data_clean\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A81FC42-23D8-41EC-890C-B67EE2513759}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6941E592-557B-4871-80FE-1FBF5B03432D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18120" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18120" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="5" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="488" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="482" uniqueCount="130">
   <si>
     <t>country</t>
   </si>
@@ -386,21 +386,9 @@
     <t>20-030971_G1_Merged_Wave2_Final_v1_18012021_IntClientUse</t>
   </si>
   <si>
-    <t>be_wk09_20201120_pB_wv01</t>
-  </si>
-  <si>
-    <t>be_wk10_19000100_pB_wv02</t>
-  </si>
-  <si>
-    <t>be_wk11_19000100_pB_wv03</t>
-  </si>
-  <si>
     <t>20_060765_BE2_Wave4_Final_v1_110121_IntClientUse</t>
   </si>
   <si>
-    <t>be_wk12_20200111_pB_wv04</t>
-  </si>
-  <si>
     <t>Temp for Belguim</t>
   </si>
   <si>
@@ -428,13 +416,7 @@
     <t>20_060765_BE2_Wave5_Final_v1_200121_IntClientUse</t>
   </si>
   <si>
-    <t>be_wk12_20200111_pB_wv05</t>
-  </si>
-  <si>
     <t>20_060765_BE2_Wave6_Final_v1_270121_IntClientUse</t>
-  </si>
-  <si>
-    <t>be_wk12_20200111_pB_wv06</t>
   </si>
   <si>
     <t>20-030971_G1_Merged_Wave1_Parents_Final_v1_12022021_IntClientUse</t>
@@ -831,8 +813,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O56"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="H34" sqref="H34"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D8" sqref="D8:D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.84375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -2854,7 +2836,7 @@
         <v>44216</v>
       </c>
       <c r="H55" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="I55" t="str">
         <f t="shared" si="0"/>
@@ -2888,7 +2870,7 @@
         <v>44224</v>
       </c>
       <c r="H56" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="I56" s="2" t="str">
         <f t="shared" si="0"/>
@@ -2907,8 +2889,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C042354-CAAB-48AD-AFC2-2197A2D12C9D}">
   <dimension ref="A1:N15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I9" sqref="I9:I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.84375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -2991,7 +2973,7 @@
         <v>65</v>
       </c>
       <c r="I2" t="str">
-        <f t="shared" ref="I2:I9" si="0">A2&amp;"_"&amp;"wk"&amp;TEXT(D2,"00")&amp;"_"&amp;YEAR(G2)&amp;TEXT(G2,"MM")&amp;TEXT(G2,"DD")&amp;"_p"&amp;E2&amp;"_wv"&amp;TEXT(F2,"00")&amp;""</f>
+        <f t="shared" ref="I2:I15" si="0">A2&amp;"_"&amp;"wk"&amp;TEXT(D2,"00")&amp;"_"&amp;YEAR(G2)&amp;TEXT(G2,"MM")&amp;TEXT(G2,"DD")&amp;"_p"&amp;E2&amp;"_wv"&amp;TEXT(F2,"00")&amp;""</f>
         <v>be_wk01_20200429_pA_wv01</v>
       </c>
       <c r="J2">
@@ -3250,8 +3232,9 @@
         <v>44155</v>
       </c>
       <c r="H10" s="2"/>
-      <c r="I10" s="2" t="s">
-        <v>114</v>
+      <c r="I10" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>be_wk09_20201120_pB_wv01</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.4">
@@ -3273,8 +3256,9 @@
       </c>
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
-      <c r="I11" s="2" t="s">
-        <v>115</v>
+      <c r="I11" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>be_wk10_19000100_pB_wv02</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.4">
@@ -3296,8 +3280,9 @@
       </c>
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
-      <c r="I12" s="2" t="s">
-        <v>116</v>
+      <c r="I12" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>be_wk11_19000100_pB_wv03</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.4">
@@ -3323,10 +3308,11 @@
         <v>44207</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="I13" s="2" t="s">
-        <v>118</v>
+        <v>114</v>
+      </c>
+      <c r="I13" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>be_wk12_20210111_pB_wv04</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.4">
@@ -3352,10 +3338,11 @@
         <v>44216</v>
       </c>
       <c r="H14" t="s">
-        <v>127</v>
-      </c>
-      <c r="I14" s="2" t="s">
-        <v>128</v>
+        <v>123</v>
+      </c>
+      <c r="I14" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>be_wk13_20210120_pB_wv05</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.4">
@@ -3369,7 +3356,7 @@
         <v>0</v>
       </c>
       <c r="D15" s="2">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E15" s="2" t="s">
         <v>15</v>
@@ -3381,10 +3368,11 @@
         <v>44223</v>
       </c>
       <c r="H15" t="s">
-        <v>129</v>
-      </c>
-      <c r="I15" s="2" t="s">
-        <v>130</v>
+        <v>124</v>
+      </c>
+      <c r="I15" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>be_wk14_20210127_pB_wv06</v>
       </c>
     </row>
   </sheetData>
@@ -3741,7 +3729,7 @@
         <v>44203</v>
       </c>
       <c r="H10" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="I10" t="str">
         <f t="shared" si="0"/>
@@ -3771,7 +3759,7 @@
         <v>44214</v>
       </c>
       <c r="H11" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="I11" t="str">
         <f t="shared" si="0"/>
@@ -4561,7 +4549,7 @@
         <v>44225</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="I16" s="2" t="str">
         <f t="shared" si="0"/>
@@ -4591,7 +4579,7 @@
         <v>44225</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="I17" s="2" t="str">
         <f t="shared" si="0"/>
@@ -4621,7 +4609,7 @@
         <v>44225</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="I18" s="2" t="str">
         <f t="shared" si="0"/>
@@ -4651,7 +4639,7 @@
         <v>44225</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="I19" s="2" t="str">
         <f t="shared" si="0"/>
@@ -4681,7 +4669,7 @@
         <v>44225</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="I20" s="2" t="str">
         <f t="shared" si="0"/>
@@ -4711,7 +4699,7 @@
         <v>44225</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="I21" s="2" t="str">
         <f t="shared" si="0"/>
@@ -4741,7 +4729,7 @@
         <v>44225</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="I22" s="2" t="str">
         <f t="shared" si="0"/>
@@ -4771,7 +4759,7 @@
         <v>44207</v>
       </c>
       <c r="H23" s="4" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="I23" s="4" t="str">
         <f t="shared" si="0"/>
@@ -4801,7 +4789,7 @@
         <v>44207</v>
       </c>
       <c r="H24" s="4" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="I24" s="4" t="str">
         <f t="shared" si="0"/>
@@ -4831,7 +4819,7 @@
         <v>44207</v>
       </c>
       <c r="H25" s="4" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="I25" s="4" t="str">
         <f t="shared" si="0"/>
@@ -4861,7 +4849,7 @@
         <v>44207</v>
       </c>
       <c r="H26" s="4" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="I26" s="4" t="str">
         <f t="shared" si="0"/>
@@ -4891,7 +4879,7 @@
         <v>44207</v>
       </c>
       <c r="H27" s="4" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="I27" s="4" t="str">
         <f t="shared" si="0"/>
@@ -4907,7 +4895,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B44EFFA-AC3D-0445-9643-71A374D3D58F}">
   <dimension ref="A1:J8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
@@ -4959,7 +4947,7 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A2" s="2" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="B2" s="2">
         <v>5</v>
@@ -4980,7 +4968,7 @@
         <v>44207</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="I2" s="2" t="str">
         <f>A2&amp;"_"&amp;"wk"&amp;TEXT(D2,"00")&amp;"_"&amp;YEAR(G3)&amp;TEXT(G3,"MM")&amp;TEXT(G3,"DD")&amp;"_p"&amp;E2&amp;"_wv"&amp;TEXT(F2,"00")&amp;""</f>
@@ -4990,7 +4978,7 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="B3" s="2">
         <v>5</v>
@@ -5011,7 +4999,7 @@
         <v>44208</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="I3" s="2" t="str">
         <f t="shared" ref="I3:I4" si="0">A3&amp;"_"&amp;"wk"&amp;TEXT(D3,"00")&amp;"_"&amp;YEAR(G4)&amp;TEXT(G4,"MM")&amp;TEXT(G4,"DD")&amp;"_p"&amp;E3&amp;"_wv"&amp;TEXT(F3,"00")&amp;""</f>
@@ -5021,7 +5009,7 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="B4" s="2">
         <v>5</v>
@@ -5042,7 +5030,7 @@
         <v>44209</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="I4" s="2" t="str">
         <f t="shared" si="0"/>
@@ -5052,7 +5040,7 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A5" s="2" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="B5" s="4">
         <v>5</v>
@@ -5073,7 +5061,7 @@
         <v>44208</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="I5" s="4" t="str">
         <f t="shared" ref="I5:I7" si="1">A5&amp;"_"&amp;"wk"&amp;TEXT(D5,"00")&amp;"_"&amp;YEAR(G5)&amp;TEXT(G5,"MM")&amp;TEXT(G5,"DD")&amp;"_p"&amp;E5&amp;"_wv"&amp;TEXT(F5,"00")&amp;""</f>
@@ -5082,7 +5070,7 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A6" s="2" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="B6" s="4">
         <v>5</v>
@@ -5103,7 +5091,7 @@
         <v>44209</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="I6" s="4" t="str">
         <f t="shared" si="1"/>
@@ -5112,7 +5100,7 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A7" s="2" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="B7" s="4">
         <v>5</v>
@@ -5133,7 +5121,7 @@
         <v>44209</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="I7" s="4" t="str">
         <f t="shared" si="1"/>
@@ -5142,7 +5130,7 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A8" s="2" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="B8" s="4">
         <v>5</v>
@@ -5163,7 +5151,7 @@
         <v>44207</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="I8" s="4" t="str">
         <f>A8&amp;"_"&amp;"wk"&amp;TEXT(D8,"00")&amp;"_"&amp;YEAR(G8)&amp;TEXT(G8,"MM")&amp;TEXT(G8,"DD")&amp;"_p"&amp;E8&amp;"_wv"&amp;TEXT(F8,"00")&amp;""</f>
@@ -5185,7 +5173,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
     </row>
   </sheetData>
@@ -5282,7 +5270,7 @@
         <v>44207</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="I2" s="4" t="str">
         <f>A2&amp;"_"&amp;"wk"&amp;TEXT(D2,"00")&amp;"_"&amp;YEAR(G2)&amp;TEXT(G2,"MM")&amp;TEXT(G2,"DD")&amp;"_p"&amp;E2&amp;"_wv"&amp;TEXT(F2,"00")&amp;""</f>
@@ -5316,7 +5304,7 @@
         <v>44207</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="I3" s="4" t="str">
         <f t="shared" ref="I3:I10" si="0">A3&amp;"_"&amp;"wk"&amp;TEXT(D3,"00")&amp;"_"&amp;YEAR(G3)&amp;TEXT(G3,"MM")&amp;TEXT(G3,"DD")&amp;"_p"&amp;E3&amp;"_wv"&amp;TEXT(F3,"00")&amp;""</f>
@@ -5350,7 +5338,7 @@
         <v>44207</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="I4" s="4" t="str">
         <f t="shared" si="0"/>
@@ -5384,7 +5372,7 @@
         <v>44207</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="I5" s="4" t="str">
         <f t="shared" si="0"/>
@@ -5418,7 +5406,7 @@
         <v>44207</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="I6" s="4" t="str">
         <f t="shared" si="0"/>
@@ -5431,7 +5419,7 @@
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A7" s="2" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="B7" s="4">
         <v>7</v>
@@ -5452,7 +5440,7 @@
         <v>44207</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="I7" s="4" t="str">
         <f t="shared" si="0"/>
@@ -5462,7 +5450,7 @@
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A8" s="2" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="B8" s="4">
         <v>7</v>
@@ -5483,7 +5471,7 @@
         <v>44208</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="I8" s="4" t="str">
         <f t="shared" si="0"/>
@@ -5493,7 +5481,7 @@
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A9" s="2" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="B9" s="4">
         <v>7</v>
@@ -5514,7 +5502,7 @@
         <v>44209</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="I9" s="4" t="str">
         <f t="shared" si="0"/>
@@ -5524,7 +5512,7 @@
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A10" s="2" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="B10" s="4">
         <v>7</v>
@@ -5545,7 +5533,7 @@
         <v>44209</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="I10" s="4" t="str">
         <f t="shared" si="0"/>

</xml_diff>

<commit_message>
update sh files for v4-v6 and spss_files.xlsx
</commit_message>
<xml_diff>
--- a/data/spss_files.xlsx
+++ b/data/spss_files.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10111"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jarvisc1\Documents\projects\comix_data_clean\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/amygimma/lshtm/comix_data_clean/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6941E592-557B-4871-80FE-1FBF5B03432D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2B29728-5FDB-5444-BC6E-B93DDCC518B7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18120" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="5" r:id="rId1"/>
@@ -21,7 +21,6 @@
     <sheet name="G1" sheetId="6" r:id="rId6"/>
     <sheet name="G2" sheetId="8" r:id="rId7"/>
     <sheet name="Sheet1" sheetId="7" r:id="rId8"/>
-    <sheet name="EUchild" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -42,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="482" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="454" uniqueCount="136">
   <si>
     <t>country</t>
   </si>
@@ -432,6 +431,24 @@
   </si>
   <si>
     <t>20-090916_NL_Wave1_Final_v1_070121_IntClientUse</t>
+  </si>
+  <si>
+    <t>20_060765_BE2_Wave7_Final_v1_220221_IntClientUse</t>
+  </si>
+  <si>
+    <t>20-090916_NL_Wave3_Final_v1_020221_IntClientUse</t>
+  </si>
+  <si>
+    <t>20-090916_NL_Wave4_Final_v1_12022021_IntClientUse</t>
+  </si>
+  <si>
+    <t>EU</t>
+  </si>
+  <si>
+    <t>panel B for BE</t>
+  </si>
+  <si>
+    <t>panel B for NL</t>
   </si>
 </sst>
 </file>
@@ -767,20 +784,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2637BBD4-AFF7-4386-815F-A64B43C0CC5D}">
-  <dimension ref="A4:B7"/>
+  <dimension ref="A4:B10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.84375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>1</v>
       </c>
@@ -788,7 +805,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>2</v>
       </c>
@@ -796,12 +813,36 @@
         <v>95</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>3</v>
       </c>
       <c r="B7" t="s">
         <v>96</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>4</v>
+      </c>
+      <c r="B8" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>5</v>
+      </c>
+      <c r="B9" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>6</v>
+      </c>
+      <c r="B10" t="s">
+        <v>135</v>
       </c>
     </row>
   </sheetData>
@@ -817,16 +858,16 @@
       <selection activeCell="D8" sqref="D8:D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.84375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.3046875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.3046875" customWidth="1"/>
-    <col min="7" max="7" width="10.69140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="58.3046875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="25.3046875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.33203125" customWidth="1"/>
+    <col min="7" max="7" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="58.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="25.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>83</v>
       </c>
@@ -873,7 +914,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -909,7 +950,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
@@ -945,7 +986,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>1</v>
       </c>
@@ -981,7 +1022,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>1</v>
       </c>
@@ -1017,7 +1058,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>1</v>
       </c>
@@ -1053,7 +1094,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>1</v>
       </c>
@@ -1089,7 +1130,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>1</v>
       </c>
@@ -1128,7 +1169,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>2</v>
       </c>
@@ -1164,7 +1205,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>1</v>
       </c>
@@ -1201,7 +1242,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>2</v>
       </c>
@@ -1238,7 +1279,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>1</v>
       </c>
@@ -1275,7 +1316,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>2</v>
       </c>
@@ -1313,7 +1354,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>1</v>
       </c>
@@ -1350,7 +1391,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>2</v>
       </c>
@@ -1387,7 +1428,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>1</v>
       </c>
@@ -1424,7 +1465,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>2</v>
       </c>
@@ -1461,7 +1502,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>1</v>
       </c>
@@ -1498,7 +1539,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>2</v>
       </c>
@@ -1535,7 +1576,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>1</v>
       </c>
@@ -1572,7 +1613,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>2</v>
       </c>
@@ -1609,7 +1650,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>1</v>
       </c>
@@ -1646,7 +1687,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>2</v>
       </c>
@@ -1683,7 +1724,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>1</v>
       </c>
@@ -1720,7 +1761,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>2</v>
       </c>
@@ -1757,7 +1798,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>1</v>
       </c>
@@ -1794,7 +1835,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>2</v>
       </c>
@@ -1831,7 +1872,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>1</v>
       </c>
@@ -1871,7 +1912,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>1</v>
       </c>
@@ -1911,7 +1952,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>1</v>
       </c>
@@ -1948,7 +1989,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>2</v>
       </c>
@@ -1984,7 +2025,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>3</v>
       </c>
@@ -2023,7 +2064,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>3</v>
       </c>
@@ -2059,7 +2100,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>3</v>
       </c>
@@ -2096,7 +2137,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>3</v>
       </c>
@@ -2133,7 +2174,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>3</v>
       </c>
@@ -2170,7 +2211,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>3</v>
       </c>
@@ -2207,7 +2248,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>3</v>
       </c>
@@ -2244,7 +2285,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>3</v>
       </c>
@@ -2281,7 +2322,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>3</v>
       </c>
@@ -2318,7 +2359,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>3</v>
       </c>
@@ -2355,7 +2396,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>3</v>
       </c>
@@ -2392,7 +2433,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>3</v>
       </c>
@@ -2429,7 +2470,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>3</v>
       </c>
@@ -2463,7 +2504,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>3</v>
       </c>
@@ -2500,7 +2541,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>3</v>
       </c>
@@ -2537,7 +2578,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>3</v>
       </c>
@@ -2574,7 +2615,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>3</v>
       </c>
@@ -2608,7 +2649,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>3</v>
       </c>
@@ -2642,7 +2683,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>3</v>
       </c>
@@ -2676,7 +2717,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>3</v>
       </c>
@@ -2710,7 +2751,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>3</v>
       </c>
@@ -2744,7 +2785,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>3</v>
       </c>
@@ -2778,7 +2819,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>3</v>
       </c>
@@ -2812,7 +2853,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A55" s="2">
         <v>3</v>
       </c>
@@ -2846,7 +2887,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A56" s="2">
         <v>3</v>
       </c>
@@ -2887,23 +2928,23 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C042354-CAAB-48AD-AFC2-2197A2D12C9D}">
-  <dimension ref="A1:N15"/>
+  <dimension ref="A1:N16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9:I15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.84375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="12.3046875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.3046875" customWidth="1"/>
+    <col min="2" max="2" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.33203125" customWidth="1"/>
     <col min="5" max="6" width="5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.4609375" customWidth="1"/>
-    <col min="8" max="8" width="58.4609375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="30.4609375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.5" customWidth="1"/>
+    <col min="8" max="8" width="58.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="30.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2947,7 +2988,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>64</v>
       </c>
@@ -2973,14 +3014,14 @@
         <v>65</v>
       </c>
       <c r="I2" t="str">
-        <f t="shared" ref="I2:I15" si="0">A2&amp;"_"&amp;"wk"&amp;TEXT(D2,"00")&amp;"_"&amp;YEAR(G2)&amp;TEXT(G2,"MM")&amp;TEXT(G2,"DD")&amp;"_p"&amp;E2&amp;"_wv"&amp;TEXT(F2,"00")&amp;""</f>
+        <f t="shared" ref="I2:I16" si="0">A2&amp;"_"&amp;"wk"&amp;TEXT(D2,"00")&amp;"_"&amp;YEAR(G2)&amp;TEXT(G2,"MM")&amp;TEXT(G2,"DD")&amp;"_p"&amp;E2&amp;"_wv"&amp;TEXT(F2,"00")&amp;""</f>
         <v>be_wk01_20200429_pA_wv01</v>
       </c>
       <c r="J2">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>64</v>
       </c>
@@ -3013,7 +3054,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>64</v>
       </c>
@@ -3046,7 +3087,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>64</v>
       </c>
@@ -3079,7 +3120,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>64</v>
       </c>
@@ -3112,7 +3153,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>64</v>
       </c>
@@ -3145,7 +3186,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>64</v>
       </c>
@@ -3178,7 +3219,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>64</v>
       </c>
@@ -3211,7 +3252,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>64</v>
       </c>
@@ -3237,7 +3278,7 @@
         <v>be_wk09_20201120_pB_wv01</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>64</v>
       </c>
@@ -3261,7 +3302,7 @@
         <v>be_wk10_19000100_pB_wv02</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>64</v>
       </c>
@@ -3285,12 +3326,12 @@
         <v>be_wk11_19000100_pB_wv03</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>64</v>
       </c>
       <c r="B13" s="2">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C13" s="2">
         <v>0</v>
@@ -3315,12 +3356,12 @@
         <v>be_wk12_20210111_pB_wv04</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>64</v>
       </c>
       <c r="B14" s="2">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C14" s="2">
         <v>0</v>
@@ -3345,12 +3386,12 @@
         <v>be_wk13_20210120_pB_wv05</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>64</v>
       </c>
       <c r="B15" s="2">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C15" s="2">
         <v>0</v>
@@ -3373,6 +3414,36 @@
       <c r="I15" s="2" t="str">
         <f t="shared" si="0"/>
         <v>be_wk14_20210127_pB_wv06</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>64</v>
+      </c>
+      <c r="B16">
+        <v>5</v>
+      </c>
+      <c r="C16">
+        <v>0</v>
+      </c>
+      <c r="D16">
+        <v>15</v>
+      </c>
+      <c r="E16" t="s">
+        <v>15</v>
+      </c>
+      <c r="F16">
+        <v>7</v>
+      </c>
+      <c r="G16" s="3">
+        <v>44249</v>
+      </c>
+      <c r="H16" t="s">
+        <v>130</v>
+      </c>
+      <c r="I16" t="str">
+        <f t="shared" si="0"/>
+        <v>be_wk15_20210222_pB_wv07</v>
       </c>
     </row>
   </sheetData>
@@ -3383,19 +3454,19 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7709FE3-57B1-4766-A5D4-6B378E0A5BA3}">
-  <dimension ref="A1:O11"/>
+  <dimension ref="A1:O13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.84375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="7" max="7" width="10.4609375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9.4609375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>83</v>
       </c>
@@ -3442,7 +3513,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -3475,7 +3546,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
@@ -3508,7 +3579,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>1</v>
       </c>
@@ -3541,7 +3612,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>1</v>
       </c>
@@ -3574,7 +3645,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>1</v>
       </c>
@@ -3607,7 +3678,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>1</v>
       </c>
@@ -3640,7 +3711,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>1</v>
       </c>
@@ -3673,7 +3744,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>1</v>
       </c>
@@ -3706,9 +3777,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A10">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B10">
         <v>0</v>
@@ -3736,9 +3807,9 @@
         <v>nl_wk09_20210107_pB_wv01</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A11">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B11">
         <v>0</v>
@@ -3764,6 +3835,68 @@
       <c r="I11" t="str">
         <f t="shared" si="0"/>
         <v>nl_wk10_20210118_pB_wv02</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A12" s="2">
+        <v>6</v>
+      </c>
+      <c r="B12" s="2">
+        <v>0</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="D12">
+        <v>11</v>
+      </c>
+      <c r="E12" t="s">
+        <v>15</v>
+      </c>
+      <c r="F12">
+        <v>3</v>
+      </c>
+      <c r="G12" s="3">
+        <v>44229</v>
+      </c>
+      <c r="H12" t="s">
+        <v>131</v>
+      </c>
+      <c r="I12" s="2" t="str">
+        <f t="shared" ref="I12:I13" si="1">C12&amp;"_"&amp;"wk"&amp;TEXT(D12,"00")&amp;"_"&amp;YEAR(G12)&amp;TEXT(G12,"MM")&amp;TEXT(G12,"DD")&amp;"_p"&amp;E12&amp;"_wv"&amp;TEXT(F12,"00")&amp;""</f>
+        <v>nl_wk11_20210202_pB_wv03</v>
+      </c>
+      <c r="J12" s="2"/>
+      <c r="K12" s="2"/>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A13" s="2">
+        <v>6</v>
+      </c>
+      <c r="B13" s="2">
+        <v>0</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="D13">
+        <v>12</v>
+      </c>
+      <c r="E13" t="s">
+        <v>15</v>
+      </c>
+      <c r="F13">
+        <v>4</v>
+      </c>
+      <c r="G13" s="3">
+        <v>44239</v>
+      </c>
+      <c r="H13" t="s">
+        <v>132</v>
+      </c>
+      <c r="I13" t="str">
+        <f t="shared" si="1"/>
+        <v>nl_wk12_20210212_pB_wv04</v>
       </c>
     </row>
   </sheetData>
@@ -3779,13 +3912,13 @@
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.84375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.3046875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.3046875" customWidth="1"/>
+    <col min="1" max="1" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>83</v>
       </c>
@@ -3832,7 +3965,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -3862,7 +3995,7 @@
         <v>no_wk01_20200501_pA_wv01</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
@@ -3895,7 +4028,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>1</v>
       </c>
@@ -3925,7 +4058,7 @@
         <v>no_wk03_20200622_pA_wv03</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>1</v>
       </c>
@@ -3958,7 +4091,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>1</v>
       </c>
@@ -3991,7 +4124,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>1</v>
       </c>
@@ -4033,18 +4166,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9984DEBA-9A58-467F-869B-4E55580BB1A4}">
   <dimension ref="A1:M27"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28:XFD28"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.84375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="7" max="7" width="10.69140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.6640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="59" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="27.3046875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="27.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4085,7 +4218,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>99</v>
       </c>
@@ -4118,7 +4251,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>100</v>
       </c>
@@ -4151,12 +4284,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>101</v>
       </c>
       <c r="B4">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C4">
         <v>0</v>
@@ -4184,12 +4317,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>102</v>
       </c>
       <c r="B5">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C5">
         <v>0</v>
@@ -4217,12 +4350,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>103</v>
       </c>
       <c r="B6">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C6">
         <v>0</v>
@@ -4250,12 +4383,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>104</v>
       </c>
-      <c r="B7">
-        <v>5</v>
+      <c r="B7" s="2">
+        <v>4</v>
       </c>
       <c r="C7">
         <v>0</v>
@@ -4283,12 +4416,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>105</v>
       </c>
-      <c r="B8">
-        <v>5</v>
+      <c r="B8" s="2">
+        <v>4</v>
       </c>
       <c r="C8">
         <v>0</v>
@@ -4316,12 +4449,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>99</v>
       </c>
-      <c r="B9">
-        <v>5</v>
+      <c r="B9" s="2">
+        <v>4</v>
       </c>
       <c r="C9">
         <v>0</v>
@@ -4346,12 +4479,12 @@
         <v>at_wk02_20210118_pA_wv02</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>100</v>
       </c>
-      <c r="B10">
-        <v>5</v>
+      <c r="B10" s="2">
+        <v>4</v>
       </c>
       <c r="C10">
         <v>0</v>
@@ -4376,12 +4509,12 @@
         <v>dk_wk02_20210118_pA_wv02</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>101</v>
       </c>
-      <c r="B11">
-        <v>5</v>
+      <c r="B11" s="2">
+        <v>4</v>
       </c>
       <c r="C11">
         <v>0</v>
@@ -4406,12 +4539,12 @@
         <v>es_wk02_20210118_pA_wv02</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>102</v>
       </c>
-      <c r="B12">
-        <v>5</v>
+      <c r="B12" s="2">
+        <v>4</v>
       </c>
       <c r="C12">
         <v>0</v>
@@ -4436,12 +4569,12 @@
         <v>fr_wk02_20210118_pA_wv02</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>103</v>
       </c>
-      <c r="B13">
-        <v>5</v>
+      <c r="B13" s="2">
+        <v>4</v>
       </c>
       <c r="C13">
         <v>0</v>
@@ -4466,12 +4599,12 @@
         <v>it_wk02_20210118_pA_wv02</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>104</v>
       </c>
-      <c r="B14">
-        <v>5</v>
+      <c r="B14" s="2">
+        <v>4</v>
       </c>
       <c r="C14">
         <v>0</v>
@@ -4496,12 +4629,12 @@
         <v>pl_wk02_20210118_pA_wv02</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>105</v>
       </c>
-      <c r="B15">
-        <v>5</v>
+      <c r="B15" s="2">
+        <v>4</v>
       </c>
       <c r="C15">
         <v>0</v>
@@ -4526,12 +4659,12 @@
         <v>pt_wk02_20210118_pA_wv02</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
         <v>99</v>
       </c>
       <c r="B16" s="2">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C16" s="2">
         <v>0</v>
@@ -4556,12 +4689,12 @@
         <v>at_wk03_20210129_pA_wv03</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
         <v>100</v>
       </c>
       <c r="B17" s="2">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C17" s="2">
         <v>0</v>
@@ -4586,12 +4719,12 @@
         <v>dk_wk03_20210129_pA_wv03</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
         <v>101</v>
       </c>
       <c r="B18" s="2">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C18" s="2">
         <v>0</v>
@@ -4616,12 +4749,12 @@
         <v>es_wk03_20210129_pA_wv03</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
         <v>102</v>
       </c>
       <c r="B19" s="2">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C19" s="2">
         <v>0</v>
@@ -4646,12 +4779,12 @@
         <v>fr_wk03_20210129_pA_wv03</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
         <v>103</v>
       </c>
       <c r="B20" s="2">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C20" s="2">
         <v>0</v>
@@ -4676,12 +4809,12 @@
         <v>it_wk03_20210129_pA_wv03</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
         <v>104</v>
       </c>
       <c r="B21" s="2">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C21" s="2">
         <v>0</v>
@@ -4706,12 +4839,12 @@
         <v>pl_wk03_20210129_pA_wv03</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
         <v>105</v>
       </c>
       <c r="B22" s="2">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C22" s="2">
         <v>0</v>
@@ -4736,12 +4869,12 @@
         <v>pt_wk03_20210129_pA_wv03</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="B23" s="4">
-        <v>5</v>
+      <c r="B23" s="2">
+        <v>4</v>
       </c>
       <c r="C23" s="4">
         <v>0</v>
@@ -4766,12 +4899,12 @@
         <v>at_wk01_20210111_pC_wv01</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="B24" s="4">
-        <v>5</v>
+      <c r="B24" s="2">
+        <v>4</v>
       </c>
       <c r="C24" s="4">
         <v>0</v>
@@ -4796,12 +4929,12 @@
         <v>dk_wk01_20210111_pC_wv01</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="B25" s="4">
-        <v>5</v>
+      <c r="B25" s="2">
+        <v>4</v>
       </c>
       <c r="C25" s="4">
         <v>0</v>
@@ -4826,12 +4959,12 @@
         <v>fr_wk01_20210111_pC_wv01</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="B26" s="4">
-        <v>5</v>
+      <c r="B26" s="2">
+        <v>4</v>
       </c>
       <c r="C26" s="4">
         <v>0</v>
@@ -4856,12 +4989,12 @@
         <v>it_wk01_20210111_pC_wv01</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" s="4" t="s">
         <v>104</v>
       </c>
       <c r="B27" s="4">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C27" s="4">
         <v>0</v>
@@ -4896,24 +5029,24 @@
   <dimension ref="A1:J8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.07421875" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.4609375" customWidth="1"/>
-    <col min="2" max="2" width="16.69140625" customWidth="1"/>
-    <col min="3" max="3" width="8.69140625" customWidth="1"/>
-    <col min="4" max="4" width="7.3046875" customWidth="1"/>
-    <col min="5" max="5" width="8.4609375" customWidth="1"/>
-    <col min="6" max="6" width="9.3046875" customWidth="1"/>
-    <col min="7" max="7" width="11.69140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="52.69140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="24.69140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="6.84375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.5" customWidth="1"/>
+    <col min="2" max="2" width="16.6640625" customWidth="1"/>
+    <col min="3" max="3" width="8.6640625" customWidth="1"/>
+    <col min="4" max="4" width="7.33203125" customWidth="1"/>
+    <col min="5" max="5" width="8.5" customWidth="1"/>
+    <col min="6" max="6" width="9.33203125" customWidth="1"/>
+    <col min="7" max="7" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="52.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="24.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="6.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -4945,12 +5078,12 @@
         <v>79</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>120</v>
       </c>
       <c r="B2" s="2">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C2" s="2">
         <v>0</v>
@@ -4976,12 +5109,12 @@
       </c>
       <c r="J2" s="2"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>121</v>
       </c>
       <c r="B3" s="2">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C3" s="2">
         <v>0</v>
@@ -5007,12 +5140,12 @@
       </c>
       <c r="J3" s="2"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>122</v>
       </c>
       <c r="B4" s="2">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C4" s="2">
         <v>0</v>
@@ -5038,12 +5171,12 @@
       </c>
       <c r="J4" s="2"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>121</v>
       </c>
       <c r="B5" s="4">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C5" s="2">
         <v>0</v>
@@ -5068,12 +5201,12 @@
         <v>fi_wk01_20210112_pC_wv01</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>122</v>
       </c>
       <c r="B6" s="4">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C6" s="2">
         <v>0</v>
@@ -5098,12 +5231,12 @@
         <v>ch_wk01_20210113_pC_wv01</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>127</v>
       </c>
       <c r="B7" s="4">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C7" s="2">
         <v>0</v>
@@ -5128,12 +5261,12 @@
         <v>gr_wk01_20210113_pC_wv01</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>120</v>
       </c>
       <c r="B8" s="4">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C8" s="2">
         <v>0</v>
@@ -5167,377 +5300,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9379CF0-E466-4164-B69D-1322B08B2D66}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="O21" sqref="O21"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.84375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>115</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BED03538-A030-6E4C-BA50-2D13272854A1}">
-  <dimension ref="A1:M10"/>
-  <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:I10"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11.07421875" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
-  <cols>
-    <col min="1" max="1" width="7.15234375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.3046875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.15234375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.3046875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.69140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="58.3046875" customWidth="1"/>
-    <col min="9" max="9" width="25" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="6.84375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="7" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="8.84375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.69140625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A1" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="J1" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="K1" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="L1" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="M1" s="4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A2" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="B2" s="4">
-        <v>7</v>
-      </c>
-      <c r="C2" s="4">
-        <v>0</v>
-      </c>
-      <c r="D2" s="4">
-        <v>1</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="F2" s="4">
-        <v>1</v>
-      </c>
-      <c r="G2" s="5">
-        <v>44207</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>125</v>
-      </c>
-      <c r="I2" s="4" t="str">
-        <f>A2&amp;"_"&amp;"wk"&amp;TEXT(D2,"00")&amp;"_"&amp;YEAR(G2)&amp;TEXT(G2,"MM")&amp;TEXT(G2,"DD")&amp;"_p"&amp;E2&amp;"_wv"&amp;TEXT(F2,"00")&amp;""</f>
-        <v>at_wk01_20210111_pC_wv01</v>
-      </c>
-      <c r="J2" s="4"/>
-      <c r="K2" s="4"/>
-      <c r="L2" s="4"/>
-      <c r="M2" s="4"/>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A3" s="4" t="s">
-        <v>100</v>
-      </c>
-      <c r="B3" s="4">
-        <v>7</v>
-      </c>
-      <c r="C3" s="4">
-        <v>0</v>
-      </c>
-      <c r="D3" s="4">
-        <v>1</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="F3" s="4">
-        <v>1</v>
-      </c>
-      <c r="G3" s="5">
-        <v>44207</v>
-      </c>
-      <c r="H3" s="4" t="s">
-        <v>125</v>
-      </c>
-      <c r="I3" s="4" t="str">
-        <f t="shared" ref="I3:I10" si="0">A3&amp;"_"&amp;"wk"&amp;TEXT(D3,"00")&amp;"_"&amp;YEAR(G3)&amp;TEXT(G3,"MM")&amp;TEXT(G3,"DD")&amp;"_p"&amp;E3&amp;"_wv"&amp;TEXT(F3,"00")&amp;""</f>
-        <v>dk_wk01_20210111_pC_wv01</v>
-      </c>
-      <c r="J3" s="4"/>
-      <c r="K3" s="4"/>
-      <c r="L3" s="4"/>
-      <c r="M3" s="4"/>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A4" s="4" t="s">
-        <v>102</v>
-      </c>
-      <c r="B4" s="4">
-        <v>7</v>
-      </c>
-      <c r="C4" s="4">
-        <v>0</v>
-      </c>
-      <c r="D4" s="4">
-        <v>1</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="F4" s="4">
-        <v>1</v>
-      </c>
-      <c r="G4" s="5">
-        <v>44207</v>
-      </c>
-      <c r="H4" s="4" t="s">
-        <v>125</v>
-      </c>
-      <c r="I4" s="4" t="str">
-        <f t="shared" si="0"/>
-        <v>fr_wk01_20210111_pC_wv01</v>
-      </c>
-      <c r="J4" s="4"/>
-      <c r="K4" s="4"/>
-      <c r="L4" s="4"/>
-      <c r="M4" s="4"/>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A5" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="B5" s="4">
-        <v>7</v>
-      </c>
-      <c r="C5" s="4">
-        <v>0</v>
-      </c>
-      <c r="D5" s="4">
-        <v>1</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="F5" s="4">
-        <v>1</v>
-      </c>
-      <c r="G5" s="5">
-        <v>44207</v>
-      </c>
-      <c r="H5" s="4" t="s">
-        <v>125</v>
-      </c>
-      <c r="I5" s="4" t="str">
-        <f t="shared" si="0"/>
-        <v>it_wk01_20210111_pC_wv01</v>
-      </c>
-      <c r="J5" s="4"/>
-      <c r="K5" s="4"/>
-      <c r="L5" s="4"/>
-      <c r="M5" s="4"/>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A6" s="4" t="s">
-        <v>104</v>
-      </c>
-      <c r="B6" s="4">
-        <v>7</v>
-      </c>
-      <c r="C6" s="4">
-        <v>0</v>
-      </c>
-      <c r="D6" s="4">
-        <v>1</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="F6" s="4">
-        <v>1</v>
-      </c>
-      <c r="G6" s="5">
-        <v>44207</v>
-      </c>
-      <c r="H6" s="4" t="s">
-        <v>125</v>
-      </c>
-      <c r="I6" s="4" t="str">
-        <f t="shared" si="0"/>
-        <v>pl_wk01_20210111_pC_wv01</v>
-      </c>
-      <c r="J6" s="4"/>
-      <c r="K6" s="4"/>
-      <c r="L6" s="4"/>
-      <c r="M6" s="4"/>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A7" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="B7" s="4">
-        <v>7</v>
-      </c>
-      <c r="C7" s="2">
-        <v>0</v>
-      </c>
-      <c r="D7" s="2">
-        <v>1</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="F7" s="2">
-        <v>1</v>
-      </c>
-      <c r="G7" s="3">
-        <v>44207</v>
-      </c>
-      <c r="H7" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="I7" s="4" t="str">
-        <f t="shared" si="0"/>
-        <v>lt_wk01_20210111_pC_wv01</v>
-      </c>
-      <c r="J7" s="2"/>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A8" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="B8" s="4">
-        <v>7</v>
-      </c>
-      <c r="C8" s="2">
-        <v>0</v>
-      </c>
-      <c r="D8" s="2">
-        <v>1</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="F8" s="2">
-        <v>1</v>
-      </c>
-      <c r="G8" s="3">
-        <v>44208</v>
-      </c>
-      <c r="H8" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="I8" s="4" t="str">
-        <f t="shared" si="0"/>
-        <v>fi_wk01_20210112_pC_wv01</v>
-      </c>
-      <c r="J8" s="2"/>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A9" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="B9" s="4">
-        <v>7</v>
-      </c>
-      <c r="C9" s="2">
-        <v>0</v>
-      </c>
-      <c r="D9" s="2">
-        <v>1</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="F9" s="2">
-        <v>1</v>
-      </c>
-      <c r="G9" s="3">
-        <v>44209</v>
-      </c>
-      <c r="H9" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="I9" s="4" t="str">
-        <f t="shared" si="0"/>
-        <v>ch_wk01_20210113_pC_wv01</v>
-      </c>
-      <c r="J9" s="2"/>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A10" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="B10" s="4">
-        <v>7</v>
-      </c>
-      <c r="C10" s="2">
-        <v>0</v>
-      </c>
-      <c r="D10" s="2">
-        <v>1</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="F10" s="2">
-        <v>1</v>
-      </c>
-      <c r="G10" s="3">
-        <v>44209</v>
-      </c>
-      <c r="H10" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="I10" s="4" t="str">
-        <f t="shared" si="0"/>
-        <v>gr_wk01_20210113_pC_wv01</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add run version 3 mac and spss files
</commit_message>
<xml_diff>
--- a/data/spss_files.xlsx
+++ b/data/spss_files.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/amygimma/lshtm/comix_data_clean/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2B29728-5FDB-5444-BC6E-B93DDCC518B7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB29EE51-EDAF-C749-9EB2-6B6D30E1262E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="5" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="454" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="457" uniqueCount="137">
   <si>
     <t>country</t>
   </si>
@@ -449,6 +449,9 @@
   </si>
   <si>
     <t>panel B for NL</t>
+  </si>
+  <si>
+    <t>20_060765_BE2_Wave8_Final_v1_250221_IntClientUse</t>
   </si>
 </sst>
 </file>
@@ -786,7 +789,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2637BBD4-AFF7-4386-815F-A64B43C0CC5D}">
   <dimension ref="A4:B10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
@@ -2928,10 +2931,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C042354-CAAB-48AD-AFC2-2197A2D12C9D}">
-  <dimension ref="A1:N16"/>
+  <dimension ref="A1:N17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H31" sqref="H31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3412,7 +3415,7 @@
         <v>124</v>
       </c>
       <c r="I15" s="2" t="str">
-        <f t="shared" si="0"/>
+        <f>A15&amp;"_"&amp;"wk"&amp;TEXT(D15,"00")&amp;"_"&amp;YEAR(G15)&amp;TEXT(G15,"MM")&amp;TEXT(G15,"DD")&amp;"_p"&amp;E15&amp;"_wv"&amp;TEXT(F15,"00")&amp;""</f>
         <v>be_wk14_20210127_pB_wv06</v>
       </c>
     </row>
@@ -3444,6 +3447,36 @@
       <c r="I16" t="str">
         <f t="shared" si="0"/>
         <v>be_wk15_20210222_pB_wv07</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A17" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B17" s="2">
+        <v>5</v>
+      </c>
+      <c r="C17" s="2">
+        <v>0</v>
+      </c>
+      <c r="D17" s="2">
+        <v>16</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F17">
+        <v>8</v>
+      </c>
+      <c r="G17" s="3">
+        <v>44253</v>
+      </c>
+      <c r="H17" t="s">
+        <v>136</v>
+      </c>
+      <c r="I17" s="2" t="str">
+        <f>A17&amp;"_"&amp;"wk"&amp;TEXT(D17,"00")&amp;"_"&amp;YEAR(G17)&amp;TEXT(G17,"MM")&amp;TEXT(G17,"DD")&amp;"_p"&amp;E17&amp;"_wv"&amp;TEXT(F17,"00")&amp;""</f>
+        <v>be_wk16_20210226_pB_wv08</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
nl wave 5 , update cnt_age_group for mass contacts and update run v3 mac sh
</commit_message>
<xml_diff>
--- a/data/spss_files.xlsx
+++ b/data/spss_files.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/amygimma/lshtm/comix_data_clean/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB29EE51-EDAF-C749-9EB2-6B6D30E1262E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C3044A0-B41B-2845-9E65-520625764146}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="5" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="457" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="460" uniqueCount="138">
   <si>
     <t>country</t>
   </si>
@@ -452,6 +452,9 @@
   </si>
   <si>
     <t>20_060765_BE2_Wave8_Final_v1_250221_IntClientUse</t>
+  </si>
+  <si>
+    <t>20-090916_NL_Wave5_Final_v1_01032021_IntClientUse</t>
   </si>
 </sst>
 </file>
@@ -2933,7 +2936,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C042354-CAAB-48AD-AFC2-2197A2D12C9D}">
   <dimension ref="A1:N17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H31" sqref="H31"/>
     </sheetView>
   </sheetViews>
@@ -3487,10 +3490,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7709FE3-57B1-4766-A5D4-6B378E0A5BA3}">
-  <dimension ref="A1:O13"/>
+  <dimension ref="A1:O14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3896,7 +3899,7 @@
         <v>131</v>
       </c>
       <c r="I12" s="2" t="str">
-        <f t="shared" ref="I12:I13" si="1">C12&amp;"_"&amp;"wk"&amp;TEXT(D12,"00")&amp;"_"&amp;YEAR(G12)&amp;TEXT(G12,"MM")&amp;TEXT(G12,"DD")&amp;"_p"&amp;E12&amp;"_wv"&amp;TEXT(F12,"00")&amp;""</f>
+        <f t="shared" ref="I12:I14" si="1">C12&amp;"_"&amp;"wk"&amp;TEXT(D12,"00")&amp;"_"&amp;YEAR(G12)&amp;TEXT(G12,"MM")&amp;TEXT(G12,"DD")&amp;"_p"&amp;E12&amp;"_wv"&amp;TEXT(F12,"00")&amp;""</f>
         <v>nl_wk11_20210202_pB_wv03</v>
       </c>
       <c r="J12" s="2"/>
@@ -3930,6 +3933,36 @@
       <c r="I13" t="str">
         <f t="shared" si="1"/>
         <v>nl_wk12_20210212_pB_wv04</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>6</v>
+      </c>
+      <c r="B14">
+        <v>0</v>
+      </c>
+      <c r="C14" t="s">
+        <v>73</v>
+      </c>
+      <c r="D14">
+        <v>13</v>
+      </c>
+      <c r="E14" t="s">
+        <v>15</v>
+      </c>
+      <c r="F14">
+        <v>5</v>
+      </c>
+      <c r="G14" s="3">
+        <v>44256</v>
+      </c>
+      <c r="H14" t="s">
+        <v>137</v>
+      </c>
+      <c r="I14" t="str">
+        <f t="shared" si="1"/>
+        <v>nl_wk13_20210301_pB_wv05</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Change week to survey round in data
</commit_message>
<xml_diff>
--- a/data/spss_files.xlsx
+++ b/data/spss_files.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/amygimma/lshtm/comix_data_clean/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jarvisc1\Documents\projects\comix_data_clean\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C3044A0-B41B-2845-9E65-520625764146}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA1E20A5-EE18-4871-8090-18695E7B5DB9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18120" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="5" r:id="rId1"/>
@@ -49,9 +49,6 @@
     <t>note</t>
   </si>
   <si>
-    <t>week</t>
-  </si>
-  <si>
     <t>panel</t>
   </si>
   <si>
@@ -455,6 +452,9 @@
   </si>
   <si>
     <t>20-090916_NL_Wave5_Final_v1_01032021_IntClientUse</t>
+  </si>
+  <si>
+    <t>survey_round</t>
   </si>
 </sst>
 </file>
@@ -796,59 +796,59 @@
       <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.84375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <sheetData>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="B5" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5">
-        <v>1</v>
-      </c>
-      <c r="B5" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A6">
         <v>2</v>
       </c>
       <c r="B6" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A7">
+        <v>3</v>
+      </c>
+      <c r="B7" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7">
-        <v>3</v>
-      </c>
-      <c r="B7" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A8">
         <v>4</v>
       </c>
       <c r="B8" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A9">
         <v>5</v>
       </c>
       <c r="B9" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A10">
         <v>6</v>
       </c>
       <c r="B10" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
   </sheetData>
@@ -861,66 +861,67 @@
   <dimension ref="A1:O56"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8:D9"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.84375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.33203125" customWidth="1"/>
-    <col min="7" max="7" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="58.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="25.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.3046875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.3046875" customWidth="1"/>
+    <col min="4" max="4" width="12.23046875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.69140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="58.3046875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="25.3046875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B1" t="s">
         <v>83</v>
       </c>
-      <c r="B1" t="s">
-        <v>84</v>
-      </c>
       <c r="C1" t="s">
         <v>0</v>
       </c>
       <c r="D1" t="s">
+        <v>137</v>
+      </c>
+      <c r="E1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
-        <v>3</v>
-      </c>
       <c r="F1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>7</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
+        <v>78</v>
+      </c>
+      <c r="L1" t="s">
         <v>8</v>
       </c>
-      <c r="K1" t="s">
-        <v>79</v>
-      </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>9</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>10</v>
       </c>
-      <c r="N1" t="s">
-        <v>11</v>
-      </c>
       <c r="O1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A2">
         <v>1</v>
       </c>
@@ -928,13 +929,13 @@
         <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D2">
         <v>1</v>
       </c>
       <c r="E2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F2">
         <v>1</v>
@@ -943,7 +944,7 @@
         <v>43923</v>
       </c>
       <c r="H2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I2" t="str">
         <f t="shared" ref="I2:I56" si="0">C2&amp;"_"&amp;"wk"&amp;TEXT(D2,"00")&amp;"_"&amp;YEAR(G2)&amp;TEXT(G2,"MM")&amp;TEXT(G2,"DD")&amp;"_p"&amp;E2&amp;"_wv"&amp;TEXT(F2,"00")&amp;""</f>
@@ -956,7 +957,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A3">
         <v>1</v>
       </c>
@@ -964,13 +965,13 @@
         <v>0</v>
       </c>
       <c r="C3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D3">
         <v>2</v>
       </c>
       <c r="E3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F3">
         <v>1</v>
@@ -979,7 +980,7 @@
         <v>43875</v>
       </c>
       <c r="H3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I3" t="str">
         <f t="shared" si="0"/>
@@ -992,7 +993,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A4">
         <v>1</v>
       </c>
@@ -1000,13 +1001,13 @@
         <v>0</v>
       </c>
       <c r="C4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D4">
         <v>3</v>
       </c>
       <c r="E4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F4">
         <v>2</v>
@@ -1015,7 +1016,7 @@
         <v>43964</v>
       </c>
       <c r="H4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I4" t="str">
         <f t="shared" si="0"/>
@@ -1028,7 +1029,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A5">
         <v>1</v>
       </c>
@@ -1036,13 +1037,13 @@
         <v>0</v>
       </c>
       <c r="C5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D5">
         <v>4</v>
       </c>
       <c r="E5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F5">
         <v>2</v>
@@ -1051,7 +1052,7 @@
         <v>43948</v>
       </c>
       <c r="H5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I5" t="str">
         <f t="shared" si="0"/>
@@ -1064,7 +1065,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A6">
         <v>1</v>
       </c>
@@ -1072,13 +1073,13 @@
         <v>0</v>
       </c>
       <c r="C6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D6">
         <v>5</v>
       </c>
       <c r="E6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F6">
         <v>3</v>
@@ -1087,7 +1088,7 @@
         <v>43949</v>
       </c>
       <c r="H6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="I6" t="str">
         <f t="shared" si="0"/>
@@ -1100,7 +1101,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A7">
         <v>1</v>
       </c>
@@ -1108,13 +1109,13 @@
         <v>0</v>
       </c>
       <c r="C7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D7">
         <v>6</v>
       </c>
       <c r="E7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F7">
         <v>3</v>
@@ -1123,7 +1124,7 @@
         <v>43963</v>
       </c>
       <c r="H7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I7" t="str">
         <f t="shared" si="0"/>
@@ -1136,7 +1137,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A8">
         <v>1</v>
       </c>
@@ -1144,13 +1145,13 @@
         <v>0</v>
       </c>
       <c r="C8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D8">
         <v>7</v>
       </c>
       <c r="E8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F8">
         <v>4</v>
@@ -1159,7 +1160,7 @@
         <v>43964</v>
       </c>
       <c r="H8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I8" t="str">
         <f t="shared" si="0"/>
@@ -1172,10 +1173,10 @@
         <v>1</v>
       </c>
       <c r="O8" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A9">
         <v>2</v>
       </c>
@@ -1183,13 +1184,13 @@
         <v>0</v>
       </c>
       <c r="C9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D9">
         <v>7</v>
       </c>
       <c r="E9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F9">
         <v>1</v>
@@ -1198,7 +1199,7 @@
         <v>43970</v>
       </c>
       <c r="H9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I9" t="str">
         <f t="shared" si="0"/>
@@ -1211,7 +1212,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A10">
         <v>1</v>
       </c>
@@ -1219,14 +1220,14 @@
         <v>0</v>
       </c>
       <c r="C10" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D10">
         <f>D8+1</f>
         <v>8</v>
       </c>
       <c r="E10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F10">
         <v>4</v>
@@ -1235,7 +1236,7 @@
         <v>43973</v>
       </c>
       <c r="H10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I10" t="str">
         <f t="shared" si="0"/>
@@ -1248,7 +1249,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A11">
         <v>2</v>
       </c>
@@ -1256,14 +1257,14 @@
         <v>0</v>
       </c>
       <c r="C11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D11">
         <f>D9+1</f>
         <v>8</v>
       </c>
       <c r="E11" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F11">
         <v>1</v>
@@ -1272,7 +1273,7 @@
         <v>43993</v>
       </c>
       <c r="H11" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I11" t="str">
         <f t="shared" si="0"/>
@@ -1285,7 +1286,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A12">
         <v>1</v>
       </c>
@@ -1293,14 +1294,14 @@
         <v>0</v>
       </c>
       <c r="C12" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D12">
         <f t="shared" ref="D12:D21" si="1">D10+1</f>
         <v>9</v>
       </c>
       <c r="E12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F12">
         <v>5</v>
@@ -1309,7 +1310,7 @@
         <v>43980</v>
       </c>
       <c r="H12" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I12" t="str">
         <f t="shared" si="0"/>
@@ -1322,7 +1323,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A13">
         <v>2</v>
       </c>
@@ -1330,14 +1331,14 @@
         <v>0</v>
       </c>
       <c r="C13" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D13">
         <f t="shared" si="1"/>
         <v>9</v>
       </c>
       <c r="E13" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F13">
         <v>2</v>
@@ -1347,7 +1348,7 @@
         <v>43979</v>
       </c>
       <c r="H13" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I13" t="str">
         <f t="shared" si="0"/>
@@ -1360,7 +1361,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A14">
         <v>1</v>
       </c>
@@ -1368,14 +1369,14 @@
         <v>0</v>
       </c>
       <c r="C14" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D14">
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
       <c r="E14" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F14">
         <v>5</v>
@@ -1384,7 +1385,7 @@
         <v>43986</v>
       </c>
       <c r="H14" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I14" t="str">
         <f t="shared" si="0"/>
@@ -1397,7 +1398,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A15">
         <v>2</v>
       </c>
@@ -1405,14 +1406,14 @@
         <v>0</v>
       </c>
       <c r="C15" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D15">
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
       <c r="E15" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F15">
         <v>2</v>
@@ -1421,7 +1422,7 @@
         <v>43990</v>
       </c>
       <c r="H15" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I15" t="str">
         <f t="shared" si="0"/>
@@ -1434,7 +1435,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A16">
         <v>1</v>
       </c>
@@ -1442,14 +1443,14 @@
         <v>0</v>
       </c>
       <c r="C16" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D16">
         <f t="shared" si="1"/>
         <v>11</v>
       </c>
       <c r="E16" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F16">
         <v>6</v>
@@ -1458,7 +1459,7 @@
         <v>43994</v>
       </c>
       <c r="H16" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I16" t="str">
         <f t="shared" si="0"/>
@@ -1471,7 +1472,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A17">
         <v>2</v>
       </c>
@@ -1479,14 +1480,14 @@
         <v>0</v>
       </c>
       <c r="C17" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D17">
         <f t="shared" si="1"/>
         <v>11</v>
       </c>
       <c r="E17" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F17">
         <v>3</v>
@@ -1495,7 +1496,7 @@
         <v>43994</v>
       </c>
       <c r="H17" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I17" t="str">
         <f t="shared" si="0"/>
@@ -1508,7 +1509,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A18">
         <v>1</v>
       </c>
@@ -1516,14 +1517,14 @@
         <v>0</v>
       </c>
       <c r="C18" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D18">
         <f t="shared" si="1"/>
         <v>12</v>
       </c>
       <c r="E18" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F18">
         <v>6</v>
@@ -1532,7 +1533,7 @@
         <v>44001</v>
       </c>
       <c r="H18" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I18" t="str">
         <f t="shared" si="0"/>
@@ -1545,7 +1546,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A19">
         <v>2</v>
       </c>
@@ -1553,14 +1554,14 @@
         <v>0</v>
       </c>
       <c r="C19" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D19">
         <f t="shared" si="1"/>
         <v>12</v>
       </c>
       <c r="E19" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F19">
         <v>3</v>
@@ -1569,7 +1570,7 @@
         <v>44001</v>
       </c>
       <c r="H19" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I19" t="str">
         <f t="shared" si="0"/>
@@ -1582,7 +1583,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A20">
         <v>1</v>
       </c>
@@ -1590,14 +1591,14 @@
         <v>0</v>
       </c>
       <c r="C20" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D20">
         <f t="shared" si="1"/>
         <v>13</v>
       </c>
       <c r="E20" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F20">
         <v>7</v>
@@ -1606,7 +1607,7 @@
         <v>44007</v>
       </c>
       <c r="H20" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I20" t="str">
         <f t="shared" si="0"/>
@@ -1619,7 +1620,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A21">
         <v>2</v>
       </c>
@@ -1627,14 +1628,14 @@
         <v>0</v>
       </c>
       <c r="C21" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D21">
         <f t="shared" si="1"/>
         <v>13</v>
       </c>
       <c r="E21" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F21">
         <v>4</v>
@@ -1643,7 +1644,7 @@
         <v>44007</v>
       </c>
       <c r="H21" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I21" t="str">
         <f t="shared" si="0"/>
@@ -1656,7 +1657,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A22">
         <v>1</v>
       </c>
@@ -1664,14 +1665,14 @@
         <v>0</v>
       </c>
       <c r="C22" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D22">
         <f>D20+1</f>
         <v>14</v>
       </c>
       <c r="E22" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F22">
         <v>7</v>
@@ -1680,7 +1681,7 @@
         <v>44014</v>
       </c>
       <c r="H22" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I22" t="str">
         <f t="shared" si="0"/>
@@ -1693,7 +1694,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A23">
         <v>2</v>
       </c>
@@ -1701,14 +1702,14 @@
         <v>0</v>
       </c>
       <c r="C23" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D23">
         <f>D21+1</f>
         <v>14</v>
       </c>
       <c r="E23" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F23">
         <v>4</v>
@@ -1717,7 +1718,7 @@
         <v>44015</v>
       </c>
       <c r="H23" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I23" t="str">
         <f t="shared" si="0"/>
@@ -1730,7 +1731,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A24">
         <v>1</v>
       </c>
@@ -1738,14 +1739,14 @@
         <v>0</v>
       </c>
       <c r="C24" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D24">
         <f t="shared" ref="D24:D28" si="3">D22+1</f>
         <v>15</v>
       </c>
       <c r="E24" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F24">
         <v>8</v>
@@ -1754,7 +1755,7 @@
         <v>44022</v>
       </c>
       <c r="H24" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I24" t="str">
         <f t="shared" si="0"/>
@@ -1767,7 +1768,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A25">
         <v>2</v>
       </c>
@@ -1775,14 +1776,14 @@
         <v>0</v>
       </c>
       <c r="C25" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D25">
         <f t="shared" si="3"/>
         <v>15</v>
       </c>
       <c r="E25" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F25">
         <v>5</v>
@@ -1791,7 +1792,7 @@
         <v>44021</v>
       </c>
       <c r="H25" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I25" t="str">
         <f t="shared" si="0"/>
@@ -1804,7 +1805,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A26">
         <v>1</v>
       </c>
@@ -1812,14 +1813,14 @@
         <v>0</v>
       </c>
       <c r="C26" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D26">
         <f t="shared" si="3"/>
         <v>16</v>
       </c>
       <c r="E26" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F26">
         <v>8</v>
@@ -1828,7 +1829,7 @@
         <v>44029</v>
       </c>
       <c r="H26" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I26" t="str">
         <f t="shared" si="0"/>
@@ -1841,7 +1842,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A27">
         <v>2</v>
       </c>
@@ -1849,14 +1850,14 @@
         <v>0</v>
       </c>
       <c r="C27" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D27">
         <f t="shared" si="3"/>
         <v>16</v>
       </c>
       <c r="E27" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F27">
         <v>5</v>
@@ -1865,7 +1866,7 @@
         <v>44029</v>
       </c>
       <c r="H27" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="I27" t="str">
         <f t="shared" si="0"/>
@@ -1878,7 +1879,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A28">
         <v>1</v>
       </c>
@@ -1886,14 +1887,14 @@
         <v>0</v>
       </c>
       <c r="C28" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D28">
         <f t="shared" si="3"/>
         <v>17</v>
       </c>
       <c r="E28" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F28">
         <v>9</v>
@@ -1902,7 +1903,7 @@
         <v>44036</v>
       </c>
       <c r="H28" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="I28" t="str">
         <f t="shared" si="0"/>
@@ -1915,10 +1916,10 @@
         <v>1</v>
       </c>
       <c r="O28" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.2">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A29">
         <v>1</v>
       </c>
@@ -1926,14 +1927,14 @@
         <v>0</v>
       </c>
       <c r="C29" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D29">
         <f>D28+1</f>
         <v>18</v>
       </c>
       <c r="E29" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F29">
         <v>9</v>
@@ -1942,7 +1943,7 @@
         <v>44043</v>
       </c>
       <c r="H29" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="I29" t="str">
         <f t="shared" si="0"/>
@@ -1955,10 +1956,10 @@
         <v>1</v>
       </c>
       <c r="O29" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.2">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A30">
         <v>1</v>
       </c>
@@ -1966,14 +1967,14 @@
         <v>0</v>
       </c>
       <c r="C30" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D30">
         <f>D29+1</f>
         <v>19</v>
       </c>
       <c r="E30" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F30">
         <v>10</v>
@@ -1982,7 +1983,7 @@
         <v>44050</v>
       </c>
       <c r="H30" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="I30" t="str">
         <f t="shared" si="0"/>
@@ -1995,7 +1996,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A31">
         <v>2</v>
       </c>
@@ -2003,13 +2004,13 @@
         <v>0</v>
       </c>
       <c r="C31" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D31">
         <v>19</v>
       </c>
       <c r="E31" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F31">
         <v>6</v>
@@ -2018,7 +2019,7 @@
         <v>44053</v>
       </c>
       <c r="H31" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I31" t="str">
         <f t="shared" si="0"/>
@@ -2031,7 +2032,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A32">
         <v>3</v>
       </c>
@@ -2039,13 +2040,13 @@
         <v>0</v>
       </c>
       <c r="C32" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D32">
         <v>20</v>
       </c>
       <c r="E32" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F32">
         <v>1</v>
@@ -2054,7 +2055,7 @@
         <v>44064</v>
       </c>
       <c r="H32" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="I32" t="str">
         <f t="shared" si="0"/>
@@ -2067,10 +2068,10 @@
         <v>1</v>
       </c>
       <c r="O32" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A33">
         <v>3</v>
       </c>
@@ -2078,13 +2079,13 @@
         <v>0</v>
       </c>
       <c r="C33" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D33">
         <v>21</v>
       </c>
       <c r="E33" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F33">
         <v>1</v>
@@ -2093,7 +2094,7 @@
         <v>44070</v>
       </c>
       <c r="H33" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="I33" t="str">
         <f t="shared" si="0"/>
@@ -2106,7 +2107,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A34">
         <v>3</v>
       </c>
@@ -2114,13 +2115,13 @@
         <v>0</v>
       </c>
       <c r="C34" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D34">
         <v>22</v>
       </c>
       <c r="E34" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F34">
         <f t="shared" ref="F34:F56" si="4">F32+1</f>
@@ -2130,7 +2131,7 @@
         <v>44077</v>
       </c>
       <c r="H34" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="I34" t="str">
         <f t="shared" si="0"/>
@@ -2143,7 +2144,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A35">
         <v>3</v>
       </c>
@@ -2151,13 +2152,13 @@
         <v>0</v>
       </c>
       <c r="C35" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D35">
         <v>23</v>
       </c>
       <c r="E35" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F35">
         <f t="shared" si="4"/>
@@ -2167,7 +2168,7 @@
         <v>44081</v>
       </c>
       <c r="H35" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="I35" t="str">
         <f t="shared" si="0"/>
@@ -2180,7 +2181,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A36">
         <v>3</v>
       </c>
@@ -2188,13 +2189,13 @@
         <v>0</v>
       </c>
       <c r="C36" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D36">
         <v>24</v>
       </c>
       <c r="E36" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F36">
         <f t="shared" si="4"/>
@@ -2204,7 +2205,7 @@
         <v>44088</v>
       </c>
       <c r="H36" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="I36" t="str">
         <f t="shared" si="0"/>
@@ -2217,7 +2218,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A37">
         <v>3</v>
       </c>
@@ -2225,13 +2226,13 @@
         <v>0</v>
       </c>
       <c r="C37" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D37">
         <v>25</v>
       </c>
       <c r="E37" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F37">
         <f t="shared" si="4"/>
@@ -2241,7 +2242,7 @@
         <v>44092</v>
       </c>
       <c r="H37" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="I37" t="str">
         <f t="shared" si="0"/>
@@ -2254,7 +2255,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A38">
         <v>3</v>
       </c>
@@ -2262,13 +2263,13 @@
         <v>0</v>
       </c>
       <c r="C38" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D38">
         <v>26</v>
       </c>
       <c r="E38" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F38">
         <f t="shared" si="4"/>
@@ -2278,7 +2279,7 @@
         <v>44099</v>
       </c>
       <c r="H38" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="I38" t="str">
         <f t="shared" si="0"/>
@@ -2291,7 +2292,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A39">
         <v>3</v>
       </c>
@@ -2299,13 +2300,13 @@
         <v>0</v>
       </c>
       <c r="C39" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D39">
         <v>27</v>
       </c>
       <c r="E39" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F39">
         <f t="shared" si="4"/>
@@ -2315,7 +2316,7 @@
         <v>44106</v>
       </c>
       <c r="H39" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="I39" t="str">
         <f t="shared" si="0"/>
@@ -2328,7 +2329,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A40">
         <v>3</v>
       </c>
@@ -2336,13 +2337,13 @@
         <v>0</v>
       </c>
       <c r="C40" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D40">
         <v>28</v>
       </c>
       <c r="E40" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F40">
         <f t="shared" si="4"/>
@@ -2352,7 +2353,7 @@
         <v>44113</v>
       </c>
       <c r="H40" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="I40" t="str">
         <f t="shared" si="0"/>
@@ -2365,7 +2366,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A41">
         <v>3</v>
       </c>
@@ -2373,13 +2374,13 @@
         <v>0</v>
       </c>
       <c r="C41" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D41">
         <v>29</v>
       </c>
       <c r="E41" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F41">
         <f t="shared" si="4"/>
@@ -2389,7 +2390,7 @@
         <v>44122</v>
       </c>
       <c r="H41" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="I41" t="str">
         <f t="shared" si="0"/>
@@ -2402,7 +2403,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A42">
         <v>3</v>
       </c>
@@ -2410,13 +2411,13 @@
         <v>0</v>
       </c>
       <c r="C42" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D42">
         <v>30</v>
       </c>
       <c r="E42" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F42">
         <f t="shared" si="4"/>
@@ -2426,7 +2427,7 @@
         <v>44127</v>
       </c>
       <c r="H42" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I42" t="str">
         <f t="shared" si="0"/>
@@ -2439,7 +2440,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A43">
         <v>3</v>
       </c>
@@ -2447,13 +2448,13 @@
         <v>0</v>
       </c>
       <c r="C43" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D43">
         <v>31</v>
       </c>
       <c r="E43" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F43">
         <f t="shared" si="4"/>
@@ -2463,7 +2464,7 @@
         <v>44134</v>
       </c>
       <c r="H43" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="I43" t="str">
         <f t="shared" si="0"/>
@@ -2476,7 +2477,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A44">
         <v>3</v>
       </c>
@@ -2484,13 +2485,13 @@
         <v>0</v>
       </c>
       <c r="C44" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D44">
         <v>32</v>
       </c>
       <c r="E44" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F44">
         <f t="shared" si="4"/>
@@ -2500,7 +2501,7 @@
         <v>44141</v>
       </c>
       <c r="H44" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="I44" t="str">
         <f t="shared" si="0"/>
@@ -2510,7 +2511,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A45">
         <v>3</v>
       </c>
@@ -2518,13 +2519,13 @@
         <v>0</v>
       </c>
       <c r="C45" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D45">
         <v>33</v>
       </c>
       <c r="E45" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F45">
         <f t="shared" si="4"/>
@@ -2534,7 +2535,7 @@
         <v>44148</v>
       </c>
       <c r="H45" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="I45" t="str">
         <f t="shared" si="0"/>
@@ -2547,7 +2548,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A46">
         <v>3</v>
       </c>
@@ -2555,13 +2556,13 @@
         <v>0</v>
       </c>
       <c r="C46" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D46">
         <v>34</v>
       </c>
       <c r="E46" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F46">
         <f t="shared" si="4"/>
@@ -2571,7 +2572,7 @@
         <v>44155</v>
       </c>
       <c r="H46" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="I46" t="str">
         <f t="shared" si="0"/>
@@ -2584,7 +2585,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A47">
         <v>3</v>
       </c>
@@ -2592,13 +2593,13 @@
         <v>0</v>
       </c>
       <c r="C47" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D47">
         <v>35</v>
       </c>
       <c r="E47" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F47">
         <f t="shared" si="4"/>
@@ -2608,7 +2609,7 @@
         <v>44161</v>
       </c>
       <c r="H47" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="I47" t="str">
         <f t="shared" si="0"/>
@@ -2621,7 +2622,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A48">
         <v>3</v>
       </c>
@@ -2629,13 +2630,13 @@
         <v>0</v>
       </c>
       <c r="C48" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D48">
         <v>36</v>
       </c>
       <c r="E48" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F48">
         <f t="shared" si="4"/>
@@ -2645,7 +2646,7 @@
         <v>43924</v>
       </c>
       <c r="H48" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="I48" t="str">
         <f t="shared" si="0"/>
@@ -2655,7 +2656,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A49">
         <v>3</v>
       </c>
@@ -2663,13 +2664,13 @@
         <v>0</v>
       </c>
       <c r="C49" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D49">
         <v>37</v>
       </c>
       <c r="E49" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F49">
         <f t="shared" si="4"/>
@@ -2679,7 +2680,7 @@
         <v>43872</v>
       </c>
       <c r="H49" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="I49" t="str">
         <f t="shared" si="0"/>
@@ -2689,7 +2690,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A50">
         <v>3</v>
       </c>
@@ -2697,13 +2698,13 @@
         <v>0</v>
       </c>
       <c r="C50" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D50">
         <v>38</v>
       </c>
       <c r="E50" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F50">
         <f t="shared" si="4"/>
@@ -2713,7 +2714,7 @@
         <v>44182</v>
       </c>
       <c r="H50" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="I50" t="str">
         <f t="shared" si="0"/>
@@ -2723,7 +2724,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A51">
         <v>3</v>
       </c>
@@ -2731,13 +2732,13 @@
         <v>0</v>
       </c>
       <c r="C51" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D51">
         <v>39</v>
       </c>
       <c r="E51" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F51">
         <f t="shared" si="4"/>
@@ -2747,7 +2748,7 @@
         <v>44189</v>
       </c>
       <c r="H51" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="I51" t="str">
         <f t="shared" si="0"/>
@@ -2757,7 +2758,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A52">
         <v>3</v>
       </c>
@@ -2765,13 +2766,13 @@
         <v>0</v>
       </c>
       <c r="C52" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D52">
         <v>40</v>
       </c>
       <c r="E52" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F52">
         <f t="shared" si="4"/>
@@ -2781,7 +2782,7 @@
         <v>44196</v>
       </c>
       <c r="H52" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="I52" t="str">
         <f t="shared" si="0"/>
@@ -2791,7 +2792,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A53">
         <v>3</v>
       </c>
@@ -2799,13 +2800,13 @@
         <v>0</v>
       </c>
       <c r="C53" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D53">
         <v>41</v>
       </c>
       <c r="E53" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F53">
         <f t="shared" si="4"/>
@@ -2815,7 +2816,7 @@
         <v>44203</v>
       </c>
       <c r="H53" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="I53" t="str">
         <f t="shared" si="0"/>
@@ -2825,7 +2826,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A54">
         <v>3</v>
       </c>
@@ -2833,13 +2834,13 @@
         <v>0</v>
       </c>
       <c r="C54" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D54">
         <v>42</v>
       </c>
       <c r="E54" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F54">
         <f t="shared" si="4"/>
@@ -2849,7 +2850,7 @@
         <v>44210</v>
       </c>
       <c r="H54" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="I54" t="str">
         <f t="shared" si="0"/>
@@ -2859,7 +2860,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A55" s="2">
         <v>3</v>
       </c>
@@ -2867,13 +2868,13 @@
         <v>0</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D55" s="2">
         <v>43</v>
       </c>
       <c r="E55" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F55" s="2">
         <f t="shared" si="4"/>
@@ -2883,7 +2884,7 @@
         <v>44216</v>
       </c>
       <c r="H55" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="I55" t="str">
         <f t="shared" si="0"/>
@@ -2893,7 +2894,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A56" s="2">
         <v>3</v>
       </c>
@@ -2901,13 +2902,13 @@
         <v>0</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D56" s="2">
         <v>44</v>
       </c>
       <c r="E56" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F56" s="2">
         <f t="shared" si="4"/>
@@ -2917,7 +2918,7 @@
         <v>44224</v>
       </c>
       <c r="H56" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="I56" s="2" t="str">
         <f t="shared" si="0"/>
@@ -2937,66 +2938,67 @@
   <dimension ref="A1:N17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H31" sqref="H31"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.84375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="2" max="2" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.33203125" customWidth="1"/>
+    <col min="2" max="2" width="12.3046875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.3046875" customWidth="1"/>
+    <col min="4" max="4" width="12.23046875" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.5" customWidth="1"/>
-    <col min="8" max="8" width="58.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="30.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.4609375" customWidth="1"/>
+    <col min="8" max="8" width="58.4609375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="30.4609375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C1" t="s">
         <v>83</v>
       </c>
-      <c r="C1" t="s">
-        <v>84</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="D1" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="E1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
-        <v>3</v>
-      </c>
       <c r="F1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" t="s">
-        <v>7</v>
-      </c>
       <c r="J1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="K1" t="s">
+        <v>8</v>
+      </c>
+      <c r="L1" t="s">
         <v>9</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>10</v>
       </c>
-      <c r="M1" t="s">
-        <v>11</v>
-      </c>
       <c r="N1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -3008,7 +3010,7 @@
         <v>1</v>
       </c>
       <c r="E2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F2">
         <v>1</v>
@@ -3017,7 +3019,7 @@
         <v>43950</v>
       </c>
       <c r="H2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="I2" t="str">
         <f t="shared" ref="I2:I16" si="0">A2&amp;"_"&amp;"wk"&amp;TEXT(D2,"00")&amp;"_"&amp;YEAR(G2)&amp;TEXT(G2,"MM")&amp;TEXT(G2,"DD")&amp;"_p"&amp;E2&amp;"_wv"&amp;TEXT(F2,"00")&amp;""</f>
@@ -3027,9 +3029,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -3041,7 +3043,7 @@
         <v>2</v>
       </c>
       <c r="E3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F3">
         <v>2</v>
@@ -3050,7 +3052,7 @@
         <v>43969</v>
       </c>
       <c r="H3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="I3" t="str">
         <f t="shared" si="0"/>
@@ -3060,9 +3062,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -3074,7 +3076,7 @@
         <v>3</v>
       </c>
       <c r="E4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F4">
         <v>3</v>
@@ -3083,7 +3085,7 @@
         <v>43983</v>
       </c>
       <c r="H4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="I4" t="str">
         <f t="shared" si="0"/>
@@ -3093,9 +3095,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -3107,7 +3109,7 @@
         <v>4</v>
       </c>
       <c r="E5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F5">
         <v>4</v>
@@ -3116,7 +3118,7 @@
         <v>43994</v>
       </c>
       <c r="H5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="I5" t="str">
         <f t="shared" si="0"/>
@@ -3126,9 +3128,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -3140,7 +3142,7 @@
         <v>5</v>
       </c>
       <c r="E6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F6">
         <v>5</v>
@@ -3149,7 +3151,7 @@
         <v>44008</v>
       </c>
       <c r="H6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="I6" t="str">
         <f t="shared" si="0"/>
@@ -3159,9 +3161,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -3173,7 +3175,7 @@
         <v>6</v>
       </c>
       <c r="E7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F7">
         <v>6</v>
@@ -3182,7 +3184,7 @@
         <v>44022</v>
       </c>
       <c r="H7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I7" t="str">
         <f t="shared" si="0"/>
@@ -3192,9 +3194,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -3206,7 +3208,7 @@
         <v>7</v>
       </c>
       <c r="E8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F8">
         <v>7</v>
@@ -3215,7 +3217,7 @@
         <v>44036</v>
       </c>
       <c r="H8" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="I8" t="str">
         <f t="shared" si="0"/>
@@ -3225,9 +3227,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -3239,7 +3241,7 @@
         <v>8</v>
       </c>
       <c r="E9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F9">
         <v>8</v>
@@ -3248,7 +3250,7 @@
         <v>44049</v>
       </c>
       <c r="H9" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="I9" t="str">
         <f t="shared" si="0"/>
@@ -3258,9 +3260,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A10" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B10" s="2"/>
       <c r="C10" s="2">
@@ -3270,7 +3272,7 @@
         <v>9</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F10" s="2">
         <v>1</v>
@@ -3284,9 +3286,9 @@
         <v>be_wk09_20201120_pB_wv01</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A11" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B11" s="2"/>
       <c r="C11" s="2">
@@ -3296,7 +3298,7 @@
         <v>10</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F11" s="2">
         <v>2</v>
@@ -3308,9 +3310,9 @@
         <v>be_wk10_19000100_pB_wv02</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A12" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B12" s="2"/>
       <c r="C12" s="2">
@@ -3320,7 +3322,7 @@
         <v>11</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F12" s="2">
         <v>3</v>
@@ -3332,9 +3334,9 @@
         <v>be_wk11_19000100_pB_wv03</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A13" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B13" s="2">
         <v>5</v>
@@ -3346,7 +3348,7 @@
         <v>12</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F13" s="2">
         <v>4</v>
@@ -3355,16 +3357,16 @@
         <v>44207</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="I13" s="2" t="str">
         <f t="shared" si="0"/>
         <v>be_wk12_20210111_pB_wv04</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A14" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B14" s="2">
         <v>5</v>
@@ -3376,7 +3378,7 @@
         <v>13</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F14" s="2">
         <v>5</v>
@@ -3385,16 +3387,16 @@
         <v>44216</v>
       </c>
       <c r="H14" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="I14" s="2" t="str">
         <f t="shared" si="0"/>
         <v>be_wk13_20210120_pB_wv05</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A15" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B15" s="2">
         <v>5</v>
@@ -3406,7 +3408,7 @@
         <v>14</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F15" s="2">
         <v>6</v>
@@ -3415,16 +3417,16 @@
         <v>44223</v>
       </c>
       <c r="H15" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="I15" s="2" t="str">
         <f>A15&amp;"_"&amp;"wk"&amp;TEXT(D15,"00")&amp;"_"&amp;YEAR(G15)&amp;TEXT(G15,"MM")&amp;TEXT(G15,"DD")&amp;"_p"&amp;E15&amp;"_wv"&amp;TEXT(F15,"00")&amp;""</f>
         <v>be_wk14_20210127_pB_wv06</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A16" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B16">
         <v>5</v>
@@ -3436,7 +3438,7 @@
         <v>15</v>
       </c>
       <c r="E16" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F16">
         <v>7</v>
@@ -3445,16 +3447,16 @@
         <v>44249</v>
       </c>
       <c r="H16" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="I16" t="str">
         <f t="shared" si="0"/>
         <v>be_wk15_20210222_pB_wv07</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A17" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B17" s="2">
         <v>5</v>
@@ -3466,7 +3468,7 @@
         <v>16</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F17">
         <v>8</v>
@@ -3475,7 +3477,7 @@
         <v>44253</v>
       </c>
       <c r="H17" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="I17" s="2" t="str">
         <f>A17&amp;"_"&amp;"wk"&amp;TEXT(D17,"00")&amp;"_"&amp;YEAR(G17)&amp;TEXT(G17,"MM")&amp;TEXT(G17,"DD")&amp;"_p"&amp;E17&amp;"_wv"&amp;TEXT(F17,"00")&amp;""</f>
@@ -3492,64 +3494,65 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7709FE3-57B1-4766-A5D4-6B378E0A5BA3}">
   <dimension ref="A1:O14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.84375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="7" max="7" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.23046875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.4609375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.4609375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B1" t="s">
         <v>83</v>
       </c>
-      <c r="B1" t="s">
-        <v>84</v>
-      </c>
       <c r="C1" t="s">
         <v>0</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="E1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
-        <v>3</v>
-      </c>
       <c r="F1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>7</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
+        <v>78</v>
+      </c>
+      <c r="L1" t="s">
         <v>8</v>
       </c>
-      <c r="K1" t="s">
-        <v>79</v>
-      </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>9</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>10</v>
       </c>
-      <c r="N1" t="s">
-        <v>11</v>
-      </c>
       <c r="O1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A2">
         <v>1</v>
       </c>
@@ -3557,13 +3560,13 @@
         <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D2">
         <v>1</v>
       </c>
       <c r="E2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F2">
         <v>1</v>
@@ -3572,7 +3575,7 @@
         <v>43950</v>
       </c>
       <c r="H2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="I2" t="str">
         <f t="shared" ref="I2:I11" si="0">C2&amp;"_"&amp;"wk"&amp;TEXT(D2,"00")&amp;"_"&amp;YEAR(G2)&amp;TEXT(G2,"MM")&amp;TEXT(G2,"DD")&amp;"_p"&amp;E2&amp;"_wv"&amp;TEXT(F2,"00")&amp;""</f>
@@ -3582,7 +3585,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A3">
         <v>1</v>
       </c>
@@ -3590,13 +3593,13 @@
         <v>0</v>
       </c>
       <c r="C3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D3">
         <v>2</v>
       </c>
       <c r="E3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F3">
         <v>2</v>
@@ -3605,7 +3608,7 @@
         <v>43969</v>
       </c>
       <c r="H3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="I3" t="str">
         <f t="shared" si="0"/>
@@ -3615,7 +3618,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A4">
         <v>1</v>
       </c>
@@ -3623,13 +3626,13 @@
         <v>0</v>
       </c>
       <c r="C4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D4">
         <v>3</v>
       </c>
       <c r="E4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F4">
         <v>3</v>
@@ -3638,7 +3641,7 @@
         <v>43983</v>
       </c>
       <c r="H4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="I4" t="str">
         <f t="shared" si="0"/>
@@ -3648,7 +3651,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A5">
         <v>1</v>
       </c>
@@ -3656,13 +3659,13 @@
         <v>0</v>
       </c>
       <c r="C5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D5">
         <v>4</v>
       </c>
       <c r="E5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F5">
         <v>4</v>
@@ -3671,7 +3674,7 @@
         <v>43994</v>
       </c>
       <c r="H5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="I5" t="str">
         <f t="shared" si="0"/>
@@ -3681,7 +3684,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A6">
         <v>1</v>
       </c>
@@ -3689,13 +3692,13 @@
         <v>0</v>
       </c>
       <c r="C6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D6">
         <v>5</v>
       </c>
       <c r="E6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F6">
         <v>5</v>
@@ -3704,7 +3707,7 @@
         <v>44008</v>
       </c>
       <c r="H6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="I6" t="str">
         <f t="shared" si="0"/>
@@ -3714,7 +3717,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A7">
         <v>1</v>
       </c>
@@ -3722,13 +3725,13 @@
         <v>0</v>
       </c>
       <c r="C7" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D7">
         <v>6</v>
       </c>
       <c r="E7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F7">
         <v>6</v>
@@ -3737,7 +3740,7 @@
         <v>44022</v>
       </c>
       <c r="H7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I7" t="str">
         <f t="shared" si="0"/>
@@ -3747,7 +3750,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A8">
         <v>1</v>
       </c>
@@ -3755,13 +3758,13 @@
         <v>0</v>
       </c>
       <c r="C8" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D8">
         <v>7</v>
       </c>
       <c r="E8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F8">
         <v>7</v>
@@ -3770,7 +3773,7 @@
         <v>44036</v>
       </c>
       <c r="H8" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="I8" t="str">
         <f t="shared" si="0"/>
@@ -3780,7 +3783,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A9">
         <v>1</v>
       </c>
@@ -3788,13 +3791,13 @@
         <v>0</v>
       </c>
       <c r="C9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D9">
         <v>8</v>
       </c>
       <c r="E9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F9">
         <v>8</v>
@@ -3803,7 +3806,7 @@
         <v>44049</v>
       </c>
       <c r="H9" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="I9" t="str">
         <f t="shared" si="0"/>
@@ -3813,7 +3816,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A10">
         <v>6</v>
       </c>
@@ -3821,13 +3824,13 @@
         <v>0</v>
       </c>
       <c r="C10" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D10">
         <v>9</v>
       </c>
       <c r="E10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F10">
         <v>1</v>
@@ -3836,14 +3839,14 @@
         <v>44203</v>
       </c>
       <c r="H10" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="I10" t="str">
         <f t="shared" si="0"/>
         <v>nl_wk09_20210107_pB_wv01</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A11">
         <v>6</v>
       </c>
@@ -3851,13 +3854,13 @@
         <v>0</v>
       </c>
       <c r="C11" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D11">
         <v>10</v>
       </c>
       <c r="E11" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F11">
         <v>2</v>
@@ -3866,14 +3869,14 @@
         <v>44214</v>
       </c>
       <c r="H11" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="I11" t="str">
         <f t="shared" si="0"/>
         <v>nl_wk10_20210118_pB_wv02</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A12" s="2">
         <v>6</v>
       </c>
@@ -3881,13 +3884,13 @@
         <v>0</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D12">
         <v>11</v>
       </c>
       <c r="E12" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F12">
         <v>3</v>
@@ -3896,7 +3899,7 @@
         <v>44229</v>
       </c>
       <c r="H12" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="I12" s="2" t="str">
         <f t="shared" ref="I12:I14" si="1">C12&amp;"_"&amp;"wk"&amp;TEXT(D12,"00")&amp;"_"&amp;YEAR(G12)&amp;TEXT(G12,"MM")&amp;TEXT(G12,"DD")&amp;"_p"&amp;E12&amp;"_wv"&amp;TEXT(F12,"00")&amp;""</f>
@@ -3905,7 +3908,7 @@
       <c r="J12" s="2"/>
       <c r="K12" s="2"/>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A13" s="2">
         <v>6</v>
       </c>
@@ -3913,13 +3916,13 @@
         <v>0</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D13">
         <v>12</v>
       </c>
       <c r="E13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F13">
         <v>4</v>
@@ -3928,14 +3931,14 @@
         <v>44239</v>
       </c>
       <c r="H13" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="I13" t="str">
         <f t="shared" si="1"/>
         <v>nl_wk12_20210212_pB_wv04</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A14">
         <v>6</v>
       </c>
@@ -3943,13 +3946,13 @@
         <v>0</v>
       </c>
       <c r="C14" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D14">
         <v>13</v>
       </c>
       <c r="E14" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F14">
         <v>5</v>
@@ -3958,7 +3961,7 @@
         <v>44256</v>
       </c>
       <c r="H14" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="I14" t="str">
         <f t="shared" si="1"/>
@@ -3975,63 +3978,64 @@
   <dimension ref="A1:O7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.84375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.33203125" customWidth="1"/>
+    <col min="1" max="1" width="12.3046875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.3046875" customWidth="1"/>
+    <col min="4" max="4" width="12.23046875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B1" t="s">
         <v>83</v>
       </c>
-      <c r="B1" t="s">
-        <v>84</v>
-      </c>
       <c r="C1" t="s">
         <v>0</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="E1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
-        <v>3</v>
-      </c>
       <c r="F1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>7</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
+        <v>78</v>
+      </c>
+      <c r="L1" t="s">
         <v>8</v>
       </c>
-      <c r="K1" t="s">
-        <v>79</v>
-      </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>9</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>10</v>
       </c>
-      <c r="N1" t="s">
-        <v>11</v>
-      </c>
       <c r="O1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A2">
         <v>1</v>
       </c>
@@ -4039,13 +4043,13 @@
         <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D2">
         <v>1</v>
       </c>
       <c r="E2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F2">
         <v>1</v>
@@ -4054,14 +4058,14 @@
         <v>43952</v>
       </c>
       <c r="H2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I2" t="str">
         <f t="shared" ref="I2:I7" si="0">C2&amp;"_"&amp;"wk"&amp;TEXT(D2,"00")&amp;"_"&amp;YEAR(G2)&amp;TEXT(G2,"MM")&amp;TEXT(G2,"DD")&amp;"_p"&amp;E2&amp;"_wv"&amp;TEXT(F2,"00")&amp;""</f>
         <v>no_wk01_20200501_pA_wv01</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A3">
         <v>1</v>
       </c>
@@ -4069,13 +4073,13 @@
         <v>0</v>
       </c>
       <c r="C3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D3">
         <v>2</v>
       </c>
       <c r="E3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F3">
         <v>2</v>
@@ -4084,7 +4088,7 @@
         <v>43980</v>
       </c>
       <c r="H3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="I3" t="str">
         <f t="shared" si="0"/>
@@ -4094,7 +4098,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A4">
         <v>1</v>
       </c>
@@ -4102,13 +4106,13 @@
         <v>0</v>
       </c>
       <c r="C4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D4">
         <v>3</v>
       </c>
       <c r="E4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F4">
         <v>3</v>
@@ -4117,14 +4121,14 @@
         <v>44004</v>
       </c>
       <c r="H4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I4" t="str">
         <f t="shared" si="0"/>
         <v>no_wk03_20200622_pA_wv03</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A5">
         <v>1</v>
       </c>
@@ -4132,13 +4136,13 @@
         <v>0</v>
       </c>
       <c r="C5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D5">
         <v>4</v>
       </c>
       <c r="E5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F5">
         <v>4</v>
@@ -4147,7 +4151,7 @@
         <v>44043</v>
       </c>
       <c r="H5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="I5" t="str">
         <f t="shared" si="0"/>
@@ -4157,7 +4161,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A6">
         <v>1</v>
       </c>
@@ -4165,13 +4169,13 @@
         <v>0</v>
       </c>
       <c r="C6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D6">
         <v>5</v>
       </c>
       <c r="E6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F6">
         <v>5</v>
@@ -4180,7 +4184,7 @@
         <v>44080</v>
       </c>
       <c r="H6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="I6" t="str">
         <f t="shared" si="0"/>
@@ -4190,7 +4194,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A7">
         <v>1</v>
       </c>
@@ -4198,13 +4202,13 @@
         <v>0</v>
       </c>
       <c r="C7" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D7">
         <v>6</v>
       </c>
       <c r="E7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F7">
         <v>6</v>
@@ -4213,7 +4217,7 @@
         <v>44105</v>
       </c>
       <c r="H7" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="I7" t="str">
         <f t="shared" si="0"/>
@@ -4233,60 +4237,61 @@
   <dimension ref="A1:M27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E29" sqref="E29"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.84375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="7" max="7" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.23046875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.69140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="59" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="27.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="27.3046875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C1" t="s">
         <v>83</v>
       </c>
-      <c r="C1" t="s">
-        <v>84</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="D1" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="E1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
-        <v>3</v>
-      </c>
       <c r="F1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" t="s">
-        <v>7</v>
-      </c>
       <c r="J1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="K1" t="s">
+        <v>8</v>
+      </c>
+      <c r="L1" t="s">
         <v>9</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>10</v>
       </c>
-      <c r="M1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B2">
         <v>5</v>
@@ -4298,7 +4303,7 @@
         <v>1</v>
       </c>
       <c r="E2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F2">
         <v>1</v>
@@ -4307,7 +4312,7 @@
         <v>44207</v>
       </c>
       <c r="H2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="I2" t="str">
         <f>A2&amp;"_"&amp;"wk"&amp;TEXT(D2,"00")&amp;"_"&amp;YEAR(G3)&amp;TEXT(G3,"MM")&amp;TEXT(G3,"DD")&amp;"_p"&amp;E2&amp;"_wv"&amp;TEXT(F2,"00")&amp;""</f>
@@ -4317,9 +4322,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B3">
         <v>5</v>
@@ -4331,7 +4336,7 @@
         <v>1</v>
       </c>
       <c r="E3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F3">
         <v>1</v>
@@ -4340,7 +4345,7 @@
         <v>44207</v>
       </c>
       <c r="H3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="I3" t="str">
         <f t="shared" ref="I3:I27" si="0">A3&amp;"_"&amp;"wk"&amp;TEXT(D3,"00")&amp;"_"&amp;YEAR(G3)&amp;TEXT(G3,"MM")&amp;TEXT(G3,"DD")&amp;"_p"&amp;E3&amp;"_wv"&amp;TEXT(F3,"00")&amp;""</f>
@@ -4350,9 +4355,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B4">
         <v>4</v>
@@ -4364,7 +4369,7 @@
         <v>1</v>
       </c>
       <c r="E4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F4">
         <v>1</v>
@@ -4373,7 +4378,7 @@
         <v>44207</v>
       </c>
       <c r="H4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="I4" t="str">
         <f t="shared" si="0"/>
@@ -4383,9 +4388,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B5">
         <v>4</v>
@@ -4397,7 +4402,7 @@
         <v>1</v>
       </c>
       <c r="E5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F5">
         <v>1</v>
@@ -4406,7 +4411,7 @@
         <v>44207</v>
       </c>
       <c r="H5" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="I5" t="str">
         <f t="shared" si="0"/>
@@ -4416,9 +4421,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B6">
         <v>4</v>
@@ -4430,7 +4435,7 @@
         <v>1</v>
       </c>
       <c r="E6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F6">
         <v>1</v>
@@ -4439,7 +4444,7 @@
         <v>44207</v>
       </c>
       <c r="H6" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="I6" t="str">
         <f t="shared" si="0"/>
@@ -4449,9 +4454,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B7" s="2">
         <v>4</v>
@@ -4463,7 +4468,7 @@
         <v>1</v>
       </c>
       <c r="E7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F7">
         <v>1</v>
@@ -4472,7 +4477,7 @@
         <v>44207</v>
       </c>
       <c r="H7" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="I7" t="str">
         <f t="shared" si="0"/>
@@ -4482,9 +4487,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B8" s="2">
         <v>4</v>
@@ -4496,7 +4501,7 @@
         <v>1</v>
       </c>
       <c r="E8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F8">
         <v>1</v>
@@ -4505,7 +4510,7 @@
         <v>44207</v>
       </c>
       <c r="H8" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="I8" t="str">
         <f t="shared" si="0"/>
@@ -4515,9 +4520,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B9" s="2">
         <v>4</v>
@@ -4529,7 +4534,7 @@
         <v>2</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F9">
         <v>2</v>
@@ -4538,16 +4543,16 @@
         <v>44214</v>
       </c>
       <c r="H9" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="I9" t="str">
         <f t="shared" si="0"/>
         <v>at_wk02_20210118_pA_wv02</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B10" s="2">
         <v>4</v>
@@ -4559,7 +4564,7 @@
         <v>2</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F10">
         <v>2</v>
@@ -4568,16 +4573,16 @@
         <v>44214</v>
       </c>
       <c r="H10" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="I10" t="str">
         <f t="shared" si="0"/>
         <v>dk_wk02_20210118_pA_wv02</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B11" s="2">
         <v>4</v>
@@ -4589,7 +4594,7 @@
         <v>2</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F11">
         <v>2</v>
@@ -4598,16 +4603,16 @@
         <v>44214</v>
       </c>
       <c r="H11" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="I11" t="str">
         <f t="shared" si="0"/>
         <v>es_wk02_20210118_pA_wv02</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A12" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B12" s="2">
         <v>4</v>
@@ -4619,7 +4624,7 @@
         <v>2</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F12">
         <v>2</v>
@@ -4628,16 +4633,16 @@
         <v>44214</v>
       </c>
       <c r="H12" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="I12" t="str">
         <f t="shared" si="0"/>
         <v>fr_wk02_20210118_pA_wv02</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A13" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B13" s="2">
         <v>4</v>
@@ -4649,7 +4654,7 @@
         <v>2</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F13">
         <v>2</v>
@@ -4658,16 +4663,16 @@
         <v>44214</v>
       </c>
       <c r="H13" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="I13" t="str">
         <f t="shared" si="0"/>
         <v>it_wk02_20210118_pA_wv02</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A14" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B14" s="2">
         <v>4</v>
@@ -4679,7 +4684,7 @@
         <v>2</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F14">
         <v>2</v>
@@ -4688,16 +4693,16 @@
         <v>44214</v>
       </c>
       <c r="H14" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="I14" t="str">
         <f t="shared" si="0"/>
         <v>pl_wk02_20210118_pA_wv02</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A15" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B15" s="2">
         <v>4</v>
@@ -4709,7 +4714,7 @@
         <v>2</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F15">
         <v>2</v>
@@ -4718,16 +4723,16 @@
         <v>44214</v>
       </c>
       <c r="H15" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="I15" t="str">
         <f t="shared" si="0"/>
         <v>pt_wk02_20210118_pA_wv02</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A16" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B16" s="2">
         <v>4</v>
@@ -4739,7 +4744,7 @@
         <v>3</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F16" s="2">
         <v>3</v>
@@ -4748,16 +4753,16 @@
         <v>44225</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="I16" s="2" t="str">
         <f t="shared" si="0"/>
         <v>at_wk03_20210129_pA_wv03</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A17" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B17" s="2">
         <v>4</v>
@@ -4769,7 +4774,7 @@
         <v>3</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F17" s="2">
         <v>3</v>
@@ -4778,16 +4783,16 @@
         <v>44225</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="I17" s="2" t="str">
         <f t="shared" si="0"/>
         <v>dk_wk03_20210129_pA_wv03</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A18" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B18" s="2">
         <v>4</v>
@@ -4799,7 +4804,7 @@
         <v>3</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F18" s="2">
         <v>3</v>
@@ -4808,16 +4813,16 @@
         <v>44225</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="I18" s="2" t="str">
         <f t="shared" si="0"/>
         <v>es_wk03_20210129_pA_wv03</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A19" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B19" s="2">
         <v>4</v>
@@ -4829,7 +4834,7 @@
         <v>3</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F19" s="2">
         <v>3</v>
@@ -4838,16 +4843,16 @@
         <v>44225</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="I19" s="2" t="str">
         <f t="shared" si="0"/>
         <v>fr_wk03_20210129_pA_wv03</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A20" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B20" s="2">
         <v>4</v>
@@ -4859,7 +4864,7 @@
         <v>3</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F20" s="2">
         <v>3</v>
@@ -4868,16 +4873,16 @@
         <v>44225</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="I20" s="2" t="str">
         <f t="shared" si="0"/>
         <v>it_wk03_20210129_pA_wv03</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A21" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B21" s="2">
         <v>4</v>
@@ -4889,7 +4894,7 @@
         <v>3</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F21" s="2">
         <v>3</v>
@@ -4898,16 +4903,16 @@
         <v>44225</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="I21" s="2" t="str">
         <f t="shared" si="0"/>
         <v>pl_wk03_20210129_pA_wv03</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A22" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B22" s="2">
         <v>4</v>
@@ -4919,7 +4924,7 @@
         <v>3</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F22" s="2">
         <v>3</v>
@@ -4928,16 +4933,16 @@
         <v>44225</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="I22" s="2" t="str">
         <f t="shared" si="0"/>
         <v>pt_wk03_20210129_pA_wv03</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A23" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B23" s="2">
         <v>4</v>
@@ -4949,7 +4954,7 @@
         <v>1</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F23" s="4">
         <v>1</v>
@@ -4958,16 +4963,16 @@
         <v>44207</v>
       </c>
       <c r="H23" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="I23" s="4" t="str">
         <f t="shared" si="0"/>
         <v>at_wk01_20210111_pC_wv01</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A24" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B24" s="2">
         <v>4</v>
@@ -4979,7 +4984,7 @@
         <v>1</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F24" s="4">
         <v>1</v>
@@ -4988,16 +4993,16 @@
         <v>44207</v>
       </c>
       <c r="H24" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="I24" s="4" t="str">
         <f t="shared" si="0"/>
         <v>dk_wk01_20210111_pC_wv01</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A25" s="4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B25" s="2">
         <v>4</v>
@@ -5009,7 +5014,7 @@
         <v>1</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F25" s="4">
         <v>1</v>
@@ -5018,16 +5023,16 @@
         <v>44207</v>
       </c>
       <c r="H25" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="I25" s="4" t="str">
         <f t="shared" si="0"/>
         <v>fr_wk01_20210111_pC_wv01</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A26" s="4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B26" s="2">
         <v>4</v>
@@ -5039,7 +5044,7 @@
         <v>1</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F26" s="4">
         <v>1</v>
@@ -5048,16 +5053,16 @@
         <v>44207</v>
       </c>
       <c r="H26" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="I26" s="4" t="str">
         <f t="shared" si="0"/>
         <v>it_wk01_20210111_pC_wv01</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A27" s="4" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B27" s="4">
         <v>4</v>
@@ -5069,7 +5074,7 @@
         <v>1</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F27" s="4">
         <v>1</v>
@@ -5078,7 +5083,7 @@
         <v>44207</v>
       </c>
       <c r="H27" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="I27" s="4" t="str">
         <f t="shared" si="0"/>
@@ -5094,59 +5099,59 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B44EFFA-AC3D-0445-9643-71A374D3D58F}">
   <dimension ref="A1:J8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="10.5" customWidth="1"/>
-    <col min="2" max="2" width="16.6640625" customWidth="1"/>
-    <col min="3" max="3" width="8.6640625" customWidth="1"/>
-    <col min="4" max="4" width="7.33203125" customWidth="1"/>
-    <col min="5" max="5" width="8.5" customWidth="1"/>
-    <col min="6" max="6" width="9.33203125" customWidth="1"/>
-    <col min="7" max="7" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="52.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="24.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="6.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.4609375" customWidth="1"/>
+    <col min="2" max="2" width="16.69140625" customWidth="1"/>
+    <col min="3" max="3" width="8.69140625" customWidth="1"/>
+    <col min="4" max="4" width="12.23046875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.4609375" customWidth="1"/>
+    <col min="6" max="6" width="9.3046875" customWidth="1"/>
+    <col min="7" max="7" width="11.69140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="52.69140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="24.69140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="6.84375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>84</v>
-      </c>
       <c r="D1" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="2" t="s">
-        <v>3</v>
-      </c>
       <c r="F1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="2" t="s">
-        <v>7</v>
-      </c>
       <c r="J1" s="2" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A2" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B2" s="2">
         <v>4</v>
@@ -5158,7 +5163,7 @@
         <v>1</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F2" s="2">
         <v>1</v>
@@ -5167,7 +5172,7 @@
         <v>44207</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="I2" s="2" t="str">
         <f>A2&amp;"_"&amp;"wk"&amp;TEXT(D2,"00")&amp;"_"&amp;YEAR(G3)&amp;TEXT(G3,"MM")&amp;TEXT(G3,"DD")&amp;"_p"&amp;E2&amp;"_wv"&amp;TEXT(F2,"00")&amp;""</f>
@@ -5175,9 +5180,9 @@
       </c>
       <c r="J2" s="2"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B3" s="2">
         <v>4</v>
@@ -5189,7 +5194,7 @@
         <v>1</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F3" s="2">
         <v>1</v>
@@ -5198,7 +5203,7 @@
         <v>44208</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="I3" s="2" t="str">
         <f t="shared" ref="I3:I4" si="0">A3&amp;"_"&amp;"wk"&amp;TEXT(D3,"00")&amp;"_"&amp;YEAR(G4)&amp;TEXT(G4,"MM")&amp;TEXT(G4,"DD")&amp;"_p"&amp;E3&amp;"_wv"&amp;TEXT(F3,"00")&amp;""</f>
@@ -5206,9 +5211,9 @@
       </c>
       <c r="J3" s="2"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B4" s="2">
         <v>4</v>
@@ -5220,7 +5225,7 @@
         <v>1</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F4" s="2">
         <v>1</v>
@@ -5229,7 +5234,7 @@
         <v>44209</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="I4" s="2" t="str">
         <f t="shared" si="0"/>
@@ -5237,9 +5242,9 @@
       </c>
       <c r="J4" s="2"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A5" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B5" s="4">
         <v>4</v>
@@ -5251,7 +5256,7 @@
         <v>1</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F5" s="2">
         <v>1</v>
@@ -5260,16 +5265,16 @@
         <v>44208</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="I5" s="4" t="str">
         <f t="shared" ref="I5:I7" si="1">A5&amp;"_"&amp;"wk"&amp;TEXT(D5,"00")&amp;"_"&amp;YEAR(G5)&amp;TEXT(G5,"MM")&amp;TEXT(G5,"DD")&amp;"_p"&amp;E5&amp;"_wv"&amp;TEXT(F5,"00")&amp;""</f>
         <v>fi_wk01_20210112_pC_wv01</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A6" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B6" s="4">
         <v>4</v>
@@ -5281,7 +5286,7 @@
         <v>1</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F6" s="2">
         <v>1</v>
@@ -5290,16 +5295,16 @@
         <v>44209</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="I6" s="4" t="str">
         <f t="shared" si="1"/>
         <v>ch_wk01_20210113_pC_wv01</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A7" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B7" s="4">
         <v>4</v>
@@ -5311,7 +5316,7 @@
         <v>1</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F7" s="2">
         <v>1</v>
@@ -5320,16 +5325,16 @@
         <v>44209</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="I7" s="4" t="str">
         <f t="shared" si="1"/>
         <v>gr_wk01_20210113_pC_wv01</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A8" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B8" s="4">
         <v>4</v>
@@ -5341,7 +5346,7 @@
         <v>1</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F8" s="2">
         <v>1</v>
@@ -5350,7 +5355,7 @@
         <v>44207</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="I8" s="4" t="str">
         <f>A8&amp;"_"&amp;"wk"&amp;TEXT(D8,"00")&amp;"_"&amp;YEAR(G8)&amp;TEXT(G8,"MM")&amp;TEXT(G8,"DD")&amp;"_p"&amp;E8&amp;"_wv"&amp;TEXT(F8,"00")&amp;""</f>
@@ -5370,11 +5375,11 @@
       <selection activeCell="O21" sqref="O21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.84375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Change wk to sr in data
</commit_message>
<xml_diff>
--- a/data/spss_files.xlsx
+++ b/data/spss_files.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jarvisc1\Documents\projects\comix_data_clean\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA1E20A5-EE18-4871-8090-18695E7B5DB9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E68AC4B-1435-4344-B387-8EF398144E00}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18120" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18120" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="5" r:id="rId1"/>
@@ -860,8 +860,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O56"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I3" sqref="I3:I56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.84375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -947,8 +947,8 @@
         <v>13</v>
       </c>
       <c r="I2" t="str">
-        <f t="shared" ref="I2:I56" si="0">C2&amp;"_"&amp;"wk"&amp;TEXT(D2,"00")&amp;"_"&amp;YEAR(G2)&amp;TEXT(G2,"MM")&amp;TEXT(G2,"DD")&amp;"_p"&amp;E2&amp;"_wv"&amp;TEXT(F2,"00")&amp;""</f>
-        <v>uk_wk01_20200402_pA_wv01</v>
+        <f>C2&amp;"_"&amp;"sr"&amp;TEXT(D2,"00")&amp;"_"&amp;YEAR(G2)&amp;TEXT(G2,"MM")&amp;TEXT(G2,"DD")&amp;"_p"&amp;E2&amp;"_wv"&amp;TEXT(F2,"00")&amp;""</f>
+        <v>uk_sr01_20200402_pA_wv01</v>
       </c>
       <c r="J2">
         <v>1</v>
@@ -982,9 +982,9 @@
       <c r="H3" t="s">
         <v>15</v>
       </c>
-      <c r="I3" t="str">
-        <f t="shared" si="0"/>
-        <v>uk_wk02_20200214_pB_wv01</v>
+      <c r="I3" s="2" t="str">
+        <f t="shared" ref="I3:I56" si="0">C3&amp;"_"&amp;"sr"&amp;TEXT(D3,"00")&amp;"_"&amp;YEAR(G3)&amp;TEXT(G3,"MM")&amp;TEXT(G3,"DD")&amp;"_p"&amp;E3&amp;"_wv"&amp;TEXT(F3,"00")&amp;""</f>
+        <v>uk_sr02_20200214_pB_wv01</v>
       </c>
       <c r="J3">
         <v>1</v>
@@ -1018,9 +1018,9 @@
       <c r="H4" t="s">
         <v>16</v>
       </c>
-      <c r="I4" t="str">
-        <f t="shared" si="0"/>
-        <v>uk_wk03_20200513_pA_wv02</v>
+      <c r="I4" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>uk_sr03_20200513_pA_wv02</v>
       </c>
       <c r="J4">
         <v>1</v>
@@ -1054,9 +1054,9 @@
       <c r="H5" t="s">
         <v>17</v>
       </c>
-      <c r="I5" t="str">
-        <f t="shared" si="0"/>
-        <v>uk_wk04_20200427_pB_wv02</v>
+      <c r="I5" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>uk_sr04_20200427_pB_wv02</v>
       </c>
       <c r="J5">
         <v>1</v>
@@ -1090,9 +1090,9 @@
       <c r="H6" t="s">
         <v>18</v>
       </c>
-      <c r="I6" t="str">
-        <f t="shared" si="0"/>
-        <v>uk_wk05_20200428_pA_wv03</v>
+      <c r="I6" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>uk_sr05_20200428_pA_wv03</v>
       </c>
       <c r="J6">
         <v>1</v>
@@ -1126,9 +1126,9 @@
       <c r="H7" t="s">
         <v>19</v>
       </c>
-      <c r="I7" t="str">
-        <f t="shared" si="0"/>
-        <v>uk_wk06_20200512_pB_wv03</v>
+      <c r="I7" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>uk_sr06_20200512_pB_wv03</v>
       </c>
       <c r="J7">
         <v>1</v>
@@ -1162,9 +1162,9 @@
       <c r="H8" t="s">
         <v>21</v>
       </c>
-      <c r="I8" t="str">
-        <f t="shared" si="0"/>
-        <v>uk_wk07_20200513_pA_wv04</v>
+      <c r="I8" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>uk_sr07_20200513_pA_wv04</v>
       </c>
       <c r="J8">
         <v>1</v>
@@ -1201,9 +1201,9 @@
       <c r="H9" t="s">
         <v>23</v>
       </c>
-      <c r="I9" t="str">
-        <f t="shared" si="0"/>
-        <v>uk_wk07_20200519_pC_wv01</v>
+      <c r="I9" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>uk_sr07_20200519_pC_wv01</v>
       </c>
       <c r="J9">
         <v>1</v>
@@ -1238,9 +1238,9 @@
       <c r="H10" t="s">
         <v>24</v>
       </c>
-      <c r="I10" t="str">
-        <f t="shared" si="0"/>
-        <v>uk_wk08_20200522_pB_wv04</v>
+      <c r="I10" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>uk_sr08_20200522_pB_wv04</v>
       </c>
       <c r="J10">
         <v>1</v>
@@ -1275,9 +1275,9 @@
       <c r="H11" t="s">
         <v>26</v>
       </c>
-      <c r="I11" t="str">
-        <f t="shared" si="0"/>
-        <v>uk_wk08_20200611_pD_wv01</v>
+      <c r="I11" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>uk_sr08_20200611_pD_wv01</v>
       </c>
       <c r="J11">
         <v>1</v>
@@ -1312,9 +1312,9 @@
       <c r="H12" t="s">
         <v>27</v>
       </c>
-      <c r="I12" t="str">
-        <f t="shared" si="0"/>
-        <v>uk_wk09_20200529_pA_wv05</v>
+      <c r="I12" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>uk_sr09_20200529_pA_wv05</v>
       </c>
       <c r="J12">
         <v>1</v>
@@ -1350,9 +1350,9 @@
       <c r="H13" t="s">
         <v>28</v>
       </c>
-      <c r="I13" t="str">
-        <f t="shared" si="0"/>
-        <v>uk_wk09_20200528_pC_wv02</v>
+      <c r="I13" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>uk_sr09_20200528_pC_wv02</v>
       </c>
       <c r="J13">
         <v>1</v>
@@ -1387,9 +1387,9 @@
       <c r="H14" t="s">
         <v>29</v>
       </c>
-      <c r="I14" t="str">
-        <f t="shared" si="0"/>
-        <v>uk_wk10_20200604_pB_wv05</v>
+      <c r="I14" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>uk_sr10_20200604_pB_wv05</v>
       </c>
       <c r="J14">
         <v>1</v>
@@ -1424,9 +1424,9 @@
       <c r="H15" t="s">
         <v>30</v>
       </c>
-      <c r="I15" t="str">
-        <f t="shared" si="0"/>
-        <v>uk_wk10_20200608_pD_wv02</v>
+      <c r="I15" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>uk_sr10_20200608_pD_wv02</v>
       </c>
       <c r="J15">
         <v>1</v>
@@ -1461,9 +1461,9 @@
       <c r="H16" t="s">
         <v>31</v>
       </c>
-      <c r="I16" t="str">
-        <f t="shared" si="0"/>
-        <v>uk_wk11_20200612_pA_wv06</v>
+      <c r="I16" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>uk_sr11_20200612_pA_wv06</v>
       </c>
       <c r="J16">
         <v>1</v>
@@ -1498,9 +1498,9 @@
       <c r="H17" t="s">
         <v>32</v>
       </c>
-      <c r="I17" t="str">
-        <f t="shared" si="0"/>
-        <v>uk_wk11_20200612_pC_wv03</v>
+      <c r="I17" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>uk_sr11_20200612_pC_wv03</v>
       </c>
       <c r="J17">
         <v>1</v>
@@ -1535,9 +1535,9 @@
       <c r="H18" t="s">
         <v>33</v>
       </c>
-      <c r="I18" t="str">
-        <f t="shared" si="0"/>
-        <v>uk_wk12_20200619_pB_wv06</v>
+      <c r="I18" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>uk_sr12_20200619_pB_wv06</v>
       </c>
       <c r="J18">
         <v>1</v>
@@ -1572,9 +1572,9 @@
       <c r="H19" t="s">
         <v>34</v>
       </c>
-      <c r="I19" t="str">
-        <f t="shared" si="0"/>
-        <v>uk_wk12_20200619_pD_wv03</v>
+      <c r="I19" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>uk_sr12_20200619_pD_wv03</v>
       </c>
       <c r="J19">
         <v>1</v>
@@ -1609,9 +1609,9 @@
       <c r="H20" t="s">
         <v>35</v>
       </c>
-      <c r="I20" t="str">
-        <f t="shared" si="0"/>
-        <v>uk_wk13_20200625_pA_wv07</v>
+      <c r="I20" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>uk_sr13_20200625_pA_wv07</v>
       </c>
       <c r="J20">
         <v>1</v>
@@ -1646,9 +1646,9 @@
       <c r="H21" t="s">
         <v>36</v>
       </c>
-      <c r="I21" t="str">
-        <f t="shared" si="0"/>
-        <v>uk_wk13_20200625_pC_wv04</v>
+      <c r="I21" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>uk_sr13_20200625_pC_wv04</v>
       </c>
       <c r="J21">
         <v>1</v>
@@ -1683,9 +1683,9 @@
       <c r="H22" t="s">
         <v>37</v>
       </c>
-      <c r="I22" t="str">
-        <f t="shared" si="0"/>
-        <v>uk_wk14_20200702_pB_wv07</v>
+      <c r="I22" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>uk_sr14_20200702_pB_wv07</v>
       </c>
       <c r="J22">
         <v>1</v>
@@ -1720,9 +1720,9 @@
       <c r="H23" t="s">
         <v>38</v>
       </c>
-      <c r="I23" t="str">
-        <f t="shared" si="0"/>
-        <v>uk_wk14_20200703_pD_wv04</v>
+      <c r="I23" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>uk_sr14_20200703_pD_wv04</v>
       </c>
       <c r="J23">
         <v>1</v>
@@ -1757,9 +1757,9 @@
       <c r="H24" t="s">
         <v>39</v>
       </c>
-      <c r="I24" t="str">
-        <f t="shared" si="0"/>
-        <v>uk_wk15_20200710_pA_wv08</v>
+      <c r="I24" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>uk_sr15_20200710_pA_wv08</v>
       </c>
       <c r="J24">
         <v>1</v>
@@ -1794,9 +1794,9 @@
       <c r="H25" t="s">
         <v>40</v>
       </c>
-      <c r="I25" t="str">
-        <f t="shared" si="0"/>
-        <v>uk_wk15_20200709_pC_wv05</v>
+      <c r="I25" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>uk_sr15_20200709_pC_wv05</v>
       </c>
       <c r="J25">
         <v>1</v>
@@ -1831,9 +1831,9 @@
       <c r="H26" t="s">
         <v>41</v>
       </c>
-      <c r="I26" t="str">
-        <f t="shared" si="0"/>
-        <v>uk_wk16_20200717_pB_wv08</v>
+      <c r="I26" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>uk_sr16_20200717_pB_wv08</v>
       </c>
       <c r="J26">
         <v>1</v>
@@ -1868,9 +1868,9 @@
       <c r="H27" t="s">
         <v>42</v>
       </c>
-      <c r="I27" t="str">
-        <f t="shared" si="0"/>
-        <v>uk_wk16_20200717_pD_wv05</v>
+      <c r="I27" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>uk_sr16_20200717_pD_wv05</v>
       </c>
       <c r="J27">
         <v>1</v>
@@ -1905,9 +1905,9 @@
       <c r="H28" t="s">
         <v>44</v>
       </c>
-      <c r="I28" t="str">
-        <f t="shared" si="0"/>
-        <v>uk_wk17_20200724_pA_wv09</v>
+      <c r="I28" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>uk_sr17_20200724_pA_wv09</v>
       </c>
       <c r="J28">
         <v>1</v>
@@ -1945,9 +1945,9 @@
       <c r="H29" t="s">
         <v>45</v>
       </c>
-      <c r="I29" t="str">
-        <f t="shared" si="0"/>
-        <v>uk_wk18_20200731_pB_wv09</v>
+      <c r="I29" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>uk_sr18_20200731_pB_wv09</v>
       </c>
       <c r="J29">
         <v>1</v>
@@ -1985,9 +1985,9 @@
       <c r="H30" t="s">
         <v>46</v>
       </c>
-      <c r="I30" t="str">
-        <f t="shared" si="0"/>
-        <v>uk_wk19_20200807_pA_wv10</v>
+      <c r="I30" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>uk_sr19_20200807_pA_wv10</v>
       </c>
       <c r="J30">
         <v>1</v>
@@ -2021,9 +2021,9 @@
       <c r="H31" t="s">
         <v>47</v>
       </c>
-      <c r="I31" t="str">
-        <f t="shared" si="0"/>
-        <v>uk_wk19_20200810_pC_wv06</v>
+      <c r="I31" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>uk_sr19_20200810_pC_wv06</v>
       </c>
       <c r="J31">
         <v>1</v>
@@ -2057,9 +2057,9 @@
       <c r="H32" t="s">
         <v>50</v>
       </c>
-      <c r="I32" t="str">
-        <f t="shared" si="0"/>
-        <v>uk_wk20_20200821_pE_wv01</v>
+      <c r="I32" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>uk_sr20_20200821_pE_wv01</v>
       </c>
       <c r="J32">
         <v>1</v>
@@ -2096,9 +2096,9 @@
       <c r="H33" t="s">
         <v>52</v>
       </c>
-      <c r="I33" t="str">
-        <f t="shared" si="0"/>
-        <v>uk_wk21_20200827_pF_wv01</v>
+      <c r="I33" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>uk_sr21_20200827_pF_wv01</v>
       </c>
       <c r="J33">
         <v>1</v>
@@ -2133,9 +2133,9 @@
       <c r="H34" t="s">
         <v>53</v>
       </c>
-      <c r="I34" t="str">
-        <f t="shared" si="0"/>
-        <v>uk_wk22_20200903_pE_wv02</v>
+      <c r="I34" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>uk_sr22_20200903_pE_wv02</v>
       </c>
       <c r="J34">
         <v>1</v>
@@ -2170,9 +2170,9 @@
       <c r="H35" t="s">
         <v>54</v>
       </c>
-      <c r="I35" t="str">
-        <f t="shared" si="0"/>
-        <v>uk_wk23_20200907_pF_wv02</v>
+      <c r="I35" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>uk_sr23_20200907_pF_wv02</v>
       </c>
       <c r="J35">
         <v>1</v>
@@ -2207,9 +2207,9 @@
       <c r="H36" t="s">
         <v>55</v>
       </c>
-      <c r="I36" t="str">
-        <f t="shared" si="0"/>
-        <v>uk_wk24_20200914_pE_wv03</v>
+      <c r="I36" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>uk_sr24_20200914_pE_wv03</v>
       </c>
       <c r="J36">
         <v>1</v>
@@ -2244,9 +2244,9 @@
       <c r="H37" t="s">
         <v>56</v>
       </c>
-      <c r="I37" t="str">
-        <f t="shared" si="0"/>
-        <v>uk_wk25_20200918_pF_wv03</v>
+      <c r="I37" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>uk_sr25_20200918_pF_wv03</v>
       </c>
       <c r="J37">
         <v>1</v>
@@ -2281,9 +2281,9 @@
       <c r="H38" t="s">
         <v>57</v>
       </c>
-      <c r="I38" t="str">
-        <f t="shared" si="0"/>
-        <v>uk_wk26_20200925_pE_wv04</v>
+      <c r="I38" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>uk_sr26_20200925_pE_wv04</v>
       </c>
       <c r="J38">
         <v>1</v>
@@ -2318,9 +2318,9 @@
       <c r="H39" t="s">
         <v>58</v>
       </c>
-      <c r="I39" t="str">
-        <f t="shared" si="0"/>
-        <v>uk_wk27_20201002_pF_wv04</v>
+      <c r="I39" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>uk_sr27_20201002_pF_wv04</v>
       </c>
       <c r="J39">
         <v>1</v>
@@ -2355,9 +2355,9 @@
       <c r="H40" t="s">
         <v>59</v>
       </c>
-      <c r="I40" t="str">
-        <f t="shared" si="0"/>
-        <v>uk_wk28_20201009_pE_wv05</v>
+      <c r="I40" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>uk_sr28_20201009_pE_wv05</v>
       </c>
       <c r="J40">
         <v>1</v>
@@ -2392,9 +2392,9 @@
       <c r="H41" t="s">
         <v>60</v>
       </c>
-      <c r="I41" t="str">
-        <f t="shared" si="0"/>
-        <v>uk_wk29_20201018_pF_wv05</v>
+      <c r="I41" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>uk_sr29_20201018_pF_wv05</v>
       </c>
       <c r="J41">
         <v>1</v>
@@ -2429,9 +2429,9 @@
       <c r="H42" t="s">
         <v>61</v>
       </c>
-      <c r="I42" t="str">
-        <f t="shared" si="0"/>
-        <v>uk_wk30_20201023_pE_wv06</v>
+      <c r="I42" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>uk_sr30_20201023_pE_wv06</v>
       </c>
       <c r="J42">
         <v>1</v>
@@ -2466,9 +2466,9 @@
       <c r="H43" t="s">
         <v>62</v>
       </c>
-      <c r="I43" t="str">
-        <f t="shared" si="0"/>
-        <v>uk_wk31_20201030_pF_wv06</v>
+      <c r="I43" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>uk_sr31_20201030_pF_wv06</v>
       </c>
       <c r="J43">
         <v>1</v>
@@ -2503,9 +2503,9 @@
       <c r="H44" t="s">
         <v>81</v>
       </c>
-      <c r="I44" t="str">
-        <f t="shared" si="0"/>
-        <v>uk_wk32_20201106_pE_wv07</v>
+      <c r="I44" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>uk_sr32_20201106_pE_wv07</v>
       </c>
       <c r="J44">
         <v>1</v>
@@ -2537,9 +2537,9 @@
       <c r="H45" t="s">
         <v>84</v>
       </c>
-      <c r="I45" t="str">
-        <f t="shared" si="0"/>
-        <v>uk_wk33_20201113_pF_wv07</v>
+      <c r="I45" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>uk_sr33_20201113_pF_wv07</v>
       </c>
       <c r="J45">
         <v>1</v>
@@ -2574,9 +2574,9 @@
       <c r="H46" t="s">
         <v>85</v>
       </c>
-      <c r="I46" t="str">
-        <f t="shared" si="0"/>
-        <v>uk_wk34_20201120_pE_wv08</v>
+      <c r="I46" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>uk_sr34_20201120_pE_wv08</v>
       </c>
       <c r="J46">
         <v>1</v>
@@ -2611,9 +2611,9 @@
       <c r="H47" t="s">
         <v>86</v>
       </c>
-      <c r="I47" t="str">
-        <f t="shared" si="0"/>
-        <v>uk_wk35_20201126_pF_wv08</v>
+      <c r="I47" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>uk_sr35_20201126_pF_wv08</v>
       </c>
       <c r="J47">
         <v>1</v>
@@ -2648,9 +2648,9 @@
       <c r="H48" t="s">
         <v>87</v>
       </c>
-      <c r="I48" t="str">
-        <f t="shared" si="0"/>
-        <v>uk_wk36_20200403_pE_wv09</v>
+      <c r="I48" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>uk_sr36_20200403_pE_wv09</v>
       </c>
       <c r="J48">
         <v>1</v>
@@ -2682,9 +2682,9 @@
       <c r="H49" t="s">
         <v>88</v>
       </c>
-      <c r="I49" t="str">
-        <f t="shared" si="0"/>
-        <v>uk_wk37_20200211_pF_wv09</v>
+      <c r="I49" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>uk_sr37_20200211_pF_wv09</v>
       </c>
       <c r="J49">
         <v>1</v>
@@ -2716,9 +2716,9 @@
       <c r="H50" t="s">
         <v>89</v>
       </c>
-      <c r="I50" t="str">
-        <f t="shared" si="0"/>
-        <v>uk_wk38_20201217_pE_wv10</v>
+      <c r="I50" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>uk_sr38_20201217_pE_wv10</v>
       </c>
       <c r="J50">
         <v>1</v>
@@ -2750,9 +2750,9 @@
       <c r="H51" t="s">
         <v>90</v>
       </c>
-      <c r="I51" t="str">
-        <f t="shared" si="0"/>
-        <v>uk_wk39_20201224_pF_wv10</v>
+      <c r="I51" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>uk_sr39_20201224_pF_wv10</v>
       </c>
       <c r="J51">
         <v>1</v>
@@ -2784,9 +2784,9 @@
       <c r="H52" t="s">
         <v>91</v>
       </c>
-      <c r="I52" t="str">
-        <f t="shared" si="0"/>
-        <v>uk_wk40_20201231_pE_wv11</v>
+      <c r="I52" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>uk_sr40_20201231_pE_wv11</v>
       </c>
       <c r="J52">
         <v>1</v>
@@ -2818,9 +2818,9 @@
       <c r="H53" t="s">
         <v>96</v>
       </c>
-      <c r="I53" t="str">
-        <f t="shared" si="0"/>
-        <v>uk_wk41_20210107_pF_wv11</v>
+      <c r="I53" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>uk_sr41_20210107_pF_wv11</v>
       </c>
       <c r="J53">
         <v>1</v>
@@ -2852,9 +2852,9 @@
       <c r="H54" t="s">
         <v>111</v>
       </c>
-      <c r="I54" t="str">
-        <f t="shared" si="0"/>
-        <v>uk_wk42_20210114_pE_wv12</v>
+      <c r="I54" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>uk_sr42_20210114_pE_wv12</v>
       </c>
       <c r="J54">
         <v>1</v>
@@ -2886,9 +2886,9 @@
       <c r="H55" t="s">
         <v>115</v>
       </c>
-      <c r="I55" t="str">
-        <f t="shared" si="0"/>
-        <v>uk_wk43_20210120_pF_wv12</v>
+      <c r="I55" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>uk_sr43_20210120_pF_wv12</v>
       </c>
       <c r="J55">
         <v>1</v>
@@ -2922,7 +2922,7 @@
       </c>
       <c r="I56" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>uk_wk44_20210128_pE_wv13</v>
+        <v>uk_sr44_20210128_pE_wv13</v>
       </c>
       <c r="J56">
         <v>1</v>
@@ -2938,7 +2938,7 @@
   <dimension ref="A1:N17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="I3" sqref="I3:I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.84375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -3022,8 +3022,8 @@
         <v>64</v>
       </c>
       <c r="I2" t="str">
-        <f t="shared" ref="I2:I16" si="0">A2&amp;"_"&amp;"wk"&amp;TEXT(D2,"00")&amp;"_"&amp;YEAR(G2)&amp;TEXT(G2,"MM")&amp;TEXT(G2,"DD")&amp;"_p"&amp;E2&amp;"_wv"&amp;TEXT(F2,"00")&amp;""</f>
-        <v>be_wk01_20200429_pA_wv01</v>
+        <f>A2&amp;"_"&amp;"sr"&amp;TEXT(D2,"00")&amp;"_"&amp;YEAR(G2)&amp;TEXT(G2,"MM")&amp;TEXT(G2,"DD")&amp;"_p"&amp;E2&amp;"_wv"&amp;TEXT(F2,"00")&amp;""</f>
+        <v>be_sr01_20200429_pA_wv01</v>
       </c>
       <c r="J2">
         <v>1</v>
@@ -3054,9 +3054,9 @@
       <c r="H3" t="s">
         <v>65</v>
       </c>
-      <c r="I3" t="str">
-        <f t="shared" si="0"/>
-        <v>be_wk02_20200518_pA_wv02</v>
+      <c r="I3" s="2" t="str">
+        <f t="shared" ref="I3:I17" si="0">A3&amp;"_"&amp;"sr"&amp;TEXT(D3,"00")&amp;"_"&amp;YEAR(G3)&amp;TEXT(G3,"MM")&amp;TEXT(G3,"DD")&amp;"_p"&amp;E3&amp;"_wv"&amp;TEXT(F3,"00")&amp;""</f>
+        <v>be_sr02_20200518_pA_wv02</v>
       </c>
       <c r="J3">
         <v>1</v>
@@ -3087,9 +3087,9 @@
       <c r="H4" t="s">
         <v>66</v>
       </c>
-      <c r="I4" t="str">
-        <f t="shared" si="0"/>
-        <v>be_wk03_20200601_pA_wv03</v>
+      <c r="I4" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>be_sr03_20200601_pA_wv03</v>
       </c>
       <c r="J4">
         <v>1</v>
@@ -3120,9 +3120,9 @@
       <c r="H5" t="s">
         <v>67</v>
       </c>
-      <c r="I5" t="str">
-        <f t="shared" si="0"/>
-        <v>be_wk04_20200612_pA_wv04</v>
+      <c r="I5" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>be_sr04_20200612_pA_wv04</v>
       </c>
       <c r="J5">
         <v>1</v>
@@ -3153,9 +3153,9 @@
       <c r="H6" t="s">
         <v>68</v>
       </c>
-      <c r="I6" t="str">
-        <f t="shared" si="0"/>
-        <v>be_wk05_20200626_pA_wv05</v>
+      <c r="I6" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>be_sr05_20200626_pA_wv05</v>
       </c>
       <c r="J6">
         <v>1</v>
@@ -3186,9 +3186,9 @@
       <c r="H7" t="s">
         <v>69</v>
       </c>
-      <c r="I7" t="str">
-        <f t="shared" si="0"/>
-        <v>be_wk06_20200710_pA_wv06</v>
+      <c r="I7" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>be_sr06_20200710_pA_wv06</v>
       </c>
       <c r="J7">
         <v>1</v>
@@ -3219,9 +3219,9 @@
       <c r="H8" t="s">
         <v>70</v>
       </c>
-      <c r="I8" t="str">
-        <f t="shared" si="0"/>
-        <v>be_wk07_20200724_pA_wv07</v>
+      <c r="I8" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>be_sr07_20200724_pA_wv07</v>
       </c>
       <c r="J8">
         <v>1</v>
@@ -3252,9 +3252,9 @@
       <c r="H9" t="s">
         <v>71</v>
       </c>
-      <c r="I9" t="str">
-        <f t="shared" si="0"/>
-        <v>be_wk08_20200806_pA_wv08</v>
+      <c r="I9" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>be_sr08_20200806_pA_wv08</v>
       </c>
       <c r="J9">
         <v>1</v>
@@ -3283,7 +3283,7 @@
       <c r="H10" s="2"/>
       <c r="I10" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>be_wk09_20201120_pB_wv01</v>
+        <v>be_sr09_20201120_pB_wv01</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.4">
@@ -3307,7 +3307,7 @@
       <c r="H11" s="2"/>
       <c r="I11" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>be_wk10_19000100_pB_wv02</v>
+        <v>be_sr10_19000100_pB_wv02</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.4">
@@ -3331,7 +3331,7 @@
       <c r="H12" s="2"/>
       <c r="I12" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>be_wk11_19000100_pB_wv03</v>
+        <v>be_sr11_19000100_pB_wv03</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.4">
@@ -3361,7 +3361,7 @@
       </c>
       <c r="I13" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>be_wk12_20210111_pB_wv04</v>
+        <v>be_sr12_20210111_pB_wv04</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.4">
@@ -3391,7 +3391,7 @@
       </c>
       <c r="I14" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>be_wk13_20210120_pB_wv05</v>
+        <v>be_sr13_20210120_pB_wv05</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.4">
@@ -3420,8 +3420,8 @@
         <v>123</v>
       </c>
       <c r="I15" s="2" t="str">
-        <f>A15&amp;"_"&amp;"wk"&amp;TEXT(D15,"00")&amp;"_"&amp;YEAR(G15)&amp;TEXT(G15,"MM")&amp;TEXT(G15,"DD")&amp;"_p"&amp;E15&amp;"_wv"&amp;TEXT(F15,"00")&amp;""</f>
-        <v>be_wk14_20210127_pB_wv06</v>
+        <f t="shared" si="0"/>
+        <v>be_sr14_20210127_pB_wv06</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.4">
@@ -3449,9 +3449,9 @@
       <c r="H16" t="s">
         <v>129</v>
       </c>
-      <c r="I16" t="str">
-        <f t="shared" si="0"/>
-        <v>be_wk15_20210222_pB_wv07</v>
+      <c r="I16" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>be_sr15_20210222_pB_wv07</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.4">
@@ -3480,8 +3480,8 @@
         <v>135</v>
       </c>
       <c r="I17" s="2" t="str">
-        <f>A17&amp;"_"&amp;"wk"&amp;TEXT(D17,"00")&amp;"_"&amp;YEAR(G17)&amp;TEXT(G17,"MM")&amp;TEXT(G17,"DD")&amp;"_p"&amp;E17&amp;"_wv"&amp;TEXT(F17,"00")&amp;""</f>
-        <v>be_wk16_20210226_pB_wv08</v>
+        <f t="shared" si="0"/>
+        <v>be_sr16_20210226_pB_wv08</v>
       </c>
     </row>
   </sheetData>
@@ -3495,7 +3495,7 @@
   <dimension ref="A1:O14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="I3" sqref="I3:I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.84375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -3578,8 +3578,8 @@
         <v>64</v>
       </c>
       <c r="I2" t="str">
-        <f t="shared" ref="I2:I11" si="0">C2&amp;"_"&amp;"wk"&amp;TEXT(D2,"00")&amp;"_"&amp;YEAR(G2)&amp;TEXT(G2,"MM")&amp;TEXT(G2,"DD")&amp;"_p"&amp;E2&amp;"_wv"&amp;TEXT(F2,"00")&amp;""</f>
-        <v>nl_wk01_20200429_pA_wv01</v>
+        <f>C2&amp;"_"&amp;"sr"&amp;TEXT(D2,"00")&amp;"_"&amp;YEAR(G2)&amp;TEXT(G2,"MM")&amp;TEXT(G2,"DD")&amp;"_p"&amp;E2&amp;"_wv"&amp;TEXT(F2,"00")&amp;""</f>
+        <v>nl_sr01_20200429_pA_wv01</v>
       </c>
       <c r="K2">
         <v>1</v>
@@ -3610,9 +3610,9 @@
       <c r="H3" t="s">
         <v>65</v>
       </c>
-      <c r="I3" t="str">
-        <f t="shared" si="0"/>
-        <v>nl_wk02_20200518_pA_wv02</v>
+      <c r="I3" s="2" t="str">
+        <f t="shared" ref="I3:I14" si="0">C3&amp;"_"&amp;"sr"&amp;TEXT(D3,"00")&amp;"_"&amp;YEAR(G3)&amp;TEXT(G3,"MM")&amp;TEXT(G3,"DD")&amp;"_p"&amp;E3&amp;"_wv"&amp;TEXT(F3,"00")&amp;""</f>
+        <v>nl_sr02_20200518_pA_wv02</v>
       </c>
       <c r="K3">
         <v>1</v>
@@ -3643,9 +3643,9 @@
       <c r="H4" t="s">
         <v>66</v>
       </c>
-      <c r="I4" t="str">
-        <f t="shared" si="0"/>
-        <v>nl_wk03_20200601_pA_wv03</v>
+      <c r="I4" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>nl_sr03_20200601_pA_wv03</v>
       </c>
       <c r="K4">
         <v>1</v>
@@ -3676,9 +3676,9 @@
       <c r="H5" t="s">
         <v>67</v>
       </c>
-      <c r="I5" t="str">
-        <f t="shared" si="0"/>
-        <v>nl_wk04_20200612_pA_wv04</v>
+      <c r="I5" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>nl_sr04_20200612_pA_wv04</v>
       </c>
       <c r="K5">
         <v>1</v>
@@ -3709,9 +3709,9 @@
       <c r="H6" t="s">
         <v>68</v>
       </c>
-      <c r="I6" t="str">
-        <f t="shared" si="0"/>
-        <v>nl_wk05_20200626_pA_wv05</v>
+      <c r="I6" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>nl_sr05_20200626_pA_wv05</v>
       </c>
       <c r="K6">
         <v>1</v>
@@ -3742,9 +3742,9 @@
       <c r="H7" t="s">
         <v>69</v>
       </c>
-      <c r="I7" t="str">
-        <f t="shared" si="0"/>
-        <v>nl_wk06_20200710_pA_wv06</v>
+      <c r="I7" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>nl_sr06_20200710_pA_wv06</v>
       </c>
       <c r="K7">
         <v>1</v>
@@ -3775,9 +3775,9 @@
       <c r="H8" t="s">
         <v>70</v>
       </c>
-      <c r="I8" t="str">
-        <f t="shared" si="0"/>
-        <v>nl_wk07_20200724_pA_wv07</v>
+      <c r="I8" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>nl_sr07_20200724_pA_wv07</v>
       </c>
       <c r="K8">
         <v>1</v>
@@ -3808,9 +3808,9 @@
       <c r="H9" t="s">
         <v>71</v>
       </c>
-      <c r="I9" t="str">
-        <f t="shared" si="0"/>
-        <v>nl_wk08_20200806_pA_wv08</v>
+      <c r="I9" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>nl_sr08_20200806_pA_wv08</v>
       </c>
       <c r="K9">
         <v>1</v>
@@ -3841,9 +3841,9 @@
       <c r="H10" t="s">
         <v>128</v>
       </c>
-      <c r="I10" t="str">
-        <f t="shared" si="0"/>
-        <v>nl_wk09_20210107_pB_wv01</v>
+      <c r="I10" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>nl_sr09_20210107_pB_wv01</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.4">
@@ -3871,9 +3871,9 @@
       <c r="H11" t="s">
         <v>127</v>
       </c>
-      <c r="I11" t="str">
-        <f t="shared" si="0"/>
-        <v>nl_wk10_20210118_pB_wv02</v>
+      <c r="I11" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>nl_sr10_20210118_pB_wv02</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.4">
@@ -3902,8 +3902,8 @@
         <v>130</v>
       </c>
       <c r="I12" s="2" t="str">
-        <f t="shared" ref="I12:I14" si="1">C12&amp;"_"&amp;"wk"&amp;TEXT(D12,"00")&amp;"_"&amp;YEAR(G12)&amp;TEXT(G12,"MM")&amp;TEXT(G12,"DD")&amp;"_p"&amp;E12&amp;"_wv"&amp;TEXT(F12,"00")&amp;""</f>
-        <v>nl_wk11_20210202_pB_wv03</v>
+        <f t="shared" si="0"/>
+        <v>nl_sr11_20210202_pB_wv03</v>
       </c>
       <c r="J12" s="2"/>
       <c r="K12" s="2"/>
@@ -3933,9 +3933,9 @@
       <c r="H13" t="s">
         <v>131</v>
       </c>
-      <c r="I13" t="str">
-        <f t="shared" si="1"/>
-        <v>nl_wk12_20210212_pB_wv04</v>
+      <c r="I13" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>nl_sr12_20210212_pB_wv04</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.4">
@@ -3963,9 +3963,9 @@
       <c r="H14" t="s">
         <v>136</v>
       </c>
-      <c r="I14" t="str">
-        <f t="shared" si="1"/>
-        <v>nl_wk13_20210301_pB_wv05</v>
+      <c r="I14" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>nl_sr13_20210301_pB_wv05</v>
       </c>
     </row>
   </sheetData>
@@ -3978,7 +3978,7 @@
   <dimension ref="A1:O7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="I3" sqref="I3:I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.84375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -4061,8 +4061,8 @@
         <v>79</v>
       </c>
       <c r="I2" t="str">
-        <f t="shared" ref="I2:I7" si="0">C2&amp;"_"&amp;"wk"&amp;TEXT(D2,"00")&amp;"_"&amp;YEAR(G2)&amp;TEXT(G2,"MM")&amp;TEXT(G2,"DD")&amp;"_p"&amp;E2&amp;"_wv"&amp;TEXT(F2,"00")&amp;""</f>
-        <v>no_wk01_20200501_pA_wv01</v>
+        <f>C2&amp;"_"&amp;"sr"&amp;TEXT(D2,"00")&amp;"_"&amp;YEAR(G2)&amp;TEXT(G2,"MM")&amp;TEXT(G2,"DD")&amp;"_p"&amp;E2&amp;"_wv"&amp;TEXT(F2,"00")&amp;""</f>
+        <v>no_sr01_20200501_pA_wv01</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.4">
@@ -4090,9 +4090,9 @@
       <c r="H3" t="s">
         <v>74</v>
       </c>
-      <c r="I3" t="str">
-        <f t="shared" si="0"/>
-        <v>no_wk02_20200529_pA_wv02</v>
+      <c r="I3" s="2" t="str">
+        <f t="shared" ref="I3:I7" si="0">C3&amp;"_"&amp;"sr"&amp;TEXT(D3,"00")&amp;"_"&amp;YEAR(G3)&amp;TEXT(G3,"MM")&amp;TEXT(G3,"DD")&amp;"_p"&amp;E3&amp;"_wv"&amp;TEXT(F3,"00")&amp;""</f>
+        <v>no_sr02_20200529_pA_wv02</v>
       </c>
       <c r="K3">
         <v>1</v>
@@ -4123,9 +4123,9 @@
       <c r="H4" t="s">
         <v>80</v>
       </c>
-      <c r="I4" t="str">
-        <f t="shared" si="0"/>
-        <v>no_wk03_20200622_pA_wv03</v>
+      <c r="I4" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>no_sr03_20200622_pA_wv03</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.4">
@@ -4153,9 +4153,9 @@
       <c r="H5" t="s">
         <v>75</v>
       </c>
-      <c r="I5" t="str">
-        <f t="shared" si="0"/>
-        <v>no_wk04_20200731_pA_wv04</v>
+      <c r="I5" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>no_sr04_20200731_pA_wv04</v>
       </c>
       <c r="K5">
         <v>1</v>
@@ -4186,9 +4186,9 @@
       <c r="H6" t="s">
         <v>76</v>
       </c>
-      <c r="I6" t="str">
-        <f t="shared" si="0"/>
-        <v>no_wk05_20200906_pA_wv05</v>
+      <c r="I6" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>no_sr05_20200906_pA_wv05</v>
       </c>
       <c r="K6">
         <v>1</v>
@@ -4219,9 +4219,9 @@
       <c r="H7" t="s">
         <v>77</v>
       </c>
-      <c r="I7" t="str">
-        <f t="shared" si="0"/>
-        <v>no_wk06_20201001_pA_wv06</v>
+      <c r="I7" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>no_sr06_20201001_pA_wv06</v>
       </c>
       <c r="K7">
         <v>1</v>
@@ -4237,7 +4237,7 @@
   <dimension ref="A1:M27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="I3" sqref="I3:I27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.84375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -4315,8 +4315,8 @@
         <v>97</v>
       </c>
       <c r="I2" t="str">
-        <f>A2&amp;"_"&amp;"wk"&amp;TEXT(D2,"00")&amp;"_"&amp;YEAR(G3)&amp;TEXT(G3,"MM")&amp;TEXT(G3,"DD")&amp;"_p"&amp;E2&amp;"_wv"&amp;TEXT(F2,"00")&amp;""</f>
-        <v>at_wk01_20210111_pA_wv01</v>
+        <f>A2&amp;"_"&amp;"sr"&amp;TEXT(D2,"00")&amp;"_"&amp;YEAR(G3)&amp;TEXT(G3,"MM")&amp;TEXT(G3,"DD")&amp;"_p"&amp;E2&amp;"_wv"&amp;TEXT(F2,"00")&amp;""</f>
+        <v>at_sr01_20210111_pA_wv01</v>
       </c>
       <c r="J2">
         <v>1</v>
@@ -4347,9 +4347,9 @@
       <c r="H3" t="s">
         <v>105</v>
       </c>
-      <c r="I3" t="str">
-        <f t="shared" ref="I3:I27" si="0">A3&amp;"_"&amp;"wk"&amp;TEXT(D3,"00")&amp;"_"&amp;YEAR(G3)&amp;TEXT(G3,"MM")&amp;TEXT(G3,"DD")&amp;"_p"&amp;E3&amp;"_wv"&amp;TEXT(F3,"00")&amp;""</f>
-        <v>dk_wk01_20210111_pA_wv01</v>
+      <c r="I3" s="2" t="str">
+        <f t="shared" ref="I3:I27" si="0">A3&amp;"_"&amp;"sr"&amp;TEXT(D3,"00")&amp;"_"&amp;YEAR(G4)&amp;TEXT(G4,"MM")&amp;TEXT(G4,"DD")&amp;"_p"&amp;E3&amp;"_wv"&amp;TEXT(F3,"00")&amp;""</f>
+        <v>dk_sr01_20210111_pA_wv01</v>
       </c>
       <c r="J3">
         <v>1</v>
@@ -4380,9 +4380,9 @@
       <c r="H4" t="s">
         <v>106</v>
       </c>
-      <c r="I4" t="str">
-        <f t="shared" si="0"/>
-        <v>es_wk01_20210111_pA_wv01</v>
+      <c r="I4" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>es_sr01_20210111_pA_wv01</v>
       </c>
       <c r="J4">
         <v>1</v>
@@ -4413,9 +4413,9 @@
       <c r="H5" t="s">
         <v>107</v>
       </c>
-      <c r="I5" t="str">
-        <f t="shared" si="0"/>
-        <v>fr_wk01_20210111_pA_wv01</v>
+      <c r="I5" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>fr_sr01_20210111_pA_wv01</v>
       </c>
       <c r="J5">
         <v>1</v>
@@ -4446,9 +4446,9 @@
       <c r="H6" t="s">
         <v>108</v>
       </c>
-      <c r="I6" t="str">
-        <f t="shared" si="0"/>
-        <v>it_wk01_20210111_pA_wv01</v>
+      <c r="I6" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>it_sr01_20210111_pA_wv01</v>
       </c>
       <c r="J6">
         <v>1</v>
@@ -4479,9 +4479,9 @@
       <c r="H7" t="s">
         <v>109</v>
       </c>
-      <c r="I7" t="str">
-        <f t="shared" si="0"/>
-        <v>pl_wk01_20210111_pA_wv01</v>
+      <c r="I7" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>pl_sr01_20210111_pA_wv01</v>
       </c>
       <c r="J7">
         <v>1</v>
@@ -4512,9 +4512,9 @@
       <c r="H8" t="s">
         <v>110</v>
       </c>
-      <c r="I8" t="str">
-        <f t="shared" si="0"/>
-        <v>pt_wk01_20210111_pA_wv01</v>
+      <c r="I8" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>pt_sr01_20210118_pA_wv01</v>
       </c>
       <c r="J8">
         <v>1</v>
@@ -4545,9 +4545,9 @@
       <c r="H9" t="s">
         <v>112</v>
       </c>
-      <c r="I9" t="str">
-        <f t="shared" si="0"/>
-        <v>at_wk02_20210118_pA_wv02</v>
+      <c r="I9" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>at_sr02_20210118_pA_wv02</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.4">
@@ -4575,9 +4575,9 @@
       <c r="H10" t="s">
         <v>112</v>
       </c>
-      <c r="I10" t="str">
-        <f t="shared" si="0"/>
-        <v>dk_wk02_20210118_pA_wv02</v>
+      <c r="I10" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>dk_sr02_20210118_pA_wv02</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.4">
@@ -4605,9 +4605,9 @@
       <c r="H11" t="s">
         <v>112</v>
       </c>
-      <c r="I11" t="str">
-        <f t="shared" si="0"/>
-        <v>es_wk02_20210118_pA_wv02</v>
+      <c r="I11" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>es_sr02_20210118_pA_wv02</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.4">
@@ -4635,9 +4635,9 @@
       <c r="H12" t="s">
         <v>112</v>
       </c>
-      <c r="I12" t="str">
-        <f t="shared" si="0"/>
-        <v>fr_wk02_20210118_pA_wv02</v>
+      <c r="I12" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>fr_sr02_20210118_pA_wv02</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.4">
@@ -4665,9 +4665,9 @@
       <c r="H13" t="s">
         <v>112</v>
       </c>
-      <c r="I13" t="str">
-        <f t="shared" si="0"/>
-        <v>it_wk02_20210118_pA_wv02</v>
+      <c r="I13" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>it_sr02_20210118_pA_wv02</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.4">
@@ -4695,9 +4695,9 @@
       <c r="H14" t="s">
         <v>112</v>
       </c>
-      <c r="I14" t="str">
-        <f t="shared" si="0"/>
-        <v>pl_wk02_20210118_pA_wv02</v>
+      <c r="I14" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>pl_sr02_20210118_pA_wv02</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.4">
@@ -4725,9 +4725,9 @@
       <c r="H15" t="s">
         <v>112</v>
       </c>
-      <c r="I15" t="str">
-        <f t="shared" si="0"/>
-        <v>pt_wk02_20210118_pA_wv02</v>
+      <c r="I15" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>pt_sr02_20210129_pA_wv02</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.4">
@@ -4757,7 +4757,7 @@
       </c>
       <c r="I16" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>at_wk03_20210129_pA_wv03</v>
+        <v>at_sr03_20210129_pA_wv03</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.4">
@@ -4787,7 +4787,7 @@
       </c>
       <c r="I17" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>dk_wk03_20210129_pA_wv03</v>
+        <v>dk_sr03_20210129_pA_wv03</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.4">
@@ -4817,7 +4817,7 @@
       </c>
       <c r="I18" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>es_wk03_20210129_pA_wv03</v>
+        <v>es_sr03_20210129_pA_wv03</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.4">
@@ -4847,7 +4847,7 @@
       </c>
       <c r="I19" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>fr_wk03_20210129_pA_wv03</v>
+        <v>fr_sr03_20210129_pA_wv03</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.4">
@@ -4877,7 +4877,7 @@
       </c>
       <c r="I20" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>it_wk03_20210129_pA_wv03</v>
+        <v>it_sr03_20210129_pA_wv03</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.4">
@@ -4907,7 +4907,7 @@
       </c>
       <c r="I21" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>pl_wk03_20210129_pA_wv03</v>
+        <v>pl_sr03_20210129_pA_wv03</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.4">
@@ -4937,7 +4937,7 @@
       </c>
       <c r="I22" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>pt_wk03_20210129_pA_wv03</v>
+        <v>pt_sr03_20210111_pA_wv03</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.4">
@@ -4965,9 +4965,9 @@
       <c r="H23" s="4" t="s">
         <v>124</v>
       </c>
-      <c r="I23" s="4" t="str">
-        <f t="shared" si="0"/>
-        <v>at_wk01_20210111_pC_wv01</v>
+      <c r="I23" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>at_sr01_20210111_pC_wv01</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.4">
@@ -4995,9 +4995,9 @@
       <c r="H24" s="4" t="s">
         <v>124</v>
       </c>
-      <c r="I24" s="4" t="str">
-        <f t="shared" si="0"/>
-        <v>dk_wk01_20210111_pC_wv01</v>
+      <c r="I24" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>dk_sr01_20210111_pC_wv01</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.4">
@@ -5025,9 +5025,9 @@
       <c r="H25" s="4" t="s">
         <v>124</v>
       </c>
-      <c r="I25" s="4" t="str">
-        <f t="shared" si="0"/>
-        <v>fr_wk01_20210111_pC_wv01</v>
+      <c r="I25" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>fr_sr01_20210111_pC_wv01</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.4">
@@ -5055,9 +5055,9 @@
       <c r="H26" s="4" t="s">
         <v>124</v>
       </c>
-      <c r="I26" s="4" t="str">
-        <f t="shared" si="0"/>
-        <v>it_wk01_20210111_pC_wv01</v>
+      <c r="I26" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>it_sr01_20210111_pC_wv01</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.4">
@@ -5085,9 +5085,9 @@
       <c r="H27" s="4" t="s">
         <v>124</v>
       </c>
-      <c r="I27" s="4" t="str">
-        <f t="shared" si="0"/>
-        <v>pl_wk01_20210111_pC_wv01</v>
+      <c r="I27" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>pl_sr01_19000100_pC_wv01</v>
       </c>
     </row>
   </sheetData>
@@ -5099,8 +5099,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B44EFFA-AC3D-0445-9643-71A374D3D58F}">
   <dimension ref="A1:J8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I3" sqref="I3:I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -5175,8 +5175,8 @@
         <v>118</v>
       </c>
       <c r="I2" s="2" t="str">
-        <f>A2&amp;"_"&amp;"wk"&amp;TEXT(D2,"00")&amp;"_"&amp;YEAR(G3)&amp;TEXT(G3,"MM")&amp;TEXT(G3,"DD")&amp;"_p"&amp;E2&amp;"_wv"&amp;TEXT(F2,"00")&amp;""</f>
-        <v>lt_wk01_20210112_pA_wv01</v>
+        <f>A2&amp;"_"&amp;"sr"&amp;TEXT(D2,"00")&amp;"_"&amp;YEAR(G3)&amp;TEXT(G3,"MM")&amp;TEXT(G3,"DD")&amp;"_p"&amp;E2&amp;"_wv"&amp;TEXT(F2,"00")&amp;""</f>
+        <v>lt_sr01_20210112_pA_wv01</v>
       </c>
       <c r="J2" s="2"/>
     </row>
@@ -5206,8 +5206,8 @@
         <v>118</v>
       </c>
       <c r="I3" s="2" t="str">
-        <f t="shared" ref="I3:I4" si="0">A3&amp;"_"&amp;"wk"&amp;TEXT(D3,"00")&amp;"_"&amp;YEAR(G4)&amp;TEXT(G4,"MM")&amp;TEXT(G4,"DD")&amp;"_p"&amp;E3&amp;"_wv"&amp;TEXT(F3,"00")&amp;""</f>
-        <v>fi_wk01_20210113_pA_wv01</v>
+        <f t="shared" ref="I3:I8" si="0">A3&amp;"_"&amp;"sr"&amp;TEXT(D3,"00")&amp;"_"&amp;YEAR(G4)&amp;TEXT(G4,"MM")&amp;TEXT(G4,"DD")&amp;"_p"&amp;E3&amp;"_wv"&amp;TEXT(F3,"00")&amp;""</f>
+        <v>fi_sr01_20210113_pA_wv01</v>
       </c>
       <c r="J3" s="2"/>
     </row>
@@ -5238,7 +5238,7 @@
       </c>
       <c r="I4" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>ch_wk01_20210112_pA_wv01</v>
+        <v>ch_sr01_20210112_pA_wv01</v>
       </c>
       <c r="J4" s="2"/>
     </row>
@@ -5267,9 +5267,9 @@
       <c r="H5" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="I5" s="4" t="str">
-        <f t="shared" ref="I5:I7" si="1">A5&amp;"_"&amp;"wk"&amp;TEXT(D5,"00")&amp;"_"&amp;YEAR(G5)&amp;TEXT(G5,"MM")&amp;TEXT(G5,"DD")&amp;"_p"&amp;E5&amp;"_wv"&amp;TEXT(F5,"00")&amp;""</f>
-        <v>fi_wk01_20210112_pC_wv01</v>
+      <c r="I5" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>fi_sr01_20210113_pC_wv01</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.4">
@@ -5297,9 +5297,9 @@
       <c r="H6" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="I6" s="4" t="str">
-        <f t="shared" si="1"/>
-        <v>ch_wk01_20210113_pC_wv01</v>
+      <c r="I6" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>ch_sr01_20210113_pC_wv01</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.4">
@@ -5327,9 +5327,9 @@
       <c r="H7" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="I7" s="4" t="str">
-        <f t="shared" si="1"/>
-        <v>gr_wk01_20210113_pC_wv01</v>
+      <c r="I7" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>gr_sr01_20210111_pC_wv01</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.4">
@@ -5357,9 +5357,9 @@
       <c r="H8" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="I8" s="4" t="str">
-        <f>A8&amp;"_"&amp;"wk"&amp;TEXT(D8,"00")&amp;"_"&amp;YEAR(G8)&amp;TEXT(G8,"MM")&amp;TEXT(G8,"DD")&amp;"_p"&amp;E8&amp;"_wv"&amp;TEXT(F8,"00")&amp;""</f>
-        <v>lt_wk01_20210111_pC_wv01</v>
+      <c r="I8" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>lt_sr01_19000100_pC_wv01</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update to be survey_round not week
</commit_message>
<xml_diff>
--- a/data/spss_files.xlsx
+++ b/data/spss_files.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jarvisc1\Documents\projects\comix_data_clean\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E68AC4B-1435-4344-B387-8EF398144E00}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A31F296C-954C-41F9-85E3-17D7A7ABCF73}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18120" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18120" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="5" r:id="rId1"/>
@@ -860,8 +860,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O56"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3:I56"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.84375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -3494,7 +3494,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7709FE3-57B1-4766-A5D4-6B378E0A5BA3}">
   <dimension ref="A1:O14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="I3" sqref="I3:I14"/>
     </sheetView>
   </sheetViews>
@@ -3502,6 +3502,7 @@
   <cols>
     <col min="4" max="4" width="12.23046875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10.4609375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="53.921875" customWidth="1"/>
     <col min="14" max="14" width="9.4609375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>

<commit_message>
updates for v4 data cleaning
</commit_message>
<xml_diff>
--- a/data/spss_files.xlsx
+++ b/data/spss_files.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10111"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jarvisc1\Documents\projects\comix_data_clean\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/amygimma/lshtm/comix_data_clean/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A31F296C-954C-41F9-85E3-17D7A7ABCF73}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{029EF437-AF7F-264C-9D11-8A7DA18A824D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18120" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16640" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="5" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="460" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="498" uniqueCount="144">
   <si>
     <t>country</t>
   </si>
@@ -455,6 +455,24 @@
   </si>
   <si>
     <t>survey_round</t>
+  </si>
+  <si>
+    <t>20-030971_G2_Main_Wave2_Merged_FI LI CH_v1_04032021_IntClientUse</t>
+  </si>
+  <si>
+    <t>20-030971_G2_Main_Wave1_EL_v1_04032021_IntClientUse</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Note </t>
+  </si>
+  <si>
+    <t>Greece is 1 survey round behind other G2 countries</t>
+  </si>
+  <si>
+    <t>20-030971_G1_Merged_Wave4_Final_v1_26022021_IntClientUse</t>
+  </si>
+  <si>
+    <t>ES &amp; PT 1 round behind (no children's round yet)</t>
   </si>
 </sst>
 </file>
@@ -796,14 +814,14 @@
       <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.84375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>1</v>
       </c>
@@ -811,7 +829,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>2</v>
       </c>
@@ -819,7 +837,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>3</v>
       </c>
@@ -827,7 +845,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>4</v>
       </c>
@@ -835,7 +853,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>5</v>
       </c>
@@ -843,7 +861,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>6</v>
       </c>
@@ -864,17 +882,17 @@
       <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.84375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.3046875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.3046875" customWidth="1"/>
-    <col min="4" max="4" width="12.23046875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.69140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="58.3046875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="25.3046875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.33203125" customWidth="1"/>
+    <col min="4" max="4" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="58.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="25.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>82</v>
       </c>
@@ -921,7 +939,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -957,7 +975,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
@@ -993,7 +1011,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>1</v>
       </c>
@@ -1029,7 +1047,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>1</v>
       </c>
@@ -1065,7 +1083,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>1</v>
       </c>
@@ -1101,7 +1119,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>1</v>
       </c>
@@ -1137,7 +1155,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>1</v>
       </c>
@@ -1176,7 +1194,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>2</v>
       </c>
@@ -1212,7 +1230,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>1</v>
       </c>
@@ -1249,7 +1267,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>2</v>
       </c>
@@ -1286,7 +1304,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>1</v>
       </c>
@@ -1323,7 +1341,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>2</v>
       </c>
@@ -1361,7 +1379,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>1</v>
       </c>
@@ -1398,7 +1416,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>2</v>
       </c>
@@ -1435,7 +1453,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>1</v>
       </c>
@@ -1472,7 +1490,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>2</v>
       </c>
@@ -1509,7 +1527,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>1</v>
       </c>
@@ -1546,7 +1564,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>2</v>
       </c>
@@ -1583,7 +1601,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>1</v>
       </c>
@@ -1620,7 +1638,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>2</v>
       </c>
@@ -1657,7 +1675,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>1</v>
       </c>
@@ -1694,7 +1712,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>2</v>
       </c>
@@ -1731,7 +1749,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>1</v>
       </c>
@@ -1768,7 +1786,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>2</v>
       </c>
@@ -1805,7 +1823,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>1</v>
       </c>
@@ -1842,7 +1860,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>2</v>
       </c>
@@ -1879,7 +1897,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>1</v>
       </c>
@@ -1919,7 +1937,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>1</v>
       </c>
@@ -1959,7 +1977,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>1</v>
       </c>
@@ -1996,7 +2014,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>2</v>
       </c>
@@ -2032,7 +2050,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>3</v>
       </c>
@@ -2071,7 +2089,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>3</v>
       </c>
@@ -2107,7 +2125,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>3</v>
       </c>
@@ -2144,7 +2162,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>3</v>
       </c>
@@ -2181,7 +2199,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>3</v>
       </c>
@@ -2218,7 +2236,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>3</v>
       </c>
@@ -2255,7 +2273,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>3</v>
       </c>
@@ -2292,7 +2310,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>3</v>
       </c>
@@ -2329,7 +2347,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>3</v>
       </c>
@@ -2366,7 +2384,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>3</v>
       </c>
@@ -2403,7 +2421,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>3</v>
       </c>
@@ -2440,7 +2458,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>3</v>
       </c>
@@ -2477,7 +2495,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>3</v>
       </c>
@@ -2511,7 +2529,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>3</v>
       </c>
@@ -2548,7 +2566,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>3</v>
       </c>
@@ -2585,7 +2603,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>3</v>
       </c>
@@ -2622,7 +2640,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>3</v>
       </c>
@@ -2656,7 +2674,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>3</v>
       </c>
@@ -2690,7 +2708,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>3</v>
       </c>
@@ -2724,7 +2742,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>3</v>
       </c>
@@ -2758,7 +2776,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>3</v>
       </c>
@@ -2792,7 +2810,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>3</v>
       </c>
@@ -2826,7 +2844,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>3</v>
       </c>
@@ -2860,7 +2878,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A55" s="2">
         <v>3</v>
       </c>
@@ -2894,7 +2912,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A56" s="2">
         <v>3</v>
       </c>
@@ -2941,18 +2959,18 @@
       <selection activeCell="I3" sqref="I3:I17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.84375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="12.3046875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.3046875" customWidth="1"/>
-    <col min="4" max="4" width="12.23046875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.33203125" customWidth="1"/>
+    <col min="4" max="4" width="12.1640625" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.4609375" customWidth="1"/>
-    <col min="8" max="8" width="58.4609375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="30.4609375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.5" customWidth="1"/>
+    <col min="8" max="8" width="58.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="30.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2996,7 +3014,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>63</v>
       </c>
@@ -3029,7 +3047,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>63</v>
       </c>
@@ -3062,7 +3080,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>63</v>
       </c>
@@ -3095,7 +3113,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>63</v>
       </c>
@@ -3128,7 +3146,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>63</v>
       </c>
@@ -3161,7 +3179,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>63</v>
       </c>
@@ -3194,7 +3212,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>63</v>
       </c>
@@ -3227,7 +3245,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>63</v>
       </c>
@@ -3260,7 +3278,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>63</v>
       </c>
@@ -3286,7 +3304,7 @@
         <v>be_sr09_20201120_pB_wv01</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>63</v>
       </c>
@@ -3310,7 +3328,7 @@
         <v>be_sr10_19000100_pB_wv02</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>63</v>
       </c>
@@ -3334,7 +3352,7 @@
         <v>be_sr11_19000100_pB_wv03</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>63</v>
       </c>
@@ -3364,7 +3382,7 @@
         <v>be_sr12_20210111_pB_wv04</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>63</v>
       </c>
@@ -3394,7 +3412,7 @@
         <v>be_sr13_20210120_pB_wv05</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>63</v>
       </c>
@@ -3424,7 +3442,7 @@
         <v>be_sr14_20210127_pB_wv06</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>63</v>
       </c>
@@ -3454,7 +3472,7 @@
         <v>be_sr15_20210222_pB_wv07</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
         <v>63</v>
       </c>
@@ -3494,19 +3512,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7709FE3-57B1-4766-A5D4-6B378E0A5BA3}">
   <dimension ref="A1:O14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I3" sqref="I3:I14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.84375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="4" max="4" width="12.23046875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.4609375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="53.921875" customWidth="1"/>
-    <col min="14" max="14" width="9.4609375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="54" customWidth="1"/>
+    <col min="14" max="14" width="9.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>82</v>
       </c>
@@ -3553,7 +3571,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -3586,7 +3604,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
@@ -3619,7 +3637,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>1</v>
       </c>
@@ -3652,7 +3670,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>1</v>
       </c>
@@ -3685,7 +3703,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>1</v>
       </c>
@@ -3718,7 +3736,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>1</v>
       </c>
@@ -3751,7 +3769,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>1</v>
       </c>
@@ -3784,7 +3802,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>1</v>
       </c>
@@ -3817,7 +3835,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>6</v>
       </c>
@@ -3847,7 +3865,7 @@
         <v>nl_sr09_20210107_pB_wv01</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>6</v>
       </c>
@@ -3877,7 +3895,7 @@
         <v>nl_sr10_20210118_pB_wv02</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
         <v>6</v>
       </c>
@@ -3909,7 +3927,7 @@
       <c r="J12" s="2"/>
       <c r="K12" s="2"/>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
         <v>6</v>
       </c>
@@ -3939,7 +3957,7 @@
         <v>nl_sr12_20210212_pB_wv04</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>6</v>
       </c>
@@ -3982,14 +4000,14 @@
       <selection activeCell="I3" sqref="I3:I7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.84375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.3046875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.3046875" customWidth="1"/>
-    <col min="4" max="4" width="12.23046875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.33203125" customWidth="1"/>
+    <col min="4" max="4" width="12.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>82</v>
       </c>
@@ -4036,7 +4054,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -4066,7 +4084,7 @@
         <v>no_sr01_20200501_pA_wv01</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
@@ -4099,7 +4117,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>1</v>
       </c>
@@ -4129,7 +4147,7 @@
         <v>no_sr03_20200622_pA_wv03</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>1</v>
       </c>
@@ -4162,7 +4180,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>1</v>
       </c>
@@ -4195,7 +4213,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>1</v>
       </c>
@@ -4235,21 +4253,21 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9984DEBA-9A58-467F-869B-4E55580BB1A4}">
-  <dimension ref="A1:M27"/>
+  <dimension ref="A1:M34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I3" sqref="I3:I27"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.84375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="4" max="4" width="12.23046875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.69140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.6640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="59" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="27.3046875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="27.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4290,12 +4308,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>98</v>
       </c>
       <c r="B2">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -4319,16 +4337,13 @@
         <f>A2&amp;"_"&amp;"sr"&amp;TEXT(D2,"00")&amp;"_"&amp;YEAR(G3)&amp;TEXT(G3,"MM")&amp;TEXT(G3,"DD")&amp;"_p"&amp;E2&amp;"_wv"&amp;TEXT(F2,"00")&amp;""</f>
         <v>at_sr01_20210111_pA_wv01</v>
       </c>
-      <c r="J2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.4">
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>99</v>
       </c>
       <c r="B3">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C3">
         <v>0</v>
@@ -4349,14 +4364,11 @@
         <v>105</v>
       </c>
       <c r="I3" s="2" t="str">
-        <f t="shared" ref="I3:I27" si="0">A3&amp;"_"&amp;"sr"&amp;TEXT(D3,"00")&amp;"_"&amp;YEAR(G4)&amp;TEXT(G4,"MM")&amp;TEXT(G4,"DD")&amp;"_p"&amp;E3&amp;"_wv"&amp;TEXT(F3,"00")&amp;""</f>
+        <f t="shared" ref="I3:I34" si="0">A3&amp;"_"&amp;"sr"&amp;TEXT(D3,"00")&amp;"_"&amp;YEAR(G4)&amp;TEXT(G4,"MM")&amp;TEXT(G4,"DD")&amp;"_p"&amp;E3&amp;"_wv"&amp;TEXT(F3,"00")&amp;""</f>
         <v>dk_sr01_20210111_pA_wv01</v>
       </c>
-      <c r="J3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.4">
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>100</v>
       </c>
@@ -4385,11 +4397,8 @@
         <f t="shared" si="0"/>
         <v>es_sr01_20210111_pA_wv01</v>
       </c>
-      <c r="J4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.4">
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>101</v>
       </c>
@@ -4418,11 +4427,8 @@
         <f t="shared" si="0"/>
         <v>fr_sr01_20210111_pA_wv01</v>
       </c>
-      <c r="J5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.4">
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>102</v>
       </c>
@@ -4451,11 +4457,8 @@
         <f t="shared" si="0"/>
         <v>it_sr01_20210111_pA_wv01</v>
       </c>
-      <c r="J6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.4">
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>103</v>
       </c>
@@ -4484,11 +4487,8 @@
         <f t="shared" si="0"/>
         <v>pl_sr01_20210111_pA_wv01</v>
       </c>
-      <c r="J7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.4">
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>104</v>
       </c>
@@ -4517,11 +4517,8 @@
         <f t="shared" si="0"/>
         <v>pt_sr01_20210118_pA_wv01</v>
       </c>
-      <c r="J8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.4">
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>98</v>
       </c>
@@ -4551,7 +4548,7 @@
         <v>at_sr02_20210118_pA_wv02</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>99</v>
       </c>
@@ -4581,7 +4578,7 @@
         <v>dk_sr02_20210118_pA_wv02</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>100</v>
       </c>
@@ -4611,7 +4608,7 @@
         <v>es_sr02_20210118_pA_wv02</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>101</v>
       </c>
@@ -4641,7 +4638,7 @@
         <v>fr_sr02_20210118_pA_wv02</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>102</v>
       </c>
@@ -4671,7 +4668,7 @@
         <v>it_sr02_20210118_pA_wv02</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>103</v>
       </c>
@@ -4701,7 +4698,7 @@
         <v>pl_sr02_20210118_pA_wv02</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>104</v>
       </c>
@@ -4731,7 +4728,7 @@
         <v>pt_sr02_20210129_pA_wv02</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
         <v>98</v>
       </c>
@@ -4761,7 +4758,7 @@
         <v>at_sr03_20210129_pA_wv03</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
         <v>99</v>
       </c>
@@ -4791,7 +4788,7 @@
         <v>dk_sr03_20210129_pA_wv03</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
         <v>100</v>
       </c>
@@ -4821,7 +4818,7 @@
         <v>es_sr03_20210129_pA_wv03</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
         <v>101</v>
       </c>
@@ -4851,7 +4848,7 @@
         <v>fr_sr03_20210129_pA_wv03</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
         <v>102</v>
       </c>
@@ -4881,7 +4878,7 @@
         <v>it_sr03_20210129_pA_wv03</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
         <v>103</v>
       </c>
@@ -4911,7 +4908,7 @@
         <v>pl_sr03_20210129_pA_wv03</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
         <v>104</v>
       </c>
@@ -4941,7 +4938,7 @@
         <v>pt_sr03_20210111_pA_wv03</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" s="4" t="s">
         <v>98</v>
       </c>
@@ -4952,7 +4949,7 @@
         <v>0</v>
       </c>
       <c r="D23" s="4">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E23" s="4" t="s">
         <v>22</v>
@@ -4968,10 +4965,10 @@
       </c>
       <c r="I23" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>at_sr01_20210111_pC_wv01</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.4">
+        <v>at_sr04_20210111_pC_wv01</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" s="4" t="s">
         <v>99</v>
       </c>
@@ -4982,7 +4979,7 @@
         <v>0</v>
       </c>
       <c r="D24" s="4">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E24" s="4" t="s">
         <v>22</v>
@@ -4998,10 +4995,10 @@
       </c>
       <c r="I24" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>dk_sr01_20210111_pC_wv01</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.4">
+        <v>dk_sr04_20210111_pC_wv01</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" s="4" t="s">
         <v>101</v>
       </c>
@@ -5012,7 +5009,7 @@
         <v>0</v>
       </c>
       <c r="D25" s="4">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E25" s="4" t="s">
         <v>22</v>
@@ -5028,10 +5025,10 @@
       </c>
       <c r="I25" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>fr_sr01_20210111_pC_wv01</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.4">
+        <v>fr_sr04_20210111_pC_wv01</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" s="4" t="s">
         <v>102</v>
       </c>
@@ -5042,7 +5039,7 @@
         <v>0</v>
       </c>
       <c r="D26" s="4">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E26" s="4" t="s">
         <v>22</v>
@@ -5058,10 +5055,10 @@
       </c>
       <c r="I26" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>it_sr01_20210111_pC_wv01</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.4">
+        <v>it_sr04_20210111_pC_wv01</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" s="4" t="s">
         <v>103</v>
       </c>
@@ -5072,7 +5069,7 @@
         <v>0</v>
       </c>
       <c r="D27" s="4">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E27" s="4" t="s">
         <v>22</v>
@@ -5088,7 +5085,223 @@
       </c>
       <c r="I27" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>pl_sr01_19000100_pC_wv01</v>
+        <v>pl_sr04_20210226_pC_wv01</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A28" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="B28">
+        <v>4</v>
+      </c>
+      <c r="C28" s="4">
+        <v>0</v>
+      </c>
+      <c r="D28" s="2">
+        <v>5</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F28" s="4">
+        <v>4</v>
+      </c>
+      <c r="G28" s="3">
+        <v>44253</v>
+      </c>
+      <c r="H28" t="s">
+        <v>142</v>
+      </c>
+      <c r="I28" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>at_sr05_20210226_pA_wv04</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A29" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="B29">
+        <v>4</v>
+      </c>
+      <c r="C29" s="4">
+        <v>0</v>
+      </c>
+      <c r="D29" s="2">
+        <v>5</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F29" s="4">
+        <v>4</v>
+      </c>
+      <c r="G29" s="3">
+        <v>44253</v>
+      </c>
+      <c r="H29" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="I29" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>dk_sr05_20210226_pA_wv04</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A30" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="B30">
+        <v>4</v>
+      </c>
+      <c r="C30" s="4">
+        <v>0</v>
+      </c>
+      <c r="D30" s="2">
+        <v>5</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F30" s="4">
+        <v>4</v>
+      </c>
+      <c r="G30" s="3">
+        <v>44253</v>
+      </c>
+      <c r="H30" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="I30" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>fr_sr05_20210226_pA_wv04</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A31" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="B31">
+        <v>4</v>
+      </c>
+      <c r="C31" s="4">
+        <v>0</v>
+      </c>
+      <c r="D31" s="2">
+        <v>5</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F31" s="4">
+        <v>4</v>
+      </c>
+      <c r="G31" s="3">
+        <v>44253</v>
+      </c>
+      <c r="H31" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="I31" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>it_sr05_20210226_pA_wv04</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A32" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="B32">
+        <v>4</v>
+      </c>
+      <c r="C32" s="4">
+        <v>0</v>
+      </c>
+      <c r="D32" s="4">
+        <v>5</v>
+      </c>
+      <c r="E32" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F32" s="4">
+        <v>4</v>
+      </c>
+      <c r="G32" s="3">
+        <v>44253</v>
+      </c>
+      <c r="H32" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="I32" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>pl_sr05_20210226_pA_wv04</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A33" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="B33">
+        <v>4</v>
+      </c>
+      <c r="C33" s="2">
+        <v>0</v>
+      </c>
+      <c r="D33" s="2">
+        <v>4</v>
+      </c>
+      <c r="E33" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F33" s="4">
+        <v>4</v>
+      </c>
+      <c r="G33" s="3">
+        <v>44253</v>
+      </c>
+      <c r="H33" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="I33" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>es_sr04_20210226_pA_wv04</v>
+      </c>
+      <c r="J33" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A34" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="B34">
+        <v>4</v>
+      </c>
+      <c r="C34" s="2">
+        <v>0</v>
+      </c>
+      <c r="D34" s="2">
+        <v>4</v>
+      </c>
+      <c r="E34" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F34" s="4">
+        <v>4</v>
+      </c>
+      <c r="G34" s="3">
+        <v>44253</v>
+      </c>
+      <c r="H34" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="I34" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>pt_sr04_19000100_pA_wv04</v>
+      </c>
+      <c r="J34" s="2" t="s">
+        <v>143</v>
       </c>
     </row>
   </sheetData>
@@ -5098,27 +5311,27 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B44EFFA-AC3D-0445-9643-71A374D3D58F}">
-  <dimension ref="A1:J8"/>
+  <dimension ref="A1:K12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I3" sqref="I3:I8"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.4609375" customWidth="1"/>
-    <col min="2" max="2" width="16.69140625" customWidth="1"/>
-    <col min="3" max="3" width="8.69140625" customWidth="1"/>
-    <col min="4" max="4" width="12.23046875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.4609375" customWidth="1"/>
-    <col min="6" max="6" width="9.3046875" customWidth="1"/>
-    <col min="7" max="7" width="11.69140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="52.69140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="24.69140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="6.84375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.5" customWidth="1"/>
+    <col min="2" max="2" width="16.6640625" customWidth="1"/>
+    <col min="3" max="3" width="8.6640625" customWidth="1"/>
+    <col min="4" max="4" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.5" customWidth="1"/>
+    <col min="6" max="6" width="9.33203125" customWidth="1"/>
+    <col min="7" max="7" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="52.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="24.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="6.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -5149,8 +5362,11 @@
       <c r="J1" s="2" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="K1" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>119</v>
       </c>
@@ -5181,7 +5397,7 @@
       </c>
       <c r="J2" s="2"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>120</v>
       </c>
@@ -5207,12 +5423,12 @@
         <v>118</v>
       </c>
       <c r="I3" s="2" t="str">
-        <f t="shared" ref="I3:I8" si="0">A3&amp;"_"&amp;"sr"&amp;TEXT(D3,"00")&amp;"_"&amp;YEAR(G4)&amp;TEXT(G4,"MM")&amp;TEXT(G4,"DD")&amp;"_p"&amp;E3&amp;"_wv"&amp;TEXT(F3,"00")&amp;""</f>
+        <f t="shared" ref="I3:I12" si="0">A3&amp;"_"&amp;"sr"&amp;TEXT(D3,"00")&amp;"_"&amp;YEAR(G4)&amp;TEXT(G4,"MM")&amp;TEXT(G4,"DD")&amp;"_p"&amp;E3&amp;"_wv"&amp;TEXT(F3,"00")&amp;""</f>
         <v>fi_sr01_20210113_pA_wv01</v>
       </c>
       <c r="J3" s="2"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>121</v>
       </c>
@@ -5243,7 +5459,7 @@
       </c>
       <c r="J4" s="2"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>120</v>
       </c>
@@ -5254,7 +5470,7 @@
         <v>0</v>
       </c>
       <c r="D5" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E5" s="4" t="s">
         <v>22</v>
@@ -5270,10 +5486,10 @@
       </c>
       <c r="I5" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>fi_sr01_20210113_pC_wv01</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.4">
+        <v>fi_sr02_20210113_pC_wv01</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>121</v>
       </c>
@@ -5284,7 +5500,7 @@
         <v>0</v>
       </c>
       <c r="D6" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E6" s="4" t="s">
         <v>22</v>
@@ -5300,10 +5516,10 @@
       </c>
       <c r="I6" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>ch_sr01_20210113_pC_wv01</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.4">
+        <v>ch_sr02_20210113_pC_wv01</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>126</v>
       </c>
@@ -5332,8 +5548,11 @@
         <f t="shared" si="0"/>
         <v>gr_sr01_20210111_pC_wv01</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="K7" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>119</v>
       </c>
@@ -5344,7 +5563,7 @@
         <v>0</v>
       </c>
       <c r="D8" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E8" s="4" t="s">
         <v>22</v>
@@ -5360,7 +5579,130 @@
       </c>
       <c r="I8" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>lt_sr01_19000100_pC_wv01</v>
+        <v>lt_sr02_20210304_pC_wv01</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="B9" s="2">
+        <v>4</v>
+      </c>
+      <c r="C9" s="2">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>3</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F9">
+        <v>2</v>
+      </c>
+      <c r="G9" s="3">
+        <v>44259</v>
+      </c>
+      <c r="H9" t="s">
+        <v>138</v>
+      </c>
+      <c r="I9" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>lt_sr03_20210305_pA_wv02</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A10" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="B10" s="2">
+        <v>4</v>
+      </c>
+      <c r="C10" s="2">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>3</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F10">
+        <v>2</v>
+      </c>
+      <c r="G10" s="3">
+        <v>44260</v>
+      </c>
+      <c r="H10" t="s">
+        <v>138</v>
+      </c>
+      <c r="I10" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>fi_sr03_20210306_pA_wv02</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A11" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="B11" s="2">
+        <v>4</v>
+      </c>
+      <c r="C11" s="2">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>3</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F11">
+        <v>2</v>
+      </c>
+      <c r="G11" s="3">
+        <v>44261</v>
+      </c>
+      <c r="H11" t="s">
+        <v>138</v>
+      </c>
+      <c r="I11" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>ch_sr03_20210307_pA_wv02</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>126</v>
+      </c>
+      <c r="B12">
+        <v>4</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <v>2</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F12">
+        <v>1</v>
+      </c>
+      <c r="G12" s="3">
+        <v>44262</v>
+      </c>
+      <c r="H12" t="s">
+        <v>139</v>
+      </c>
+      <c r="I12" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>gr_sr02_19000100_pA_wv01</v>
+      </c>
+      <c r="K12" s="2" t="s">
+        <v>141</v>
       </c>
     </row>
   </sheetData>
@@ -5376,9 +5718,9 @@
       <selection activeCell="O21" sqref="O21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.84375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>114</v>
       </c>

</xml_diff>